<commit_message>
- finished data extraction from `10.1016/j.jmrt.2024.12.256`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE206828-8640-C54E-9F92-0C7A4581402D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DF877A-0E26-8343-93F1-F309097F03D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="4460" windowWidth="31020" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="5880" windowWidth="34240" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="99">
   <si>
     <r>
       <rPr>
@@ -324,10 +324,16 @@
     <t>hardness</t>
   </si>
   <si>
+    <t>T2</t>
+  </si>
+  <si>
     <t>BCC</t>
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>F7b</t>
   </si>
   <si>
     <t>tensile yield stress</t>
@@ -385,6 +391,42 @@
   </si>
   <si>
     <t>poissons ratio</t>
+  </si>
+  <si>
+    <t>Al0.3NbTi3VZr1.5</t>
+  </si>
+  <si>
+    <t>DED+T</t>
+  </si>
+  <si>
+    <t>AM DED followed by tempering at 873K for 2h to remove residual stress</t>
+  </si>
+  <si>
+    <t>AM DED followed by tempering at 873K for 2h to remove residual stress; homogenized at 1473K for 1h and quenched in water</t>
+  </si>
+  <si>
+    <t>DED+T+H+WQ</t>
+  </si>
+  <si>
+    <t>AM DED followed by tempering at 873K for 2h to remove residual stress; homogenized at 1473K for 1h and quenched in water; cold-rolled to 70% thickness reduction</t>
+  </si>
+  <si>
+    <t>DED+T+H+WQ+CR</t>
+  </si>
+  <si>
+    <t>DED+T+H+WQ+CR+AT</t>
+  </si>
+  <si>
+    <t>AM DED followed by tempering at 873K for 2h to remove residual stress; homogenized at 1473K for 1h and quenched in water; cold-rolled to 70% thickness reduction; aged at 573K for 7 days</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijplas.2024.104237</t>
+  </si>
+  <si>
+    <t>F7a</t>
+  </si>
+  <si>
+    <t>F9b</t>
   </si>
 </sst>
 </file>
@@ -2660,8 +2702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="86" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3019,16 +3061,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="54"/>
       <c r="B10" s="55" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F10" s="56" t="s">
         <v>63</v>
@@ -3040,35 +3082,49 @@
       <c r="I10" s="58">
         <v>298</v>
       </c>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="J10" s="59">
+        <f>P10*9807000</f>
+        <v>2765313472.485765</v>
+      </c>
+      <c r="K10" s="59">
+        <f>(Q10-R10)*9807000</f>
+        <v>101233548.38710338</v>
+      </c>
       <c r="L10" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="56"/>
+      <c r="M10" s="56" t="s">
+        <v>97</v>
+      </c>
       <c r="N10" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O10" s="9"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="9"/>
+      <c r="P10" s="4">
+        <v>281.97343453510399</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>284.70588235294099</v>
+      </c>
+      <c r="R10" s="4">
+        <v>274.38330170777903</v>
+      </c>
       <c r="S10" s="51"/>
       <c r="T10" s="51"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="54"/>
       <c r="B11" s="55" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F11" s="56" t="s">
         <v>63</v>
@@ -3080,35 +3136,49 @@
       <c r="I11" s="58">
         <v>298</v>
       </c>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
+      <c r="J11" s="59">
+        <f t="shared" ref="J11:J14" si="0">P11*9807000</f>
+        <v>2951404554.0796909</v>
+      </c>
+      <c r="K11" s="59">
+        <f t="shared" ref="K11:K14" si="1">(Q11-R11)*9807000</f>
+        <v>276903529.41176373</v>
+      </c>
       <c r="L11" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="56"/>
+      <c r="M11" s="56" t="s">
+        <v>97</v>
+      </c>
       <c r="N11" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O11" s="9"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="9"/>
+      <c r="P11" s="4">
+        <v>300.94876660341498</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>310.81593927893698</v>
+      </c>
+      <c r="R11" s="4">
+        <v>282.58064516129002</v>
+      </c>
       <c r="S11" s="9"/>
       <c r="T11" s="9"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="54"/>
       <c r="B12" s="55" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F12" s="56" t="s">
         <v>63</v>
@@ -3120,35 +3190,49 @@
       <c r="I12" s="58">
         <v>298</v>
       </c>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
+      <c r="J12" s="59">
+        <f t="shared" si="0"/>
+        <v>3323586717.2675428</v>
+      </c>
+      <c r="K12" s="59">
+        <f t="shared" si="1"/>
+        <v>208422011.38520369</v>
+      </c>
       <c r="L12" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="56"/>
+      <c r="M12" s="56" t="s">
+        <v>97</v>
+      </c>
       <c r="N12" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O12" s="9"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="9"/>
+      <c r="P12" s="4">
+        <v>338.89943074003702</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>346.48956356736198</v>
+      </c>
+      <c r="R12" s="4">
+        <v>325.23719165085299</v>
+      </c>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="54"/>
       <c r="B13" s="55" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>63</v>
@@ -3160,35 +3244,49 @@
       <c r="I13" s="58">
         <v>298</v>
       </c>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
+      <c r="J13" s="59">
+        <f t="shared" si="0"/>
+        <v>3472459582.5426855</v>
+      </c>
+      <c r="K13" s="59">
+        <f t="shared" si="1"/>
+        <v>165248880.45541432</v>
+      </c>
       <c r="L13" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="56"/>
+      <c r="M13" s="56" t="s">
+        <v>97</v>
+      </c>
       <c r="N13" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O13" s="9"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="9"/>
+      <c r="P13" s="4">
+        <v>354.07969639468598</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>364.09867172675501</v>
+      </c>
+      <c r="R13" s="4">
+        <v>347.24857685009403</v>
+      </c>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="54"/>
       <c r="B14" s="55" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F14" s="56" t="s">
         <v>63</v>
@@ -3200,38 +3298,52 @@
       <c r="I14" s="58">
         <v>298</v>
       </c>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
+      <c r="J14" s="59">
+        <f t="shared" si="0"/>
+        <v>3555828387.0967712</v>
+      </c>
+      <c r="K14" s="59">
+        <f t="shared" si="1"/>
+        <v>98256091.081590965</v>
+      </c>
       <c r="L14" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M14" s="56"/>
+      <c r="M14" s="56" t="s">
+        <v>97</v>
+      </c>
       <c r="N14" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O14" s="9"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="9"/>
+      <c r="P14" s="4">
+        <v>362.58064516129002</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>368.95635673624201</v>
+      </c>
+      <c r="R14" s="4">
+        <v>358.937381404174</v>
+      </c>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="54"/>
       <c r="B15" s="55" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G15" s="56" t="s">
         <v>29</v>
@@ -3240,14 +3352,18 @@
       <c r="I15" s="58">
         <v>298</v>
       </c>
-      <c r="J15" s="59"/>
+      <c r="J15" s="9">
+        <v>727045.07512520801</v>
+      </c>
       <c r="K15" s="59"/>
       <c r="L15" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M15" s="56"/>
+      <c r="M15" s="56" t="s">
+        <v>98</v>
+      </c>
       <c r="N15" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="4"/>
@@ -3259,19 +3375,19 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="54"/>
       <c r="B16" s="55" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G16" s="56" t="s">
         <v>29</v>
@@ -3280,14 +3396,18 @@
       <c r="I16" s="58">
         <v>298</v>
       </c>
-      <c r="J16" s="59"/>
+      <c r="J16" s="9">
+        <v>790651.08514190302</v>
+      </c>
       <c r="K16" s="4"/>
       <c r="L16" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="56"/>
+      <c r="M16" s="56" t="s">
+        <v>98</v>
+      </c>
       <c r="N16" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="4"/>
@@ -3299,19 +3419,19 @@
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="55" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G17" s="56" t="s">
         <v>29</v>
@@ -3320,14 +3440,18 @@
       <c r="I17" s="58">
         <v>298</v>
       </c>
-      <c r="J17" s="4"/>
+      <c r="J17" s="9">
+        <v>814190.31719532504</v>
+      </c>
       <c r="K17" s="4"/>
       <c r="L17" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="4"/>
+      <c r="M17" s="56" t="s">
+        <v>98</v>
+      </c>
       <c r="N17" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="4"/>
@@ -3339,19 +3463,19 @@
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="55" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G18" s="56" t="s">
         <v>29</v>
@@ -3360,14 +3484,18 @@
       <c r="I18" s="58">
         <v>298</v>
       </c>
-      <c r="J18" s="4"/>
+      <c r="J18" s="9">
+        <v>869282.13689482398</v>
+      </c>
       <c r="K18" s="4"/>
       <c r="L18" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="56" t="s">
+        <v>98</v>
+      </c>
       <c r="N18" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="4"/>
@@ -3379,19 +3507,19 @@
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="55" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G19" s="56" t="s">
         <v>29</v>
@@ -3400,14 +3528,18 @@
       <c r="I19" s="58">
         <v>298</v>
       </c>
-      <c r="J19" s="4"/>
+      <c r="J19" s="9">
+        <v>996994.99165275402</v>
+      </c>
       <c r="K19" s="4"/>
       <c r="L19" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="4"/>
+      <c r="M19" s="56" t="s">
+        <v>98</v>
+      </c>
       <c r="N19" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="4"/>
@@ -3419,19 +3551,19 @@
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="56" t="s">
         <v>70</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="56" t="s">
-        <v>68</v>
       </c>
       <c r="G20" s="56" t="s">
         <v>29</v>
@@ -3440,14 +3572,18 @@
       <c r="I20" s="58">
         <v>298</v>
       </c>
-      <c r="J20" s="4"/>
+      <c r="J20" s="9">
+        <v>872763.419483101</v>
+      </c>
       <c r="K20" s="4"/>
       <c r="L20" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="4"/>
+      <c r="M20" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N20" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="4"/>
@@ -3459,19 +3595,19 @@
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="55" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F21" s="56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G21" s="56" t="s">
         <v>29</v>
@@ -3480,14 +3616,18 @@
       <c r="I21" s="58">
         <v>298</v>
       </c>
-      <c r="J21" s="4"/>
+      <c r="J21" s="9">
+        <v>914115.30815109296</v>
+      </c>
       <c r="K21" s="4"/>
       <c r="L21" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M21" s="4"/>
+      <c r="M21" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N21" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="4"/>
@@ -3499,19 +3639,19 @@
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="55" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G22" s="56" t="s">
         <v>29</v>
@@ -3520,14 +3660,18 @@
       <c r="I22" s="58">
         <v>298</v>
       </c>
-      <c r="J22" s="4"/>
+      <c r="J22" s="9">
+        <v>958648.11133200699</v>
+      </c>
       <c r="K22" s="59"/>
       <c r="L22" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M22" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N22" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="4"/>
@@ -3539,19 +3683,19 @@
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="54"/>
       <c r="B23" s="55" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F23" s="56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G23" s="56" t="s">
         <v>29</v>
@@ -3560,14 +3704,18 @@
       <c r="I23" s="58">
         <v>298</v>
       </c>
-      <c r="J23" s="59"/>
+      <c r="J23" s="9">
+        <v>1023856.8588469099</v>
+      </c>
       <c r="K23" s="59"/>
       <c r="L23" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="56"/>
+      <c r="M23" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N23" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="4"/>
@@ -3579,19 +3727,19 @@
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="54"/>
       <c r="B24" s="55" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G24" s="56" t="s">
         <v>29</v>
@@ -3600,14 +3748,18 @@
       <c r="I24" s="58">
         <v>298</v>
       </c>
-      <c r="J24" s="59"/>
+      <c r="J24" s="9">
+        <v>1058846.9184890599</v>
+      </c>
       <c r="K24" s="59"/>
       <c r="L24" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M24" s="56"/>
+      <c r="M24" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N24" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O24" s="9"/>
       <c r="P24" s="4"/>
@@ -3619,19 +3771,19 @@
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="54"/>
       <c r="B25" s="115" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C25" s="116" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D25" s="116" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E25" s="117" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F25" s="56" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G25" s="56" t="s">
         <v>29</v>
@@ -3640,14 +3792,18 @@
       <c r="I25" s="58">
         <v>298</v>
       </c>
-      <c r="J25" s="59"/>
+      <c r="J25" s="9">
+        <v>26.924686192468599</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="M25" s="56"/>
+        <v>66</v>
+      </c>
+      <c r="M25" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N25" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O25" s="9"/>
       <c r="P25" s="4"/>
@@ -3659,19 +3815,19 @@
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="54"/>
       <c r="B26" s="118" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C26" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" s="119" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E26" s="120" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G26" s="56" t="s">
         <v>29</v>
@@ -3680,14 +3836,18 @@
       <c r="I26" s="58">
         <v>298</v>
       </c>
-      <c r="J26" s="4"/>
+      <c r="J26" s="9">
+        <v>20.9832635983263</v>
+      </c>
       <c r="K26" s="4"/>
       <c r="L26" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="M26" s="56"/>
+        <v>66</v>
+      </c>
+      <c r="M26" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N26" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="61"/>
@@ -3699,19 +3859,19 @@
     <row r="27" spans="1:20" ht="18.75" customHeight="1">
       <c r="A27" s="54"/>
       <c r="B27" s="118" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C27" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D27" s="119" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E27" s="120" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F27" s="56" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G27" s="56" t="s">
         <v>29</v>
@@ -3720,14 +3880,18 @@
       <c r="I27" s="58">
         <v>298</v>
       </c>
-      <c r="J27" s="4"/>
+      <c r="J27" s="9">
+        <v>19.449093444909298</v>
+      </c>
       <c r="K27" s="4"/>
       <c r="L27" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="M27" s="56"/>
+        <v>66</v>
+      </c>
+      <c r="M27" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N27" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O27" s="9"/>
       <c r="P27" s="61"/>
@@ -3739,19 +3903,19 @@
     <row r="28" spans="1:20" ht="18.75" customHeight="1">
       <c r="A28" s="54"/>
       <c r="B28" s="118" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C28" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D28" s="119" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E28" s="120" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F28" s="56" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G28" s="56" t="s">
         <v>29</v>
@@ -3760,14 +3924,18 @@
       <c r="I28" s="58">
         <v>298</v>
       </c>
-      <c r="J28" s="4"/>
+      <c r="J28" s="9">
+        <v>18.891213389121301</v>
+      </c>
       <c r="K28" s="4"/>
       <c r="L28" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="M28" s="56"/>
+        <v>66</v>
+      </c>
+      <c r="M28" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N28" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O28" s="9"/>
       <c r="P28" s="61"/>
@@ -3779,19 +3947,19 @@
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
       <c r="A29" s="54"/>
       <c r="B29" s="118" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C29" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" s="119" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E29" s="120" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F29" s="56" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G29" s="56" t="s">
         <v>29</v>
@@ -3800,14 +3968,18 @@
       <c r="I29" s="58">
         <v>298</v>
       </c>
-      <c r="J29" s="4"/>
+      <c r="J29" s="9">
+        <v>14.288702928870199</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="M29" s="56"/>
+        <v>66</v>
+      </c>
+      <c r="M29" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="N29" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O29" s="9"/>
       <c r="P29" s="61"/>
@@ -3819,23 +3991,23 @@
     <row r="30" spans="1:20" ht="18.75" customHeight="1">
       <c r="A30" s="54"/>
       <c r="B30" s="115" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" s="116" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D30" s="54"/>
       <c r="E30" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F30" s="56" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G30" s="56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H30" s="77" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="1">
@@ -3843,9 +4015,11 @@
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
+      <c r="M30" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N30" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O30" s="9"/>
       <c r="P30" s="61"/>
@@ -3857,23 +4031,23 @@
     <row r="31" spans="1:20" ht="18.75" customHeight="1">
       <c r="A31" s="54"/>
       <c r="B31" s="118" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C31" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D31" s="54"/>
       <c r="E31" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F31" s="56" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G31" s="56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H31" s="77" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="1">
@@ -3881,9 +4055,11 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
+      <c r="M31" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N31" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O31" s="9"/>
       <c r="P31" s="61"/>
@@ -3895,23 +4071,23 @@
     <row r="32" spans="1:20" ht="18.75" customHeight="1">
       <c r="A32" s="54"/>
       <c r="B32" s="118" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C32" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F32" s="56" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G32" s="56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H32" s="77" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="1">
@@ -3919,9 +4095,11 @@
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
+      <c r="M32" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N32" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O32" s="9"/>
       <c r="P32" s="61"/>
@@ -3933,23 +4111,23 @@
     <row r="33" spans="1:20" ht="18.75" customHeight="1">
       <c r="A33" s="54"/>
       <c r="B33" s="118" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C33" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F33" s="56" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G33" s="56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H33" s="77" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="1">
@@ -3957,9 +4135,11 @@
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
+      <c r="M33" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N33" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="61"/>
@@ -3971,23 +4151,23 @@
     <row r="34" spans="1:20" ht="18.75" customHeight="1">
       <c r="A34" s="54"/>
       <c r="B34" s="118" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C34" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D34" s="54"/>
       <c r="E34" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F34" s="56" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G34" s="56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H34" s="77" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="1">
@@ -3995,9 +4175,11 @@
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
+      <c r="M34" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N34" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O34" s="9"/>
       <c r="P34" s="4"/>
@@ -4009,23 +4191,23 @@
     <row r="35" spans="1:20" ht="18.75" customHeight="1">
       <c r="A35" s="54"/>
       <c r="B35" s="115" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C35" s="116" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D35" s="54"/>
       <c r="E35" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F35" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H35" s="77" t="s">
         <v>84</v>
-      </c>
-      <c r="G35" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="H35" s="77" t="s">
-        <v>82</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4">
@@ -4033,9 +4215,11 @@
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
+      <c r="M35" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N35" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O35" s="9"/>
       <c r="P35" s="4"/>
@@ -4047,23 +4231,23 @@
     <row r="36" spans="1:20" ht="18.75" customHeight="1">
       <c r="A36" s="54"/>
       <c r="B36" s="118" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C36" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D36" s="54"/>
       <c r="E36" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F36" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H36" s="77" t="s">
         <v>84</v>
-      </c>
-      <c r="G36" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="H36" s="77" t="s">
-        <v>82</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4">
@@ -4071,9 +4255,11 @@
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="56"/>
-      <c r="M36" s="56"/>
+      <c r="M36" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N36" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="4"/>
@@ -4085,23 +4271,23 @@
     <row r="37" spans="1:20" ht="18.75" customHeight="1">
       <c r="A37" s="54"/>
       <c r="B37" s="118" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C37" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D37" s="54"/>
       <c r="E37" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F37" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H37" s="77" t="s">
         <v>84</v>
-      </c>
-      <c r="G37" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="H37" s="77" t="s">
-        <v>82</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4">
@@ -4109,9 +4295,11 @@
       </c>
       <c r="K37" s="59"/>
       <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
+      <c r="M37" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N37" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O37" s="9"/>
       <c r="P37" s="4"/>
@@ -4123,23 +4311,23 @@
     <row r="38" spans="1:20" ht="18.75" customHeight="1">
       <c r="A38" s="54"/>
       <c r="B38" s="118" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C38" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D38" s="54"/>
       <c r="E38" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F38" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H38" s="77" t="s">
         <v>84</v>
-      </c>
-      <c r="G38" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="H38" s="77" t="s">
-        <v>82</v>
       </c>
       <c r="I38" s="58"/>
       <c r="J38" s="4">
@@ -4147,9 +4335,11 @@
       </c>
       <c r="K38" s="59"/>
       <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
+      <c r="M38" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N38" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O38" s="63"/>
       <c r="P38" s="64"/>
@@ -4161,23 +4351,23 @@
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
       <c r="A39" s="54"/>
       <c r="B39" s="118" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C39" s="119" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D39" s="54"/>
       <c r="E39" s="55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F39" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="77" t="s">
         <v>84</v>
-      </c>
-      <c r="G39" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="H39" s="77" t="s">
-        <v>82</v>
       </c>
       <c r="I39" s="58"/>
       <c r="J39" s="4">
@@ -4185,9 +4375,11 @@
       </c>
       <c r="K39" s="59"/>
       <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
+      <c r="M39" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="N39" s="60" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O39" s="63"/>
       <c r="P39" s="64"/>
@@ -4198,10 +4390,16 @@
     </row>
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
       <c r="A40" s="54"/>
-      <c r="B40" s="55"/>
+      <c r="B40" s="55" t="s">
+        <v>87</v>
+      </c>
       <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="55"/>
+      <c r="D40" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="55" t="s">
+        <v>89</v>
+      </c>
       <c r="F40" s="56"/>
       <c r="G40" s="56"/>
       <c r="H40" s="77"/>
@@ -4210,7 +4408,9 @@
       <c r="K40" s="59"/>
       <c r="L40" s="56"/>
       <c r="M40" s="56"/>
-      <c r="N40" s="54"/>
+      <c r="N40" s="54" t="s">
+        <v>96</v>
+      </c>
       <c r="O40" s="63"/>
       <c r="P40" s="64"/>
       <c r="Q40" s="64"/>
@@ -4220,10 +4420,16 @@
     </row>
     <row r="41" spans="1:20" ht="18.75" customHeight="1">
       <c r="A41" s="54"/>
-      <c r="B41" s="55"/>
+      <c r="B41" s="55" t="s">
+        <v>87</v>
+      </c>
       <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="55"/>
+      <c r="D41" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="55" t="s">
+        <v>90</v>
+      </c>
       <c r="F41" s="56"/>
       <c r="G41" s="56"/>
       <c r="H41" s="57"/>
@@ -4242,10 +4448,16 @@
     </row>
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
       <c r="A42" s="54"/>
-      <c r="B42" s="55"/>
+      <c r="B42" s="55" t="s">
+        <v>87</v>
+      </c>
       <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="55"/>
+      <c r="D42" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="55" t="s">
+        <v>92</v>
+      </c>
       <c r="F42" s="65"/>
       <c r="G42" s="56"/>
       <c r="H42" s="57"/>
@@ -4264,10 +4476,16 @@
     </row>
     <row r="43" spans="1:20" ht="18" customHeight="1">
       <c r="A43" s="54"/>
-      <c r="B43" s="55"/>
+      <c r="B43" s="55" t="s">
+        <v>87</v>
+      </c>
       <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="55"/>
+      <c r="D43" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="55" t="s">
+        <v>95</v>
+      </c>
       <c r="F43" s="65"/>
       <c r="G43" s="56"/>
       <c r="H43" s="57"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.ijplas.2024.104237`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DF877A-0E26-8343-93F1-F309097F03D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067F420F-4B5D-BE4B-BE08-EABF0B19953F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="5880" windowWidth="34240" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="107">
   <si>
     <r>
       <rPr>
@@ -324,6 +324,9 @@
     <t>hardness</t>
   </si>
   <si>
+    <t>nanohardness</t>
+  </si>
+  <si>
     <t>T2</t>
   </si>
   <si>
@@ -396,12 +399,6 @@
     <t>Al0.3NbTi3VZr1.5</t>
   </si>
   <si>
-    <t>DED+T</t>
-  </si>
-  <si>
-    <t>AM DED followed by tempering at 873K for 2h to remove residual stress</t>
-  </si>
-  <si>
     <t>AM DED followed by tempering at 873K for 2h to remove residual stress; homogenized at 1473K for 1h and quenched in water</t>
   </si>
   <si>
@@ -414,12 +411,6 @@
     <t>DED+T+H+WQ+CR</t>
   </si>
   <si>
-    <t>DED+T+H+WQ+CR+AT</t>
-  </si>
-  <si>
-    <t>AM DED followed by tempering at 873K for 2h to remove residual stress; homogenized at 1473K for 1h and quenched in water; cold-rolled to 70% thickness reduction; aged at 573K for 7 days</t>
-  </si>
-  <si>
     <t>10.1016/j.ijplas.2024.104237</t>
   </si>
   <si>
@@ -427,6 +418,39 @@
   </si>
   <si>
     <t>F9b</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>AM DED followed by tempering at 873K for 2h to remove residual stress; homogenized at 1473K for 1h and quenched in water; cold-rolled to 70% thickness reduction; recrystallized at 1173K for 1h and quenched</t>
+  </si>
+  <si>
+    <t>DED+T+H+WQ+CR+RX+WQ</t>
+  </si>
+  <si>
+    <t>DED+T+H+WQ+CR+RX+WQ+AT</t>
+  </si>
+  <si>
+    <t>AM DED followed by tempering at 873K for 2h to remove residual stress; homogenized at 1473K for 1h and quenched in water; cold-rolled to 70% thickness reduction; recrystallized at 1173K for 1h and quenched; aged at 573K for 7 days</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>BCC+C14</t>
+  </si>
+  <si>
+    <t>F6b</t>
+  </si>
+  <si>
+    <t>F7c</t>
   </si>
 </sst>
 </file>
@@ -2702,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T859"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="86" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3061,16 +3085,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="54"/>
       <c r="B10" s="55" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F10" s="56" t="s">
         <v>63</v>
@@ -3094,10 +3118,10 @@
         <v>33</v>
       </c>
       <c r="M10" s="56" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N10" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="4">
@@ -3115,16 +3139,16 @@
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="54"/>
       <c r="B11" s="55" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F11" s="56" t="s">
         <v>63</v>
@@ -3148,10 +3172,10 @@
         <v>33</v>
       </c>
       <c r="M11" s="56" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N11" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="4">
@@ -3169,16 +3193,16 @@
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="54"/>
       <c r="B12" s="55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F12" s="56" t="s">
         <v>63</v>
@@ -3202,10 +3226,10 @@
         <v>33</v>
       </c>
       <c r="M12" s="56" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N12" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="4">
@@ -3223,16 +3247,16 @@
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="54"/>
       <c r="B13" s="55" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>63</v>
@@ -3256,10 +3280,10 @@
         <v>33</v>
       </c>
       <c r="M13" s="56" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N13" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="4">
@@ -3277,16 +3301,16 @@
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="54"/>
       <c r="B14" s="55" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F14" s="56" t="s">
         <v>63</v>
@@ -3310,10 +3334,10 @@
         <v>33</v>
       </c>
       <c r="M14" s="56" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N14" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="4">
@@ -3331,19 +3355,19 @@
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="54"/>
       <c r="B15" s="55" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G15" s="56" t="s">
         <v>29</v>
@@ -3360,10 +3384,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N15" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="4"/>
@@ -3375,19 +3399,19 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="54"/>
       <c r="B16" s="55" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G16" s="56" t="s">
         <v>29</v>
@@ -3404,10 +3428,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N16" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="4"/>
@@ -3419,19 +3443,19 @@
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G17" s="56" t="s">
         <v>29</v>
@@ -3448,10 +3472,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N17" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="4"/>
@@ -3463,19 +3487,19 @@
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="55" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G18" s="56" t="s">
         <v>29</v>
@@ -3492,10 +3516,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N18" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="4"/>
@@ -3507,19 +3531,19 @@
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="55" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G19" s="56" t="s">
         <v>29</v>
@@ -3536,10 +3560,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N19" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="4"/>
@@ -3551,19 +3575,19 @@
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="55" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G20" s="56" t="s">
         <v>29</v>
@@ -3580,10 +3604,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N20" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="4"/>
@@ -3595,19 +3619,19 @@
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="55" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G21" s="56" t="s">
         <v>29</v>
@@ -3624,10 +3648,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N21" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="4"/>
@@ -3639,19 +3663,19 @@
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G22" s="56" t="s">
         <v>29</v>
@@ -3668,10 +3692,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N22" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="4"/>
@@ -3683,19 +3707,19 @@
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="54"/>
       <c r="B23" s="55" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F23" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G23" s="56" t="s">
         <v>29</v>
@@ -3712,10 +3736,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N23" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="4"/>
@@ -3727,19 +3751,19 @@
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="54"/>
       <c r="B24" s="55" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G24" s="56" t="s">
         <v>29</v>
@@ -3756,10 +3780,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N24" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O24" s="9"/>
       <c r="P24" s="4"/>
@@ -3771,19 +3795,19 @@
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="54"/>
       <c r="B25" s="115" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" s="116" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D25" s="116" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E25" s="117" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F25" s="56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G25" s="56" t="s">
         <v>29</v>
@@ -3797,13 +3821,13 @@
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M25" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N25" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O25" s="9"/>
       <c r="P25" s="4"/>
@@ -3815,19 +3839,19 @@
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="54"/>
       <c r="B26" s="118" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D26" s="119" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E26" s="120" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G26" s="56" t="s">
         <v>29</v>
@@ -3841,13 +3865,13 @@
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M26" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N26" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="61"/>
@@ -3859,19 +3883,19 @@
     <row r="27" spans="1:20" ht="18.75" customHeight="1">
       <c r="A27" s="54"/>
       <c r="B27" s="118" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C27" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D27" s="119" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E27" s="120" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F27" s="56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G27" s="56" t="s">
         <v>29</v>
@@ -3885,13 +3909,13 @@
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M27" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N27" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O27" s="9"/>
       <c r="P27" s="61"/>
@@ -3903,19 +3927,19 @@
     <row r="28" spans="1:20" ht="18.75" customHeight="1">
       <c r="A28" s="54"/>
       <c r="B28" s="118" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C28" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D28" s="119" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E28" s="120" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F28" s="56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G28" s="56" t="s">
         <v>29</v>
@@ -3929,13 +3953,13 @@
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M28" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N28" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O28" s="9"/>
       <c r="P28" s="61"/>
@@ -3947,19 +3971,19 @@
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
       <c r="A29" s="54"/>
       <c r="B29" s="118" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C29" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D29" s="119" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E29" s="120" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F29" s="56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G29" s="56" t="s">
         <v>29</v>
@@ -3973,13 +3997,13 @@
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M29" s="77" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N29" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O29" s="9"/>
       <c r="P29" s="61"/>
@@ -3991,23 +4015,23 @@
     <row r="30" spans="1:20" ht="18.75" customHeight="1">
       <c r="A30" s="54"/>
       <c r="B30" s="115" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C30" s="116" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="54"/>
       <c r="E30" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F30" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="G30" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H30" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="1">
@@ -4016,10 +4040,10 @@
       <c r="K30" s="4"/>
       <c r="L30" s="56"/>
       <c r="M30" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N30" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O30" s="9"/>
       <c r="P30" s="61"/>
@@ -4031,23 +4055,23 @@
     <row r="31" spans="1:20" ht="18.75" customHeight="1">
       <c r="A31" s="54"/>
       <c r="B31" s="118" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C31" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D31" s="54"/>
       <c r="E31" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F31" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="G31" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H31" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="1">
@@ -4056,10 +4080,10 @@
       <c r="K31" s="4"/>
       <c r="L31" s="56"/>
       <c r="M31" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N31" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O31" s="9"/>
       <c r="P31" s="61"/>
@@ -4071,23 +4095,23 @@
     <row r="32" spans="1:20" ht="18.75" customHeight="1">
       <c r="A32" s="54"/>
       <c r="B32" s="118" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C32" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F32" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="G32" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H32" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="1">
@@ -4096,10 +4120,10 @@
       <c r="K32" s="4"/>
       <c r="L32" s="56"/>
       <c r="M32" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N32" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O32" s="9"/>
       <c r="P32" s="61"/>
@@ -4111,23 +4135,23 @@
     <row r="33" spans="1:20" ht="18.75" customHeight="1">
       <c r="A33" s="54"/>
       <c r="B33" s="118" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C33" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F33" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="G33" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H33" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="1">
@@ -4136,10 +4160,10 @@
       <c r="K33" s="4"/>
       <c r="L33" s="56"/>
       <c r="M33" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N33" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="61"/>
@@ -4151,23 +4175,23 @@
     <row r="34" spans="1:20" ht="18.75" customHeight="1">
       <c r="A34" s="54"/>
       <c r="B34" s="118" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C34" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D34" s="54"/>
       <c r="E34" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F34" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="G34" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H34" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="1">
@@ -4176,10 +4200,10 @@
       <c r="K34" s="4"/>
       <c r="L34" s="56"/>
       <c r="M34" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N34" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O34" s="9"/>
       <c r="P34" s="4"/>
@@ -4191,23 +4215,23 @@
     <row r="35" spans="1:20" ht="18.75" customHeight="1">
       <c r="A35" s="54"/>
       <c r="B35" s="115" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C35" s="116" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D35" s="54"/>
       <c r="E35" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F35" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H35" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4">
@@ -4216,10 +4240,10 @@
       <c r="K35" s="4"/>
       <c r="L35" s="56"/>
       <c r="M35" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N35" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O35" s="9"/>
       <c r="P35" s="4"/>
@@ -4231,23 +4255,23 @@
     <row r="36" spans="1:20" ht="18.75" customHeight="1">
       <c r="A36" s="54"/>
       <c r="B36" s="118" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C36" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D36" s="54"/>
       <c r="E36" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F36" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H36" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4">
@@ -4256,10 +4280,10 @@
       <c r="K36" s="4"/>
       <c r="L36" s="56"/>
       <c r="M36" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N36" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="4"/>
@@ -4271,23 +4295,23 @@
     <row r="37" spans="1:20" ht="18.75" customHeight="1">
       <c r="A37" s="54"/>
       <c r="B37" s="118" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C37" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D37" s="54"/>
       <c r="E37" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F37" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="G37" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4">
@@ -4296,10 +4320,10 @@
       <c r="K37" s="59"/>
       <c r="L37" s="56"/>
       <c r="M37" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N37" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O37" s="9"/>
       <c r="P37" s="4"/>
@@ -4311,23 +4335,23 @@
     <row r="38" spans="1:20" ht="18.75" customHeight="1">
       <c r="A38" s="54"/>
       <c r="B38" s="118" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C38" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D38" s="54"/>
       <c r="E38" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G38" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H38" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F38" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="G38" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H38" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I38" s="58"/>
       <c r="J38" s="4">
@@ -4336,10 +4360,10 @@
       <c r="K38" s="59"/>
       <c r="L38" s="56"/>
       <c r="M38" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N38" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O38" s="63"/>
       <c r="P38" s="64"/>
@@ -4351,23 +4375,23 @@
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
       <c r="A39" s="54"/>
       <c r="B39" s="118" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C39" s="119" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D39" s="54"/>
       <c r="E39" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H39" s="77" t="s">
         <v>85</v>
-      </c>
-      <c r="F39" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="G39" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H39" s="77" t="s">
-        <v>84</v>
       </c>
       <c r="I39" s="58"/>
       <c r="J39" s="4">
@@ -4376,10 +4400,10 @@
       <c r="K39" s="59"/>
       <c r="L39" s="56"/>
       <c r="M39" s="56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N39" s="60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O39" s="63"/>
       <c r="P39" s="64"/>
@@ -4389,134 +4413,248 @@
       <c r="T39" s="9"/>
     </row>
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A40" s="54"/>
+      <c r="A40" s="54" t="s">
+        <v>96</v>
+      </c>
       <c r="B40" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="54"/>
+        <v>88</v>
+      </c>
+      <c r="C40" s="54" t="s">
+        <v>66</v>
+      </c>
       <c r="D40" s="54" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E40" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
+      <c r="F40" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="57"/>
+      <c r="I40" s="58">
+        <v>298</v>
+      </c>
+      <c r="J40" s="63">
+        <v>4137236084.45297</v>
+      </c>
+      <c r="K40" s="67">
+        <f>Q40-J40</f>
+        <v>119001919.38579988</v>
+      </c>
+      <c r="L40" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M40" s="56" t="s">
+        <v>105</v>
+      </c>
       <c r="N40" s="54" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O40" s="63"/>
       <c r="P40" s="64"/>
-      <c r="Q40" s="64"/>
+      <c r="Q40" s="63">
+        <v>4256238003.8387699</v>
+      </c>
       <c r="R40" s="63"/>
       <c r="S40" s="9"/>
       <c r="T40" s="9"/>
     </row>
     <row r="41" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A41" s="54"/>
+      <c r="A41" s="54" t="s">
+        <v>97</v>
+      </c>
       <c r="B41" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="54"/>
+        <v>88</v>
+      </c>
+      <c r="C41" s="54" t="s">
+        <v>66</v>
+      </c>
       <c r="D41" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="55" t="s">
-        <v>90</v>
-      </c>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
+      <c r="F41" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H41" s="57"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="59"/>
-      <c r="K41" s="67"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="54"/>
+      <c r="I41" s="58">
+        <v>298</v>
+      </c>
+      <c r="J41" s="63">
+        <v>5223608445.2974997</v>
+      </c>
+      <c r="K41" s="67">
+        <f t="shared" ref="K41:K43" si="2">Q41-J41</f>
+        <v>322456813.81958008</v>
+      </c>
+      <c r="L41" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M41" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="N41" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O41" s="63"/>
       <c r="P41" s="64"/>
-      <c r="Q41" s="64"/>
+      <c r="Q41" s="63">
+        <v>5546065259.1170797</v>
+      </c>
       <c r="R41" s="63"/>
       <c r="S41" s="9"/>
       <c r="T41" s="9"/>
     </row>
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A42" s="54"/>
+      <c r="A42" s="54" t="s">
+        <v>102</v>
+      </c>
       <c r="B42" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="54"/>
+        <v>88</v>
+      </c>
+      <c r="C42" s="54" t="s">
+        <v>104</v>
+      </c>
       <c r="D42" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F42" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="57"/>
+      <c r="I42" s="58">
+        <v>298</v>
+      </c>
+      <c r="J42" s="63">
+        <v>4283109404.9903998</v>
+      </c>
+      <c r="K42" s="67">
+        <f t="shared" si="2"/>
+        <v>218809980.80614042</v>
+      </c>
+      <c r="L42" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M42" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="N42" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="F42" s="65"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="57"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="54"/>
       <c r="O42" s="63"/>
       <c r="P42" s="67"/>
-      <c r="Q42" s="64"/>
+      <c r="Q42" s="63">
+        <v>4501919385.7965403</v>
+      </c>
       <c r="R42" s="63"/>
       <c r="S42" s="9"/>
       <c r="T42" s="9"/>
     </row>
     <row r="43" spans="1:20" ht="18" customHeight="1">
-      <c r="A43" s="54"/>
+      <c r="A43" s="54" t="s">
+        <v>103</v>
+      </c>
       <c r="B43" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="54"/>
+        <v>88</v>
+      </c>
+      <c r="C43" s="54" t="s">
+        <v>104</v>
+      </c>
       <c r="D43" s="54" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E43" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="65"/>
-      <c r="G43" s="56"/>
+        <v>101</v>
+      </c>
+      <c r="F43" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H43" s="57"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="66"/>
-      <c r="K43" s="66"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="54"/>
+      <c r="I43" s="58">
+        <v>298</v>
+      </c>
+      <c r="J43" s="63">
+        <v>4494241842.6103601</v>
+      </c>
+      <c r="K43" s="67">
+        <f t="shared" si="2"/>
+        <v>218809980.80613995</v>
+      </c>
+      <c r="L43" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M43" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="N43" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O43" s="63"/>
       <c r="P43" s="67"/>
-      <c r="Q43" s="64"/>
+      <c r="Q43" s="63">
+        <v>4713051823.4165001</v>
+      </c>
       <c r="R43" s="63"/>
       <c r="S43" s="9"/>
       <c r="T43" s="9"/>
     </row>
     <row r="44" spans="1:20" ht="18" customHeight="1">
-      <c r="A44" s="54"/>
-      <c r="B44" s="55"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="56"/>
+      <c r="A44" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H44" s="57"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="66"/>
+      <c r="I44" s="58">
+        <v>298</v>
+      </c>
+      <c r="J44" s="63">
+        <v>933971.29186602798</v>
+      </c>
       <c r="K44" s="66"/>
-      <c r="L44" s="68"/>
-      <c r="M44" s="68"/>
-      <c r="N44" s="54"/>
+      <c r="L44" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M44" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="N44" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O44" s="63"/>
       <c r="P44" s="67"/>
       <c r="Q44" s="64"/>
@@ -4525,20 +4663,44 @@
       <c r="T44" s="9"/>
     </row>
     <row r="45" spans="1:20" ht="18" customHeight="1">
-      <c r="A45" s="54"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="56"/>
+      <c r="A45" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H45" s="57"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="66"/>
+      <c r="I45" s="58">
+        <v>298</v>
+      </c>
+      <c r="J45" s="63">
+        <v>1341626.7942583701</v>
+      </c>
       <c r="K45" s="66"/>
-      <c r="L45" s="68"/>
-      <c r="M45" s="68"/>
-      <c r="N45" s="54"/>
+      <c r="L45" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="N45" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O45" s="63"/>
       <c r="P45" s="67"/>
       <c r="Q45" s="64"/>
@@ -4547,20 +4709,44 @@
       <c r="T45" s="9"/>
     </row>
     <row r="46" spans="1:20" ht="18" customHeight="1">
-      <c r="A46" s="54"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="56"/>
+      <c r="A46" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="G46" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H46" s="57"/>
-      <c r="I46" s="69"/>
-      <c r="J46" s="66"/>
+      <c r="I46" s="58">
+        <v>298</v>
+      </c>
+      <c r="J46" s="63">
+        <v>1025837.32057416</v>
+      </c>
       <c r="K46" s="66"/>
-      <c r="L46" s="68"/>
-      <c r="M46" s="68"/>
-      <c r="N46" s="54"/>
+      <c r="L46" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M46" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="N46" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O46" s="63"/>
       <c r="P46" s="67"/>
       <c r="Q46" s="64"/>
@@ -4569,20 +4755,44 @@
       <c r="T46" s="9"/>
     </row>
     <row r="47" spans="1:20" ht="18" customHeight="1">
-      <c r="A47" s="54"/>
-      <c r="B47" s="55"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="56"/>
+      <c r="A47" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H47" s="57"/>
-      <c r="I47" s="69"/>
-      <c r="J47" s="66"/>
+      <c r="I47" s="58">
+        <v>298</v>
+      </c>
+      <c r="J47" s="63">
+        <v>1063157.8947368399</v>
+      </c>
       <c r="K47" s="66"/>
-      <c r="L47" s="68"/>
-      <c r="M47" s="68"/>
-      <c r="N47" s="54"/>
+      <c r="L47" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M47" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="N47" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O47" s="63"/>
       <c r="P47" s="67"/>
       <c r="Q47" s="64"/>
@@ -4591,20 +4801,44 @@
       <c r="T47" s="9"/>
     </row>
     <row r="48" spans="1:20" ht="18" customHeight="1">
-      <c r="A48" s="54"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="54"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="65"/>
-      <c r="G48" s="56"/>
+      <c r="A48" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="G48" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H48" s="57"/>
-      <c r="I48" s="69"/>
-      <c r="J48" s="66"/>
+      <c r="I48" s="58">
+        <v>298</v>
+      </c>
+      <c r="J48" s="63">
+        <v>941784.03755868506</v>
+      </c>
       <c r="K48" s="66"/>
-      <c r="L48" s="68"/>
-      <c r="M48" s="68"/>
-      <c r="N48" s="54"/>
+      <c r="L48" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M48" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="N48" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O48" s="63"/>
       <c r="P48" s="67"/>
       <c r="Q48" s="64"/>
@@ -4613,20 +4847,44 @@
       <c r="T48" s="9"/>
     </row>
     <row r="49" spans="1:20" ht="18" customHeight="1">
-      <c r="A49" s="54"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="56"/>
+      <c r="A49" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E49" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="G49" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H49" s="57"/>
-      <c r="I49" s="69"/>
-      <c r="J49" s="66"/>
+      <c r="I49" s="58">
+        <v>298</v>
+      </c>
+      <c r="J49" s="63">
+        <v>1467605.63380281</v>
+      </c>
       <c r="K49" s="66"/>
-      <c r="L49" s="68"/>
-      <c r="M49" s="68"/>
-      <c r="N49" s="54"/>
+      <c r="L49" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M49" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="N49" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O49" s="63"/>
       <c r="P49" s="67"/>
       <c r="Q49" s="64"/>
@@ -4635,20 +4893,44 @@
       <c r="T49" s="9"/>
     </row>
     <row r="50" spans="1:20" ht="18" customHeight="1">
-      <c r="A50" s="54"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="56"/>
+      <c r="A50" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="E50" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H50" s="57"/>
-      <c r="I50" s="69"/>
-      <c r="J50" s="66"/>
+      <c r="I50" s="58">
+        <v>298</v>
+      </c>
+      <c r="J50" s="63">
+        <v>1122065.7276995301</v>
+      </c>
       <c r="K50" s="66"/>
-      <c r="L50" s="68"/>
-      <c r="M50" s="68"/>
-      <c r="N50" s="54"/>
+      <c r="L50" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M50" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="N50" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O50" s="63"/>
       <c r="P50" s="67"/>
       <c r="Q50" s="64"/>
@@ -4657,20 +4939,44 @@
       <c r="T50" s="9"/>
     </row>
     <row r="51" spans="1:20" ht="18" customHeight="1">
-      <c r="A51" s="54"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="65"/>
-      <c r="G51" s="56"/>
+      <c r="A51" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="F51" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H51" s="57"/>
-      <c r="I51" s="69"/>
-      <c r="J51" s="66"/>
+      <c r="I51" s="58">
+        <v>298</v>
+      </c>
+      <c r="J51" s="63">
+        <v>1180281.6901408399</v>
+      </c>
       <c r="K51" s="66"/>
-      <c r="L51" s="68"/>
-      <c r="M51" s="68"/>
-      <c r="N51" s="54"/>
+      <c r="L51" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M51" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="N51" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O51" s="63"/>
       <c r="P51" s="67"/>
       <c r="Q51" s="64"/>
@@ -4679,20 +4985,44 @@
       <c r="T51" s="9"/>
     </row>
     <row r="52" spans="1:20" ht="18" customHeight="1">
-      <c r="A52" s="54"/>
-      <c r="B52" s="55"/>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="65"/>
-      <c r="G52" s="56"/>
+      <c r="A52" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F52" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="G52" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H52" s="57"/>
-      <c r="I52" s="69"/>
-      <c r="J52" s="66"/>
+      <c r="I52" s="58">
+        <v>298</v>
+      </c>
+      <c r="J52" s="66">
+        <v>10.452830188679201</v>
+      </c>
       <c r="K52" s="66"/>
-      <c r="L52" s="68"/>
-      <c r="M52" s="68"/>
-      <c r="N52" s="54"/>
+      <c r="L52" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="M52" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="N52" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O52" s="63"/>
       <c r="P52" s="67"/>
       <c r="Q52" s="64"/>
@@ -4701,20 +5031,44 @@
       <c r="T52" s="9"/>
     </row>
     <row r="53" spans="1:20" ht="18" customHeight="1">
-      <c r="A53" s="54"/>
-      <c r="B53" s="55"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="65"/>
-      <c r="G53" s="56"/>
+      <c r="A53" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="F53" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H53" s="57"/>
-      <c r="I53" s="69"/>
-      <c r="J53" s="66"/>
+      <c r="I53" s="58">
+        <v>298</v>
+      </c>
+      <c r="J53" s="66">
+        <v>9.8113207547169807</v>
+      </c>
       <c r="K53" s="66"/>
-      <c r="L53" s="68"/>
-      <c r="M53" s="68"/>
-      <c r="N53" s="54"/>
+      <c r="L53" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="M53" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="N53" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O53" s="63"/>
       <c r="P53" s="67"/>
       <c r="Q53" s="64"/>
@@ -4723,20 +5077,44 @@
       <c r="T53" s="9"/>
     </row>
     <row r="54" spans="1:20" ht="18" customHeight="1">
-      <c r="A54" s="54"/>
-      <c r="B54" s="55"/>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="65"/>
-      <c r="G54" s="56"/>
+      <c r="A54" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="E54" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="G54" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H54" s="57"/>
-      <c r="I54" s="69"/>
-      <c r="J54" s="66"/>
+      <c r="I54" s="58">
+        <v>298</v>
+      </c>
+      <c r="J54" s="66">
+        <v>15.943396226415</v>
+      </c>
       <c r="K54" s="66"/>
-      <c r="L54" s="68"/>
-      <c r="M54" s="68"/>
-      <c r="N54" s="54"/>
+      <c r="L54" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="M54" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="N54" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O54" s="63"/>
       <c r="P54" s="67"/>
       <c r="Q54" s="64"/>
@@ -4745,20 +5123,44 @@
       <c r="T54" s="9"/>
     </row>
     <row r="55" spans="1:20" ht="18" customHeight="1">
-      <c r="A55" s="54"/>
-      <c r="B55" s="55"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="65"/>
-      <c r="G55" s="56"/>
+      <c r="A55" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E55" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="F55" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="G55" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H55" s="57"/>
-      <c r="I55" s="69"/>
-      <c r="J55" s="66"/>
+      <c r="I55" s="58">
+        <v>298</v>
+      </c>
+      <c r="J55" s="66">
+        <v>18.018867924528301</v>
+      </c>
       <c r="K55" s="66"/>
-      <c r="L55" s="68"/>
-      <c r="M55" s="68"/>
-      <c r="N55" s="54"/>
+      <c r="L55" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="M55" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="N55" s="54" t="s">
+        <v>93</v>
+      </c>
       <c r="O55" s="63"/>
       <c r="P55" s="67"/>
       <c r="Q55" s="64"/>
@@ -4797,7 +5199,7 @@
       <c r="F57" s="65"/>
       <c r="G57" s="56"/>
       <c r="H57" s="57"/>
-      <c r="I57" s="69"/>
+      <c r="I57" s="58"/>
       <c r="J57" s="66"/>
       <c r="K57" s="66"/>
       <c r="L57" s="68"/>
@@ -4885,7 +5287,7 @@
       <c r="F61" s="65"/>
       <c r="G61" s="56"/>
       <c r="H61" s="57"/>
-      <c r="I61" s="58"/>
+      <c r="I61" s="69"/>
       <c r="J61" s="66"/>
       <c r="K61" s="66"/>
       <c r="L61" s="68"/>
@@ -4997,7 +5399,7 @@
       <c r="H66" s="57"/>
       <c r="I66" s="69"/>
       <c r="J66" s="66"/>
-      <c r="K66" s="66"/>
+      <c r="K66" s="70"/>
       <c r="L66" s="68"/>
       <c r="M66" s="68"/>
       <c r="N66" s="54"/>
@@ -5019,7 +5421,7 @@
       <c r="H67" s="57"/>
       <c r="I67" s="69"/>
       <c r="J67" s="66"/>
-      <c r="K67" s="70"/>
+      <c r="K67" s="54"/>
       <c r="L67" s="68"/>
       <c r="M67" s="68"/>
       <c r="N67" s="54"/>
@@ -5041,7 +5443,7 @@
       <c r="H68" s="57"/>
       <c r="I68" s="69"/>
       <c r="J68" s="66"/>
-      <c r="K68" s="54"/>
+      <c r="K68" s="67"/>
       <c r="L68" s="68"/>
       <c r="M68" s="68"/>
       <c r="N68" s="54"/>
@@ -5129,7 +5531,7 @@
       <c r="H72" s="57"/>
       <c r="I72" s="69"/>
       <c r="J72" s="66"/>
-      <c r="K72" s="67"/>
+      <c r="K72" s="54"/>
       <c r="L72" s="68"/>
       <c r="M72" s="68"/>
       <c r="N72" s="54"/>
@@ -5149,9 +5551,9 @@
       <c r="F73" s="65"/>
       <c r="G73" s="56"/>
       <c r="H73" s="57"/>
-      <c r="I73" s="69"/>
-      <c r="J73" s="66"/>
-      <c r="K73" s="54"/>
+      <c r="I73" s="58"/>
+      <c r="J73" s="67"/>
+      <c r="K73" s="67"/>
       <c r="L73" s="68"/>
       <c r="M73" s="68"/>
       <c r="N73" s="54"/>
@@ -5237,9 +5639,9 @@
       <c r="F77" s="65"/>
       <c r="G77" s="56"/>
       <c r="H77" s="57"/>
-      <c r="I77" s="58"/>
-      <c r="J77" s="67"/>
-      <c r="K77" s="67"/>
+      <c r="I77" s="69"/>
+      <c r="J77" s="64"/>
+      <c r="K77" s="54"/>
       <c r="L77" s="68"/>
       <c r="M77" s="68"/>
       <c r="N77" s="54"/>
@@ -5261,7 +5663,7 @@
       <c r="H78" s="57"/>
       <c r="I78" s="69"/>
       <c r="J78" s="64"/>
-      <c r="K78" s="54"/>
+      <c r="K78" s="67"/>
       <c r="L78" s="68"/>
       <c r="M78" s="68"/>
       <c r="N78" s="54"/>
@@ -5349,7 +5751,7 @@
       <c r="H82" s="57"/>
       <c r="I82" s="69"/>
       <c r="J82" s="64"/>
-      <c r="K82" s="67"/>
+      <c r="K82" s="54"/>
       <c r="L82" s="68"/>
       <c r="M82" s="68"/>
       <c r="N82" s="54"/>
@@ -5371,7 +5773,7 @@
       <c r="H83" s="57"/>
       <c r="I83" s="69"/>
       <c r="J83" s="64"/>
-      <c r="K83" s="54"/>
+      <c r="K83" s="67"/>
       <c r="L83" s="68"/>
       <c r="M83" s="68"/>
       <c r="N83" s="54"/>
@@ -5459,7 +5861,7 @@
       <c r="H87" s="57"/>
       <c r="I87" s="69"/>
       <c r="J87" s="64"/>
-      <c r="K87" s="67"/>
+      <c r="K87" s="66"/>
       <c r="L87" s="68"/>
       <c r="M87" s="68"/>
       <c r="N87" s="54"/>
@@ -5498,11 +5900,11 @@
       <c r="C89" s="54"/>
       <c r="D89" s="54"/>
       <c r="E89" s="55"/>
-      <c r="F89" s="65"/>
+      <c r="F89" s="56"/>
       <c r="G89" s="56"/>
       <c r="H89" s="57"/>
-      <c r="I89" s="69"/>
-      <c r="J89" s="64"/>
+      <c r="I89" s="58"/>
+      <c r="J89" s="66"/>
       <c r="K89" s="66"/>
       <c r="L89" s="68"/>
       <c r="M89" s="68"/>
@@ -5569,7 +5971,7 @@
       <c r="H92" s="57"/>
       <c r="I92" s="58"/>
       <c r="J92" s="66"/>
-      <c r="K92" s="66"/>
+      <c r="K92" s="59"/>
       <c r="L92" s="68"/>
       <c r="M92" s="68"/>
       <c r="N92" s="54"/>
@@ -5590,7 +5992,7 @@
       <c r="G93" s="56"/>
       <c r="H93" s="57"/>
       <c r="I93" s="58"/>
-      <c r="J93" s="66"/>
+      <c r="J93" s="59"/>
       <c r="K93" s="59"/>
       <c r="L93" s="68"/>
       <c r="M93" s="68"/>
@@ -5745,7 +6147,7 @@
       <c r="H100" s="57"/>
       <c r="I100" s="58"/>
       <c r="J100" s="59"/>
-      <c r="K100" s="59"/>
+      <c r="K100" s="66"/>
       <c r="L100" s="56"/>
       <c r="M100" s="56"/>
       <c r="N100" s="54"/>
@@ -5757,7 +6159,7 @@
       <c r="T100" s="9"/>
     </row>
     <row r="101" spans="1:20" ht="18" customHeight="1">
-      <c r="A101" s="54"/>
+      <c r="A101" s="71"/>
       <c r="B101" s="55"/>
       <c r="C101" s="54"/>
       <c r="D101" s="54"/>
@@ -5854,7 +6256,7 @@
       <c r="G105" s="56"/>
       <c r="H105" s="57"/>
       <c r="I105" s="58"/>
-      <c r="J105" s="59"/>
+      <c r="J105" s="64"/>
       <c r="K105" s="66"/>
       <c r="L105" s="56"/>
       <c r="M105" s="56"/>
@@ -6013,7 +6415,7 @@
       <c r="L112" s="68"/>
       <c r="M112" s="56"/>
       <c r="N112" s="54"/>
-      <c r="O112" s="63"/>
+      <c r="O112" s="9"/>
       <c r="P112" s="64"/>
       <c r="Q112" s="64"/>
       <c r="R112" s="63"/>
@@ -6030,12 +6432,12 @@
       <c r="G113" s="56"/>
       <c r="H113" s="57"/>
       <c r="I113" s="58"/>
-      <c r="J113" s="64"/>
+      <c r="J113" s="66"/>
       <c r="K113" s="66"/>
       <c r="L113" s="68"/>
       <c r="M113" s="56"/>
       <c r="N113" s="54"/>
-      <c r="O113" s="63"/>
+      <c r="O113" s="9"/>
       <c r="P113" s="64"/>
       <c r="Q113" s="64"/>
       <c r="R113" s="63"/>
@@ -6140,7 +6542,7 @@
       <c r="G118" s="56"/>
       <c r="H118" s="57"/>
       <c r="I118" s="58"/>
-      <c r="J118" s="66"/>
+      <c r="J118" s="64"/>
       <c r="K118" s="66"/>
       <c r="L118" s="68"/>
       <c r="M118" s="68"/>
@@ -6162,7 +6564,7 @@
       <c r="G119" s="56"/>
       <c r="H119" s="57"/>
       <c r="I119" s="58"/>
-      <c r="J119" s="64"/>
+      <c r="J119" s="67"/>
       <c r="K119" s="66"/>
       <c r="L119" s="68"/>
       <c r="M119" s="68"/>
@@ -6185,7 +6587,7 @@
       <c r="H120" s="57"/>
       <c r="I120" s="58"/>
       <c r="J120" s="67"/>
-      <c r="K120" s="66"/>
+      <c r="K120" s="73"/>
       <c r="L120" s="68"/>
       <c r="M120" s="68"/>
       <c r="N120" s="54"/>
@@ -6197,16 +6599,16 @@
       <c r="T120" s="9"/>
     </row>
     <row r="121" spans="1:20" ht="18" customHeight="1">
-      <c r="A121" s="71"/>
-      <c r="B121" s="55"/>
-      <c r="C121" s="54"/>
-      <c r="D121" s="54"/>
-      <c r="E121" s="55"/>
-      <c r="F121" s="56"/>
-      <c r="G121" s="56"/>
+      <c r="A121" s="4"/>
+      <c r="B121" s="72"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="72"/>
+      <c r="F121" s="52"/>
+      <c r="G121" s="52"/>
       <c r="H121" s="57"/>
-      <c r="I121" s="58"/>
-      <c r="J121" s="67"/>
+      <c r="I121" s="4"/>
+      <c r="J121" s="73"/>
       <c r="K121" s="73"/>
       <c r="L121" s="68"/>
       <c r="M121" s="68"/>
@@ -6229,11 +6631,11 @@
       <c r="H122" s="57"/>
       <c r="I122" s="4"/>
       <c r="J122" s="73"/>
-      <c r="K122" s="73"/>
+      <c r="K122" s="66"/>
       <c r="L122" s="52"/>
       <c r="M122" s="52"/>
       <c r="N122" s="4"/>
-      <c r="O122" s="9"/>
+      <c r="O122" s="63"/>
       <c r="P122" s="4"/>
       <c r="Q122" s="4"/>
       <c r="R122" s="9"/>
@@ -6241,21 +6643,21 @@
       <c r="T122" s="9"/>
     </row>
     <row r="123" spans="1:20" ht="18" customHeight="1">
-      <c r="A123" s="4"/>
-      <c r="B123" s="72"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="72"/>
-      <c r="F123" s="52"/>
-      <c r="G123" s="52"/>
+      <c r="A123" s="54"/>
+      <c r="B123" s="55"/>
+      <c r="C123" s="54"/>
+      <c r="D123" s="54"/>
+      <c r="E123" s="55"/>
+      <c r="F123" s="56"/>
+      <c r="G123" s="56"/>
       <c r="H123" s="57"/>
-      <c r="I123" s="4"/>
-      <c r="J123" s="73"/>
+      <c r="I123" s="69"/>
+      <c r="J123" s="74"/>
       <c r="K123" s="66"/>
       <c r="L123" s="52"/>
       <c r="M123" s="52"/>
       <c r="N123" s="4"/>
-      <c r="O123" s="9"/>
+      <c r="O123" s="63"/>
       <c r="P123" s="4"/>
       <c r="Q123" s="4"/>
       <c r="R123" s="9"/>
@@ -6285,7 +6687,7 @@
       <c r="T124" s="9"/>
     </row>
     <row r="125" spans="1:20" ht="18" customHeight="1">
-      <c r="A125" s="54"/>
+      <c r="A125" s="71"/>
       <c r="B125" s="55"/>
       <c r="C125" s="54"/>
       <c r="D125" s="54"/>
@@ -6293,8 +6695,8 @@
       <c r="F125" s="56"/>
       <c r="G125" s="56"/>
       <c r="H125" s="57"/>
-      <c r="I125" s="69"/>
-      <c r="J125" s="74"/>
+      <c r="I125" s="54"/>
+      <c r="J125" s="59"/>
       <c r="K125" s="66"/>
       <c r="L125" s="56"/>
       <c r="M125" s="56"/>
@@ -6337,13 +6739,13 @@
       <c r="F127" s="56"/>
       <c r="G127" s="56"/>
       <c r="H127" s="57"/>
-      <c r="I127" s="54"/>
-      <c r="J127" s="59"/>
+      <c r="I127" s="69"/>
+      <c r="J127" s="74"/>
       <c r="K127" s="66"/>
       <c r="L127" s="56"/>
       <c r="M127" s="68"/>
       <c r="N127" s="54"/>
-      <c r="O127" s="63"/>
+      <c r="O127" s="9"/>
       <c r="P127" s="64"/>
       <c r="Q127" s="4"/>
       <c r="R127" s="63"/>
@@ -6365,7 +6767,7 @@
       <c r="L128" s="56"/>
       <c r="M128" s="68"/>
       <c r="N128" s="54"/>
-      <c r="O128" s="63"/>
+      <c r="O128" s="9"/>
       <c r="P128" s="64"/>
       <c r="Q128" s="4"/>
       <c r="R128" s="63"/>
@@ -6381,13 +6783,13 @@
       <c r="F129" s="56"/>
       <c r="G129" s="56"/>
       <c r="H129" s="57"/>
-      <c r="I129" s="69"/>
-      <c r="J129" s="74"/>
+      <c r="I129" s="54"/>
+      <c r="J129" s="54"/>
       <c r="K129" s="66"/>
       <c r="L129" s="56"/>
       <c r="M129" s="68"/>
       <c r="N129" s="54"/>
-      <c r="O129" s="63"/>
+      <c r="O129" s="9"/>
       <c r="P129" s="64"/>
       <c r="Q129" s="4"/>
       <c r="R129" s="63"/>
@@ -6409,7 +6811,7 @@
       <c r="L130" s="68"/>
       <c r="M130" s="68"/>
       <c r="N130" s="54"/>
-      <c r="O130" s="63"/>
+      <c r="O130" s="9"/>
       <c r="P130" s="64"/>
       <c r="Q130" s="4"/>
       <c r="R130" s="63"/>
@@ -6425,13 +6827,13 @@
       <c r="F131" s="56"/>
       <c r="G131" s="56"/>
       <c r="H131" s="57"/>
-      <c r="I131" s="54"/>
-      <c r="J131" s="54"/>
+      <c r="I131" s="69"/>
+      <c r="J131" s="67"/>
       <c r="K131" s="66"/>
       <c r="L131" s="68"/>
       <c r="M131" s="68"/>
       <c r="N131" s="54"/>
-      <c r="O131" s="63"/>
+      <c r="O131" s="9"/>
       <c r="P131" s="64"/>
       <c r="Q131" s="4"/>
       <c r="R131" s="63"/>
@@ -6449,11 +6851,11 @@
       <c r="H132" s="57"/>
       <c r="I132" s="69"/>
       <c r="J132" s="67"/>
-      <c r="K132" s="66"/>
+      <c r="K132" s="59"/>
       <c r="L132" s="68"/>
       <c r="M132" s="68"/>
       <c r="N132" s="54"/>
-      <c r="O132" s="63"/>
+      <c r="O132" s="9"/>
       <c r="P132" s="64"/>
       <c r="Q132" s="4"/>
       <c r="R132" s="63"/>
@@ -6461,7 +6863,7 @@
       <c r="T132" s="9"/>
     </row>
     <row r="133" spans="1:20" ht="18" customHeight="1">
-      <c r="A133" s="71"/>
+      <c r="A133" s="54"/>
       <c r="B133" s="55"/>
       <c r="C133" s="54"/>
       <c r="D133" s="54"/>
@@ -6469,13 +6871,13 @@
       <c r="F133" s="56"/>
       <c r="G133" s="56"/>
       <c r="H133" s="57"/>
-      <c r="I133" s="69"/>
-      <c r="J133" s="67"/>
+      <c r="I133" s="58"/>
+      <c r="J133" s="59"/>
       <c r="K133" s="59"/>
       <c r="L133" s="68"/>
       <c r="M133" s="68"/>
       <c r="N133" s="54"/>
-      <c r="O133" s="63"/>
+      <c r="O133" s="9"/>
       <c r="P133" s="64"/>
       <c r="Q133" s="4"/>
       <c r="R133" s="63"/>
@@ -6497,7 +6899,7 @@
       <c r="L134" s="56"/>
       <c r="M134" s="56"/>
       <c r="N134" s="75"/>
-      <c r="O134" s="63"/>
+      <c r="O134" s="9"/>
       <c r="P134" s="64"/>
       <c r="Q134" s="4"/>
       <c r="R134" s="63"/>
@@ -6519,7 +6921,7 @@
       <c r="L135" s="56"/>
       <c r="M135" s="56"/>
       <c r="N135" s="75"/>
-      <c r="O135" s="63"/>
+      <c r="O135" s="9"/>
       <c r="P135" s="64"/>
       <c r="Q135" s="4"/>
       <c r="R135" s="63"/>
@@ -6541,7 +6943,7 @@
       <c r="L136" s="56"/>
       <c r="M136" s="56"/>
       <c r="N136" s="75"/>
-      <c r="O136" s="63"/>
+      <c r="O136" s="9"/>
       <c r="P136" s="64"/>
       <c r="Q136" s="4"/>
       <c r="R136" s="63"/>
@@ -6625,7 +7027,7 @@
       <c r="H140" s="57"/>
       <c r="I140" s="58"/>
       <c r="J140" s="59"/>
-      <c r="K140" s="59"/>
+      <c r="K140" s="4"/>
       <c r="L140" s="56"/>
       <c r="M140" s="56"/>
       <c r="N140" s="75"/>
@@ -6645,8 +7047,8 @@
       <c r="F141" s="56"/>
       <c r="G141" s="56"/>
       <c r="H141" s="57"/>
-      <c r="I141" s="58"/>
-      <c r="J141" s="59"/>
+      <c r="I141" s="4"/>
+      <c r="J141" s="4"/>
       <c r="K141" s="4"/>
       <c r="L141" s="56"/>
       <c r="M141" s="56"/>
@@ -6801,7 +7203,7 @@
       <c r="H148" s="57"/>
       <c r="I148" s="4"/>
       <c r="J148" s="4"/>
-      <c r="K148" s="4"/>
+      <c r="K148" s="59"/>
       <c r="L148" s="56"/>
       <c r="M148" s="4"/>
       <c r="N148" s="75"/>
@@ -6815,14 +7217,14 @@
     <row r="149" spans="1:20" ht="18" customHeight="1">
       <c r="A149" s="54"/>
       <c r="B149" s="55"/>
-      <c r="C149" s="54"/>
+      <c r="C149" s="56"/>
       <c r="D149" s="54"/>
       <c r="E149" s="55"/>
       <c r="F149" s="56"/>
       <c r="G149" s="56"/>
       <c r="H149" s="57"/>
-      <c r="I149" s="4"/>
-      <c r="J149" s="4"/>
+      <c r="I149" s="58"/>
+      <c r="J149" s="59"/>
       <c r="K149" s="59"/>
       <c r="L149" s="56"/>
       <c r="M149" s="4"/>
@@ -6977,7 +7379,7 @@
       <c r="H156" s="57"/>
       <c r="I156" s="58"/>
       <c r="J156" s="59"/>
-      <c r="K156" s="59"/>
+      <c r="K156" s="4"/>
       <c r="L156" s="56"/>
       <c r="M156" s="56"/>
       <c r="N156" s="75"/>
@@ -6998,7 +7400,7 @@
       <c r="G157" s="56"/>
       <c r="H157" s="57"/>
       <c r="I157" s="58"/>
-      <c r="J157" s="59"/>
+      <c r="J157" s="4"/>
       <c r="K157" s="4"/>
       <c r="L157" s="56"/>
       <c r="M157" s="56"/>
@@ -7121,15 +7523,15 @@
       <c r="T162" s="9"/>
     </row>
     <row r="163" spans="1:20" ht="18" customHeight="1">
-      <c r="A163" s="54"/>
+      <c r="A163" s="4"/>
       <c r="B163" s="55"/>
-      <c r="C163" s="56"/>
+      <c r="C163" s="54"/>
       <c r="D163" s="54"/>
-      <c r="E163" s="55"/>
-      <c r="F163" s="56"/>
+      <c r="E163" s="63"/>
+      <c r="F163" s="76"/>
       <c r="G163" s="56"/>
-      <c r="H163" s="57"/>
-      <c r="I163" s="58"/>
+      <c r="H163" s="65"/>
+      <c r="I163" s="4"/>
       <c r="J163" s="4"/>
       <c r="K163" s="4"/>
       <c r="L163" s="4"/>
@@ -7321,12 +7723,12 @@
     <row r="172" spans="1:20" ht="18" customHeight="1">
       <c r="A172" s="4"/>
       <c r="B172" s="55"/>
-      <c r="C172" s="54"/>
-      <c r="D172" s="54"/>
+      <c r="C172" s="4"/>
+      <c r="D172" s="4"/>
       <c r="E172" s="63"/>
-      <c r="F172" s="76"/>
+      <c r="F172" s="4"/>
       <c r="G172" s="56"/>
-      <c r="H172" s="65"/>
+      <c r="H172" s="4"/>
       <c r="I172" s="4"/>
       <c r="J172" s="4"/>
       <c r="K172" s="4"/>
@@ -8185,7 +8587,7 @@
       <c r="F211" s="4"/>
       <c r="G211" s="56"/>
       <c r="H211" s="4"/>
-      <c r="I211" s="4"/>
+      <c r="I211" s="53"/>
       <c r="J211" s="4"/>
       <c r="K211" s="4"/>
       <c r="L211" s="4"/>
@@ -8357,11 +8759,11 @@
       <c r="B219" s="55"/>
       <c r="C219" s="4"/>
       <c r="D219" s="4"/>
-      <c r="E219" s="63"/>
+      <c r="E219" s="9"/>
       <c r="F219" s="4"/>
-      <c r="G219" s="56"/>
+      <c r="G219" s="4"/>
       <c r="H219" s="4"/>
-      <c r="I219" s="53"/>
+      <c r="I219" s="4"/>
       <c r="J219" s="4"/>
       <c r="K219" s="4"/>
       <c r="L219" s="4"/>
@@ -8620,7 +9022,6 @@
       <c r="L231" s="4"/>
       <c r="M231" s="4"/>
       <c r="N231" s="4"/>
-      <c r="O231" s="9"/>
       <c r="P231" s="4"/>
       <c r="R231" s="9"/>
       <c r="S231" s="9"/>
@@ -8641,7 +9042,6 @@
       <c r="L232" s="4"/>
       <c r="M232" s="4"/>
       <c r="N232" s="4"/>
-      <c r="O232" s="9"/>
       <c r="P232" s="4"/>
       <c r="R232" s="9"/>
       <c r="S232" s="9"/>
@@ -8662,7 +9062,6 @@
       <c r="L233" s="4"/>
       <c r="M233" s="4"/>
       <c r="N233" s="4"/>
-      <c r="O233" s="9"/>
       <c r="P233" s="4"/>
       <c r="R233" s="9"/>
       <c r="S233" s="9"/>
@@ -8683,7 +9082,6 @@
       <c r="L234" s="4"/>
       <c r="M234" s="4"/>
       <c r="N234" s="4"/>
-      <c r="O234" s="9"/>
       <c r="P234" s="4"/>
       <c r="R234" s="9"/>
       <c r="S234" s="9"/>
@@ -8704,7 +9102,6 @@
       <c r="L235" s="4"/>
       <c r="M235" s="4"/>
       <c r="N235" s="4"/>
-      <c r="O235" s="9"/>
       <c r="P235" s="4"/>
       <c r="R235" s="9"/>
       <c r="S235" s="9"/>
@@ -8725,7 +9122,6 @@
       <c r="L236" s="4"/>
       <c r="M236" s="4"/>
       <c r="N236" s="4"/>
-      <c r="O236" s="9"/>
       <c r="P236" s="4"/>
       <c r="R236" s="9"/>
       <c r="S236" s="9"/>
@@ -8746,7 +9142,6 @@
       <c r="L237" s="4"/>
       <c r="M237" s="4"/>
       <c r="N237" s="4"/>
-      <c r="O237" s="9"/>
       <c r="P237" s="4"/>
       <c r="R237" s="9"/>
       <c r="S237" s="9"/>
@@ -8767,7 +9162,6 @@
       <c r="L238" s="4"/>
       <c r="M238" s="4"/>
       <c r="N238" s="4"/>
-      <c r="O238" s="9"/>
       <c r="P238" s="4"/>
       <c r="R238" s="9"/>
       <c r="S238" s="9"/>
@@ -8784,31 +9178,18 @@
       <c r="H239" s="4"/>
       <c r="I239" s="4"/>
       <c r="J239" s="4"/>
-      <c r="K239" s="4"/>
       <c r="L239" s="4"/>
       <c r="M239" s="4"/>
       <c r="N239" s="4"/>
-      <c r="O239" s="9"/>
       <c r="P239" s="4"/>
       <c r="R239" s="9"/>
       <c r="S239" s="9"/>
       <c r="T239" s="9"/>
     </row>
     <row r="240" spans="1:20" ht="18" customHeight="1">
-      <c r="A240" s="4"/>
-      <c r="B240" s="55"/>
-      <c r="C240" s="4"/>
-      <c r="D240" s="4"/>
-      <c r="E240" s="9"/>
-      <c r="F240" s="4"/>
-      <c r="G240" s="4"/>
-      <c r="H240" s="4"/>
-      <c r="I240" s="4"/>
-      <c r="J240" s="4"/>
       <c r="L240" s="4"/>
       <c r="M240" s="4"/>
       <c r="N240" s="4"/>
-      <c r="O240" s="9"/>
       <c r="P240" s="4"/>
       <c r="R240" s="9"/>
       <c r="S240" s="9"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.ijrmhm.2025.107039`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEE59B9-3726-D24D-9EB7-BA55ED86117E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040EB067-3A85-3E46-B9BE-7E43CC5AC362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="6040" windowWidth="31040" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="8800" windowWidth="31040" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="139">
   <si>
     <r>
       <rPr>
@@ -327,6 +327,9 @@
     <t>nanohardness</t>
   </si>
   <si>
+    <t>F11</t>
+  </si>
+  <si>
     <t>AAM</t>
   </si>
   <si>
@@ -345,9 +348,15 @@
     <t>%</t>
   </si>
   <si>
+    <t>AAM+A</t>
+  </si>
+  <si>
     <t>UCS</t>
   </si>
   <si>
+    <t>T5</t>
+  </si>
+  <si>
     <t>minimum compressive ductility</t>
   </si>
   <si>
@@ -504,10 +513,40 @@
     <t>BCC+oxide</t>
   </si>
   <si>
+    <t>F12</t>
+  </si>
+  <si>
     <t>F9a</t>
   </si>
   <si>
     <t>10.1016/j.msea.2025.147800</t>
+  </si>
+  <si>
+    <t>NbMoZrTi</t>
+  </si>
+  <si>
+    <t>annealed at 873K in Ar for 10h and furnace cooled</t>
+  </si>
+  <si>
+    <t>annealed at 1073K in Ar for 10h and furnace cooled</t>
+  </si>
+  <si>
+    <t>annealed at 1273K in Ar for 10h and furnace cooled</t>
+  </si>
+  <si>
+    <t>HT0</t>
+  </si>
+  <si>
+    <t>HT600</t>
+  </si>
+  <si>
+    <t>HT800</t>
+  </si>
+  <si>
+    <t>HT1000</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijrmhm.2025.107039</t>
   </si>
 </sst>
 </file>
@@ -2775,8 +2814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T856"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E23" zoomScale="86" workbookViewId="0">
-      <selection activeCell="O80" sqref="O80"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B90" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N106" sqref="N106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3134,16 +3173,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="54"/>
       <c r="B10" s="55" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F10" s="56" t="s">
         <v>63</v>
@@ -3167,10 +3206,10 @@
         <v>33</v>
       </c>
       <c r="M10" s="56" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N10" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="4">
@@ -3188,16 +3227,16 @@
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="54"/>
       <c r="B11" s="55" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F11" s="56" t="s">
         <v>63</v>
@@ -3221,10 +3260,10 @@
         <v>33</v>
       </c>
       <c r="M11" s="56" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N11" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="4">
@@ -3242,16 +3281,16 @@
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="54"/>
       <c r="B12" s="55" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F12" s="56" t="s">
         <v>63</v>
@@ -3275,10 +3314,10 @@
         <v>33</v>
       </c>
       <c r="M12" s="56" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N12" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="4">
@@ -3296,16 +3335,16 @@
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="54"/>
       <c r="B13" s="55" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>63</v>
@@ -3329,10 +3368,10 @@
         <v>33</v>
       </c>
       <c r="M13" s="56" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N13" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="4">
@@ -3350,16 +3389,16 @@
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="54"/>
       <c r="B14" s="55" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F14" s="56" t="s">
         <v>63</v>
@@ -3383,10 +3422,10 @@
         <v>33</v>
       </c>
       <c r="M14" s="56" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N14" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="4">
@@ -3404,19 +3443,19 @@
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="54"/>
       <c r="B15" s="55" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G15" s="56" t="s">
         <v>29</v>
@@ -3434,10 +3473,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="56" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N15" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9">
@@ -3451,19 +3490,19 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="54"/>
       <c r="B16" s="55" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G16" s="56" t="s">
         <v>29</v>
@@ -3481,10 +3520,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="56" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N16" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="9">
@@ -3498,19 +3537,19 @@
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="55" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G17" s="56" t="s">
         <v>29</v>
@@ -3528,10 +3567,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="56" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N17" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="9">
@@ -3545,19 +3584,19 @@
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="55" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G18" s="56" t="s">
         <v>29</v>
@@ -3575,10 +3614,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="56" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N18" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="9">
@@ -3592,19 +3631,19 @@
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="55" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G19" s="56" t="s">
         <v>29</v>
@@ -3622,10 +3661,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="56" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N19" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="9">
@@ -3639,19 +3678,19 @@
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="56" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="56" t="s">
-        <v>76</v>
       </c>
       <c r="G20" s="56" t="s">
         <v>29</v>
@@ -3669,10 +3708,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N20" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9">
@@ -3686,19 +3725,19 @@
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="55" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F21" s="56" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G21" s="56" t="s">
         <v>29</v>
@@ -3716,10 +3755,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N21" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="9">
@@ -3733,19 +3772,19 @@
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="55" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G22" s="56" t="s">
         <v>29</v>
@@ -3763,10 +3802,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N22" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9">
@@ -3780,19 +3819,19 @@
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="54"/>
       <c r="B23" s="55" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F23" s="56" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G23" s="56" t="s">
         <v>29</v>
@@ -3810,10 +3849,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N23" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="9">
@@ -3827,19 +3866,19 @@
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="54"/>
       <c r="B24" s="55" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G24" s="56" t="s">
         <v>29</v>
@@ -3857,10 +3896,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N24" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O24" s="9"/>
       <c r="P24" s="9">
@@ -3874,19 +3913,19 @@
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="54"/>
       <c r="B25" s="114" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C25" s="115" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D25" s="115" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E25" s="116" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F25" s="56" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G25" s="56" t="s">
         <v>29</v>
@@ -3900,13 +3939,13 @@
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M25" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N25" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O25" s="9"/>
       <c r="P25" s="4"/>
@@ -3918,19 +3957,19 @@
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="54"/>
       <c r="B26" s="117" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C26" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" s="118" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E26" s="119" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G26" s="56" t="s">
         <v>29</v>
@@ -3944,13 +3983,13 @@
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M26" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N26" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="61"/>
@@ -3962,19 +4001,19 @@
     <row r="27" spans="1:20" ht="18.75" customHeight="1">
       <c r="A27" s="54"/>
       <c r="B27" s="117" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C27" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D27" s="118" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E27" s="119" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F27" s="56" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G27" s="56" t="s">
         <v>29</v>
@@ -3988,13 +4027,13 @@
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M27" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N27" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O27" s="9"/>
       <c r="P27" s="61"/>
@@ -4006,19 +4045,19 @@
     <row r="28" spans="1:20" ht="18.75" customHeight="1">
       <c r="A28" s="54"/>
       <c r="B28" s="117" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C28" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D28" s="118" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E28" s="119" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F28" s="56" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G28" s="56" t="s">
         <v>29</v>
@@ -4032,13 +4071,13 @@
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M28" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N28" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O28" s="9"/>
       <c r="P28" s="61"/>
@@ -4050,19 +4089,19 @@
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
       <c r="A29" s="54"/>
       <c r="B29" s="117" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C29" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="118" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E29" s="119" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F29" s="56" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G29" s="56" t="s">
         <v>29</v>
@@ -4076,13 +4115,13 @@
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M29" s="76" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N29" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O29" s="9"/>
       <c r="P29" s="61"/>
@@ -4094,23 +4133,23 @@
     <row r="30" spans="1:20" ht="18.75" customHeight="1">
       <c r="A30" s="54"/>
       <c r="B30" s="114" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C30" s="115" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="54"/>
       <c r="E30" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F30" s="56" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G30" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H30" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="1">
@@ -4119,10 +4158,10 @@
       <c r="K30" s="4"/>
       <c r="L30" s="56"/>
       <c r="M30" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N30" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O30" s="9"/>
       <c r="P30" s="61"/>
@@ -4134,23 +4173,23 @@
     <row r="31" spans="1:20" ht="18.75" customHeight="1">
       <c r="A31" s="54"/>
       <c r="B31" s="117" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C31" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="54"/>
       <c r="E31" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F31" s="56" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G31" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H31" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="1">
@@ -4159,10 +4198,10 @@
       <c r="K31" s="4"/>
       <c r="L31" s="56"/>
       <c r="M31" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N31" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O31" s="9"/>
       <c r="P31" s="61"/>
@@ -4174,23 +4213,23 @@
     <row r="32" spans="1:20" ht="18.75" customHeight="1">
       <c r="A32" s="54"/>
       <c r="B32" s="117" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C32" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F32" s="56" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G32" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H32" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="1">
@@ -4199,10 +4238,10 @@
       <c r="K32" s="4"/>
       <c r="L32" s="56"/>
       <c r="M32" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N32" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O32" s="9"/>
       <c r="P32" s="61"/>
@@ -4214,23 +4253,23 @@
     <row r="33" spans="1:20" ht="18.75" customHeight="1">
       <c r="A33" s="54"/>
       <c r="B33" s="117" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C33" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F33" s="56" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G33" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H33" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="1">
@@ -4239,10 +4278,10 @@
       <c r="K33" s="4"/>
       <c r="L33" s="56"/>
       <c r="M33" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N33" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="61"/>
@@ -4254,23 +4293,23 @@
     <row r="34" spans="1:20" ht="18.75" customHeight="1">
       <c r="A34" s="54"/>
       <c r="B34" s="117" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C34" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D34" s="54"/>
       <c r="E34" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F34" s="56" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G34" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H34" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="1">
@@ -4279,10 +4318,10 @@
       <c r="K34" s="4"/>
       <c r="L34" s="56"/>
       <c r="M34" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N34" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O34" s="9"/>
       <c r="P34" s="4"/>
@@ -4294,23 +4333,23 @@
     <row r="35" spans="1:20" ht="18.75" customHeight="1">
       <c r="A35" s="54"/>
       <c r="B35" s="114" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C35" s="115" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D35" s="54"/>
       <c r="E35" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F35" s="56" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G35" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H35" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4">
@@ -4319,10 +4358,10 @@
       <c r="K35" s="4"/>
       <c r="L35" s="56"/>
       <c r="M35" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N35" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O35" s="9"/>
       <c r="P35" s="4"/>
@@ -4334,23 +4373,23 @@
     <row r="36" spans="1:20" ht="18.75" customHeight="1">
       <c r="A36" s="54"/>
       <c r="B36" s="117" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C36" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D36" s="54"/>
       <c r="E36" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F36" s="56" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G36" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H36" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4">
@@ -4359,10 +4398,10 @@
       <c r="K36" s="4"/>
       <c r="L36" s="56"/>
       <c r="M36" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N36" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="4"/>
@@ -4374,23 +4413,23 @@
     <row r="37" spans="1:20" ht="18.75" customHeight="1">
       <c r="A37" s="54"/>
       <c r="B37" s="117" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C37" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D37" s="54"/>
       <c r="E37" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F37" s="56" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G37" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H37" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4">
@@ -4399,10 +4438,10 @@
       <c r="K37" s="59"/>
       <c r="L37" s="56"/>
       <c r="M37" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N37" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O37" s="9"/>
       <c r="P37" s="4"/>
@@ -4414,23 +4453,23 @@
     <row r="38" spans="1:20" ht="18.75" customHeight="1">
       <c r="A38" s="54"/>
       <c r="B38" s="117" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C38" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D38" s="54"/>
       <c r="E38" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F38" s="56" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G38" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H38" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I38" s="58"/>
       <c r="J38" s="4">
@@ -4439,10 +4478,10 @@
       <c r="K38" s="59"/>
       <c r="L38" s="56"/>
       <c r="M38" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N38" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O38" s="63"/>
       <c r="P38" s="64"/>
@@ -4454,23 +4493,23 @@
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
       <c r="A39" s="54"/>
       <c r="B39" s="117" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C39" s="118" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D39" s="54"/>
       <c r="E39" s="55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F39" s="56" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G39" s="56" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H39" s="76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I39" s="58"/>
       <c r="J39" s="4">
@@ -4479,10 +4518,10 @@
       <c r="K39" s="59"/>
       <c r="L39" s="56"/>
       <c r="M39" s="56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N39" s="60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O39" s="63"/>
       <c r="P39" s="64"/>
@@ -4493,19 +4532,19 @@
     </row>
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
       <c r="A40" s="54" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D40" s="54" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F40" s="56" t="s">
         <v>64</v>
@@ -4528,10 +4567,10 @@
         <v>33</v>
       </c>
       <c r="M40" s="56" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N40" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O40" s="63"/>
       <c r="P40" s="64"/>
@@ -4544,19 +4583,19 @@
     </row>
     <row r="41" spans="1:20" ht="18.75" customHeight="1">
       <c r="A41" s="54" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B41" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D41" s="54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E41" s="55" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F41" s="56" t="s">
         <v>64</v>
@@ -4579,10 +4618,10 @@
         <v>33</v>
       </c>
       <c r="M41" s="56" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N41" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O41" s="63"/>
       <c r="P41" s="64"/>
@@ -4595,19 +4634,19 @@
     </row>
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
       <c r="A42" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="54" t="s">
-        <v>105</v>
-      </c>
       <c r="E42" s="55" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F42" s="56" t="s">
         <v>64</v>
@@ -4630,10 +4669,10 @@
         <v>33</v>
       </c>
       <c r="M42" s="56" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N42" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O42" s="63"/>
       <c r="P42" s="67"/>
@@ -4646,19 +4685,19 @@
     </row>
     <row r="43" spans="1:20" ht="18" customHeight="1">
       <c r="A43" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B43" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="54" t="s">
+      <c r="E43" s="55" t="s">
         <v>110</v>
-      </c>
-      <c r="D43" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" s="55" t="s">
-        <v>107</v>
       </c>
       <c r="F43" s="56" t="s">
         <v>64</v>
@@ -4681,10 +4720,10 @@
         <v>33</v>
       </c>
       <c r="M43" s="56" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="N43" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O43" s="63"/>
       <c r="P43" s="67"/>
@@ -4697,22 +4736,22 @@
     </row>
     <row r="44" spans="1:20" ht="18" customHeight="1">
       <c r="A44" s="54" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C44" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D44" s="54" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E44" s="55" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F44" s="65" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G44" s="56" t="s">
         <v>29</v>
@@ -4730,10 +4769,10 @@
         <v>33</v>
       </c>
       <c r="M44" s="68" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="N44" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O44" s="63"/>
       <c r="P44" s="63">
@@ -4746,22 +4785,22 @@
     </row>
     <row r="45" spans="1:20" ht="18" customHeight="1">
       <c r="A45" s="54" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D45" s="54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E45" s="55" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F45" s="65" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G45" s="56" t="s">
         <v>29</v>
@@ -4779,10 +4818,10 @@
         <v>33</v>
       </c>
       <c r="M45" s="68" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="N45" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O45" s="63"/>
       <c r="P45" s="63">
@@ -4795,22 +4834,22 @@
     </row>
     <row r="46" spans="1:20" ht="18" customHeight="1">
       <c r="A46" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="B46" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" s="54" t="s">
-        <v>105</v>
-      </c>
       <c r="E46" s="55" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F46" s="65" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G46" s="56" t="s">
         <v>29</v>
@@ -4828,10 +4867,10 @@
         <v>33</v>
       </c>
       <c r="M46" s="68" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="N46" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O46" s="63"/>
       <c r="P46" s="63">
@@ -4844,22 +4883,22 @@
     </row>
     <row r="47" spans="1:20" ht="18" customHeight="1">
       <c r="A47" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B47" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="54" t="s">
+      <c r="E47" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="E47" s="55" t="s">
-        <v>107</v>
-      </c>
       <c r="F47" s="65" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G47" s="56" t="s">
         <v>29</v>
@@ -4877,10 +4916,10 @@
         <v>33</v>
       </c>
       <c r="M47" s="68" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="N47" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O47" s="63"/>
       <c r="P47" s="63">
@@ -4893,22 +4932,22 @@
     </row>
     <row r="48" spans="1:20" ht="18" customHeight="1">
       <c r="A48" s="54" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B48" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C48" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D48" s="54" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E48" s="55" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F48" s="65" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G48" s="56" t="s">
         <v>29</v>
@@ -4926,10 +4965,10 @@
         <v>33</v>
       </c>
       <c r="M48" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N48" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O48" s="63"/>
       <c r="P48" s="63">
@@ -4942,22 +4981,22 @@
     </row>
     <row r="49" spans="1:20" ht="18" customHeight="1">
       <c r="A49" s="54" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B49" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C49" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D49" s="54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E49" s="55" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F49" s="65" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G49" s="56" t="s">
         <v>29</v>
@@ -4975,10 +5014,10 @@
         <v>33</v>
       </c>
       <c r="M49" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N49" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O49" s="63"/>
       <c r="P49" s="63">
@@ -4991,22 +5030,22 @@
     </row>
     <row r="50" spans="1:20" ht="18" customHeight="1">
       <c r="A50" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="D50" s="54" t="s">
-        <v>105</v>
-      </c>
       <c r="E50" s="55" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F50" s="65" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G50" s="56" t="s">
         <v>29</v>
@@ -5024,10 +5063,10 @@
         <v>33</v>
       </c>
       <c r="M50" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N50" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O50" s="63"/>
       <c r="P50" s="63">
@@ -5040,22 +5079,22 @@
     </row>
     <row r="51" spans="1:20" ht="18" customHeight="1">
       <c r="A51" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="54" t="s">
+      <c r="E51" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D51" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="E51" s="55" t="s">
-        <v>107</v>
-      </c>
       <c r="F51" s="65" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G51" s="56" t="s">
         <v>29</v>
@@ -5073,10 +5112,10 @@
         <v>33</v>
       </c>
       <c r="M51" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N51" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O51" s="63"/>
       <c r="P51" s="63">
@@ -5089,22 +5128,22 @@
     </row>
     <row r="52" spans="1:20" ht="18" customHeight="1">
       <c r="A52" s="54" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B52" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C52" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D52" s="54" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E52" s="55" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F52" s="65" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G52" s="56" t="s">
         <v>29</v>
@@ -5118,13 +5157,13 @@
       </c>
       <c r="K52" s="66"/>
       <c r="L52" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M52" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N52" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O52" s="63"/>
       <c r="P52" s="67"/>
@@ -5135,22 +5174,22 @@
     </row>
     <row r="53" spans="1:20" ht="18" customHeight="1">
       <c r="A53" s="54" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C53" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D53" s="54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E53" s="55" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F53" s="65" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G53" s="56" t="s">
         <v>29</v>
@@ -5164,13 +5203,13 @@
       </c>
       <c r="K53" s="66"/>
       <c r="L53" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M53" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N53" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O53" s="63"/>
       <c r="P53" s="67"/>
@@ -5181,22 +5220,22 @@
     </row>
     <row r="54" spans="1:20" ht="18" customHeight="1">
       <c r="A54" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="54" t="s">
-        <v>105</v>
-      </c>
       <c r="E54" s="55" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F54" s="65" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G54" s="56" t="s">
         <v>29</v>
@@ -5210,13 +5249,13 @@
       </c>
       <c r="K54" s="66"/>
       <c r="L54" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M54" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N54" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O54" s="63"/>
       <c r="P54" s="67"/>
@@ -5227,22 +5266,22 @@
     </row>
     <row r="55" spans="1:20" ht="18" customHeight="1">
       <c r="A55" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B55" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="54" t="s">
+      <c r="E55" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D55" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="E55" s="55" t="s">
-        <v>107</v>
-      </c>
       <c r="F55" s="65" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G55" s="56" t="s">
         <v>29</v>
@@ -5256,13 +5295,13 @@
       </c>
       <c r="K55" s="66"/>
       <c r="L55" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M55" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="N55" s="54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O55" s="63"/>
       <c r="P55" s="67"/>
@@ -5274,13 +5313,13 @@
     <row r="56" spans="1:20" ht="18" customHeight="1">
       <c r="A56" s="54"/>
       <c r="B56" s="55" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C56" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D56" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E56" s="55"/>
       <c r="F56" s="65" t="s">
@@ -5305,10 +5344,10 @@
         <v>33</v>
       </c>
       <c r="M56" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N56" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O56" s="63"/>
       <c r="P56" s="63">
@@ -5324,13 +5363,13 @@
     <row r="57" spans="1:20" ht="18" customHeight="1">
       <c r="A57" s="54"/>
       <c r="B57" s="55" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C57" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D57" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E57" s="55"/>
       <c r="F57" s="65" t="s">
@@ -5355,10 +5394,10 @@
         <v>33</v>
       </c>
       <c r="M57" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N57" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O57" s="63"/>
       <c r="P57" s="63">
@@ -5374,13 +5413,13 @@
     <row r="58" spans="1:20" ht="18" customHeight="1">
       <c r="A58" s="54"/>
       <c r="B58" s="55" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C58" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D58" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E58" s="55"/>
       <c r="F58" s="65" t="s">
@@ -5405,10 +5444,10 @@
         <v>33</v>
       </c>
       <c r="M58" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N58" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O58" s="63"/>
       <c r="P58" s="63">
@@ -5424,13 +5463,13 @@
     <row r="59" spans="1:20" ht="18" customHeight="1">
       <c r="A59" s="54"/>
       <c r="B59" s="55" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C59" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D59" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E59" s="55"/>
       <c r="F59" s="65" t="s">
@@ -5455,10 +5494,10 @@
         <v>33</v>
       </c>
       <c r="M59" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N59" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O59" s="63"/>
       <c r="P59" s="63">
@@ -5474,13 +5513,13 @@
     <row r="60" spans="1:20" ht="18" customHeight="1">
       <c r="A60" s="54"/>
       <c r="B60" s="55" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C60" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D60" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E60" s="55"/>
       <c r="F60" s="65" t="s">
@@ -5505,10 +5544,10 @@
         <v>33</v>
       </c>
       <c r="M60" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N60" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O60" s="63"/>
       <c r="P60" s="63">
@@ -5524,13 +5563,13 @@
     <row r="61" spans="1:20" ht="18" customHeight="1">
       <c r="A61" s="54"/>
       <c r="B61" s="55" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C61" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D61" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E61" s="55"/>
       <c r="F61" s="65" t="s">
@@ -5555,10 +5594,10 @@
         <v>33</v>
       </c>
       <c r="M61" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N61" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O61" s="63"/>
       <c r="P61" s="63">
@@ -5574,13 +5613,13 @@
     <row r="62" spans="1:20" ht="18" customHeight="1">
       <c r="A62" s="54"/>
       <c r="B62" s="55" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C62" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D62" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E62" s="55"/>
       <c r="F62" s="65"/>
@@ -5592,7 +5631,7 @@
       <c r="L62" s="68"/>
       <c r="M62" s="68"/>
       <c r="N62" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O62" s="63"/>
       <c r="P62" s="63"/>
@@ -5604,13 +5643,13 @@
     <row r="63" spans="1:20" ht="18" customHeight="1">
       <c r="A63" s="54"/>
       <c r="B63" s="55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C63" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D63" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E63" s="55"/>
       <c r="F63" s="65" t="s">
@@ -5635,10 +5674,10 @@
         <v>33</v>
       </c>
       <c r="M63" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N63" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O63" s="63"/>
       <c r="P63" s="63">
@@ -5654,13 +5693,13 @@
     <row r="64" spans="1:20" ht="18" customHeight="1">
       <c r="A64" s="54"/>
       <c r="B64" s="55" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C64" s="54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D64" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E64" s="55"/>
       <c r="F64" s="65" t="s">
@@ -5685,10 +5724,10 @@
         <v>33</v>
       </c>
       <c r="M64" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N64" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O64" s="63"/>
       <c r="P64" s="63">
@@ -5704,13 +5743,13 @@
     <row r="65" spans="1:20" ht="18" customHeight="1">
       <c r="A65" s="54"/>
       <c r="B65" s="55" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C65" s="54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D65" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E65" s="55"/>
       <c r="F65" s="65" t="s">
@@ -5735,10 +5774,10 @@
         <v>33</v>
       </c>
       <c r="M65" s="68" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N65" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O65" s="63"/>
       <c r="P65" s="63">
@@ -5754,17 +5793,17 @@
     <row r="66" spans="1:20" ht="18" customHeight="1">
       <c r="A66" s="54"/>
       <c r="B66" s="55" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C66" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D66" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E66" s="55"/>
       <c r="F66" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G66" s="56" t="s">
         <v>29</v>
@@ -5785,10 +5824,10 @@
         <v>33</v>
       </c>
       <c r="M66" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N66" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O66" s="63"/>
       <c r="P66" s="63">
@@ -5804,17 +5843,17 @@
     <row r="67" spans="1:20" ht="18" customHeight="1">
       <c r="A67" s="54"/>
       <c r="B67" s="55" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C67" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D67" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E67" s="55"/>
       <c r="F67" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G67" s="56" t="s">
         <v>29</v>
@@ -5835,10 +5874,10 @@
         <v>33</v>
       </c>
       <c r="M67" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N67" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O67" s="63"/>
       <c r="P67" s="63">
@@ -5854,17 +5893,17 @@
     <row r="68" spans="1:20" ht="18" customHeight="1">
       <c r="A68" s="54"/>
       <c r="B68" s="55" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C68" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D68" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E68" s="55"/>
       <c r="F68" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G68" s="56" t="s">
         <v>29</v>
@@ -5885,10 +5924,10 @@
         <v>33</v>
       </c>
       <c r="M68" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N68" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O68" s="63"/>
       <c r="P68" s="63">
@@ -5904,17 +5943,17 @@
     <row r="69" spans="1:20" ht="18" customHeight="1">
       <c r="A69" s="54"/>
       <c r="B69" s="55" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C69" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D69" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E69" s="55"/>
       <c r="F69" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G69" s="56" t="s">
         <v>29</v>
@@ -5935,10 +5974,10 @@
         <v>33</v>
       </c>
       <c r="M69" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N69" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O69" s="63"/>
       <c r="P69" s="63">
@@ -5954,17 +5993,17 @@
     <row r="70" spans="1:20" ht="18" customHeight="1">
       <c r="A70" s="54"/>
       <c r="B70" s="55" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C70" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D70" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E70" s="55"/>
       <c r="F70" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G70" s="56" t="s">
         <v>29</v>
@@ -5985,10 +6024,10 @@
         <v>33</v>
       </c>
       <c r="M70" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N70" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O70" s="63"/>
       <c r="P70" s="63">
@@ -6004,17 +6043,17 @@
     <row r="71" spans="1:20" ht="18" customHeight="1">
       <c r="A71" s="54"/>
       <c r="B71" s="55" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C71" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D71" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E71" s="55"/>
       <c r="F71" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G71" s="56" t="s">
         <v>29</v>
@@ -6035,10 +6074,10 @@
         <v>33</v>
       </c>
       <c r="M71" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N71" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O71" s="63"/>
       <c r="P71" s="63">
@@ -6054,17 +6093,17 @@
     <row r="72" spans="1:20" ht="18" customHeight="1">
       <c r="A72" s="54"/>
       <c r="B72" s="55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C72" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D72" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E72" s="55"/>
       <c r="F72" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G72" s="56" t="s">
         <v>29</v>
@@ -6085,10 +6124,10 @@
         <v>33</v>
       </c>
       <c r="M72" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N72" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O72" s="63"/>
       <c r="P72" s="63">
@@ -6104,17 +6143,17 @@
     <row r="73" spans="1:20" ht="18" customHeight="1">
       <c r="A73" s="54"/>
       <c r="B73" s="55" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C73" s="54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D73" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E73" s="55"/>
       <c r="F73" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G73" s="56" t="s">
         <v>29</v>
@@ -6135,10 +6174,10 @@
         <v>33</v>
       </c>
       <c r="M73" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N73" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O73" s="63"/>
       <c r="P73" s="63">
@@ -6154,17 +6193,17 @@
     <row r="74" spans="1:20" ht="18" customHeight="1">
       <c r="A74" s="54"/>
       <c r="B74" s="55" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C74" s="54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D74" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E74" s="55"/>
       <c r="F74" s="65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G74" s="56" t="s">
         <v>29</v>
@@ -6185,10 +6224,10 @@
         <v>33</v>
       </c>
       <c r="M74" s="68" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="N74" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O74" s="63"/>
       <c r="P74" s="63">
@@ -6204,17 +6243,17 @@
     <row r="75" spans="1:20" ht="18" customHeight="1">
       <c r="A75" s="54"/>
       <c r="B75" s="55" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C75" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D75" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E75" s="55"/>
       <c r="F75" s="65" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G75" s="56" t="s">
         <v>29</v>
@@ -6232,10 +6271,10 @@
         <v>33</v>
       </c>
       <c r="M75" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N75" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O75" s="63"/>
       <c r="P75" s="63">
@@ -6249,17 +6288,17 @@
     <row r="76" spans="1:20" ht="18" customHeight="1">
       <c r="A76" s="54"/>
       <c r="B76" s="55" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C76" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D76" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E76" s="55"/>
       <c r="F76" s="65" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G76" s="56" t="s">
         <v>29</v>
@@ -6277,10 +6316,10 @@
         <v>33</v>
       </c>
       <c r="M76" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N76" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O76" s="63"/>
       <c r="P76" s="63">
@@ -6294,17 +6333,17 @@
     <row r="77" spans="1:20" ht="18" customHeight="1">
       <c r="A77" s="54"/>
       <c r="B77" s="55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C77" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D77" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E77" s="55"/>
       <c r="F77" s="65" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G77" s="56" t="s">
         <v>29</v>
@@ -6322,10 +6361,10 @@
         <v>33</v>
       </c>
       <c r="M77" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N77" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O77" s="63"/>
       <c r="P77" s="63">
@@ -6339,17 +6378,17 @@
     <row r="78" spans="1:20" ht="18" customHeight="1">
       <c r="A78" s="54"/>
       <c r="B78" s="55" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C78" s="54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D78" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E78" s="55"/>
       <c r="F78" s="65" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G78" s="56" t="s">
         <v>29</v>
@@ -6367,10 +6406,10 @@
         <v>33</v>
       </c>
       <c r="M78" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N78" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O78" s="63"/>
       <c r="P78" s="63">
@@ -6384,17 +6423,17 @@
     <row r="79" spans="1:20" ht="18" customHeight="1">
       <c r="A79" s="54"/>
       <c r="B79" s="55" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C79" s="54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D79" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E79" s="55"/>
       <c r="F79" s="65" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G79" s="56" t="s">
         <v>29</v>
@@ -6412,10 +6451,10 @@
         <v>33</v>
       </c>
       <c r="M79" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N79" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O79" s="63"/>
       <c r="P79" s="63">
@@ -6429,17 +6468,17 @@
     <row r="80" spans="1:20" ht="18" customHeight="1">
       <c r="A80" s="54"/>
       <c r="B80" s="55" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D80" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E80" s="55"/>
       <c r="F80" s="65" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G80" s="56" t="s">
         <v>29</v>
@@ -6453,13 +6492,13 @@
       </c>
       <c r="K80" s="67"/>
       <c r="L80" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M80" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N80" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O80" s="63"/>
       <c r="P80" s="64"/>
@@ -6471,17 +6510,17 @@
     <row r="81" spans="1:20" ht="18" customHeight="1">
       <c r="A81" s="54"/>
       <c r="B81" s="55" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C81" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D81" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E81" s="55"/>
       <c r="F81" s="65" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G81" s="56" t="s">
         <v>29</v>
@@ -6495,13 +6534,13 @@
       </c>
       <c r="K81" s="67"/>
       <c r="L81" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M81" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N81" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O81" s="63"/>
       <c r="P81" s="64"/>
@@ -6513,17 +6552,17 @@
     <row r="82" spans="1:20" ht="18" customHeight="1">
       <c r="A82" s="54"/>
       <c r="B82" s="55" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C82" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D82" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E82" s="55"/>
       <c r="F82" s="65" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G82" s="56" t="s">
         <v>29</v>
@@ -6537,13 +6576,13 @@
       </c>
       <c r="K82" s="67"/>
       <c r="L82" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M82" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N82" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O82" s="63"/>
       <c r="P82" s="64"/>
@@ -6555,17 +6594,17 @@
     <row r="83" spans="1:20" ht="18" customHeight="1">
       <c r="A83" s="54"/>
       <c r="B83" s="55" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C83" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D83" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E83" s="55"/>
       <c r="F83" s="65" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G83" s="56" t="s">
         <v>29</v>
@@ -6579,13 +6618,13 @@
       </c>
       <c r="K83" s="67"/>
       <c r="L83" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M83" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N83" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O83" s="63"/>
       <c r="P83" s="64"/>
@@ -6597,17 +6636,17 @@
     <row r="84" spans="1:20" ht="18" customHeight="1">
       <c r="A84" s="54"/>
       <c r="B84" s="55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C84" s="54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D84" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E84" s="55"/>
       <c r="F84" s="65" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G84" s="56" t="s">
         <v>29</v>
@@ -6621,13 +6660,13 @@
       </c>
       <c r="K84" s="66"/>
       <c r="L84" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M84" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N84" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O84" s="63"/>
       <c r="P84" s="64"/>
@@ -6639,17 +6678,17 @@
     <row r="85" spans="1:20" ht="18" customHeight="1">
       <c r="A85" s="54"/>
       <c r="B85" s="55" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C85" s="54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D85" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E85" s="55"/>
       <c r="F85" s="65" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G85" s="56" t="s">
         <v>29</v>
@@ -6663,13 +6702,13 @@
       </c>
       <c r="K85" s="66"/>
       <c r="L85" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M85" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N85" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O85" s="63"/>
       <c r="P85" s="64"/>
@@ -6681,17 +6720,17 @@
     <row r="86" spans="1:20" ht="18" customHeight="1">
       <c r="A86" s="54"/>
       <c r="B86" s="55" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C86" s="54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D86" s="54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E86" s="55"/>
       <c r="F86" s="65" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G86" s="56" t="s">
         <v>29</v>
@@ -6705,13 +6744,13 @@
       </c>
       <c r="K86" s="66"/>
       <c r="L86" s="68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M86" s="68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N86" s="54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O86" s="63"/>
       <c r="P86" s="64"/>
@@ -6721,108 +6760,256 @@
       <c r="T86" s="9"/>
     </row>
     <row r="87" spans="1:20" ht="18" customHeight="1">
-      <c r="A87" s="54"/>
-      <c r="B87" s="55"/>
-      <c r="C87" s="54"/>
-      <c r="D87" s="54"/>
+      <c r="A87" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B87" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C87" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D87" s="54" t="s">
+        <v>66</v>
+      </c>
       <c r="E87" s="55"/>
-      <c r="F87" s="56"/>
-      <c r="G87" s="56"/>
+      <c r="F87" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="G87" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H87" s="57"/>
-      <c r="I87" s="58"/>
-      <c r="J87" s="66"/>
-      <c r="K87" s="66"/>
-      <c r="L87" s="68"/>
-      <c r="M87" s="68"/>
-      <c r="N87" s="54"/>
+      <c r="I87" s="58">
+        <v>298</v>
+      </c>
+      <c r="J87" s="66">
+        <f t="shared" ref="J87:K90" si="10">P87*9807000</f>
+        <v>5118273300</v>
+      </c>
+      <c r="K87" s="66">
+        <f t="shared" si="10"/>
+        <v>196140000</v>
+      </c>
+      <c r="L87" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M87" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="N87" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O87" s="63"/>
-      <c r="P87" s="64"/>
-      <c r="Q87" s="64"/>
+      <c r="P87" s="64">
+        <v>521.9</v>
+      </c>
+      <c r="Q87" s="64">
+        <v>20</v>
+      </c>
       <c r="R87" s="63"/>
       <c r="S87" s="9"/>
       <c r="T87" s="9"/>
     </row>
     <row r="88" spans="1:20" ht="18" customHeight="1">
-      <c r="A88" s="54"/>
-      <c r="B88" s="55"/>
-      <c r="C88" s="54"/>
-      <c r="D88" s="54"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="56"/>
-      <c r="G88" s="56"/>
+      <c r="A88" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B88" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C88" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D88" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E88" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="F88" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="G88" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H88" s="57"/>
-      <c r="I88" s="58"/>
-      <c r="J88" s="66"/>
-      <c r="K88" s="66"/>
-      <c r="L88" s="68"/>
-      <c r="M88" s="68"/>
-      <c r="N88" s="54"/>
+      <c r="I88" s="58">
+        <v>298</v>
+      </c>
+      <c r="J88" s="66">
+        <f t="shared" si="10"/>
+        <v>5797898400</v>
+      </c>
+      <c r="K88" s="66">
+        <f t="shared" si="10"/>
+        <v>196140000</v>
+      </c>
+      <c r="L88" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M88" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="N88" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O88" s="63"/>
-      <c r="P88" s="64"/>
-      <c r="Q88" s="64"/>
+      <c r="P88" s="64">
+        <v>591.20000000000005</v>
+      </c>
+      <c r="Q88" s="64">
+        <v>20</v>
+      </c>
       <c r="R88" s="63"/>
       <c r="S88" s="9"/>
       <c r="T88" s="9"/>
     </row>
     <row r="89" spans="1:20" ht="18" customHeight="1">
-      <c r="A89" s="54"/>
-      <c r="B89" s="55"/>
-      <c r="C89" s="54"/>
-      <c r="D89" s="54"/>
-      <c r="E89" s="55"/>
-      <c r="F89" s="56"/>
-      <c r="G89" s="56"/>
+      <c r="A89" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B89" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C89" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D89" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E89" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F89" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="G89" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H89" s="57"/>
-      <c r="I89" s="58"/>
-      <c r="J89" s="66"/>
-      <c r="K89" s="59"/>
-      <c r="L89" s="68"/>
-      <c r="M89" s="68"/>
-      <c r="N89" s="54"/>
+      <c r="I89" s="58">
+        <v>298</v>
+      </c>
+      <c r="J89" s="66">
+        <f t="shared" si="10"/>
+        <v>4983917400</v>
+      </c>
+      <c r="K89" s="66">
+        <f t="shared" si="10"/>
+        <v>196140000</v>
+      </c>
+      <c r="L89" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M89" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="N89" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O89" s="63"/>
-      <c r="P89" s="64"/>
-      <c r="Q89" s="64"/>
+      <c r="P89" s="64">
+        <v>508.2</v>
+      </c>
+      <c r="Q89" s="64">
+        <v>20</v>
+      </c>
       <c r="R89" s="63"/>
       <c r="S89" s="9"/>
       <c r="T89" s="9"/>
     </row>
     <row r="90" spans="1:20" ht="18" customHeight="1">
-      <c r="A90" s="54"/>
-      <c r="B90" s="55"/>
-      <c r="C90" s="54"/>
-      <c r="D90" s="54"/>
-      <c r="E90" s="55"/>
-      <c r="F90" s="56"/>
-      <c r="G90" s="56"/>
+      <c r="A90" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C90" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D90" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E90" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F90" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="G90" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H90" s="57"/>
-      <c r="I90" s="58"/>
-      <c r="J90" s="59"/>
-      <c r="K90" s="59"/>
-      <c r="L90" s="68"/>
-      <c r="M90" s="68"/>
-      <c r="N90" s="54"/>
+      <c r="I90" s="58">
+        <v>298</v>
+      </c>
+      <c r="J90" s="66">
+        <f t="shared" si="10"/>
+        <v>4635768900</v>
+      </c>
+      <c r="K90" s="66">
+        <f t="shared" si="10"/>
+        <v>294210000</v>
+      </c>
+      <c r="L90" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M90" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="N90" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O90" s="63"/>
-      <c r="P90" s="64"/>
-      <c r="Q90" s="64"/>
+      <c r="P90" s="64">
+        <v>472.7</v>
+      </c>
+      <c r="Q90" s="64">
+        <v>30</v>
+      </c>
       <c r="R90" s="63"/>
       <c r="S90" s="9"/>
       <c r="T90" s="9"/>
     </row>
     <row r="91" spans="1:20" ht="18" customHeight="1">
-      <c r="A91" s="54"/>
-      <c r="B91" s="55"/>
-      <c r="C91" s="54"/>
-      <c r="D91" s="54"/>
+      <c r="A91" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C91" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D91" s="54" t="s">
+        <v>66</v>
+      </c>
       <c r="E91" s="55"/>
-      <c r="F91" s="56"/>
-      <c r="G91" s="56"/>
+      <c r="F91" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G91" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H91" s="57"/>
-      <c r="I91" s="58"/>
-      <c r="J91" s="59"/>
+      <c r="I91" s="58">
+        <v>298</v>
+      </c>
+      <c r="J91" s="59">
+        <v>1462000000</v>
+      </c>
       <c r="K91" s="59"/>
-      <c r="L91" s="56"/>
-      <c r="M91" s="56"/>
-      <c r="N91" s="54"/>
+      <c r="L91" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M91" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N91" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O91" s="63"/>
       <c r="P91" s="67"/>
       <c r="Q91" s="64"/>
@@ -6831,20 +7018,44 @@
       <c r="T91" s="9"/>
     </row>
     <row r="92" spans="1:20" ht="18" customHeight="1">
-      <c r="A92" s="54"/>
-      <c r="B92" s="55"/>
-      <c r="C92" s="54"/>
-      <c r="D92" s="54"/>
-      <c r="E92" s="55"/>
-      <c r="F92" s="56"/>
-      <c r="G92" s="56"/>
+      <c r="A92" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C92" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D92" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E92" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="F92" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G92" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H92" s="57"/>
-      <c r="I92" s="58"/>
-      <c r="J92" s="59"/>
+      <c r="I92" s="58">
+        <v>298</v>
+      </c>
+      <c r="J92" s="59">
+        <v>1538000000</v>
+      </c>
       <c r="K92" s="59"/>
-      <c r="L92" s="56"/>
-      <c r="M92" s="56"/>
-      <c r="N92" s="54"/>
+      <c r="L92" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M92" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N92" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O92" s="63"/>
       <c r="P92" s="67"/>
       <c r="Q92" s="64"/>
@@ -6853,20 +7064,44 @@
       <c r="T92" s="9"/>
     </row>
     <row r="93" spans="1:20" ht="18" customHeight="1">
-      <c r="A93" s="54"/>
-      <c r="B93" s="55"/>
-      <c r="C93" s="54"/>
-      <c r="D93" s="54"/>
-      <c r="E93" s="55"/>
-      <c r="F93" s="56"/>
-      <c r="G93" s="56"/>
+      <c r="A93" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D93" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E93" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F93" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G93" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H93" s="57"/>
-      <c r="I93" s="58"/>
-      <c r="J93" s="59"/>
+      <c r="I93" s="58">
+        <v>298</v>
+      </c>
+      <c r="J93" s="59">
+        <v>1474000000</v>
+      </c>
       <c r="K93" s="59"/>
-      <c r="L93" s="56"/>
-      <c r="M93" s="56"/>
-      <c r="N93" s="54"/>
+      <c r="L93" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M93" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N93" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O93" s="63"/>
       <c r="P93" s="67"/>
       <c r="Q93" s="64"/>
@@ -6875,20 +7110,44 @@
       <c r="T93" s="9"/>
     </row>
     <row r="94" spans="1:20" ht="18" customHeight="1">
-      <c r="A94" s="54"/>
-      <c r="B94" s="55"/>
-      <c r="C94" s="54"/>
-      <c r="D94" s="54"/>
-      <c r="E94" s="55"/>
-      <c r="F94" s="56"/>
-      <c r="G94" s="56"/>
+      <c r="A94" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B94" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C94" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D94" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E94" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F94" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G94" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H94" s="57"/>
-      <c r="I94" s="58"/>
-      <c r="J94" s="59"/>
+      <c r="I94" s="58">
+        <v>298</v>
+      </c>
+      <c r="J94" s="59">
+        <v>1458000000</v>
+      </c>
       <c r="K94" s="59"/>
-      <c r="L94" s="56"/>
-      <c r="M94" s="56"/>
-      <c r="N94" s="54"/>
+      <c r="L94" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M94" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N94" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O94" s="63"/>
       <c r="P94" s="67"/>
       <c r="Q94" s="64"/>
@@ -6897,20 +7156,42 @@
       <c r="T94" s="9"/>
     </row>
     <row r="95" spans="1:20" ht="18" customHeight="1">
-      <c r="A95" s="54"/>
-      <c r="B95" s="55"/>
-      <c r="C95" s="54"/>
-      <c r="D95" s="54"/>
+      <c r="A95" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B95" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C95" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D95" s="54" t="s">
+        <v>66</v>
+      </c>
       <c r="E95" s="55"/>
-      <c r="F95" s="56"/>
-      <c r="G95" s="56"/>
+      <c r="F95" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="G95" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H95" s="57"/>
-      <c r="I95" s="58"/>
-      <c r="J95" s="59"/>
+      <c r="I95" s="58">
+        <v>298</v>
+      </c>
+      <c r="J95" s="59">
+        <v>2158000000</v>
+      </c>
       <c r="K95" s="59"/>
-      <c r="L95" s="56"/>
-      <c r="M95" s="56"/>
-      <c r="N95" s="54"/>
+      <c r="L95" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M95" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N95" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O95" s="63"/>
       <c r="P95" s="67"/>
       <c r="Q95" s="64"/>
@@ -6919,20 +7200,44 @@
       <c r="T95" s="9"/>
     </row>
     <row r="96" spans="1:20" ht="18" customHeight="1">
-      <c r="A96" s="70"/>
-      <c r="B96" s="55"/>
-      <c r="C96" s="54"/>
-      <c r="D96" s="54"/>
-      <c r="E96" s="55"/>
-      <c r="F96" s="56"/>
-      <c r="G96" s="56"/>
+      <c r="A96" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B96" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C96" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D96" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E96" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="F96" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="G96" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H96" s="57"/>
-      <c r="I96" s="58"/>
-      <c r="J96" s="59"/>
+      <c r="I96" s="58">
+        <v>298</v>
+      </c>
+      <c r="J96" s="59">
+        <v>2193000000</v>
+      </c>
       <c r="K96" s="59"/>
-      <c r="L96" s="56"/>
-      <c r="M96" s="56"/>
-      <c r="N96" s="54"/>
+      <c r="L96" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M96" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N96" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O96" s="63"/>
       <c r="P96" s="67"/>
       <c r="Q96" s="64"/>
@@ -6941,20 +7246,44 @@
       <c r="T96" s="9"/>
     </row>
     <row r="97" spans="1:20" ht="18" customHeight="1">
-      <c r="A97" s="70"/>
-      <c r="B97" s="55"/>
-      <c r="C97" s="54"/>
-      <c r="D97" s="54"/>
-      <c r="E97" s="55"/>
-      <c r="F97" s="56"/>
-      <c r="G97" s="56"/>
+      <c r="A97" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B97" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C97" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D97" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E97" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F97" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="G97" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H97" s="57"/>
-      <c r="I97" s="58"/>
-      <c r="J97" s="59"/>
+      <c r="I97" s="58">
+        <v>298</v>
+      </c>
+      <c r="J97" s="59">
+        <v>2105000000</v>
+      </c>
       <c r="K97" s="66"/>
-      <c r="L97" s="56"/>
-      <c r="M97" s="56"/>
-      <c r="N97" s="54"/>
+      <c r="L97" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M97" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N97" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O97" s="63"/>
       <c r="P97" s="64"/>
       <c r="Q97" s="64"/>
@@ -6963,20 +7292,44 @@
       <c r="T97" s="9"/>
     </row>
     <row r="98" spans="1:20" ht="18" customHeight="1">
-      <c r="A98" s="70"/>
-      <c r="B98" s="55"/>
-      <c r="C98" s="54"/>
-      <c r="D98" s="54"/>
-      <c r="E98" s="55"/>
-      <c r="F98" s="56"/>
-      <c r="G98" s="56"/>
+      <c r="A98" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B98" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C98" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D98" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E98" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F98" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="G98" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H98" s="57"/>
-      <c r="I98" s="58"/>
-      <c r="J98" s="59"/>
+      <c r="I98" s="58">
+        <v>298</v>
+      </c>
+      <c r="J98" s="59">
+        <v>2017000000</v>
+      </c>
       <c r="K98" s="66"/>
-      <c r="L98" s="56"/>
-      <c r="M98" s="56"/>
-      <c r="N98" s="54"/>
+      <c r="L98" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M98" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N98" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O98" s="63"/>
       <c r="P98" s="64"/>
       <c r="Q98" s="4"/>
@@ -6985,20 +7338,42 @@
       <c r="T98" s="9"/>
     </row>
     <row r="99" spans="1:20" ht="18" customHeight="1">
-      <c r="A99" s="70"/>
-      <c r="B99" s="55"/>
-      <c r="C99" s="54"/>
-      <c r="D99" s="54"/>
+      <c r="A99" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B99" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C99" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D99" s="54" t="s">
+        <v>66</v>
+      </c>
       <c r="E99" s="55"/>
-      <c r="F99" s="56"/>
-      <c r="G99" s="56"/>
+      <c r="F99" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G99" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H99" s="57"/>
-      <c r="I99" s="58"/>
-      <c r="J99" s="59"/>
+      <c r="I99" s="58">
+        <v>298</v>
+      </c>
+      <c r="J99" s="63">
+        <v>26.481481481481399</v>
+      </c>
       <c r="K99" s="66"/>
-      <c r="L99" s="56"/>
-      <c r="M99" s="56"/>
-      <c r="N99" s="54"/>
+      <c r="L99" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="M99" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="N99" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O99" s="63"/>
       <c r="P99" s="67"/>
       <c r="Q99" s="4"/>
@@ -7007,20 +7382,44 @@
       <c r="T99" s="9"/>
     </row>
     <row r="100" spans="1:20" ht="18" customHeight="1">
-      <c r="A100" s="70"/>
-      <c r="B100" s="55"/>
-      <c r="C100" s="54"/>
-      <c r="D100" s="54"/>
-      <c r="E100" s="55"/>
-      <c r="F100" s="56"/>
-      <c r="G100" s="56"/>
+      <c r="A100" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B100" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C100" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D100" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E100" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="F100" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G100" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H100" s="57"/>
-      <c r="I100" s="58"/>
-      <c r="J100" s="59"/>
+      <c r="I100" s="58">
+        <v>298</v>
+      </c>
+      <c r="J100" s="63">
+        <v>23.796296296296202</v>
+      </c>
       <c r="K100" s="66"/>
-      <c r="L100" s="56"/>
-      <c r="M100" s="56"/>
-      <c r="N100" s="54"/>
+      <c r="L100" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="M100" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="N100" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O100" s="63"/>
       <c r="P100" s="67"/>
       <c r="Q100" s="64"/>
@@ -7029,20 +7428,44 @@
       <c r="T100" s="9"/>
     </row>
     <row r="101" spans="1:20" ht="18" customHeight="1">
-      <c r="A101" s="70"/>
-      <c r="B101" s="55"/>
-      <c r="C101" s="54"/>
-      <c r="D101" s="54"/>
-      <c r="E101" s="55"/>
-      <c r="F101" s="56"/>
-      <c r="G101" s="56"/>
+      <c r="A101" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B101" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C101" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D101" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E101" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F101" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G101" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H101" s="57"/>
-      <c r="I101" s="58"/>
-      <c r="J101" s="59"/>
+      <c r="I101" s="58">
+        <v>298</v>
+      </c>
+      <c r="J101" s="63">
+        <v>27.469135802469101</v>
+      </c>
       <c r="K101" s="66"/>
-      <c r="L101" s="56"/>
-      <c r="M101" s="56"/>
-      <c r="N101" s="54"/>
+      <c r="L101" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="M101" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="N101" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O101" s="63"/>
       <c r="P101" s="64"/>
       <c r="Q101" s="64"/>
@@ -7051,20 +7474,44 @@
       <c r="T101" s="9"/>
     </row>
     <row r="102" spans="1:20" ht="18" customHeight="1">
-      <c r="A102" s="70"/>
-      <c r="B102" s="55"/>
-      <c r="C102" s="54"/>
-      <c r="D102" s="54"/>
-      <c r="E102" s="55"/>
-      <c r="F102" s="56"/>
-      <c r="G102" s="56"/>
+      <c r="A102" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B102" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C102" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D102" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E102" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F102" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G102" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H102" s="57"/>
-      <c r="I102" s="58"/>
-      <c r="J102" s="64"/>
+      <c r="I102" s="58">
+        <v>298</v>
+      </c>
+      <c r="J102" s="63">
+        <v>28.858024691358001</v>
+      </c>
       <c r="K102" s="66"/>
-      <c r="L102" s="56"/>
-      <c r="M102" s="56"/>
-      <c r="N102" s="54"/>
+      <c r="L102" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="M102" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="N102" s="54" t="s">
+        <v>138</v>
+      </c>
       <c r="O102" s="63"/>
       <c r="P102" s="64"/>
       <c r="Q102" s="64"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2025.147831`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040EB067-3A85-3E46-B9BE-7E43CC5AC362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D9847F-4AF4-D14C-BE86-BEDA6FDF7C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="8800" windowWidth="31040" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="4740" windowWidth="31040" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="144">
   <si>
     <r>
       <rPr>
@@ -354,6 +354,9 @@
     <t>UCS</t>
   </si>
   <si>
+    <t>VAM</t>
+  </si>
+  <si>
     <t>T5</t>
   </si>
   <si>
@@ -547,6 +550,18 @@
   </si>
   <si>
     <t>10.1016/j.ijrmhm.2025.107039</t>
+  </si>
+  <si>
+    <t>Al6.3 Ti34.28 Zr25.81 Nb16.9 Ta16.71</t>
+  </si>
+  <si>
+    <t>DED</t>
+  </si>
+  <si>
+    <t>LDED with laser power of 1200-1800W scanning 300-600 mm/min at powder feed 4 g/min in protective gas flow rate of 4-8 L/min rising height of 1.5 mm and alternating scanning strategy between layers; properties averaged for 2 directions</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2025.147831</t>
   </si>
 </sst>
 </file>
@@ -2814,8 +2829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T856"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B90" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N106" sqref="N106"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B93" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N113" sqref="N113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3173,16 +3188,16 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="54"/>
       <c r="B10" s="55" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C10" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F10" s="56" t="s">
         <v>63</v>
@@ -3206,10 +3221,10 @@
         <v>33</v>
       </c>
       <c r="M10" s="56" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N10" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="4">
@@ -3227,16 +3242,16 @@
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="54"/>
       <c r="B11" s="55" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C11" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F11" s="56" t="s">
         <v>63</v>
@@ -3260,10 +3275,10 @@
         <v>33</v>
       </c>
       <c r="M11" s="56" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N11" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="4">
@@ -3281,16 +3296,16 @@
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="54"/>
       <c r="B12" s="55" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C12" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F12" s="56" t="s">
         <v>63</v>
@@ -3314,10 +3329,10 @@
         <v>33</v>
       </c>
       <c r="M12" s="56" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N12" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="4">
@@ -3335,16 +3350,16 @@
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="54"/>
       <c r="B13" s="55" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C13" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>63</v>
@@ -3368,10 +3383,10 @@
         <v>33</v>
       </c>
       <c r="M13" s="56" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N13" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="4">
@@ -3389,16 +3404,16 @@
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="54"/>
       <c r="B14" s="55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C14" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F14" s="56" t="s">
         <v>63</v>
@@ -3422,10 +3437,10 @@
         <v>33</v>
       </c>
       <c r="M14" s="56" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N14" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="4">
@@ -3443,19 +3458,19 @@
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="54"/>
       <c r="B15" s="55" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C15" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G15" s="56" t="s">
         <v>29</v>
@@ -3473,10 +3488,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="56" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N15" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9">
@@ -3490,19 +3505,19 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="54"/>
       <c r="B16" s="55" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G16" s="56" t="s">
         <v>29</v>
@@ -3520,10 +3535,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="56" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N16" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="9">
@@ -3537,19 +3552,19 @@
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="55" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C17" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G17" s="56" t="s">
         <v>29</v>
@@ -3567,10 +3582,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="56" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N17" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="9">
@@ -3584,19 +3599,19 @@
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="55" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G18" s="56" t="s">
         <v>29</v>
@@ -3614,10 +3629,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="56" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N18" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="9">
@@ -3631,19 +3646,19 @@
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C19" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G19" s="56" t="s">
         <v>29</v>
@@ -3661,10 +3676,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="56" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N19" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="9">
@@ -3678,19 +3693,19 @@
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="55" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C20" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F20" s="56" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G20" s="56" t="s">
         <v>29</v>
@@ -3708,10 +3723,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N20" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9">
@@ -3725,19 +3740,19 @@
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="55" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C21" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F21" s="56" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G21" s="56" t="s">
         <v>29</v>
@@ -3755,10 +3770,10 @@
         <v>33</v>
       </c>
       <c r="M21" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N21" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="9">
@@ -3772,19 +3787,19 @@
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="55" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C22" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G22" s="56" t="s">
         <v>29</v>
@@ -3802,10 +3817,10 @@
         <v>33</v>
       </c>
       <c r="M22" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N22" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9">
@@ -3819,19 +3834,19 @@
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="54"/>
       <c r="B23" s="55" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C23" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F23" s="56" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G23" s="56" t="s">
         <v>29</v>
@@ -3849,10 +3864,10 @@
         <v>33</v>
       </c>
       <c r="M23" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N23" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="9">
@@ -3866,19 +3881,19 @@
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="54"/>
       <c r="B24" s="55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C24" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G24" s="56" t="s">
         <v>29</v>
@@ -3896,10 +3911,10 @@
         <v>33</v>
       </c>
       <c r="M24" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N24" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O24" s="9"/>
       <c r="P24" s="9">
@@ -3913,19 +3928,19 @@
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="54"/>
       <c r="B25" s="114" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C25" s="115" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="115" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E25" s="116" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F25" s="56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G25" s="56" t="s">
         <v>29</v>
@@ -3942,10 +3957,10 @@
         <v>71</v>
       </c>
       <c r="M25" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N25" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O25" s="9"/>
       <c r="P25" s="4"/>
@@ -3957,19 +3972,19 @@
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="54"/>
       <c r="B26" s="117" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D26" s="118" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E26" s="119" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G26" s="56" t="s">
         <v>29</v>
@@ -3986,10 +4001,10 @@
         <v>71</v>
       </c>
       <c r="M26" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N26" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="61"/>
@@ -4001,19 +4016,19 @@
     <row r="27" spans="1:20" ht="18.75" customHeight="1">
       <c r="A27" s="54"/>
       <c r="B27" s="117" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C27" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D27" s="118" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E27" s="119" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F27" s="56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G27" s="56" t="s">
         <v>29</v>
@@ -4030,10 +4045,10 @@
         <v>71</v>
       </c>
       <c r="M27" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N27" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O27" s="9"/>
       <c r="P27" s="61"/>
@@ -4045,19 +4060,19 @@
     <row r="28" spans="1:20" ht="18.75" customHeight="1">
       <c r="A28" s="54"/>
       <c r="B28" s="117" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C28" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D28" s="118" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E28" s="119" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F28" s="56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G28" s="56" t="s">
         <v>29</v>
@@ -4074,10 +4089,10 @@
         <v>71</v>
       </c>
       <c r="M28" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N28" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O28" s="9"/>
       <c r="P28" s="61"/>
@@ -4089,19 +4104,19 @@
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
       <c r="A29" s="54"/>
       <c r="B29" s="117" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D29" s="118" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E29" s="119" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F29" s="56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G29" s="56" t="s">
         <v>29</v>
@@ -4118,10 +4133,10 @@
         <v>71</v>
       </c>
       <c r="M29" s="76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N29" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O29" s="9"/>
       <c r="P29" s="61"/>
@@ -4133,23 +4148,23 @@
     <row r="30" spans="1:20" ht="18.75" customHeight="1">
       <c r="A30" s="54"/>
       <c r="B30" s="114" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C30" s="115" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="54"/>
       <c r="E30" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F30" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H30" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="1">
@@ -4161,7 +4176,7 @@
         <v>67</v>
       </c>
       <c r="N30" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O30" s="9"/>
       <c r="P30" s="61"/>
@@ -4173,23 +4188,23 @@
     <row r="31" spans="1:20" ht="18.75" customHeight="1">
       <c r="A31" s="54"/>
       <c r="B31" s="117" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C31" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="54"/>
       <c r="E31" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F31" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="G31" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H31" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="1">
@@ -4201,7 +4216,7 @@
         <v>67</v>
       </c>
       <c r="N31" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O31" s="9"/>
       <c r="P31" s="61"/>
@@ -4213,23 +4228,23 @@
     <row r="32" spans="1:20" ht="18.75" customHeight="1">
       <c r="A32" s="54"/>
       <c r="B32" s="117" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C32" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H32" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F32" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="G32" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H32" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="1">
@@ -4241,7 +4256,7 @@
         <v>67</v>
       </c>
       <c r="N32" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O32" s="9"/>
       <c r="P32" s="61"/>
@@ -4253,23 +4268,23 @@
     <row r="33" spans="1:20" ht="18.75" customHeight="1">
       <c r="A33" s="54"/>
       <c r="B33" s="117" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C33" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H33" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F33" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="G33" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="1">
@@ -4281,7 +4296,7 @@
         <v>67</v>
       </c>
       <c r="N33" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="61"/>
@@ -4293,23 +4308,23 @@
     <row r="34" spans="1:20" ht="18.75" customHeight="1">
       <c r="A34" s="54"/>
       <c r="B34" s="117" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C34" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D34" s="54"/>
       <c r="E34" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F34" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H34" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="1">
@@ -4321,7 +4336,7 @@
         <v>67</v>
       </c>
       <c r="N34" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O34" s="9"/>
       <c r="P34" s="4"/>
@@ -4333,23 +4348,23 @@
     <row r="35" spans="1:20" ht="18.75" customHeight="1">
       <c r="A35" s="54"/>
       <c r="B35" s="114" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C35" s="115" t="s">
         <v>68</v>
       </c>
       <c r="D35" s="54"/>
       <c r="E35" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F35" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H35" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4">
@@ -4361,7 +4376,7 @@
         <v>67</v>
       </c>
       <c r="N35" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O35" s="9"/>
       <c r="P35" s="4"/>
@@ -4373,23 +4388,23 @@
     <row r="36" spans="1:20" ht="18.75" customHeight="1">
       <c r="A36" s="54"/>
       <c r="B36" s="117" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D36" s="54"/>
       <c r="E36" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F36" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="G36" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H36" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4">
@@ -4401,7 +4416,7 @@
         <v>67</v>
       </c>
       <c r="N36" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="4"/>
@@ -4413,23 +4428,23 @@
     <row r="37" spans="1:20" ht="18.75" customHeight="1">
       <c r="A37" s="54"/>
       <c r="B37" s="117" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C37" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D37" s="54"/>
       <c r="E37" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H37" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F37" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="G37" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H37" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4">
@@ -4441,7 +4456,7 @@
         <v>67</v>
       </c>
       <c r="N37" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O37" s="9"/>
       <c r="P37" s="4"/>
@@ -4453,23 +4468,23 @@
     <row r="38" spans="1:20" ht="18.75" customHeight="1">
       <c r="A38" s="54"/>
       <c r="B38" s="117" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C38" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D38" s="54"/>
       <c r="E38" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H38" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F38" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="G38" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H38" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I38" s="58"/>
       <c r="J38" s="4">
@@ -4481,7 +4496,7 @@
         <v>67</v>
       </c>
       <c r="N38" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O38" s="63"/>
       <c r="P38" s="64"/>
@@ -4493,23 +4508,23 @@
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
       <c r="A39" s="54"/>
       <c r="B39" s="117" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C39" s="118" t="s">
         <v>68</v>
       </c>
       <c r="D39" s="54"/>
       <c r="E39" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G39" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" s="76" t="s">
         <v>95</v>
-      </c>
-      <c r="F39" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="G39" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H39" s="76" t="s">
-        <v>94</v>
       </c>
       <c r="I39" s="58"/>
       <c r="J39" s="4">
@@ -4521,7 +4536,7 @@
         <v>67</v>
       </c>
       <c r="N39" s="60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O39" s="63"/>
       <c r="P39" s="64"/>
@@ -4532,19 +4547,19 @@
     </row>
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
       <c r="A40" s="54" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C40" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D40" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="55" t="s">
         <v>99</v>
-      </c>
-      <c r="E40" s="55" t="s">
-        <v>98</v>
       </c>
       <c r="F40" s="56" t="s">
         <v>64</v>
@@ -4567,10 +4582,10 @@
         <v>33</v>
       </c>
       <c r="M40" s="56" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N40" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O40" s="63"/>
       <c r="P40" s="64"/>
@@ -4583,19 +4598,19 @@
     </row>
     <row r="41" spans="1:20" ht="18.75" customHeight="1">
       <c r="A41" s="54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B41" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C41" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D41" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="55" t="s">
         <v>101</v>
-      </c>
-      <c r="E41" s="55" t="s">
-        <v>100</v>
       </c>
       <c r="F41" s="56" t="s">
         <v>64</v>
@@ -4618,10 +4633,10 @@
         <v>33</v>
       </c>
       <c r="M41" s="56" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N41" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O41" s="63"/>
       <c r="P41" s="64"/>
@@ -4634,19 +4649,19 @@
     </row>
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
       <c r="A42" s="54" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B42" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D42" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="55" t="s">
         <v>108</v>
-      </c>
-      <c r="E42" s="55" t="s">
-        <v>107</v>
       </c>
       <c r="F42" s="56" t="s">
         <v>64</v>
@@ -4669,10 +4684,10 @@
         <v>33</v>
       </c>
       <c r="M42" s="56" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N42" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O42" s="63"/>
       <c r="P42" s="67"/>
@@ -4685,19 +4700,19 @@
     </row>
     <row r="43" spans="1:20" ht="18" customHeight="1">
       <c r="A43" s="54" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B43" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D43" s="54" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E43" s="55" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F43" s="56" t="s">
         <v>64</v>
@@ -4720,10 +4735,10 @@
         <v>33</v>
       </c>
       <c r="M43" s="56" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N43" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O43" s="63"/>
       <c r="P43" s="67"/>
@@ -4736,22 +4751,22 @@
     </row>
     <row r="44" spans="1:20" ht="18" customHeight="1">
       <c r="A44" s="54" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C44" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D44" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="E44" s="55" t="s">
-        <v>98</v>
-      </c>
       <c r="F44" s="65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G44" s="56" t="s">
         <v>29</v>
@@ -4769,10 +4784,10 @@
         <v>33</v>
       </c>
       <c r="M44" s="68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N44" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O44" s="63"/>
       <c r="P44" s="63">
@@ -4785,22 +4800,22 @@
     </row>
     <row r="45" spans="1:20" ht="18" customHeight="1">
       <c r="A45" s="54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C45" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D45" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="E45" s="55" t="s">
-        <v>100</v>
-      </c>
       <c r="F45" s="65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G45" s="56" t="s">
         <v>29</v>
@@ -4818,10 +4833,10 @@
         <v>33</v>
       </c>
       <c r="M45" s="68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N45" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O45" s="63"/>
       <c r="P45" s="63">
@@ -4834,22 +4849,22 @@
     </row>
     <row r="46" spans="1:20" ht="18" customHeight="1">
       <c r="A46" s="54" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B46" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C46" s="54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D46" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="55" t="s">
-        <v>107</v>
-      </c>
       <c r="F46" s="65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G46" s="56" t="s">
         <v>29</v>
@@ -4867,10 +4882,10 @@
         <v>33</v>
       </c>
       <c r="M46" s="68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N46" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O46" s="63"/>
       <c r="P46" s="63">
@@ -4883,22 +4898,22 @@
     </row>
     <row r="47" spans="1:20" ht="18" customHeight="1">
       <c r="A47" s="54" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B47" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C47" s="54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D47" s="54" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E47" s="55" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F47" s="65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G47" s="56" t="s">
         <v>29</v>
@@ -4916,10 +4931,10 @@
         <v>33</v>
       </c>
       <c r="M47" s="68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N47" s="54" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O47" s="63"/>
       <c r="P47" s="63">
@@ -4932,22 +4947,22 @@
     </row>
     <row r="48" spans="1:20" ht="18" customHeight="1">
       <c r="A48" s="54" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B48" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C48" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D48" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="55" t="s">
-        <v>98</v>
-      </c>
       <c r="F48" s="65" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G48" s="56" t="s">
         <v>29</v>
@@ -4965,10 +4980,10 @@
         <v>33</v>
       </c>
       <c r="M48" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N48" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="N48" s="54" t="s">
-        <v>102</v>
       </c>
       <c r="O48" s="63"/>
       <c r="P48" s="63">
@@ -4981,22 +4996,22 @@
     </row>
     <row r="49" spans="1:20" ht="18" customHeight="1">
       <c r="A49" s="54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B49" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C49" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D49" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="E49" s="55" t="s">
-        <v>100</v>
-      </c>
       <c r="F49" s="65" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G49" s="56" t="s">
         <v>29</v>
@@ -5014,10 +5029,10 @@
         <v>33</v>
       </c>
       <c r="M49" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N49" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="N49" s="54" t="s">
-        <v>102</v>
       </c>
       <c r="O49" s="63"/>
       <c r="P49" s="63">
@@ -5030,22 +5045,22 @@
     </row>
     <row r="50" spans="1:20" ht="18" customHeight="1">
       <c r="A50" s="54" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B50" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C50" s="54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D50" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="E50" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="E50" s="55" t="s">
-        <v>107</v>
-      </c>
       <c r="F50" s="65" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G50" s="56" t="s">
         <v>29</v>
@@ -5063,10 +5078,10 @@
         <v>33</v>
       </c>
       <c r="M50" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N50" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="N50" s="54" t="s">
-        <v>102</v>
       </c>
       <c r="O50" s="63"/>
       <c r="P50" s="63">
@@ -5079,22 +5094,22 @@
     </row>
     <row r="51" spans="1:20" ht="18" customHeight="1">
       <c r="A51" s="54" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B51" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C51" s="54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D51" s="54" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E51" s="55" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F51" s="65" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G51" s="56" t="s">
         <v>29</v>
@@ -5112,10 +5127,10 @@
         <v>33</v>
       </c>
       <c r="M51" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N51" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="N51" s="54" t="s">
-        <v>102</v>
       </c>
       <c r="O51" s="63"/>
       <c r="P51" s="63">
@@ -5128,22 +5143,22 @@
     </row>
     <row r="52" spans="1:20" ht="18" customHeight="1">
       <c r="A52" s="54" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B52" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C52" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D52" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="55" t="s">
-        <v>98</v>
-      </c>
       <c r="F52" s="65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G52" s="56" t="s">
         <v>29</v>
@@ -5160,10 +5175,10 @@
         <v>71</v>
       </c>
       <c r="M52" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N52" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="N52" s="54" t="s">
-        <v>102</v>
       </c>
       <c r="O52" s="63"/>
       <c r="P52" s="67"/>
@@ -5174,22 +5189,22 @@
     </row>
     <row r="53" spans="1:20" ht="18" customHeight="1">
       <c r="A53" s="54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C53" s="54" t="s">
         <v>68</v>
       </c>
       <c r="D53" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="E53" s="55" t="s">
-        <v>100</v>
-      </c>
       <c r="F53" s="65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G53" s="56" t="s">
         <v>29</v>
@@ -5206,10 +5221,10 @@
         <v>71</v>
       </c>
       <c r="M53" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N53" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="N53" s="54" t="s">
-        <v>102</v>
       </c>
       <c r="O53" s="63"/>
       <c r="P53" s="67"/>
@@ -5220,22 +5235,22 @@
     </row>
     <row r="54" spans="1:20" ht="18" customHeight="1">
       <c r="A54" s="54" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B54" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C54" s="54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D54" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="E54" s="55" t="s">
-        <v>107</v>
-      </c>
       <c r="F54" s="65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G54" s="56" t="s">
         <v>29</v>
@@ -5252,10 +5267,10 @@
         <v>71</v>
       </c>
       <c r="M54" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N54" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="N54" s="54" t="s">
-        <v>102</v>
       </c>
       <c r="O54" s="63"/>
       <c r="P54" s="67"/>
@@ -5266,22 +5281,22 @@
     </row>
     <row r="55" spans="1:20" ht="18" customHeight="1">
       <c r="A55" s="54" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B55" s="55" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C55" s="54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D55" s="54" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E55" s="55" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F55" s="65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G55" s="56" t="s">
         <v>29</v>
@@ -5298,10 +5313,10 @@
         <v>71</v>
       </c>
       <c r="M55" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="N55" s="54" t="s">
         <v>103</v>
-      </c>
-      <c r="N55" s="54" t="s">
-        <v>102</v>
       </c>
       <c r="O55" s="63"/>
       <c r="P55" s="67"/>
@@ -5313,7 +5328,7 @@
     <row r="56" spans="1:20" ht="18" customHeight="1">
       <c r="A56" s="54"/>
       <c r="B56" s="55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C56" s="54" t="s">
         <v>68</v>
@@ -5344,10 +5359,10 @@
         <v>33</v>
       </c>
       <c r="M56" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N56" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O56" s="63"/>
       <c r="P56" s="63">
@@ -5363,7 +5378,7 @@
     <row r="57" spans="1:20" ht="18" customHeight="1">
       <c r="A57" s="54"/>
       <c r="B57" s="55" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C57" s="54" t="s">
         <v>68</v>
@@ -5394,10 +5409,10 @@
         <v>33</v>
       </c>
       <c r="M57" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N57" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O57" s="63"/>
       <c r="P57" s="63">
@@ -5413,7 +5428,7 @@
     <row r="58" spans="1:20" ht="18" customHeight="1">
       <c r="A58" s="54"/>
       <c r="B58" s="55" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C58" s="54" t="s">
         <v>68</v>
@@ -5444,10 +5459,10 @@
         <v>33</v>
       </c>
       <c r="M58" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N58" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O58" s="63"/>
       <c r="P58" s="63">
@@ -5463,7 +5478,7 @@
     <row r="59" spans="1:20" ht="18" customHeight="1">
       <c r="A59" s="54"/>
       <c r="B59" s="55" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C59" s="54" t="s">
         <v>68</v>
@@ -5494,10 +5509,10 @@
         <v>33</v>
       </c>
       <c r="M59" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N59" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O59" s="63"/>
       <c r="P59" s="63">
@@ -5513,7 +5528,7 @@
     <row r="60" spans="1:20" ht="18" customHeight="1">
       <c r="A60" s="54"/>
       <c r="B60" s="55" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C60" s="54" t="s">
         <v>68</v>
@@ -5544,10 +5559,10 @@
         <v>33</v>
       </c>
       <c r="M60" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N60" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O60" s="63"/>
       <c r="P60" s="63">
@@ -5563,7 +5578,7 @@
     <row r="61" spans="1:20" ht="18" customHeight="1">
       <c r="A61" s="54"/>
       <c r="B61" s="55" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C61" s="54" t="s">
         <v>68</v>
@@ -5594,10 +5609,10 @@
         <v>33</v>
       </c>
       <c r="M61" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N61" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O61" s="63"/>
       <c r="P61" s="63">
@@ -5613,7 +5628,7 @@
     <row r="62" spans="1:20" ht="18" customHeight="1">
       <c r="A62" s="54"/>
       <c r="B62" s="55" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C62" s="54" t="s">
         <v>68</v>
@@ -5631,7 +5646,7 @@
       <c r="L62" s="68"/>
       <c r="M62" s="68"/>
       <c r="N62" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O62" s="63"/>
       <c r="P62" s="63"/>
@@ -5643,7 +5658,7 @@
     <row r="63" spans="1:20" ht="18" customHeight="1">
       <c r="A63" s="54"/>
       <c r="B63" s="55" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C63" s="54" t="s">
         <v>68</v>
@@ -5674,10 +5689,10 @@
         <v>33</v>
       </c>
       <c r="M63" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N63" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O63" s="63"/>
       <c r="P63" s="63">
@@ -5693,10 +5708,10 @@
     <row r="64" spans="1:20" ht="18" customHeight="1">
       <c r="A64" s="54"/>
       <c r="B64" s="55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C64" s="54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D64" s="54" t="s">
         <v>66</v>
@@ -5724,10 +5739,10 @@
         <v>33</v>
       </c>
       <c r="M64" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N64" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O64" s="63"/>
       <c r="P64" s="63">
@@ -5743,10 +5758,10 @@
     <row r="65" spans="1:20" ht="18" customHeight="1">
       <c r="A65" s="54"/>
       <c r="B65" s="55" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C65" s="54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D65" s="54" t="s">
         <v>66</v>
@@ -5774,10 +5789,10 @@
         <v>33</v>
       </c>
       <c r="M65" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N65" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O65" s="63"/>
       <c r="P65" s="63">
@@ -5793,7 +5808,7 @@
     <row r="66" spans="1:20" ht="18" customHeight="1">
       <c r="A66" s="54"/>
       <c r="B66" s="55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C66" s="54" t="s">
         <v>68</v>
@@ -5824,10 +5839,10 @@
         <v>33</v>
       </c>
       <c r="M66" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N66" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O66" s="63"/>
       <c r="P66" s="63">
@@ -5843,7 +5858,7 @@
     <row r="67" spans="1:20" ht="18" customHeight="1">
       <c r="A67" s="54"/>
       <c r="B67" s="55" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C67" s="54" t="s">
         <v>68</v>
@@ -5874,10 +5889,10 @@
         <v>33</v>
       </c>
       <c r="M67" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N67" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O67" s="63"/>
       <c r="P67" s="63">
@@ -5893,7 +5908,7 @@
     <row r="68" spans="1:20" ht="18" customHeight="1">
       <c r="A68" s="54"/>
       <c r="B68" s="55" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C68" s="54" t="s">
         <v>68</v>
@@ -5924,10 +5939,10 @@
         <v>33</v>
       </c>
       <c r="M68" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N68" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O68" s="63"/>
       <c r="P68" s="63">
@@ -5943,7 +5958,7 @@
     <row r="69" spans="1:20" ht="18" customHeight="1">
       <c r="A69" s="54"/>
       <c r="B69" s="55" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C69" s="54" t="s">
         <v>68</v>
@@ -5974,10 +5989,10 @@
         <v>33</v>
       </c>
       <c r="M69" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N69" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O69" s="63"/>
       <c r="P69" s="63">
@@ -5993,7 +6008,7 @@
     <row r="70" spans="1:20" ht="18" customHeight="1">
       <c r="A70" s="54"/>
       <c r="B70" s="55" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C70" s="54" t="s">
         <v>68</v>
@@ -6024,10 +6039,10 @@
         <v>33</v>
       </c>
       <c r="M70" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N70" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O70" s="63"/>
       <c r="P70" s="63">
@@ -6043,7 +6058,7 @@
     <row r="71" spans="1:20" ht="18" customHeight="1">
       <c r="A71" s="54"/>
       <c r="B71" s="55" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C71" s="54" t="s">
         <v>68</v>
@@ -6074,10 +6089,10 @@
         <v>33</v>
       </c>
       <c r="M71" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N71" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O71" s="63"/>
       <c r="P71" s="63">
@@ -6093,7 +6108,7 @@
     <row r="72" spans="1:20" ht="18" customHeight="1">
       <c r="A72" s="54"/>
       <c r="B72" s="55" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C72" s="54" t="s">
         <v>68</v>
@@ -6124,10 +6139,10 @@
         <v>33</v>
       </c>
       <c r="M72" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N72" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O72" s="63"/>
       <c r="P72" s="63">
@@ -6143,10 +6158,10 @@
     <row r="73" spans="1:20" ht="18" customHeight="1">
       <c r="A73" s="54"/>
       <c r="B73" s="55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C73" s="54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D73" s="54" t="s">
         <v>66</v>
@@ -6174,10 +6189,10 @@
         <v>33</v>
       </c>
       <c r="M73" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N73" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O73" s="63"/>
       <c r="P73" s="63">
@@ -6193,10 +6208,10 @@
     <row r="74" spans="1:20" ht="18" customHeight="1">
       <c r="A74" s="54"/>
       <c r="B74" s="55" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C74" s="54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D74" s="54" t="s">
         <v>66</v>
@@ -6224,10 +6239,10 @@
         <v>33</v>
       </c>
       <c r="M74" s="68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N74" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O74" s="63"/>
       <c r="P74" s="63">
@@ -6243,7 +6258,7 @@
     <row r="75" spans="1:20" ht="18" customHeight="1">
       <c r="A75" s="54"/>
       <c r="B75" s="55" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C75" s="54" t="s">
         <v>68</v>
@@ -6271,10 +6286,10 @@
         <v>33</v>
       </c>
       <c r="M75" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N75" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O75" s="63"/>
       <c r="P75" s="63">
@@ -6288,7 +6303,7 @@
     <row r="76" spans="1:20" ht="18" customHeight="1">
       <c r="A76" s="54"/>
       <c r="B76" s="55" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C76" s="54" t="s">
         <v>68</v>
@@ -6316,10 +6331,10 @@
         <v>33</v>
       </c>
       <c r="M76" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N76" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O76" s="63"/>
       <c r="P76" s="63">
@@ -6333,7 +6348,7 @@
     <row r="77" spans="1:20" ht="18" customHeight="1">
       <c r="A77" s="54"/>
       <c r="B77" s="55" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C77" s="54" t="s">
         <v>68</v>
@@ -6361,10 +6376,10 @@
         <v>33</v>
       </c>
       <c r="M77" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N77" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O77" s="63"/>
       <c r="P77" s="63">
@@ -6378,10 +6393,10 @@
     <row r="78" spans="1:20" ht="18" customHeight="1">
       <c r="A78" s="54"/>
       <c r="B78" s="55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C78" s="54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D78" s="54" t="s">
         <v>66</v>
@@ -6406,10 +6421,10 @@
         <v>33</v>
       </c>
       <c r="M78" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N78" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O78" s="63"/>
       <c r="P78" s="63">
@@ -6423,10 +6438,10 @@
     <row r="79" spans="1:20" ht="18" customHeight="1">
       <c r="A79" s="54"/>
       <c r="B79" s="55" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C79" s="54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D79" s="54" t="s">
         <v>66</v>
@@ -6451,10 +6466,10 @@
         <v>33</v>
       </c>
       <c r="M79" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N79" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O79" s="63"/>
       <c r="P79" s="63">
@@ -6468,7 +6483,7 @@
     <row r="80" spans="1:20" ht="18" customHeight="1">
       <c r="A80" s="54"/>
       <c r="B80" s="55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C80" s="54" t="s">
         <v>68</v>
@@ -6478,7 +6493,7 @@
       </c>
       <c r="E80" s="55"/>
       <c r="F80" s="65" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G80" s="56" t="s">
         <v>29</v>
@@ -6495,10 +6510,10 @@
         <v>71</v>
       </c>
       <c r="M80" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N80" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O80" s="63"/>
       <c r="P80" s="64"/>
@@ -6510,7 +6525,7 @@
     <row r="81" spans="1:20" ht="18" customHeight="1">
       <c r="A81" s="54"/>
       <c r="B81" s="55" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C81" s="54" t="s">
         <v>68</v>
@@ -6520,7 +6535,7 @@
       </c>
       <c r="E81" s="55"/>
       <c r="F81" s="65" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G81" s="56" t="s">
         <v>29</v>
@@ -6537,10 +6552,10 @@
         <v>71</v>
       </c>
       <c r="M81" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N81" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O81" s="63"/>
       <c r="P81" s="64"/>
@@ -6552,7 +6567,7 @@
     <row r="82" spans="1:20" ht="18" customHeight="1">
       <c r="A82" s="54"/>
       <c r="B82" s="55" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C82" s="54" t="s">
         <v>68</v>
@@ -6579,10 +6594,10 @@
         <v>71</v>
       </c>
       <c r="M82" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N82" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O82" s="63"/>
       <c r="P82" s="64"/>
@@ -6594,7 +6609,7 @@
     <row r="83" spans="1:20" ht="18" customHeight="1">
       <c r="A83" s="54"/>
       <c r="B83" s="55" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C83" s="54" t="s">
         <v>68</v>
@@ -6621,10 +6636,10 @@
         <v>71</v>
       </c>
       <c r="M83" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N83" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O83" s="63"/>
       <c r="P83" s="64"/>
@@ -6636,7 +6651,7 @@
     <row r="84" spans="1:20" ht="18" customHeight="1">
       <c r="A84" s="54"/>
       <c r="B84" s="55" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C84" s="54" t="s">
         <v>68</v>
@@ -6663,10 +6678,10 @@
         <v>71</v>
       </c>
       <c r="M84" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N84" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O84" s="63"/>
       <c r="P84" s="64"/>
@@ -6678,10 +6693,10 @@
     <row r="85" spans="1:20" ht="18" customHeight="1">
       <c r="A85" s="54"/>
       <c r="B85" s="55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C85" s="54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D85" s="54" t="s">
         <v>66</v>
@@ -6705,10 +6720,10 @@
         <v>71</v>
       </c>
       <c r="M85" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N85" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O85" s="63"/>
       <c r="P85" s="64"/>
@@ -6720,10 +6735,10 @@
     <row r="86" spans="1:20" ht="18" customHeight="1">
       <c r="A86" s="54"/>
       <c r="B86" s="55" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C86" s="54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D86" s="54" t="s">
         <v>66</v>
@@ -6747,10 +6762,10 @@
         <v>71</v>
       </c>
       <c r="M86" s="68" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N86" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O86" s="63"/>
       <c r="P86" s="64"/>
@@ -6761,10 +6776,10 @@
     </row>
     <row r="87" spans="1:20" ht="18" customHeight="1">
       <c r="A87" s="54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B87" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C87" s="54" t="s">
         <v>68</v>
@@ -6798,7 +6813,7 @@
         <v>65</v>
       </c>
       <c r="N87" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O87" s="63"/>
       <c r="P87" s="64">
@@ -6813,10 +6828,10 @@
     </row>
     <row r="88" spans="1:20" ht="18" customHeight="1">
       <c r="A88" s="54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B88" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C88" s="54" t="s">
         <v>68</v>
@@ -6825,7 +6840,7 @@
         <v>72</v>
       </c>
       <c r="E88" s="55" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F88" s="56" t="s">
         <v>63</v>
@@ -6852,7 +6867,7 @@
         <v>65</v>
       </c>
       <c r="N88" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O88" s="63"/>
       <c r="P88" s="64">
@@ -6867,10 +6882,10 @@
     </row>
     <row r="89" spans="1:20" ht="18" customHeight="1">
       <c r="A89" s="54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B89" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C89" s="54" t="s">
         <v>68</v>
@@ -6879,7 +6894,7 @@
         <v>72</v>
       </c>
       <c r="E89" s="55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F89" s="56" t="s">
         <v>63</v>
@@ -6906,7 +6921,7 @@
         <v>65</v>
       </c>
       <c r="N89" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O89" s="63"/>
       <c r="P89" s="64">
@@ -6921,10 +6936,10 @@
     </row>
     <row r="90" spans="1:20" ht="18" customHeight="1">
       <c r="A90" s="54" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B90" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C90" s="54" t="s">
         <v>68</v>
@@ -6933,7 +6948,7 @@
         <v>72</v>
       </c>
       <c r="E90" s="55" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F90" s="56" t="s">
         <v>63</v>
@@ -6960,7 +6975,7 @@
         <v>65</v>
       </c>
       <c r="N90" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O90" s="63"/>
       <c r="P90" s="64">
@@ -6975,10 +6990,10 @@
     </row>
     <row r="91" spans="1:20" ht="18" customHeight="1">
       <c r="A91" s="54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B91" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C91" s="54" t="s">
         <v>68</v>
@@ -7005,10 +7020,10 @@
         <v>33</v>
       </c>
       <c r="M91" s="56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N91" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O91" s="63"/>
       <c r="P91" s="67"/>
@@ -7019,10 +7034,10 @@
     </row>
     <row r="92" spans="1:20" ht="18" customHeight="1">
       <c r="A92" s="54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B92" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C92" s="54" t="s">
         <v>68</v>
@@ -7031,7 +7046,7 @@
         <v>72</v>
       </c>
       <c r="E92" s="55" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F92" s="56" t="s">
         <v>69</v>
@@ -7051,10 +7066,10 @@
         <v>33</v>
       </c>
       <c r="M92" s="56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N92" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O92" s="63"/>
       <c r="P92" s="67"/>
@@ -7065,10 +7080,10 @@
     </row>
     <row r="93" spans="1:20" ht="18" customHeight="1">
       <c r="A93" s="54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B93" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C93" s="54" t="s">
         <v>68</v>
@@ -7077,7 +7092,7 @@
         <v>72</v>
       </c>
       <c r="E93" s="55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F93" s="56" t="s">
         <v>69</v>
@@ -7097,10 +7112,10 @@
         <v>33</v>
       </c>
       <c r="M93" s="56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N93" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O93" s="63"/>
       <c r="P93" s="67"/>
@@ -7111,10 +7126,10 @@
     </row>
     <row r="94" spans="1:20" ht="18" customHeight="1">
       <c r="A94" s="54" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B94" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C94" s="54" t="s">
         <v>68</v>
@@ -7123,7 +7138,7 @@
         <v>72</v>
       </c>
       <c r="E94" s="55" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F94" s="56" t="s">
         <v>69</v>
@@ -7143,10 +7158,10 @@
         <v>33</v>
       </c>
       <c r="M94" s="56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N94" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O94" s="63"/>
       <c r="P94" s="67"/>
@@ -7157,10 +7172,10 @@
     </row>
     <row r="95" spans="1:20" ht="18" customHeight="1">
       <c r="A95" s="54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B95" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C95" s="54" t="s">
         <v>68</v>
@@ -7187,10 +7202,10 @@
         <v>33</v>
       </c>
       <c r="M95" s="56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N95" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O95" s="63"/>
       <c r="P95" s="67"/>
@@ -7201,10 +7216,10 @@
     </row>
     <row r="96" spans="1:20" ht="18" customHeight="1">
       <c r="A96" s="54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B96" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C96" s="54" t="s">
         <v>68</v>
@@ -7213,7 +7228,7 @@
         <v>72</v>
       </c>
       <c r="E96" s="55" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F96" s="56" t="s">
         <v>73</v>
@@ -7233,10 +7248,10 @@
         <v>33</v>
       </c>
       <c r="M96" s="56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N96" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O96" s="63"/>
       <c r="P96" s="67"/>
@@ -7247,10 +7262,10 @@
     </row>
     <row r="97" spans="1:20" ht="18" customHeight="1">
       <c r="A97" s="54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B97" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C97" s="54" t="s">
         <v>68</v>
@@ -7259,7 +7274,7 @@
         <v>72</v>
       </c>
       <c r="E97" s="55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F97" s="56" t="s">
         <v>73</v>
@@ -7279,10 +7294,10 @@
         <v>33</v>
       </c>
       <c r="M97" s="56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N97" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O97" s="63"/>
       <c r="P97" s="64"/>
@@ -7293,10 +7308,10 @@
     </row>
     <row r="98" spans="1:20" ht="18" customHeight="1">
       <c r="A98" s="54" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B98" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C98" s="54" t="s">
         <v>68</v>
@@ -7305,7 +7320,7 @@
         <v>72</v>
       </c>
       <c r="E98" s="55" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F98" s="56" t="s">
         <v>73</v>
@@ -7325,10 +7340,10 @@
         <v>33</v>
       </c>
       <c r="M98" s="56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N98" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O98" s="63"/>
       <c r="P98" s="64"/>
@@ -7339,10 +7354,10 @@
     </row>
     <row r="99" spans="1:20" ht="18" customHeight="1">
       <c r="A99" s="54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B99" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C99" s="54" t="s">
         <v>68</v>
@@ -7369,10 +7384,10 @@
         <v>71</v>
       </c>
       <c r="M99" s="56" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N99" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O99" s="63"/>
       <c r="P99" s="67"/>
@@ -7383,10 +7398,10 @@
     </row>
     <row r="100" spans="1:20" ht="18" customHeight="1">
       <c r="A100" s="54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B100" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C100" s="54" t="s">
         <v>68</v>
@@ -7395,7 +7410,7 @@
         <v>72</v>
       </c>
       <c r="E100" s="55" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F100" s="56" t="s">
         <v>70</v>
@@ -7415,10 +7430,10 @@
         <v>71</v>
       </c>
       <c r="M100" s="56" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N100" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O100" s="63"/>
       <c r="P100" s="67"/>
@@ -7429,10 +7444,10 @@
     </row>
     <row r="101" spans="1:20" ht="18" customHeight="1">
       <c r="A101" s="54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B101" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C101" s="54" t="s">
         <v>68</v>
@@ -7441,7 +7456,7 @@
         <v>72</v>
       </c>
       <c r="E101" s="55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F101" s="56" t="s">
         <v>70</v>
@@ -7461,10 +7476,10 @@
         <v>71</v>
       </c>
       <c r="M101" s="56" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N101" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O101" s="63"/>
       <c r="P101" s="64"/>
@@ -7475,10 +7490,10 @@
     </row>
     <row r="102" spans="1:20" ht="18" customHeight="1">
       <c r="A102" s="54" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B102" s="55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C102" s="54" t="s">
         <v>68</v>
@@ -7487,7 +7502,7 @@
         <v>72</v>
       </c>
       <c r="E102" s="55" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F102" s="56" t="s">
         <v>70</v>
@@ -7507,10 +7522,10 @@
         <v>71</v>
       </c>
       <c r="M102" s="56" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N102" s="54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O102" s="63"/>
       <c r="P102" s="64"/>
@@ -7521,19 +7536,39 @@
     </row>
     <row r="103" spans="1:20" ht="18" customHeight="1">
       <c r="A103" s="70"/>
-      <c r="B103" s="55"/>
-      <c r="C103" s="54"/>
-      <c r="D103" s="54"/>
+      <c r="B103" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C103" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D103" s="54" t="s">
+        <v>74</v>
+      </c>
       <c r="E103" s="55"/>
-      <c r="F103" s="56"/>
-      <c r="G103" s="56"/>
+      <c r="F103" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G103" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H103" s="57"/>
-      <c r="I103" s="58"/>
-      <c r="J103" s="64"/>
+      <c r="I103" s="58">
+        <v>298</v>
+      </c>
+      <c r="J103" s="64">
+        <v>1075000000</v>
+      </c>
       <c r="K103" s="66"/>
-      <c r="L103" s="68"/>
-      <c r="M103" s="56"/>
-      <c r="N103" s="54"/>
+      <c r="L103" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M103" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N103" s="54" t="s">
+        <v>143</v>
+      </c>
       <c r="O103" s="63"/>
       <c r="P103" s="64"/>
       <c r="Q103" s="64"/>
@@ -7543,19 +7578,43 @@
     </row>
     <row r="104" spans="1:20" ht="18" customHeight="1">
       <c r="A104" s="70"/>
-      <c r="B104" s="55"/>
-      <c r="C104" s="54"/>
-      <c r="D104" s="54"/>
-      <c r="E104" s="55"/>
-      <c r="F104" s="56"/>
-      <c r="G104" s="56"/>
+      <c r="B104" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C104" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D104" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="E104" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F104" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G104" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H104" s="57"/>
-      <c r="I104" s="58"/>
-      <c r="J104" s="64"/>
-      <c r="K104" s="66"/>
-      <c r="L104" s="68"/>
-      <c r="M104" s="56"/>
-      <c r="N104" s="54"/>
+      <c r="I104" s="58">
+        <v>298</v>
+      </c>
+      <c r="J104" s="64">
+        <v>1603000000</v>
+      </c>
+      <c r="K104" s="66">
+        <v>50000000</v>
+      </c>
+      <c r="L104" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M104" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N104" s="54" t="s">
+        <v>143</v>
+      </c>
       <c r="O104" s="63"/>
       <c r="P104" s="64"/>
       <c r="Q104" s="64"/>
@@ -7565,19 +7624,39 @@
     </row>
     <row r="105" spans="1:20" ht="18" customHeight="1">
       <c r="A105" s="70"/>
-      <c r="B105" s="55"/>
-      <c r="C105" s="54"/>
-      <c r="D105" s="54"/>
+      <c r="B105" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C105" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D105" s="54" t="s">
+        <v>74</v>
+      </c>
       <c r="E105" s="55"/>
-      <c r="F105" s="56"/>
-      <c r="G105" s="56"/>
+      <c r="F105" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="G105" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H105" s="57"/>
-      <c r="I105" s="58"/>
-      <c r="J105" s="64"/>
+      <c r="I105" s="58">
+        <v>298</v>
+      </c>
+      <c r="J105" s="64">
+        <v>1460000000</v>
+      </c>
       <c r="K105" s="66"/>
-      <c r="L105" s="68"/>
-      <c r="M105" s="56"/>
-      <c r="N105" s="54"/>
+      <c r="L105" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M105" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N105" s="54" t="s">
+        <v>143</v>
+      </c>
       <c r="O105" s="63"/>
       <c r="P105" s="64"/>
       <c r="Q105" s="64"/>
@@ -7587,19 +7666,43 @@
     </row>
     <row r="106" spans="1:20" ht="18" customHeight="1">
       <c r="A106" s="70"/>
-      <c r="B106" s="55"/>
-      <c r="C106" s="54"/>
-      <c r="D106" s="54"/>
-      <c r="E106" s="55"/>
-      <c r="F106" s="56"/>
-      <c r="G106" s="56"/>
+      <c r="B106" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C106" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D106" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="E106" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F106" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="G106" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H106" s="57"/>
-      <c r="I106" s="58"/>
-      <c r="J106" s="64"/>
-      <c r="K106" s="66"/>
-      <c r="L106" s="68"/>
-      <c r="M106" s="56"/>
-      <c r="N106" s="54"/>
+      <c r="I106" s="58">
+        <v>298</v>
+      </c>
+      <c r="J106" s="64">
+        <v>2001000000</v>
+      </c>
+      <c r="K106" s="66">
+        <v>10000000</v>
+      </c>
+      <c r="L106" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M106" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N106" s="54" t="s">
+        <v>143</v>
+      </c>
       <c r="O106" s="63"/>
       <c r="P106" s="64"/>
       <c r="Q106" s="64"/>
@@ -7609,19 +7712,39 @@
     </row>
     <row r="107" spans="1:20" ht="18" customHeight="1">
       <c r="A107" s="70"/>
-      <c r="B107" s="55"/>
-      <c r="C107" s="54"/>
-      <c r="D107" s="54"/>
+      <c r="B107" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C107" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D107" s="54" t="s">
+        <v>74</v>
+      </c>
       <c r="E107" s="55"/>
-      <c r="F107" s="56"/>
-      <c r="G107" s="56"/>
+      <c r="F107" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G107" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H107" s="57"/>
-      <c r="I107" s="58"/>
-      <c r="J107" s="64"/>
+      <c r="I107" s="58">
+        <v>298</v>
+      </c>
+      <c r="J107" s="64">
+        <v>22</v>
+      </c>
       <c r="K107" s="66"/>
-      <c r="L107" s="68"/>
-      <c r="M107" s="56"/>
-      <c r="N107" s="54"/>
+      <c r="L107" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="M107" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N107" s="54" t="s">
+        <v>143</v>
+      </c>
       <c r="O107" s="63"/>
       <c r="P107" s="64"/>
       <c r="Q107" s="64"/>
@@ -7631,19 +7754,43 @@
     </row>
     <row r="108" spans="1:20" ht="18" customHeight="1">
       <c r="A108" s="70"/>
-      <c r="B108" s="55"/>
-      <c r="C108" s="54"/>
-      <c r="D108" s="54"/>
-      <c r="E108" s="55"/>
-      <c r="F108" s="56"/>
-      <c r="G108" s="56"/>
+      <c r="B108" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C108" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D108" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="E108" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F108" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G108" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H108" s="57"/>
-      <c r="I108" s="58"/>
-      <c r="J108" s="64"/>
-      <c r="K108" s="66"/>
-      <c r="L108" s="68"/>
-      <c r="M108" s="56"/>
-      <c r="N108" s="54"/>
+      <c r="I108" s="58">
+        <v>298</v>
+      </c>
+      <c r="J108" s="64">
+        <v>37</v>
+      </c>
+      <c r="K108" s="66">
+        <v>2</v>
+      </c>
+      <c r="L108" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="M108" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N108" s="54" t="s">
+        <v>143</v>
+      </c>
       <c r="O108" s="63"/>
       <c r="P108" s="64"/>
       <c r="Q108" s="64"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jmst.2024.11.057`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D9847F-4AF4-D14C-BE86-BEDA6FDF7C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5706BCC3-86B4-4A4E-AE06-29C93F950471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="4740" windowWidth="31040" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="10920" windowWidth="31040" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="149">
   <si>
     <r>
       <rPr>
@@ -562,6 +562,21 @@
   </si>
   <si>
     <t>10.1016/j.msea.2025.147831</t>
+  </si>
+  <si>
+    <t>Al7(CoNiV)31</t>
+  </si>
+  <si>
+    <t>VIM+H+WQ+CR+RX+WQ</t>
+  </si>
+  <si>
+    <t>FCC+L21</t>
+  </si>
+  <si>
+    <t>homogenized in Ar at 1373 K for 6h then quenched and cold rolled to 84% reduction then recrystallized at 1173K for 1h and water quenched again; FCC majority and L21 (ordered BCC) minority</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmst.2024.11.057</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1557,6 @@
     <xf numFmtId="3" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1667,6 +1681,7 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2829,8 +2844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T856"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B93" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N113" sqref="N113"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A104" zoomScale="86" workbookViewId="0">
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -2887,19 +2902,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="85"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="84"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -2915,17 +2930,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="89"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="88"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -2966,43 +2981,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="92" t="s">
+      <c r="F5" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="92" t="s">
+      <c r="G5" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="93" t="s">
+      <c r="H5" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="92" t="s">
+      <c r="I5" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="92" t="s">
+      <c r="J5" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="92" t="s">
+      <c r="K5" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="92" t="s">
+      <c r="L5" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="92" t="s">
+      <c r="M5" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="92" t="s">
+      <c r="N5" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="97" t="s">
+      <c r="O5" s="96" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3018,19 +3033,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="96"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="98"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3080,7 +3095,7 @@
       <c r="N7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="99"/>
+      <c r="O7" s="98"/>
       <c r="P7" s="33" t="s">
         <v>36</v>
       </c>
@@ -3095,35 +3110,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1">
       <c r="A8" s="36"/>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103" t="s">
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="108" t="s">
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="107" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="109"/>
+      <c r="N8" s="108"/>
       <c r="O8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="110" t="s">
+      <c r="P8" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="111"/>
-      <c r="R8" s="112"/>
-      <c r="S8" s="112"/>
-      <c r="T8" s="113"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="111"/>
+      <c r="T8" s="112"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="38" t="s">
@@ -3722,7 +3737,7 @@
       <c r="L20" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="76" t="s">
+      <c r="M20" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N20" s="60" t="s">
@@ -3769,7 +3784,7 @@
       <c r="L21" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M21" s="76" t="s">
+      <c r="M21" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N21" s="60" t="s">
@@ -3816,7 +3831,7 @@
       <c r="L22" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M22" s="76" t="s">
+      <c r="M22" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N22" s="60" t="s">
@@ -3863,7 +3878,7 @@
       <c r="L23" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="76" t="s">
+      <c r="M23" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N23" s="60" t="s">
@@ -3910,7 +3925,7 @@
       <c r="L24" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M24" s="76" t="s">
+      <c r="M24" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N24" s="60" t="s">
@@ -3927,16 +3942,16 @@
     </row>
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="54"/>
-      <c r="B25" s="114" t="s">
+      <c r="B25" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="115" t="s">
+      <c r="C25" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="115" t="s">
+      <c r="D25" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="116" t="s">
+      <c r="E25" s="115" t="s">
         <v>89</v>
       </c>
       <c r="F25" s="56" t="s">
@@ -3956,7 +3971,7 @@
       <c r="L25" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="M25" s="76" t="s">
+      <c r="M25" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N25" s="60" t="s">
@@ -3971,16 +3986,16 @@
     </row>
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="54"/>
-      <c r="B26" s="117" t="s">
+      <c r="B26" s="116" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="118" t="s">
+      <c r="C26" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="118" t="s">
+      <c r="D26" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="E26" s="119" t="s">
+      <c r="E26" s="118" t="s">
         <v>89</v>
       </c>
       <c r="F26" s="56" t="s">
@@ -4000,7 +4015,7 @@
       <c r="L26" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="M26" s="76" t="s">
+      <c r="M26" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N26" s="60" t="s">
@@ -4015,16 +4030,16 @@
     </row>
     <row r="27" spans="1:20" ht="18.75" customHeight="1">
       <c r="A27" s="54"/>
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="116" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="118" t="s">
+      <c r="D27" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="119" t="s">
+      <c r="E27" s="118" t="s">
         <v>89</v>
       </c>
       <c r="F27" s="56" t="s">
@@ -4044,7 +4059,7 @@
       <c r="L27" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="M27" s="76" t="s">
+      <c r="M27" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N27" s="60" t="s">
@@ -4059,16 +4074,16 @@
     </row>
     <row r="28" spans="1:20" ht="18.75" customHeight="1">
       <c r="A28" s="54"/>
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="118" t="s">
+      <c r="C28" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="118" t="s">
+      <c r="D28" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="119" t="s">
+      <c r="E28" s="118" t="s">
         <v>89</v>
       </c>
       <c r="F28" s="56" t="s">
@@ -4088,7 +4103,7 @@
       <c r="L28" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="M28" s="76" t="s">
+      <c r="M28" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N28" s="60" t="s">
@@ -4103,16 +4118,16 @@
     </row>
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
       <c r="A29" s="54"/>
-      <c r="B29" s="117" t="s">
+      <c r="B29" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="118" t="s">
+      <c r="C29" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="118" t="s">
+      <c r="D29" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="E29" s="119" t="s">
+      <c r="E29" s="118" t="s">
         <v>89</v>
       </c>
       <c r="F29" s="56" t="s">
@@ -4132,7 +4147,7 @@
       <c r="L29" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="M29" s="76" t="s">
+      <c r="M29" s="75" t="s">
         <v>77</v>
       </c>
       <c r="N29" s="60" t="s">
@@ -4147,10 +4162,10 @@
     </row>
     <row r="30" spans="1:20" ht="18.75" customHeight="1">
       <c r="A30" s="54"/>
-      <c r="B30" s="114" t="s">
+      <c r="B30" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="115" t="s">
+      <c r="C30" s="114" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="54"/>
@@ -4163,7 +4178,7 @@
       <c r="G30" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H30" s="76" t="s">
+      <c r="H30" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I30" s="4"/>
@@ -4187,10 +4202,10 @@
     </row>
     <row r="31" spans="1:20" ht="18.75" customHeight="1">
       <c r="A31" s="54"/>
-      <c r="B31" s="117" t="s">
+      <c r="B31" s="116" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="118" t="s">
+      <c r="C31" s="117" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="54"/>
@@ -4203,7 +4218,7 @@
       <c r="G31" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H31" s="76" t="s">
+      <c r="H31" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I31" s="4"/>
@@ -4227,10 +4242,10 @@
     </row>
     <row r="32" spans="1:20" ht="18.75" customHeight="1">
       <c r="A32" s="54"/>
-      <c r="B32" s="117" t="s">
+      <c r="B32" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="118" t="s">
+      <c r="C32" s="117" t="s">
         <v>68</v>
       </c>
       <c r="D32" s="54"/>
@@ -4243,7 +4258,7 @@
       <c r="G32" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H32" s="76" t="s">
+      <c r="H32" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I32" s="4"/>
@@ -4267,10 +4282,10 @@
     </row>
     <row r="33" spans="1:20" ht="18.75" customHeight="1">
       <c r="A33" s="54"/>
-      <c r="B33" s="117" t="s">
+      <c r="B33" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="118" t="s">
+      <c r="C33" s="117" t="s">
         <v>68</v>
       </c>
       <c r="D33" s="54"/>
@@ -4283,7 +4298,7 @@
       <c r="G33" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H33" s="76" t="s">
+      <c r="H33" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I33" s="4"/>
@@ -4307,10 +4322,10 @@
     </row>
     <row r="34" spans="1:20" ht="18.75" customHeight="1">
       <c r="A34" s="54"/>
-      <c r="B34" s="117" t="s">
+      <c r="B34" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="118" t="s">
+      <c r="C34" s="117" t="s">
         <v>68</v>
       </c>
       <c r="D34" s="54"/>
@@ -4323,7 +4338,7 @@
       <c r="G34" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H34" s="76" t="s">
+      <c r="H34" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I34" s="4"/>
@@ -4347,10 +4362,10 @@
     </row>
     <row r="35" spans="1:20" ht="18.75" customHeight="1">
       <c r="A35" s="54"/>
-      <c r="B35" s="114" t="s">
+      <c r="B35" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="115" t="s">
+      <c r="C35" s="114" t="s">
         <v>68</v>
       </c>
       <c r="D35" s="54"/>
@@ -4363,7 +4378,7 @@
       <c r="G35" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H35" s="76" t="s">
+      <c r="H35" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I35" s="4"/>
@@ -4387,10 +4402,10 @@
     </row>
     <row r="36" spans="1:20" ht="18.75" customHeight="1">
       <c r="A36" s="54"/>
-      <c r="B36" s="117" t="s">
+      <c r="B36" s="116" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="118" t="s">
+      <c r="C36" s="117" t="s">
         <v>68</v>
       </c>
       <c r="D36" s="54"/>
@@ -4403,7 +4418,7 @@
       <c r="G36" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H36" s="76" t="s">
+      <c r="H36" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I36" s="4"/>
@@ -4427,10 +4442,10 @@
     </row>
     <row r="37" spans="1:20" ht="18.75" customHeight="1">
       <c r="A37" s="54"/>
-      <c r="B37" s="117" t="s">
+      <c r="B37" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="118" t="s">
+      <c r="C37" s="117" t="s">
         <v>68</v>
       </c>
       <c r="D37" s="54"/>
@@ -4443,7 +4458,7 @@
       <c r="G37" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H37" s="76" t="s">
+      <c r="H37" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I37" s="4"/>
@@ -4467,10 +4482,10 @@
     </row>
     <row r="38" spans="1:20" ht="18.75" customHeight="1">
       <c r="A38" s="54"/>
-      <c r="B38" s="117" t="s">
+      <c r="B38" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="118" t="s">
+      <c r="C38" s="117" t="s">
         <v>68</v>
       </c>
       <c r="D38" s="54"/>
@@ -4483,7 +4498,7 @@
       <c r="G38" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H38" s="76" t="s">
+      <c r="H38" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I38" s="58"/>
@@ -4507,10 +4522,10 @@
     </row>
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
       <c r="A39" s="54"/>
-      <c r="B39" s="117" t="s">
+      <c r="B39" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="117" t="s">
         <v>68</v>
       </c>
       <c r="D39" s="54"/>
@@ -4523,7 +4538,7 @@
       <c r="G39" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="H39" s="76" t="s">
+      <c r="H39" s="75" t="s">
         <v>95</v>
       </c>
       <c r="I39" s="58"/>
@@ -7800,19 +7815,43 @@
     </row>
     <row r="109" spans="1:20" ht="18" customHeight="1">
       <c r="A109" s="70"/>
-      <c r="B109" s="55"/>
-      <c r="C109" s="54"/>
-      <c r="D109" s="54"/>
-      <c r="E109" s="55"/>
-      <c r="F109" s="56"/>
-      <c r="G109" s="56"/>
+      <c r="B109" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C109" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="D109" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="E109" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="F109" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="G109" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H109" s="57"/>
-      <c r="I109" s="58"/>
-      <c r="J109" s="64"/>
-      <c r="K109" s="66"/>
-      <c r="L109" s="68"/>
-      <c r="M109" s="56"/>
-      <c r="N109" s="54"/>
+      <c r="I109" s="58">
+        <v>77</v>
+      </c>
+      <c r="J109" s="64">
+        <v>1270000000</v>
+      </c>
+      <c r="K109" s="66">
+        <v>13000000</v>
+      </c>
+      <c r="L109" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M109" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N109" s="54" t="s">
+        <v>148</v>
+      </c>
       <c r="O109" s="9"/>
       <c r="P109" s="64"/>
       <c r="Q109" s="64"/>
@@ -7822,19 +7861,43 @@
     </row>
     <row r="110" spans="1:20" ht="18" customHeight="1">
       <c r="A110" s="70"/>
-      <c r="B110" s="55"/>
-      <c r="C110" s="54"/>
-      <c r="D110" s="54"/>
-      <c r="E110" s="55"/>
-      <c r="F110" s="56"/>
-      <c r="G110" s="56"/>
+      <c r="B110" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C110" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="D110" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="E110" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="F110" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G110" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H110" s="57"/>
-      <c r="I110" s="58"/>
-      <c r="J110" s="66"/>
-      <c r="K110" s="66"/>
-      <c r="L110" s="68"/>
-      <c r="M110" s="56"/>
-      <c r="N110" s="54"/>
+      <c r="I110" s="58">
+        <v>77</v>
+      </c>
+      <c r="J110" s="66">
+        <v>1844000000</v>
+      </c>
+      <c r="K110" s="66">
+        <v>15000000</v>
+      </c>
+      <c r="L110" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M110" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N110" s="54" t="s">
+        <v>148</v>
+      </c>
       <c r="O110" s="9"/>
       <c r="P110" s="64"/>
       <c r="Q110" s="64"/>
@@ -7844,19 +7907,43 @@
     </row>
     <row r="111" spans="1:20" ht="18" customHeight="1">
       <c r="A111" s="70"/>
-      <c r="B111" s="55"/>
-      <c r="C111" s="54"/>
-      <c r="D111" s="54"/>
-      <c r="E111" s="55"/>
-      <c r="F111" s="56"/>
-      <c r="G111" s="56"/>
+      <c r="B111" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C111" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="D111" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="E111" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="F111" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="G111" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H111" s="57"/>
-      <c r="I111" s="58"/>
-      <c r="J111" s="66"/>
-      <c r="K111" s="66"/>
-      <c r="L111" s="68"/>
-      <c r="M111" s="68"/>
-      <c r="N111" s="54"/>
+      <c r="I111" s="58">
+        <v>77</v>
+      </c>
+      <c r="J111" s="66">
+        <v>29</v>
+      </c>
+      <c r="K111" s="66">
+        <v>2</v>
+      </c>
+      <c r="L111" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="M111" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N111" s="54" t="s">
+        <v>148</v>
+      </c>
       <c r="O111" s="63"/>
       <c r="P111" s="67"/>
       <c r="Q111" s="64"/>
@@ -7866,19 +7953,43 @@
     </row>
     <row r="112" spans="1:20" ht="18" customHeight="1">
       <c r="A112" s="70"/>
-      <c r="B112" s="71"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="71"/>
-      <c r="F112" s="52"/>
-      <c r="G112" s="52"/>
+      <c r="B112" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C112" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="D112" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="E112" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="F112" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="G112" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H112" s="57"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="66"/>
-      <c r="K112" s="66"/>
-      <c r="L112" s="68"/>
-      <c r="M112" s="68"/>
-      <c r="N112" s="54"/>
+      <c r="I112" s="4">
+        <v>298</v>
+      </c>
+      <c r="J112" s="66">
+        <v>1145000000</v>
+      </c>
+      <c r="K112" s="66">
+        <v>9000000</v>
+      </c>
+      <c r="L112" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M112" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N112" s="54" t="s">
+        <v>148</v>
+      </c>
       <c r="O112" s="63"/>
       <c r="P112" s="67"/>
       <c r="Q112" s="64"/>
@@ -7888,19 +7999,43 @@
     </row>
     <row r="113" spans="1:20" ht="18" customHeight="1">
       <c r="A113" s="70"/>
-      <c r="B113" s="71"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="71"/>
-      <c r="F113" s="52"/>
-      <c r="G113" s="52"/>
+      <c r="B113" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C113" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="D113" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="E113" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="F113" s="119" t="s">
+        <v>80</v>
+      </c>
+      <c r="G113" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H113" s="57"/>
-      <c r="I113" s="4"/>
-      <c r="J113" s="66"/>
-      <c r="K113" s="66"/>
-      <c r="L113" s="68"/>
-      <c r="M113" s="68"/>
-      <c r="N113" s="54"/>
+      <c r="I113" s="4">
+        <v>298</v>
+      </c>
+      <c r="J113" s="66">
+        <v>1556000000</v>
+      </c>
+      <c r="K113" s="66">
+        <v>16000000</v>
+      </c>
+      <c r="L113" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M113" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N113" s="54" t="s">
+        <v>148</v>
+      </c>
       <c r="O113" s="63"/>
       <c r="P113" s="67"/>
       <c r="Q113" s="4"/>
@@ -7910,19 +8045,43 @@
     </row>
     <row r="114" spans="1:20" ht="18" customHeight="1">
       <c r="A114" s="70"/>
-      <c r="B114" s="55"/>
-      <c r="C114" s="54"/>
-      <c r="D114" s="54"/>
-      <c r="E114" s="55"/>
-      <c r="F114" s="56"/>
-      <c r="G114" s="56"/>
+      <c r="B114" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C114" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="D114" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="E114" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="F114" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="G114" s="56" t="s">
+        <v>29</v>
+      </c>
       <c r="H114" s="57"/>
-      <c r="I114" s="69"/>
-      <c r="J114" s="66"/>
-      <c r="K114" s="66"/>
-      <c r="L114" s="68"/>
-      <c r="M114" s="68"/>
-      <c r="N114" s="54"/>
+      <c r="I114" s="69">
+        <v>298</v>
+      </c>
+      <c r="J114" s="66">
+        <v>43</v>
+      </c>
+      <c r="K114" s="66">
+        <v>5</v>
+      </c>
+      <c r="L114" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="M114" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N114" s="54" t="s">
+        <v>148</v>
+      </c>
       <c r="O114" s="63"/>
       <c r="P114" s="67"/>
       <c r="Q114" s="4"/>
@@ -7985,7 +8144,7 @@
       <c r="H117" s="57"/>
       <c r="I117" s="54"/>
       <c r="J117" s="67"/>
-      <c r="K117" s="72"/>
+      <c r="K117" s="71"/>
       <c r="L117" s="68"/>
       <c r="M117" s="68"/>
       <c r="N117" s="54"/>
@@ -8006,8 +8165,8 @@
       <c r="G118" s="56"/>
       <c r="H118" s="57"/>
       <c r="I118" s="69"/>
-      <c r="J118" s="72"/>
-      <c r="K118" s="72"/>
+      <c r="J118" s="71"/>
+      <c r="K118" s="71"/>
       <c r="L118" s="68"/>
       <c r="M118" s="68"/>
       <c r="N118" s="54"/>
@@ -8028,7 +8187,7 @@
       <c r="G119" s="56"/>
       <c r="H119" s="57"/>
       <c r="I119" s="69"/>
-      <c r="J119" s="72"/>
+      <c r="J119" s="71"/>
       <c r="K119" s="66"/>
       <c r="L119" s="52"/>
       <c r="M119" s="52"/>
@@ -8050,7 +8209,7 @@
       <c r="G120" s="56"/>
       <c r="H120" s="57"/>
       <c r="I120" s="54"/>
-      <c r="J120" s="73"/>
+      <c r="J120" s="72"/>
       <c r="K120" s="66"/>
       <c r="L120" s="52"/>
       <c r="M120" s="52"/>
@@ -8072,7 +8231,7 @@
       <c r="G121" s="56"/>
       <c r="H121" s="57"/>
       <c r="I121" s="54"/>
-      <c r="J121" s="73"/>
+      <c r="J121" s="72"/>
       <c r="K121" s="66"/>
       <c r="L121" s="56"/>
       <c r="M121" s="56"/>
@@ -8138,7 +8297,7 @@
       <c r="G124" s="56"/>
       <c r="H124" s="57"/>
       <c r="I124" s="58"/>
-      <c r="J124" s="73"/>
+      <c r="J124" s="72"/>
       <c r="K124" s="66"/>
       <c r="L124" s="56"/>
       <c r="M124" s="68"/>
@@ -8160,7 +8319,7 @@
       <c r="G125" s="56"/>
       <c r="H125" s="57"/>
       <c r="I125" s="58"/>
-      <c r="J125" s="73"/>
+      <c r="J125" s="72"/>
       <c r="K125" s="66"/>
       <c r="L125" s="56"/>
       <c r="M125" s="68"/>
@@ -8296,7 +8455,7 @@
       <c r="K131" s="59"/>
       <c r="L131" s="56"/>
       <c r="M131" s="56"/>
-      <c r="N131" s="74"/>
+      <c r="N131" s="73"/>
       <c r="O131" s="9"/>
       <c r="P131" s="64"/>
       <c r="Q131" s="4"/>
@@ -8318,7 +8477,7 @@
       <c r="K132" s="59"/>
       <c r="L132" s="56"/>
       <c r="M132" s="56"/>
-      <c r="N132" s="74"/>
+      <c r="N132" s="73"/>
       <c r="O132" s="9"/>
       <c r="P132" s="64"/>
       <c r="Q132" s="4"/>
@@ -8340,7 +8499,7 @@
       <c r="K133" s="59"/>
       <c r="L133" s="56"/>
       <c r="M133" s="56"/>
-      <c r="N133" s="74"/>
+      <c r="N133" s="73"/>
       <c r="O133" s="9"/>
       <c r="P133" s="64"/>
       <c r="Q133" s="4"/>
@@ -8362,7 +8521,7 @@
       <c r="K134" s="59"/>
       <c r="L134" s="56"/>
       <c r="M134" s="56"/>
-      <c r="N134" s="74"/>
+      <c r="N134" s="73"/>
       <c r="O134" s="9"/>
       <c r="P134" s="4"/>
       <c r="Q134" s="4"/>
@@ -8384,7 +8543,7 @@
       <c r="K135" s="59"/>
       <c r="L135" s="56"/>
       <c r="M135" s="56"/>
-      <c r="N135" s="74"/>
+      <c r="N135" s="73"/>
       <c r="O135" s="9"/>
       <c r="P135" s="4"/>
       <c r="Q135" s="4"/>
@@ -8406,7 +8565,7 @@
       <c r="K136" s="59"/>
       <c r="L136" s="56"/>
       <c r="M136" s="56"/>
-      <c r="N136" s="74"/>
+      <c r="N136" s="73"/>
       <c r="O136" s="9"/>
       <c r="P136" s="4"/>
       <c r="Q136" s="4"/>
@@ -8428,7 +8587,7 @@
       <c r="K137" s="4"/>
       <c r="L137" s="56"/>
       <c r="M137" s="56"/>
-      <c r="N137" s="74"/>
+      <c r="N137" s="73"/>
       <c r="O137" s="9"/>
       <c r="P137" s="4"/>
       <c r="Q137" s="4"/>
@@ -8450,7 +8609,7 @@
       <c r="K138" s="4"/>
       <c r="L138" s="56"/>
       <c r="M138" s="56"/>
-      <c r="N138" s="74"/>
+      <c r="N138" s="73"/>
       <c r="O138" s="9"/>
       <c r="P138" s="4"/>
       <c r="Q138" s="4"/>
@@ -8472,7 +8631,7 @@
       <c r="K139" s="4"/>
       <c r="L139" s="56"/>
       <c r="M139" s="4"/>
-      <c r="N139" s="74"/>
+      <c r="N139" s="73"/>
       <c r="O139" s="9"/>
       <c r="P139" s="4"/>
       <c r="Q139" s="4"/>
@@ -8494,7 +8653,7 @@
       <c r="K140" s="4"/>
       <c r="L140" s="56"/>
       <c r="M140" s="4"/>
-      <c r="N140" s="74"/>
+      <c r="N140" s="73"/>
       <c r="O140" s="9"/>
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
@@ -8516,7 +8675,7 @@
       <c r="K141" s="4"/>
       <c r="L141" s="56"/>
       <c r="M141" s="4"/>
-      <c r="N141" s="74"/>
+      <c r="N141" s="73"/>
       <c r="O141" s="9"/>
       <c r="P141" s="4"/>
       <c r="Q141" s="4"/>
@@ -8538,7 +8697,7 @@
       <c r="K142" s="4"/>
       <c r="L142" s="56"/>
       <c r="M142" s="4"/>
-      <c r="N142" s="74"/>
+      <c r="N142" s="73"/>
       <c r="O142" s="9"/>
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
@@ -8560,7 +8719,7 @@
       <c r="K143" s="4"/>
       <c r="L143" s="56"/>
       <c r="M143" s="4"/>
-      <c r="N143" s="74"/>
+      <c r="N143" s="73"/>
       <c r="O143" s="9"/>
       <c r="P143" s="4"/>
       <c r="Q143" s="4"/>
@@ -8582,7 +8741,7 @@
       <c r="K144" s="4"/>
       <c r="L144" s="56"/>
       <c r="M144" s="4"/>
-      <c r="N144" s="74"/>
+      <c r="N144" s="73"/>
       <c r="O144" s="9"/>
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
@@ -8604,7 +8763,7 @@
       <c r="K145" s="59"/>
       <c r="L145" s="56"/>
       <c r="M145" s="4"/>
-      <c r="N145" s="74"/>
+      <c r="N145" s="73"/>
       <c r="O145" s="9"/>
       <c r="P145" s="4"/>
       <c r="Q145" s="4"/>
@@ -8626,7 +8785,7 @@
       <c r="K146" s="59"/>
       <c r="L146" s="56"/>
       <c r="M146" s="4"/>
-      <c r="N146" s="74"/>
+      <c r="N146" s="73"/>
       <c r="O146" s="9"/>
       <c r="P146" s="4"/>
       <c r="Q146" s="4"/>
@@ -8648,7 +8807,7 @@
       <c r="K147" s="59"/>
       <c r="L147" s="56"/>
       <c r="M147" s="56"/>
-      <c r="N147" s="74"/>
+      <c r="N147" s="73"/>
       <c r="O147" s="9"/>
       <c r="P147" s="4"/>
       <c r="Q147" s="4"/>
@@ -8758,7 +8917,7 @@
       <c r="K152" s="59"/>
       <c r="L152" s="56"/>
       <c r="M152" s="56"/>
-      <c r="N152" s="74"/>
+      <c r="N152" s="73"/>
       <c r="O152" s="9"/>
       <c r="P152" s="4"/>
       <c r="Q152" s="4"/>
@@ -8780,7 +8939,7 @@
       <c r="K153" s="4"/>
       <c r="L153" s="56"/>
       <c r="M153" s="56"/>
-      <c r="N153" s="74"/>
+      <c r="N153" s="73"/>
       <c r="O153" s="9"/>
       <c r="P153" s="4"/>
       <c r="Q153" s="4"/>
@@ -8794,7 +8953,7 @@
       <c r="C154" s="54"/>
       <c r="D154" s="54"/>
       <c r="E154" s="63"/>
-      <c r="F154" s="75"/>
+      <c r="F154" s="74"/>
       <c r="G154" s="56"/>
       <c r="H154" s="65"/>
       <c r="I154" s="4"/>
@@ -8802,7 +8961,7 @@
       <c r="K154" s="4"/>
       <c r="L154" s="56"/>
       <c r="M154" s="56"/>
-      <c r="N154" s="74"/>
+      <c r="N154" s="73"/>
       <c r="O154" s="9"/>
       <c r="P154" s="4"/>
       <c r="Q154" s="4"/>
@@ -8816,7 +8975,7 @@
       <c r="C155" s="54"/>
       <c r="D155" s="54"/>
       <c r="E155" s="63"/>
-      <c r="F155" s="75"/>
+      <c r="F155" s="74"/>
       <c r="G155" s="56"/>
       <c r="H155" s="65"/>
       <c r="I155" s="4"/>
@@ -8824,7 +8983,7 @@
       <c r="K155" s="4"/>
       <c r="L155" s="56"/>
       <c r="M155" s="4"/>
-      <c r="N155" s="74"/>
+      <c r="N155" s="73"/>
       <c r="O155" s="9"/>
       <c r="P155" s="4"/>
       <c r="Q155" s="4"/>
@@ -8838,7 +8997,7 @@
       <c r="C156" s="54"/>
       <c r="D156" s="54"/>
       <c r="E156" s="63"/>
-      <c r="F156" s="75"/>
+      <c r="F156" s="74"/>
       <c r="G156" s="56"/>
       <c r="H156" s="65"/>
       <c r="I156" s="4"/>
@@ -8846,7 +9005,7 @@
       <c r="K156" s="4"/>
       <c r="L156" s="56"/>
       <c r="M156" s="4"/>
-      <c r="N156" s="74"/>
+      <c r="N156" s="73"/>
       <c r="O156" s="9"/>
       <c r="P156" s="4"/>
       <c r="Q156" s="4"/>
@@ -8860,7 +9019,7 @@
       <c r="C157" s="54"/>
       <c r="D157" s="54"/>
       <c r="E157" s="63"/>
-      <c r="F157" s="75"/>
+      <c r="F157" s="74"/>
       <c r="G157" s="56"/>
       <c r="H157" s="65"/>
       <c r="I157" s="4"/>
@@ -8868,7 +9027,7 @@
       <c r="K157" s="4"/>
       <c r="L157" s="56"/>
       <c r="M157" s="4"/>
-      <c r="N157" s="74"/>
+      <c r="N157" s="73"/>
       <c r="O157" s="9"/>
       <c r="P157" s="4"/>
       <c r="Q157" s="4"/>
@@ -8882,7 +9041,7 @@
       <c r="C158" s="54"/>
       <c r="D158" s="54"/>
       <c r="E158" s="63"/>
-      <c r="F158" s="75"/>
+      <c r="F158" s="74"/>
       <c r="G158" s="56"/>
       <c r="H158" s="65"/>
       <c r="I158" s="4"/>
@@ -8890,7 +9049,7 @@
       <c r="K158" s="4"/>
       <c r="L158" s="4"/>
       <c r="M158" s="4"/>
-      <c r="N158" s="74"/>
+      <c r="N158" s="73"/>
       <c r="O158" s="9"/>
       <c r="P158" s="4"/>
       <c r="Q158" s="4"/>
@@ -8904,7 +9063,7 @@
       <c r="C159" s="54"/>
       <c r="D159" s="54"/>
       <c r="E159" s="63"/>
-      <c r="F159" s="75"/>
+      <c r="F159" s="74"/>
       <c r="G159" s="56"/>
       <c r="H159" s="65"/>
       <c r="I159" s="4"/>
@@ -8912,7 +9071,7 @@
       <c r="K159" s="4"/>
       <c r="L159" s="4"/>
       <c r="M159" s="4"/>
-      <c r="N159" s="74"/>
+      <c r="N159" s="73"/>
       <c r="O159" s="9"/>
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
@@ -8926,7 +9085,7 @@
       <c r="C160" s="54"/>
       <c r="D160" s="54"/>
       <c r="E160" s="63"/>
-      <c r="F160" s="75"/>
+      <c r="F160" s="74"/>
       <c r="G160" s="56"/>
       <c r="H160" s="65"/>
       <c r="I160" s="4"/>
@@ -8934,7 +9093,7 @@
       <c r="K160" s="4"/>
       <c r="L160" s="4"/>
       <c r="M160" s="4"/>
-      <c r="N160" s="74"/>
+      <c r="N160" s="73"/>
       <c r="O160" s="9"/>
       <c r="P160" s="64"/>
       <c r="Q160" s="4"/>
@@ -8948,7 +9107,7 @@
       <c r="C161" s="54"/>
       <c r="D161" s="54"/>
       <c r="E161" s="63"/>
-      <c r="F161" s="75"/>
+      <c r="F161" s="74"/>
       <c r="G161" s="56"/>
       <c r="H161" s="65"/>
       <c r="I161" s="4"/>
@@ -8970,7 +9129,7 @@
       <c r="C162" s="54"/>
       <c r="D162" s="54"/>
       <c r="E162" s="63"/>
-      <c r="F162" s="75"/>
+      <c r="F162" s="74"/>
       <c r="G162" s="56"/>
       <c r="H162" s="65"/>
       <c r="I162" s="4"/>

</xml_diff>

<commit_message>
- extracted data from `10.1063/5.0160762`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF2A46B-60FE-B349-921C-C89EEE507195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E0204D-C5EE-9D45-B660-F4CA3C3CED3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8220" windowWidth="34560" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="172">
   <si>
     <r>
       <rPr>
@@ -607,6 +607,45 @@
   </si>
   <si>
     <t>10.1007/s11837-023-06129-2</t>
+  </si>
+  <si>
+    <t>Hf20Nb31Ta31Ti18</t>
+  </si>
+  <si>
+    <t>HNTT</t>
+  </si>
+  <si>
+    <t>HNTT-Mn</t>
+  </si>
+  <si>
+    <t>HNTT-Cu</t>
+  </si>
+  <si>
+    <t>HNTT-Fe</t>
+  </si>
+  <si>
+    <t>Hf20 Nb29.75 Ta29.75 Ti18 Mn2.5</t>
+  </si>
+  <si>
+    <t>Hf20 Nb29.75 Ta29.75 Ti18 Cu2.5</t>
+  </si>
+  <si>
+    <t>Hf20 Nb29.75 Ta29.75 Ti18 Al2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HNTT-Al </t>
+  </si>
+  <si>
+    <t>Hf20 Nb29.75 Ta29.75 Ti18 Fe2.5</t>
+  </si>
+  <si>
+    <t>prepared and tested under vacuum</t>
+  </si>
+  <si>
+    <t>prepared and tested under vacuum; significant loss of Mn observed</t>
+  </si>
+  <si>
+    <t>10.1063/5.0160762</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1713,6 +1752,10 @@
     </xf>
     <xf numFmtId="49" fontId="15" fillId="10" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="10" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="15" fillId="10" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2875,8 +2918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T856"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N128" sqref="N128"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A116" zoomScale="86" workbookViewId="0">
+      <selection activeCell="O151" sqref="O151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -8657,661 +8700,1626 @@
       <c r="T126" s="9"/>
     </row>
     <row r="127" spans="1:20" ht="18" customHeight="1">
-      <c r="A127" s="69"/>
-      <c r="B127" s="54"/>
-      <c r="C127" s="53"/>
-      <c r="D127" s="53"/>
-      <c r="E127" s="54"/>
-      <c r="F127" s="55"/>
-      <c r="G127" s="55"/>
+      <c r="A127" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="B127" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C127" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D127" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E127" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F127" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G127" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H127" s="56"/>
-      <c r="I127" s="57"/>
-      <c r="J127" s="53"/>
-      <c r="K127" s="65"/>
-      <c r="L127" s="67"/>
-      <c r="M127" s="67"/>
-      <c r="N127" s="53"/>
+      <c r="I127" s="57">
+        <v>298</v>
+      </c>
+      <c r="J127" s="65">
+        <f t="shared" ref="J127:K156" si="13">P127*9807000</f>
+        <v>2883258000</v>
+      </c>
+      <c r="K127" s="65">
+        <f t="shared" si="13"/>
+        <v>49035000</v>
+      </c>
+      <c r="L127" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M127" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N127" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O127" s="9"/>
-      <c r="P127" s="63"/>
-      <c r="Q127" s="4"/>
+      <c r="P127" s="63">
+        <v>294</v>
+      </c>
+      <c r="Q127" s="4">
+        <v>5</v>
+      </c>
       <c r="R127" s="62"/>
       <c r="S127" s="9"/>
       <c r="T127" s="9"/>
     </row>
     <row r="128" spans="1:20" ht="18" customHeight="1">
-      <c r="A128" s="53"/>
-      <c r="B128" s="54"/>
-      <c r="C128" s="53"/>
-      <c r="D128" s="53"/>
-      <c r="E128" s="54"/>
-      <c r="F128" s="55"/>
-      <c r="G128" s="55"/>
+      <c r="A128" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="B128" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="C128" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D128" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E128" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="F128" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G128" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H128" s="56"/>
-      <c r="I128" s="57"/>
-      <c r="J128" s="66"/>
-      <c r="K128" s="65"/>
-      <c r="L128" s="67"/>
-      <c r="M128" s="67"/>
-      <c r="N128" s="53"/>
+      <c r="I128" s="57">
+        <v>298</v>
+      </c>
+      <c r="J128" s="65">
+        <f t="shared" si="13"/>
+        <v>2314452000</v>
+      </c>
+      <c r="K128" s="65">
+        <f t="shared" si="13"/>
+        <v>58842000</v>
+      </c>
+      <c r="L128" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M128" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N128" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O128" s="9"/>
-      <c r="P128" s="63"/>
-      <c r="Q128" s="4"/>
+      <c r="P128" s="63">
+        <v>236</v>
+      </c>
+      <c r="Q128" s="4">
+        <v>6</v>
+      </c>
       <c r="R128" s="62"/>
       <c r="S128" s="9"/>
       <c r="T128" s="9"/>
     </row>
     <row r="129" spans="1:20" ht="18" customHeight="1">
-      <c r="A129" s="53"/>
-      <c r="B129" s="54"/>
-      <c r="C129" s="53"/>
-      <c r="D129" s="53"/>
-      <c r="E129" s="54"/>
-      <c r="F129" s="55"/>
-      <c r="G129" s="55"/>
+      <c r="A129" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="B129" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="C129" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D129" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E129" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F129" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G129" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H129" s="56"/>
-      <c r="I129" s="57"/>
-      <c r="J129" s="66"/>
-      <c r="K129" s="58"/>
-      <c r="L129" s="67"/>
-      <c r="M129" s="67"/>
-      <c r="N129" s="53"/>
+      <c r="I129" s="57">
+        <v>298</v>
+      </c>
+      <c r="J129" s="65">
+        <f t="shared" si="13"/>
+        <v>2363487000</v>
+      </c>
+      <c r="K129" s="65">
+        <f t="shared" si="13"/>
+        <v>39228000</v>
+      </c>
+      <c r="L129" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M129" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N129" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O129" s="9"/>
-      <c r="P129" s="63"/>
-      <c r="Q129" s="4"/>
+      <c r="P129" s="63">
+        <v>241</v>
+      </c>
+      <c r="Q129" s="4">
+        <v>4</v>
+      </c>
       <c r="R129" s="62"/>
       <c r="S129" s="9"/>
       <c r="T129" s="9"/>
     </row>
     <row r="130" spans="1:20" ht="18" customHeight="1">
-      <c r="A130" s="53"/>
-      <c r="B130" s="54"/>
-      <c r="C130" s="53"/>
-      <c r="D130" s="53"/>
-      <c r="E130" s="54"/>
-      <c r="F130" s="55"/>
-      <c r="G130" s="55"/>
+      <c r="A130" s="53" t="s">
+        <v>162</v>
+      </c>
+      <c r="B130" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="C130" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D130" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E130" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F130" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G130" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H130" s="56"/>
-      <c r="I130" s="57"/>
-      <c r="J130" s="58"/>
-      <c r="K130" s="58"/>
-      <c r="L130" s="67"/>
-      <c r="M130" s="67"/>
-      <c r="N130" s="53"/>
+      <c r="I130" s="57">
+        <v>298</v>
+      </c>
+      <c r="J130" s="65">
+        <f t="shared" si="13"/>
+        <v>2500785000</v>
+      </c>
+      <c r="K130" s="65">
+        <f t="shared" si="13"/>
+        <v>9807000</v>
+      </c>
+      <c r="L130" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M130" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N130" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O130" s="9"/>
-      <c r="P130" s="63"/>
-      <c r="Q130" s="4"/>
+      <c r="P130" s="63">
+        <v>255</v>
+      </c>
+      <c r="Q130" s="4">
+        <v>1</v>
+      </c>
       <c r="R130" s="62"/>
       <c r="S130" s="9"/>
       <c r="T130" s="9"/>
     </row>
     <row r="131" spans="1:20" ht="18" customHeight="1">
-      <c r="A131" s="53"/>
-      <c r="B131" s="54"/>
-      <c r="C131" s="53"/>
-      <c r="D131" s="53"/>
-      <c r="E131" s="54"/>
-      <c r="F131" s="55"/>
-      <c r="G131" s="55"/>
+      <c r="A131" s="53" t="s">
+        <v>163</v>
+      </c>
+      <c r="B131" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="C131" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D131" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E131" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F131" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G131" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H131" s="56"/>
-      <c r="I131" s="57"/>
-      <c r="J131" s="58"/>
-      <c r="K131" s="58"/>
-      <c r="L131" s="55"/>
-      <c r="M131" s="55"/>
-      <c r="N131" s="72"/>
+      <c r="I131" s="57">
+        <v>298</v>
+      </c>
+      <c r="J131" s="65">
+        <f t="shared" si="13"/>
+        <v>3040170000</v>
+      </c>
+      <c r="K131" s="65">
+        <f t="shared" si="13"/>
+        <v>39228000</v>
+      </c>
+      <c r="L131" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M131" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N131" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O131" s="9"/>
-      <c r="P131" s="63"/>
-      <c r="Q131" s="4"/>
+      <c r="P131" s="63">
+        <v>310</v>
+      </c>
+      <c r="Q131" s="4">
+        <v>4</v>
+      </c>
       <c r="R131" s="62"/>
       <c r="S131" s="9"/>
       <c r="T131" s="9"/>
     </row>
     <row r="132" spans="1:20" ht="18" customHeight="1">
-      <c r="A132" s="53"/>
-      <c r="B132" s="54"/>
-      <c r="C132" s="53"/>
-      <c r="D132" s="53"/>
-      <c r="E132" s="54"/>
-      <c r="F132" s="55"/>
-      <c r="G132" s="55"/>
+      <c r="A132" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="B132" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C132" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D132" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E132" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F132" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G132" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H132" s="56"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="58"/>
-      <c r="K132" s="58"/>
-      <c r="L132" s="55"/>
-      <c r="M132" s="55"/>
-      <c r="N132" s="72"/>
+      <c r="I132" s="4">
+        <f>273+300</f>
+        <v>573</v>
+      </c>
+      <c r="J132" s="65">
+        <f t="shared" si="13"/>
+        <v>2216382000</v>
+      </c>
+      <c r="K132" s="65">
+        <f t="shared" si="13"/>
+        <v>19614000</v>
+      </c>
+      <c r="L132" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M132" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N132" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O132" s="9"/>
-      <c r="P132" s="63"/>
-      <c r="Q132" s="4"/>
+      <c r="P132" s="63">
+        <v>226</v>
+      </c>
+      <c r="Q132" s="4">
+        <v>2</v>
+      </c>
       <c r="R132" s="62"/>
       <c r="S132" s="9"/>
       <c r="T132" s="9"/>
     </row>
     <row r="133" spans="1:20" ht="18" customHeight="1">
-      <c r="A133" s="53"/>
-      <c r="B133" s="54"/>
-      <c r="C133" s="53"/>
-      <c r="D133" s="53"/>
-      <c r="E133" s="54"/>
-      <c r="F133" s="55"/>
-      <c r="G133" s="55"/>
+      <c r="A133" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="B133" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="C133" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D133" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E133" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="F133" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G133" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H133" s="56"/>
-      <c r="I133" s="4"/>
-      <c r="J133" s="58"/>
-      <c r="K133" s="58"/>
-      <c r="L133" s="55"/>
-      <c r="M133" s="55"/>
-      <c r="N133" s="72"/>
+      <c r="I133" s="4">
+        <f t="shared" ref="I133:I136" si="14">273+300</f>
+        <v>573</v>
+      </c>
+      <c r="J133" s="65">
+        <f t="shared" si="13"/>
+        <v>1922172000</v>
+      </c>
+      <c r="K133" s="65">
+        <f t="shared" si="13"/>
+        <v>19614000</v>
+      </c>
+      <c r="L133" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M133" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N133" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O133" s="9"/>
-      <c r="P133" s="63"/>
-      <c r="Q133" s="4"/>
+      <c r="P133" s="63">
+        <v>196</v>
+      </c>
+      <c r="Q133" s="4">
+        <v>2</v>
+      </c>
       <c r="R133" s="62"/>
       <c r="S133" s="9"/>
       <c r="T133" s="9"/>
     </row>
     <row r="134" spans="1:20" ht="18" customHeight="1">
-      <c r="A134" s="53"/>
-      <c r="B134" s="54"/>
-      <c r="C134" s="53"/>
-      <c r="D134" s="53"/>
-      <c r="E134" s="54"/>
-      <c r="F134" s="55"/>
-      <c r="G134" s="55"/>
+      <c r="A134" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="B134" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="C134" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D134" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E134" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F134" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G134" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H134" s="56"/>
-      <c r="I134" s="4"/>
-      <c r="J134" s="58"/>
-      <c r="K134" s="58"/>
-      <c r="L134" s="55"/>
-      <c r="M134" s="55"/>
-      <c r="N134" s="72"/>
+      <c r="I134" s="4">
+        <f t="shared" si="14"/>
+        <v>573</v>
+      </c>
+      <c r="J134" s="65">
+        <f t="shared" si="13"/>
+        <v>1873137000</v>
+      </c>
+      <c r="K134" s="65">
+        <f t="shared" si="13"/>
+        <v>49035000</v>
+      </c>
+      <c r="L134" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M134" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N134" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O134" s="9"/>
-      <c r="P134" s="4"/>
-      <c r="Q134" s="4"/>
+      <c r="P134" s="4">
+        <v>191</v>
+      </c>
+      <c r="Q134" s="4">
+        <v>5</v>
+      </c>
       <c r="R134" s="9"/>
       <c r="S134" s="9"/>
       <c r="T134" s="9"/>
     </row>
     <row r="135" spans="1:20" ht="18" customHeight="1">
-      <c r="A135" s="53"/>
-      <c r="B135" s="54"/>
-      <c r="C135" s="53"/>
-      <c r="D135" s="53"/>
-      <c r="E135" s="54"/>
-      <c r="F135" s="55"/>
-      <c r="G135" s="55"/>
+      <c r="A135" s="53" t="s">
+        <v>162</v>
+      </c>
+      <c r="B135" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="C135" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D135" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E135" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F135" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G135" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H135" s="56"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="58"/>
-      <c r="K135" s="58"/>
-      <c r="L135" s="55"/>
-      <c r="M135" s="55"/>
-      <c r="N135" s="72"/>
+      <c r="I135" s="4">
+        <f t="shared" si="14"/>
+        <v>573</v>
+      </c>
+      <c r="J135" s="65">
+        <f t="shared" si="13"/>
+        <v>2039856000</v>
+      </c>
+      <c r="K135" s="65">
+        <f t="shared" si="13"/>
+        <v>29421000</v>
+      </c>
+      <c r="L135" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M135" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N135" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O135" s="9"/>
-      <c r="P135" s="4"/>
-      <c r="Q135" s="4"/>
+      <c r="P135" s="4">
+        <v>208</v>
+      </c>
+      <c r="Q135" s="4">
+        <v>3</v>
+      </c>
       <c r="R135" s="9"/>
       <c r="S135" s="9"/>
       <c r="T135" s="9"/>
     </row>
     <row r="136" spans="1:20" ht="18" customHeight="1">
-      <c r="A136" s="53"/>
-      <c r="B136" s="54"/>
-      <c r="C136" s="53"/>
-      <c r="D136" s="53"/>
-      <c r="E136" s="54"/>
-      <c r="F136" s="55"/>
-      <c r="G136" s="55"/>
+      <c r="A136" s="53" t="s">
+        <v>163</v>
+      </c>
+      <c r="B136" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="C136" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D136" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E136" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F136" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G136" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H136" s="56"/>
-      <c r="I136" s="4"/>
-      <c r="J136" s="58"/>
-      <c r="K136" s="58"/>
-      <c r="L136" s="55"/>
-      <c r="M136" s="55"/>
-      <c r="N136" s="72"/>
+      <c r="I136" s="4">
+        <f t="shared" si="14"/>
+        <v>573</v>
+      </c>
+      <c r="J136" s="65">
+        <f t="shared" si="13"/>
+        <v>2569434000</v>
+      </c>
+      <c r="K136" s="65">
+        <f t="shared" si="13"/>
+        <v>49035000</v>
+      </c>
+      <c r="L136" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M136" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N136" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O136" s="9"/>
-      <c r="P136" s="4"/>
-      <c r="Q136" s="4"/>
+      <c r="P136" s="4">
+        <v>262</v>
+      </c>
+      <c r="Q136" s="4">
+        <v>5</v>
+      </c>
       <c r="R136" s="9"/>
       <c r="S136" s="9"/>
       <c r="T136" s="9"/>
     </row>
     <row r="137" spans="1:20" ht="18" customHeight="1">
-      <c r="A137" s="53"/>
-      <c r="B137" s="54"/>
-      <c r="C137" s="53"/>
-      <c r="D137" s="53"/>
-      <c r="E137" s="54"/>
-      <c r="F137" s="55"/>
-      <c r="G137" s="55"/>
+      <c r="A137" s="121" t="s">
+        <v>160</v>
+      </c>
+      <c r="B137" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="C137" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="D137" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E137" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="F137" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G137" s="119" t="s">
+        <v>29</v>
+      </c>
       <c r="H137" s="56"/>
-      <c r="I137" s="4"/>
-      <c r="J137" s="58"/>
-      <c r="K137" s="4"/>
-      <c r="L137" s="55"/>
-      <c r="M137" s="55"/>
-      <c r="N137" s="72"/>
+      <c r="I137" s="4">
+        <v>673</v>
+      </c>
+      <c r="J137" s="65">
+        <f t="shared" si="13"/>
+        <v>2206575000</v>
+      </c>
+      <c r="K137" s="65">
+        <f t="shared" si="13"/>
+        <v>39228000</v>
+      </c>
+      <c r="L137" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M137" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N137" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O137" s="9"/>
-      <c r="P137" s="4"/>
-      <c r="Q137" s="4"/>
+      <c r="P137" s="4">
+        <v>225</v>
+      </c>
+      <c r="Q137" s="4">
+        <v>4</v>
+      </c>
       <c r="R137" s="9"/>
       <c r="S137" s="9"/>
       <c r="T137" s="9"/>
     </row>
     <row r="138" spans="1:20" ht="18" customHeight="1">
-      <c r="A138" s="53"/>
-      <c r="B138" s="54"/>
-      <c r="C138" s="53"/>
-      <c r="D138" s="53"/>
-      <c r="E138" s="54"/>
-      <c r="F138" s="55"/>
-      <c r="G138" s="55"/>
+      <c r="A138" s="122" t="s">
+        <v>161</v>
+      </c>
+      <c r="B138" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C138" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D138" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E138" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="F138" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G138" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H138" s="56"/>
-      <c r="I138" s="4"/>
-      <c r="J138" s="4"/>
-      <c r="K138" s="4"/>
-      <c r="L138" s="55"/>
-      <c r="M138" s="55"/>
-      <c r="N138" s="72"/>
+      <c r="I138" s="4">
+        <v>673</v>
+      </c>
+      <c r="J138" s="65">
+        <f t="shared" si="13"/>
+        <v>1873137000</v>
+      </c>
+      <c r="K138" s="65">
+        <f t="shared" si="13"/>
+        <v>39228000</v>
+      </c>
+      <c r="L138" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M138" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N138" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O138" s="9"/>
-      <c r="P138" s="4"/>
-      <c r="Q138" s="4"/>
+      <c r="P138" s="4">
+        <v>191</v>
+      </c>
+      <c r="Q138" s="4">
+        <v>4</v>
+      </c>
       <c r="R138" s="9"/>
       <c r="S138" s="9"/>
       <c r="T138" s="9"/>
     </row>
     <row r="139" spans="1:20" ht="18" customHeight="1">
-      <c r="A139" s="53"/>
-      <c r="B139" s="54"/>
-      <c r="C139" s="53"/>
-      <c r="D139" s="53"/>
-      <c r="E139" s="54"/>
-      <c r="F139" s="55"/>
-      <c r="G139" s="55"/>
+      <c r="A139" s="122" t="s">
+        <v>167</v>
+      </c>
+      <c r="B139" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="C139" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D139" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E139" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F139" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G139" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H139" s="56"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="55"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="72"/>
+      <c r="I139" s="4">
+        <v>673</v>
+      </c>
+      <c r="J139" s="65">
+        <f t="shared" si="13"/>
+        <v>1843716000</v>
+      </c>
+      <c r="K139" s="65">
+        <f t="shared" si="13"/>
+        <v>39228000</v>
+      </c>
+      <c r="L139" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M139" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N139" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O139" s="9"/>
-      <c r="P139" s="4"/>
-      <c r="Q139" s="4"/>
+      <c r="P139" s="4">
+        <v>188</v>
+      </c>
+      <c r="Q139" s="4">
+        <v>4</v>
+      </c>
       <c r="R139" s="9"/>
       <c r="S139" s="9"/>
       <c r="T139" s="9"/>
     </row>
     <row r="140" spans="1:20" ht="18" customHeight="1">
-      <c r="A140" s="53"/>
-      <c r="B140" s="54"/>
-      <c r="C140" s="55"/>
-      <c r="D140" s="53"/>
-      <c r="E140" s="54"/>
-      <c r="F140" s="55"/>
-      <c r="G140" s="55"/>
+      <c r="A140" s="122" t="s">
+        <v>162</v>
+      </c>
+      <c r="B140" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="C140" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D140" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E140" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F140" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G140" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H140" s="56"/>
-      <c r="I140" s="57"/>
-      <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
-      <c r="L140" s="55"/>
-      <c r="M140" s="4"/>
-      <c r="N140" s="72"/>
+      <c r="I140" s="4">
+        <v>673</v>
+      </c>
+      <c r="J140" s="65">
+        <f t="shared" si="13"/>
+        <v>1981014000</v>
+      </c>
+      <c r="K140" s="65">
+        <f t="shared" si="13"/>
+        <v>19614000</v>
+      </c>
+      <c r="L140" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M140" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N140" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O140" s="9"/>
-      <c r="P140" s="4"/>
-      <c r="Q140" s="4"/>
+      <c r="P140" s="4">
+        <v>202</v>
+      </c>
+      <c r="Q140" s="4">
+        <v>2</v>
+      </c>
       <c r="R140" s="9"/>
       <c r="S140" s="9"/>
       <c r="T140" s="9"/>
     </row>
     <row r="141" spans="1:20" ht="18" customHeight="1">
-      <c r="A141" s="53"/>
-      <c r="B141" s="54"/>
-      <c r="C141" s="55"/>
-      <c r="D141" s="53"/>
-      <c r="E141" s="54"/>
-      <c r="F141" s="55"/>
-      <c r="G141" s="55"/>
+      <c r="A141" s="122" t="s">
+        <v>163</v>
+      </c>
+      <c r="B141" s="80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C141" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D141" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E141" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F141" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G141" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H141" s="56"/>
-      <c r="I141" s="57"/>
-      <c r="J141" s="4"/>
-      <c r="K141" s="4"/>
-      <c r="L141" s="55"/>
-      <c r="M141" s="4"/>
-      <c r="N141" s="72"/>
+      <c r="I141" s="4">
+        <v>673</v>
+      </c>
+      <c r="J141" s="65">
+        <f t="shared" si="13"/>
+        <v>2216382000</v>
+      </c>
+      <c r="K141" s="65">
+        <f t="shared" si="13"/>
+        <v>29421000</v>
+      </c>
+      <c r="L141" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M141" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N141" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O141" s="9"/>
-      <c r="P141" s="4"/>
-      <c r="Q141" s="4"/>
+      <c r="P141" s="4">
+        <v>226</v>
+      </c>
+      <c r="Q141" s="4">
+        <v>3</v>
+      </c>
       <c r="R141" s="9"/>
       <c r="S141" s="9"/>
       <c r="T141" s="9"/>
     </row>
     <row r="142" spans="1:20" ht="18" customHeight="1">
-      <c r="A142" s="53"/>
-      <c r="B142" s="54"/>
-      <c r="C142" s="55"/>
-      <c r="D142" s="53"/>
-      <c r="E142" s="54"/>
-      <c r="F142" s="55"/>
-      <c r="G142" s="55"/>
+      <c r="A142" s="121" t="s">
+        <v>160</v>
+      </c>
+      <c r="B142" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="C142" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="D142" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E142" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="F142" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G142" s="119" t="s">
+        <v>29</v>
+      </c>
       <c r="H142" s="56"/>
-      <c r="I142" s="57"/>
-      <c r="J142" s="4"/>
-      <c r="K142" s="4"/>
-      <c r="L142" s="55"/>
-      <c r="M142" s="4"/>
-      <c r="N142" s="72"/>
+      <c r="I142" s="57">
+        <v>873</v>
+      </c>
+      <c r="J142" s="65">
+        <f t="shared" si="13"/>
+        <v>2216382000</v>
+      </c>
+      <c r="K142" s="65">
+        <f t="shared" si="13"/>
+        <v>29421000</v>
+      </c>
+      <c r="L142" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M142" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N142" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O142" s="9"/>
-      <c r="P142" s="4"/>
-      <c r="Q142" s="4"/>
+      <c r="P142" s="4">
+        <v>226</v>
+      </c>
+      <c r="Q142" s="4">
+        <v>3</v>
+      </c>
       <c r="R142" s="9"/>
       <c r="S142" s="9"/>
       <c r="T142" s="9"/>
     </row>
     <row r="143" spans="1:20" ht="18" customHeight="1">
-      <c r="A143" s="53"/>
-      <c r="B143" s="54"/>
-      <c r="C143" s="55"/>
-      <c r="D143" s="53"/>
-      <c r="E143" s="54"/>
-      <c r="F143" s="55"/>
-      <c r="G143" s="55"/>
+      <c r="A143" s="122" t="s">
+        <v>161</v>
+      </c>
+      <c r="B143" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C143" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D143" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E143" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="F143" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G143" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H143" s="56"/>
-      <c r="I143" s="57"/>
-      <c r="J143" s="4"/>
-      <c r="K143" s="4"/>
-      <c r="L143" s="55"/>
-      <c r="M143" s="4"/>
-      <c r="N143" s="72"/>
+      <c r="I143" s="57">
+        <v>873</v>
+      </c>
+      <c r="J143" s="65">
+        <f t="shared" si="13"/>
+        <v>1902558000</v>
+      </c>
+      <c r="K143" s="65">
+        <f t="shared" si="13"/>
+        <v>19614000</v>
+      </c>
+      <c r="L143" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M143" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N143" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O143" s="9"/>
-      <c r="P143" s="4"/>
-      <c r="Q143" s="4"/>
+      <c r="P143" s="4">
+        <v>194</v>
+      </c>
+      <c r="Q143" s="4">
+        <v>2</v>
+      </c>
       <c r="R143" s="9"/>
       <c r="S143" s="9"/>
       <c r="T143" s="9"/>
     </row>
     <row r="144" spans="1:20" ht="18" customHeight="1">
-      <c r="A144" s="53"/>
-      <c r="B144" s="54"/>
-      <c r="C144" s="55"/>
-      <c r="D144" s="53"/>
-      <c r="E144" s="54"/>
-      <c r="F144" s="55"/>
-      <c r="G144" s="55"/>
+      <c r="A144" s="122" t="s">
+        <v>167</v>
+      </c>
+      <c r="B144" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="C144" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D144" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E144" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F144" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G144" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H144" s="56"/>
-      <c r="I144" s="57"/>
-      <c r="J144" s="4"/>
-      <c r="K144" s="4"/>
-      <c r="L144" s="55"/>
-      <c r="M144" s="4"/>
-      <c r="N144" s="72"/>
+      <c r="I144" s="57">
+        <v>873</v>
+      </c>
+      <c r="J144" s="65">
+        <f t="shared" si="13"/>
+        <v>1833909000</v>
+      </c>
+      <c r="K144" s="65">
+        <f t="shared" si="13"/>
+        <v>39228000</v>
+      </c>
+      <c r="L144" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M144" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N144" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O144" s="9"/>
-      <c r="P144" s="4"/>
-      <c r="Q144" s="4"/>
+      <c r="P144" s="4">
+        <v>187</v>
+      </c>
+      <c r="Q144" s="4">
+        <v>4</v>
+      </c>
       <c r="R144" s="9"/>
       <c r="S144" s="9"/>
       <c r="T144" s="9"/>
     </row>
     <row r="145" spans="1:20" ht="18" customHeight="1">
-      <c r="A145" s="53"/>
-      <c r="B145" s="54"/>
-      <c r="C145" s="55"/>
-      <c r="D145" s="53"/>
-      <c r="E145" s="54"/>
-      <c r="F145" s="55"/>
-      <c r="G145" s="55"/>
+      <c r="A145" s="122" t="s">
+        <v>162</v>
+      </c>
+      <c r="B145" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="C145" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D145" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E145" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F145" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G145" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H145" s="56"/>
-      <c r="I145" s="57"/>
-      <c r="J145" s="4"/>
-      <c r="K145" s="58"/>
-      <c r="L145" s="55"/>
-      <c r="M145" s="4"/>
-      <c r="N145" s="72"/>
+      <c r="I145" s="57">
+        <v>873</v>
+      </c>
+      <c r="J145" s="65">
+        <f t="shared" si="13"/>
+        <v>1931979000</v>
+      </c>
+      <c r="K145" s="65">
+        <f t="shared" si="13"/>
+        <v>78456000</v>
+      </c>
+      <c r="L145" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M145" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N145" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O145" s="9"/>
-      <c r="P145" s="4"/>
-      <c r="Q145" s="4"/>
+      <c r="P145" s="4">
+        <v>197</v>
+      </c>
+      <c r="Q145" s="4">
+        <v>8</v>
+      </c>
       <c r="R145" s="9"/>
       <c r="S145" s="9"/>
       <c r="T145" s="9"/>
     </row>
     <row r="146" spans="1:20" ht="18" customHeight="1">
-      <c r="A146" s="53"/>
-      <c r="B146" s="54"/>
-      <c r="C146" s="55"/>
-      <c r="D146" s="53"/>
-      <c r="E146" s="54"/>
-      <c r="F146" s="55"/>
-      <c r="G146" s="55"/>
+      <c r="A146" s="122" t="s">
+        <v>163</v>
+      </c>
+      <c r="B146" s="80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C146" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D146" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E146" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F146" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G146" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H146" s="56"/>
-      <c r="I146" s="57"/>
-      <c r="J146" s="58"/>
-      <c r="K146" s="58"/>
-      <c r="L146" s="55"/>
-      <c r="M146" s="4"/>
-      <c r="N146" s="72"/>
+      <c r="I146" s="57">
+        <v>873</v>
+      </c>
+      <c r="J146" s="65">
+        <f t="shared" si="13"/>
+        <v>2294838000</v>
+      </c>
+      <c r="K146" s="65">
+        <f t="shared" si="13"/>
+        <v>98070000</v>
+      </c>
+      <c r="L146" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M146" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N146" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O146" s="9"/>
-      <c r="P146" s="4"/>
-      <c r="Q146" s="4"/>
+      <c r="P146" s="4">
+        <v>234</v>
+      </c>
+      <c r="Q146" s="4">
+        <v>10</v>
+      </c>
       <c r="R146" s="9"/>
       <c r="S146" s="9"/>
       <c r="T146" s="9"/>
     </row>
     <row r="147" spans="1:20" ht="18" customHeight="1">
-      <c r="A147" s="53"/>
-      <c r="B147" s="54"/>
-      <c r="C147" s="55"/>
-      <c r="D147" s="53"/>
-      <c r="E147" s="54"/>
-      <c r="F147" s="55"/>
-      <c r="G147" s="55"/>
+      <c r="A147" s="121" t="s">
+        <v>160</v>
+      </c>
+      <c r="B147" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="C147" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="D147" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E147" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="F147" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G147" s="119" t="s">
+        <v>29</v>
+      </c>
       <c r="H147" s="56"/>
-      <c r="I147" s="57"/>
-      <c r="J147" s="58"/>
-      <c r="K147" s="58"/>
-      <c r="L147" s="55"/>
-      <c r="M147" s="55"/>
-      <c r="N147" s="72"/>
+      <c r="I147" s="57">
+        <v>1073</v>
+      </c>
+      <c r="J147" s="65">
+        <f t="shared" si="13"/>
+        <v>2010435000</v>
+      </c>
+      <c r="K147" s="65">
+        <f t="shared" si="13"/>
+        <v>39228000</v>
+      </c>
+      <c r="L147" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M147" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N147" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O147" s="9"/>
-      <c r="P147" s="4"/>
-      <c r="Q147" s="4"/>
+      <c r="P147" s="4">
+        <v>205</v>
+      </c>
+      <c r="Q147" s="4">
+        <v>4</v>
+      </c>
       <c r="R147" s="9"/>
       <c r="S147" s="9"/>
       <c r="T147" s="9"/>
     </row>
     <row r="148" spans="1:20" ht="18" customHeight="1">
-      <c r="A148" s="53"/>
-      <c r="B148" s="54"/>
-      <c r="C148" s="55"/>
-      <c r="D148" s="53"/>
-      <c r="E148" s="54"/>
-      <c r="F148" s="55"/>
-      <c r="G148" s="55"/>
+      <c r="A148" s="122" t="s">
+        <v>161</v>
+      </c>
+      <c r="B148" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C148" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D148" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E148" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="F148" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G148" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H148" s="56"/>
-      <c r="I148" s="57"/>
-      <c r="J148" s="58"/>
-      <c r="K148" s="58"/>
-      <c r="L148" s="55"/>
-      <c r="M148" s="55"/>
-      <c r="N148" s="53"/>
+      <c r="I148" s="57">
+        <v>1073</v>
+      </c>
+      <c r="J148" s="65">
+        <f t="shared" si="13"/>
+        <v>1824102000</v>
+      </c>
+      <c r="K148" s="65">
+        <f t="shared" si="13"/>
+        <v>19614000</v>
+      </c>
+      <c r="L148" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M148" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N148" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O148" s="9"/>
-      <c r="P148" s="4"/>
-      <c r="Q148" s="4"/>
+      <c r="P148" s="4">
+        <v>186</v>
+      </c>
+      <c r="Q148" s="4">
+        <v>2</v>
+      </c>
       <c r="R148" s="9"/>
       <c r="S148" s="9"/>
       <c r="T148" s="9"/>
     </row>
     <row r="149" spans="1:20" ht="18" customHeight="1">
-      <c r="A149" s="53"/>
-      <c r="B149" s="54"/>
-      <c r="C149" s="55"/>
-      <c r="D149" s="53"/>
-      <c r="E149" s="54"/>
-      <c r="F149" s="55"/>
-      <c r="G149" s="55"/>
+      <c r="A149" s="122" t="s">
+        <v>167</v>
+      </c>
+      <c r="B149" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="C149" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D149" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E149" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F149" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G149" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H149" s="56"/>
-      <c r="I149" s="57"/>
-      <c r="J149" s="58"/>
-      <c r="K149" s="58"/>
-      <c r="L149" s="55"/>
-      <c r="M149" s="55"/>
-      <c r="N149" s="53"/>
+      <c r="I149" s="57">
+        <v>1073</v>
+      </c>
+      <c r="J149" s="65">
+        <f t="shared" si="13"/>
+        <v>1824102000</v>
+      </c>
+      <c r="K149" s="65">
+        <f t="shared" si="13"/>
+        <v>29421000</v>
+      </c>
+      <c r="L149" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M149" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N149" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O149" s="9"/>
-      <c r="P149" s="4"/>
-      <c r="Q149" s="4"/>
+      <c r="P149" s="4">
+        <v>186</v>
+      </c>
+      <c r="Q149" s="4">
+        <v>3</v>
+      </c>
       <c r="R149" s="9"/>
       <c r="S149" s="9"/>
       <c r="T149" s="9"/>
     </row>
     <row r="150" spans="1:20" ht="18" customHeight="1">
-      <c r="A150" s="53"/>
-      <c r="B150" s="54"/>
-      <c r="C150" s="55"/>
-      <c r="D150" s="53"/>
-      <c r="E150" s="54"/>
-      <c r="F150" s="55"/>
-      <c r="G150" s="55"/>
+      <c r="A150" s="122" t="s">
+        <v>162</v>
+      </c>
+      <c r="B150" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="C150" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D150" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E150" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F150" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G150" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H150" s="56"/>
-      <c r="I150" s="57"/>
-      <c r="J150" s="58"/>
-      <c r="K150" s="58"/>
-      <c r="L150" s="55"/>
-      <c r="M150" s="55"/>
-      <c r="N150" s="53"/>
+      <c r="I150" s="57">
+        <v>1073</v>
+      </c>
+      <c r="J150" s="65">
+        <f t="shared" si="13"/>
+        <v>1824102000</v>
+      </c>
+      <c r="K150" s="65">
+        <f t="shared" si="13"/>
+        <v>29421000</v>
+      </c>
+      <c r="L150" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M150" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N150" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O150" s="9"/>
-      <c r="P150" s="4"/>
-      <c r="Q150" s="4"/>
+      <c r="P150" s="4">
+        <v>186</v>
+      </c>
+      <c r="Q150" s="4">
+        <v>3</v>
+      </c>
       <c r="R150" s="9"/>
       <c r="S150" s="9"/>
       <c r="T150" s="9"/>
     </row>
     <row r="151" spans="1:20" ht="18" customHeight="1">
-      <c r="A151" s="53"/>
-      <c r="B151" s="54"/>
-      <c r="C151" s="55"/>
-      <c r="D151" s="53"/>
-      <c r="E151" s="54"/>
-      <c r="F151" s="55"/>
-      <c r="G151" s="55"/>
+      <c r="A151" s="122" t="s">
+        <v>163</v>
+      </c>
+      <c r="B151" s="80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C151" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D151" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E151" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F151" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G151" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H151" s="56"/>
-      <c r="I151" s="57"/>
-      <c r="J151" s="58"/>
-      <c r="K151" s="58"/>
-      <c r="L151" s="55"/>
-      <c r="M151" s="55"/>
-      <c r="N151" s="53"/>
+      <c r="I151" s="57">
+        <v>1073</v>
+      </c>
+      <c r="J151" s="65">
+        <f t="shared" si="13"/>
+        <v>2177154000</v>
+      </c>
+      <c r="K151" s="65">
+        <f t="shared" si="13"/>
+        <v>58842000</v>
+      </c>
+      <c r="L151" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M151" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N151" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O151" s="9"/>
-      <c r="P151" s="4"/>
-      <c r="Q151" s="4"/>
+      <c r="P151" s="4">
+        <v>222</v>
+      </c>
+      <c r="Q151" s="4">
+        <v>6</v>
+      </c>
       <c r="R151" s="9"/>
       <c r="S151" s="9"/>
       <c r="T151" s="9"/>
     </row>
     <row r="152" spans="1:20" ht="18" customHeight="1">
-      <c r="A152" s="53"/>
-      <c r="B152" s="54"/>
-      <c r="C152" s="55"/>
-      <c r="D152" s="53"/>
-      <c r="E152" s="54"/>
-      <c r="F152" s="55"/>
-      <c r="G152" s="55"/>
+      <c r="A152" s="121" t="s">
+        <v>160</v>
+      </c>
+      <c r="B152" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="C152" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="D152" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E152" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="F152" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G152" s="119" t="s">
+        <v>29</v>
+      </c>
       <c r="H152" s="56"/>
-      <c r="I152" s="57"/>
-      <c r="J152" s="58"/>
-      <c r="K152" s="58"/>
-      <c r="L152" s="55"/>
-      <c r="M152" s="55"/>
-      <c r="N152" s="72"/>
+      <c r="I152" s="57">
+        <v>1273</v>
+      </c>
+      <c r="J152" s="65">
+        <f t="shared" si="13"/>
+        <v>1500471000</v>
+      </c>
+      <c r="K152" s="65">
+        <f t="shared" si="13"/>
+        <v>49035000</v>
+      </c>
+      <c r="L152" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M152" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N152" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O152" s="9"/>
-      <c r="P152" s="4"/>
-      <c r="Q152" s="4"/>
+      <c r="P152" s="4">
+        <v>153</v>
+      </c>
+      <c r="Q152" s="4">
+        <v>5</v>
+      </c>
       <c r="R152" s="9"/>
       <c r="S152" s="9"/>
       <c r="T152" s="9"/>
     </row>
     <row r="153" spans="1:20" ht="18" customHeight="1">
-      <c r="A153" s="53"/>
-      <c r="B153" s="54"/>
-      <c r="C153" s="55"/>
-      <c r="D153" s="53"/>
-      <c r="E153" s="54"/>
-      <c r="F153" s="55"/>
-      <c r="G153" s="55"/>
+      <c r="A153" s="122" t="s">
+        <v>161</v>
+      </c>
+      <c r="B153" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C153" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D153" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E153" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="F153" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G153" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H153" s="56"/>
-      <c r="I153" s="57"/>
-      <c r="J153" s="58"/>
-      <c r="K153" s="4"/>
-      <c r="L153" s="55"/>
-      <c r="M153" s="55"/>
-      <c r="N153" s="72"/>
+      <c r="I153" s="57">
+        <v>1273</v>
+      </c>
+      <c r="J153" s="65">
+        <f t="shared" si="13"/>
+        <v>1284717000</v>
+      </c>
+      <c r="K153" s="65">
+        <f t="shared" si="13"/>
+        <v>58842000</v>
+      </c>
+      <c r="L153" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M153" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N153" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O153" s="9"/>
-      <c r="P153" s="4"/>
-      <c r="Q153" s="4"/>
+      <c r="P153" s="4">
+        <v>131</v>
+      </c>
+      <c r="Q153" s="4">
+        <v>6</v>
+      </c>
       <c r="R153" s="9"/>
       <c r="S153" s="9"/>
       <c r="T153" s="9"/>
     </row>
     <row r="154" spans="1:20" ht="18" customHeight="1">
-      <c r="A154" s="53"/>
-      <c r="B154" s="54"/>
-      <c r="C154" s="53"/>
-      <c r="D154" s="53"/>
-      <c r="E154" s="62"/>
-      <c r="F154" s="73"/>
-      <c r="G154" s="55"/>
+      <c r="A154" s="122" t="s">
+        <v>167</v>
+      </c>
+      <c r="B154" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="C154" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D154" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E154" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F154" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G154" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H154" s="64"/>
-      <c r="I154" s="4"/>
-      <c r="J154" s="4"/>
-      <c r="K154" s="4"/>
-      <c r="L154" s="55"/>
-      <c r="M154" s="55"/>
-      <c r="N154" s="72"/>
+      <c r="I154" s="57">
+        <v>1273</v>
+      </c>
+      <c r="J154" s="65">
+        <f t="shared" si="13"/>
+        <v>1284717000</v>
+      </c>
+      <c r="K154" s="65">
+        <f t="shared" si="13"/>
+        <v>29421000</v>
+      </c>
+      <c r="L154" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M154" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N154" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O154" s="9"/>
-      <c r="P154" s="4"/>
-      <c r="Q154" s="4"/>
+      <c r="P154" s="4">
+        <v>131</v>
+      </c>
+      <c r="Q154" s="4">
+        <v>3</v>
+      </c>
       <c r="R154" s="9"/>
       <c r="S154" s="9"/>
       <c r="T154" s="9"/>
     </row>
     <row r="155" spans="1:20" ht="18" customHeight="1">
-      <c r="A155" s="53"/>
-      <c r="B155" s="54"/>
-      <c r="C155" s="53"/>
-      <c r="D155" s="53"/>
-      <c r="E155" s="62"/>
-      <c r="F155" s="73"/>
-      <c r="G155" s="55"/>
+      <c r="A155" s="122" t="s">
+        <v>162</v>
+      </c>
+      <c r="B155" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="C155" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D155" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E155" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F155" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G155" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H155" s="64"/>
-      <c r="I155" s="4"/>
-      <c r="J155" s="4"/>
-      <c r="K155" s="4"/>
-      <c r="L155" s="55"/>
-      <c r="M155" s="4"/>
-      <c r="N155" s="72"/>
+      <c r="I155" s="57">
+        <v>1273</v>
+      </c>
+      <c r="J155" s="65">
+        <f t="shared" si="13"/>
+        <v>1333752000</v>
+      </c>
+      <c r="K155" s="65">
+        <f t="shared" si="13"/>
+        <v>29421000</v>
+      </c>
+      <c r="L155" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M155" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N155" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O155" s="9"/>
-      <c r="P155" s="4"/>
-      <c r="Q155" s="4"/>
+      <c r="P155" s="4">
+        <v>136</v>
+      </c>
+      <c r="Q155" s="4">
+        <v>3</v>
+      </c>
       <c r="R155" s="9"/>
       <c r="S155" s="9"/>
       <c r="T155" s="9"/>
     </row>
     <row r="156" spans="1:20" ht="18" customHeight="1">
-      <c r="A156" s="53"/>
-      <c r="B156" s="54"/>
-      <c r="C156" s="53"/>
-      <c r="D156" s="53"/>
-      <c r="E156" s="62"/>
-      <c r="F156" s="73"/>
-      <c r="G156" s="55"/>
+      <c r="A156" s="122" t="s">
+        <v>163</v>
+      </c>
+      <c r="B156" s="80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C156" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D156" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E156" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F156" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="G156" s="120" t="s">
+        <v>29</v>
+      </c>
       <c r="H156" s="64"/>
-      <c r="I156" s="4"/>
-      <c r="J156" s="4"/>
-      <c r="K156" s="4"/>
-      <c r="L156" s="55"/>
-      <c r="M156" s="4"/>
-      <c r="N156" s="72"/>
+      <c r="I156" s="57">
+        <v>1273</v>
+      </c>
+      <c r="J156" s="65">
+        <f t="shared" si="13"/>
+        <v>1216068000</v>
+      </c>
+      <c r="K156" s="65">
+        <f t="shared" si="13"/>
+        <v>49035000</v>
+      </c>
+      <c r="L156" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="M156" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="N156" s="53" t="s">
+        <v>171</v>
+      </c>
       <c r="O156" s="9"/>
-      <c r="P156" s="4"/>
-      <c r="Q156" s="4"/>
+      <c r="P156" s="4">
+        <v>124</v>
+      </c>
+      <c r="Q156" s="4">
+        <v>5</v>
+      </c>
       <c r="R156" s="9"/>
       <c r="S156" s="9"/>
       <c r="T156" s="9"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matchar.2023.113321`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E0204D-C5EE-9D45-B660-F4CA3C3CED3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6809A4-2A1B-4B41-8082-709283BBA149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8220" windowWidth="34560" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="180">
   <si>
     <r>
       <rPr>
@@ -646,6 +646,30 @@
   </si>
   <si>
     <t>10.1063/5.0160762</t>
+  </si>
+  <si>
+    <t>Nb40 Ti25 Al15 V10 Ta5 Hf3 W2</t>
+  </si>
+  <si>
+    <t>strain rate 1e-3</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>AAM+H+AT</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 10h and aged at 923K for 120h</t>
+  </si>
+  <si>
+    <t>homogenized at 1473K for 10h and aged at 1123K for 120h</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchar.2023.113321</t>
   </si>
 </sst>
 </file>
@@ -2918,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T856"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A116" zoomScale="86" workbookViewId="0">
-      <selection activeCell="O151" sqref="O151"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A148" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M169" sqref="M169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -10326,19 +10350,43 @@
     </row>
     <row r="157" spans="1:20" ht="18" customHeight="1">
       <c r="A157" s="53"/>
-      <c r="B157" s="54"/>
-      <c r="C157" s="53"/>
-      <c r="D157" s="53"/>
+      <c r="B157" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C157" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D157" s="53" t="s">
+        <v>66</v>
+      </c>
       <c r="E157" s="62"/>
-      <c r="F157" s="73"/>
-      <c r="G157" s="55"/>
-      <c r="H157" s="64"/>
-      <c r="I157" s="4"/>
-      <c r="J157" s="4"/>
-      <c r="K157" s="4"/>
-      <c r="L157" s="55"/>
-      <c r="M157" s="4"/>
-      <c r="N157" s="72"/>
+      <c r="F157" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="G157" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="H157" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="I157" s="4">
+        <v>298</v>
+      </c>
+      <c r="J157" s="70">
+        <v>1024000000</v>
+      </c>
+      <c r="K157" s="70">
+        <v>7000000</v>
+      </c>
+      <c r="L157" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="M157" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="N157" s="72" t="s">
+        <v>179</v>
+      </c>
       <c r="O157" s="9"/>
       <c r="P157" s="4"/>
       <c r="Q157" s="4"/>
@@ -10348,19 +10396,43 @@
     </row>
     <row r="158" spans="1:20" ht="18" customHeight="1">
       <c r="A158" s="4"/>
-      <c r="B158" s="54"/>
-      <c r="C158" s="53"/>
-      <c r="D158" s="53"/>
+      <c r="B158" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C158" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D158" s="53" t="s">
+        <v>66</v>
+      </c>
       <c r="E158" s="62"/>
-      <c r="F158" s="73"/>
-      <c r="G158" s="55"/>
-      <c r="H158" s="64"/>
-      <c r="I158" s="4"/>
-      <c r="J158" s="4"/>
-      <c r="K158" s="4"/>
-      <c r="L158" s="4"/>
-      <c r="M158" s="4"/>
-      <c r="N158" s="72"/>
+      <c r="F158" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="G158" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="H158" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="I158" s="4">
+        <v>1073</v>
+      </c>
+      <c r="J158" s="70">
+        <v>611000000</v>
+      </c>
+      <c r="K158" s="70">
+        <v>24000000</v>
+      </c>
+      <c r="L158" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="M158" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="N158" s="72" t="s">
+        <v>179</v>
+      </c>
       <c r="O158" s="9"/>
       <c r="P158" s="4"/>
       <c r="Q158" s="4"/>
@@ -10370,19 +10442,43 @@
     </row>
     <row r="159" spans="1:20" ht="18" customHeight="1">
       <c r="A159" s="4"/>
-      <c r="B159" s="54"/>
-      <c r="C159" s="53"/>
-      <c r="D159" s="53"/>
+      <c r="B159" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C159" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D159" s="53" t="s">
+        <v>66</v>
+      </c>
       <c r="E159" s="62"/>
-      <c r="F159" s="73"/>
-      <c r="G159" s="55"/>
-      <c r="H159" s="64"/>
-      <c r="I159" s="4"/>
-      <c r="J159" s="4"/>
-      <c r="K159" s="4"/>
-      <c r="L159" s="4"/>
-      <c r="M159" s="4"/>
-      <c r="N159" s="72"/>
+      <c r="F159" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="G159" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="H159" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="I159" s="4">
+        <v>1173</v>
+      </c>
+      <c r="J159" s="70">
+        <v>437000000</v>
+      </c>
+      <c r="K159" s="70">
+        <v>8000000</v>
+      </c>
+      <c r="L159" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="M159" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="N159" s="72" t="s">
+        <v>179</v>
+      </c>
       <c r="O159" s="9"/>
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
@@ -10392,19 +10488,43 @@
     </row>
     <row r="160" spans="1:20" ht="18" customHeight="1">
       <c r="A160" s="4"/>
-      <c r="B160" s="54"/>
-      <c r="C160" s="53"/>
-      <c r="D160" s="53"/>
+      <c r="B160" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C160" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D160" s="53" t="s">
+        <v>66</v>
+      </c>
       <c r="E160" s="62"/>
-      <c r="F160" s="73"/>
-      <c r="G160" s="55"/>
-      <c r="H160" s="64"/>
-      <c r="I160" s="4"/>
-      <c r="J160" s="4"/>
-      <c r="K160" s="4"/>
-      <c r="L160" s="4"/>
-      <c r="M160" s="4"/>
-      <c r="N160" s="72"/>
+      <c r="F160" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="G160" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="H160" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="I160" s="4">
+        <v>1273</v>
+      </c>
+      <c r="J160" s="70">
+        <v>237000000</v>
+      </c>
+      <c r="K160" s="70">
+        <v>8000000</v>
+      </c>
+      <c r="L160" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="M160" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="N160" s="72" t="s">
+        <v>179</v>
+      </c>
       <c r="O160" s="9"/>
       <c r="P160" s="63"/>
       <c r="Q160" s="4"/>
@@ -10414,44 +10534,100 @@
     </row>
     <row r="161" spans="1:20" ht="18" customHeight="1">
       <c r="A161" s="4"/>
-      <c r="B161" s="54"/>
-      <c r="C161" s="53"/>
-      <c r="D161" s="53"/>
-      <c r="E161" s="62"/>
+      <c r="B161" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C161" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D161" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="E161" s="62" t="s">
+        <v>176</v>
+      </c>
       <c r="F161" s="73"/>
-      <c r="G161" s="55"/>
+      <c r="G161" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H161" s="64"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="4"/>
-      <c r="K161" s="4"/>
-      <c r="L161" s="4"/>
-      <c r="M161" s="4"/>
-      <c r="N161" s="4"/>
+      <c r="I161" s="4">
+        <v>298</v>
+      </c>
+      <c r="J161" s="65">
+        <f t="shared" ref="J161:K162" si="15">P161*9807000</f>
+        <v>3671740800</v>
+      </c>
+      <c r="K161" s="65">
+        <f t="shared" si="15"/>
+        <v>10787700</v>
+      </c>
+      <c r="L161" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="M161" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="N161" s="72" t="s">
+        <v>179</v>
+      </c>
       <c r="O161" s="9"/>
-      <c r="P161" s="66"/>
-      <c r="Q161" s="4"/>
+      <c r="P161" s="66">
+        <v>374.4</v>
+      </c>
+      <c r="Q161" s="4">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="R161" s="9"/>
       <c r="S161" s="9"/>
       <c r="T161" s="9"/>
     </row>
     <row r="162" spans="1:20" ht="18" customHeight="1">
       <c r="A162" s="4"/>
-      <c r="B162" s="54"/>
-      <c r="C162" s="53"/>
-      <c r="D162" s="53"/>
-      <c r="E162" s="62"/>
+      <c r="B162" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C162" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D162" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="E162" s="62" t="s">
+        <v>177</v>
+      </c>
       <c r="F162" s="73"/>
-      <c r="G162" s="55"/>
+      <c r="G162" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="H162" s="64"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
-      <c r="L162" s="4"/>
-      <c r="M162" s="4"/>
-      <c r="N162" s="4"/>
+      <c r="I162" s="4">
+        <v>298</v>
+      </c>
+      <c r="J162" s="65">
+        <f t="shared" si="15"/>
+        <v>3471678000</v>
+      </c>
+      <c r="K162" s="65">
+        <f t="shared" si="15"/>
+        <v>16671900</v>
+      </c>
+      <c r="L162" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="M162" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="N162" s="72" t="s">
+        <v>179</v>
+      </c>
       <c r="O162" s="9"/>
-      <c r="P162" s="66"/>
-      <c r="Q162" s="4"/>
+      <c r="P162" s="66">
+        <v>354</v>
+      </c>
+      <c r="Q162" s="4">
+        <v>1.7</v>
+      </c>
       <c r="R162" s="9"/>
       <c r="S162" s="9"/>
       <c r="T162" s="9"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2024.147225`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16409B35-3E37-5F48-A579-FDA01EAC6414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6678C2C-8414-5848-90E9-E1E71880E7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="4980" windowWidth="43540" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="7960" windowWidth="43540" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="203">
   <si>
     <r>
       <rPr>
@@ -724,6 +724,21 @@
   </si>
   <si>
     <t>10.1016/j.actamat.2023.118784</t>
+  </si>
+  <si>
+    <t>Ti42 Hf21 Nb21 V16</t>
+  </si>
+  <si>
+    <t>T42</t>
+  </si>
+  <si>
+    <t>aka T42</t>
+  </si>
+  <si>
+    <t>LENS(DED)</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2024.147225</t>
   </si>
 </sst>
 </file>
@@ -3060,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B249" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O281" sqref="O281"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A270" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G299" sqref="G299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -15911,20 +15926,41 @@
       <c r="T281" s="139"/>
     </row>
     <row r="282" spans="1:20" ht="18" customHeight="1">
-      <c r="A282" s="138"/>
-      <c r="B282" s="138"/>
-      <c r="C282" s="138"/>
-      <c r="D282" s="138"/>
-      <c r="E282" s="138"/>
-      <c r="F282" s="138"/>
-      <c r="G282" s="138"/>
-      <c r="H282" s="138"/>
-      <c r="I282" s="138"/>
-      <c r="J282" s="138"/>
+      <c r="A282" s="142" t="s">
+        <v>199</v>
+      </c>
+      <c r="B282" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C282" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D282" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E282" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F282" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G282" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I282" s="138">
+        <v>298</v>
+      </c>
+      <c r="J282" s="144">
+        <v>1030000000</v>
+      </c>
       <c r="K282" s="138"/>
-      <c r="L282" s="138"/>
+      <c r="L282" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M282" s="138"/>
-      <c r="N282" s="138"/>
+      <c r="N282" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O282" s="138"/>
       <c r="P282" s="138"/>
       <c r="Q282" s="138"/>
@@ -15934,19 +15970,38 @@
     </row>
     <row r="283" spans="1:20" ht="18" customHeight="1">
       <c r="A283" s="138"/>
-      <c r="B283" s="138"/>
-      <c r="C283" s="138"/>
-      <c r="D283" s="138"/>
-      <c r="E283" s="138"/>
-      <c r="F283" s="138"/>
-      <c r="G283" s="138"/>
-      <c r="H283" s="138"/>
-      <c r="I283" s="138"/>
-      <c r="J283" s="138"/>
+      <c r="B283" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C283" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D283" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E283" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F283" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G283" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I283" s="138">
+        <v>298</v>
+      </c>
+      <c r="J283" s="138">
+        <v>22.5</v>
+      </c>
       <c r="K283" s="138"/>
-      <c r="L283" s="138"/>
+      <c r="L283" s="142" t="s">
+        <v>71</v>
+      </c>
       <c r="M283" s="138"/>
-      <c r="N283" s="138"/>
+      <c r="N283" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O283" s="138"/>
       <c r="P283" s="138"/>
       <c r="Q283" s="138"/>
@@ -15956,19 +16011,38 @@
     </row>
     <row r="284" spans="1:20" ht="18" customHeight="1">
       <c r="A284" s="138"/>
-      <c r="B284" s="138"/>
-      <c r="C284" s="138"/>
-      <c r="D284" s="138"/>
-      <c r="E284" s="138"/>
-      <c r="F284" s="138"/>
-      <c r="G284" s="138"/>
-      <c r="H284" s="138"/>
-      <c r="I284" s="138"/>
-      <c r="J284" s="138"/>
+      <c r="B284" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C284" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D284" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E284" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F284" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G284" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I284" s="138">
+        <v>298</v>
+      </c>
+      <c r="J284" s="144">
+        <v>1017000000</v>
+      </c>
       <c r="K284" s="138"/>
-      <c r="L284" s="138"/>
+      <c r="L284" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M284" s="138"/>
-      <c r="N284" s="138"/>
+      <c r="N284" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O284" s="138"/>
       <c r="P284" s="138"/>
       <c r="Q284" s="138"/>
@@ -15978,19 +16052,38 @@
     </row>
     <row r="285" spans="1:20" ht="18" customHeight="1">
       <c r="A285" s="138"/>
-      <c r="B285" s="138"/>
-      <c r="C285" s="138"/>
-      <c r="D285" s="138"/>
-      <c r="E285" s="138"/>
-      <c r="F285" s="138"/>
-      <c r="G285" s="138"/>
-      <c r="H285" s="138"/>
-      <c r="I285" s="138"/>
-      <c r="J285" s="138"/>
+      <c r="B285" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C285" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D285" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E285" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F285" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G285" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I285" s="138">
+        <v>673</v>
+      </c>
+      <c r="J285" s="144">
+        <v>681000000</v>
+      </c>
       <c r="K285" s="138"/>
-      <c r="L285" s="138"/>
+      <c r="L285" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M285" s="138"/>
-      <c r="N285" s="138"/>
+      <c r="N285" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O285" s="138"/>
       <c r="P285" s="138"/>
       <c r="Q285" s="138"/>
@@ -16000,19 +16093,38 @@
     </row>
     <row r="286" spans="1:20" ht="18" customHeight="1">
       <c r="A286" s="138"/>
-      <c r="B286" s="138"/>
-      <c r="C286" s="138"/>
-      <c r="D286" s="138"/>
-      <c r="E286" s="138"/>
-      <c r="F286" s="138"/>
-      <c r="G286" s="138"/>
-      <c r="H286" s="138"/>
-      <c r="I286" s="138"/>
-      <c r="J286" s="138"/>
+      <c r="B286" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C286" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D286" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E286" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F286" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G286" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I286" s="138">
+        <v>673</v>
+      </c>
+      <c r="J286" s="138">
+        <v>27.8</v>
+      </c>
       <c r="K286" s="138"/>
-      <c r="L286" s="138"/>
+      <c r="L286" s="142" t="s">
+        <v>71</v>
+      </c>
       <c r="M286" s="138"/>
-      <c r="N286" s="138"/>
+      <c r="N286" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O286" s="138"/>
       <c r="P286" s="138"/>
       <c r="Q286" s="138"/>
@@ -16022,19 +16134,38 @@
     </row>
     <row r="287" spans="1:20" ht="18" customHeight="1">
       <c r="A287" s="138"/>
-      <c r="B287" s="138"/>
-      <c r="C287" s="138"/>
-      <c r="D287" s="138"/>
-      <c r="E287" s="138"/>
-      <c r="F287" s="138"/>
-      <c r="G287" s="138"/>
-      <c r="H287" s="138"/>
-      <c r="I287" s="138"/>
-      <c r="J287" s="138"/>
+      <c r="B287" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C287" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D287" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E287" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F287" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G287" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I287" s="138">
+        <v>673</v>
+      </c>
+      <c r="J287" s="144">
+        <v>802000000</v>
+      </c>
       <c r="K287" s="138"/>
-      <c r="L287" s="138"/>
+      <c r="L287" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M287" s="138"/>
-      <c r="N287" s="138"/>
+      <c r="N287" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O287" s="138"/>
       <c r="P287" s="138"/>
       <c r="Q287" s="138"/>
@@ -16044,19 +16175,38 @@
     </row>
     <row r="288" spans="1:20" ht="18" customHeight="1">
       <c r="A288" s="138"/>
-      <c r="B288" s="138"/>
-      <c r="C288" s="138"/>
-      <c r="D288" s="138"/>
-      <c r="E288" s="138"/>
-      <c r="F288" s="138"/>
-      <c r="G288" s="138"/>
-      <c r="H288" s="138"/>
-      <c r="I288" s="138"/>
-      <c r="J288" s="138"/>
+      <c r="B288" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C288" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D288" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E288" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F288" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G288" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I288" s="138">
+        <v>773</v>
+      </c>
+      <c r="J288" s="144">
+        <v>661000000</v>
+      </c>
       <c r="K288" s="138"/>
-      <c r="L288" s="138"/>
+      <c r="L288" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M288" s="138"/>
-      <c r="N288" s="138"/>
+      <c r="N288" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O288" s="138"/>
       <c r="P288" s="138"/>
       <c r="Q288" s="138"/>
@@ -16066,19 +16216,38 @@
     </row>
     <row r="289" spans="1:20" ht="18" customHeight="1">
       <c r="A289" s="138"/>
-      <c r="B289" s="138"/>
-      <c r="C289" s="138"/>
-      <c r="D289" s="138"/>
-      <c r="E289" s="138"/>
-      <c r="F289" s="138"/>
-      <c r="G289" s="138"/>
-      <c r="H289" s="138"/>
-      <c r="I289" s="138"/>
-      <c r="J289" s="138"/>
+      <c r="B289" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C289" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D289" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E289" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F289" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G289" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I289" s="138">
+        <v>773</v>
+      </c>
+      <c r="J289" s="138">
+        <v>16.8</v>
+      </c>
       <c r="K289" s="138"/>
-      <c r="L289" s="138"/>
+      <c r="L289" s="142" t="s">
+        <v>71</v>
+      </c>
       <c r="M289" s="138"/>
-      <c r="N289" s="138"/>
+      <c r="N289" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O289" s="138"/>
       <c r="P289" s="138"/>
       <c r="Q289" s="138"/>
@@ -16088,19 +16257,38 @@
     </row>
     <row r="290" spans="1:20" ht="18" customHeight="1">
       <c r="A290" s="138"/>
-      <c r="B290" s="138"/>
-      <c r="C290" s="138"/>
-      <c r="D290" s="138"/>
-      <c r="E290" s="138"/>
-      <c r="F290" s="138"/>
-      <c r="G290" s="138"/>
-      <c r="H290" s="138"/>
-      <c r="I290" s="138"/>
-      <c r="J290" s="138"/>
+      <c r="B290" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C290" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D290" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E290" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F290" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G290" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I290" s="138">
+        <v>773</v>
+      </c>
+      <c r="J290" s="144">
+        <v>767000000</v>
+      </c>
       <c r="K290" s="138"/>
-      <c r="L290" s="138"/>
+      <c r="L290" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M290" s="138"/>
-      <c r="N290" s="138"/>
+      <c r="N290" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O290" s="138"/>
       <c r="P290" s="138"/>
       <c r="Q290" s="138"/>
@@ -16110,19 +16298,38 @@
     </row>
     <row r="291" spans="1:20" ht="18" customHeight="1">
       <c r="A291" s="138"/>
-      <c r="B291" s="138"/>
-      <c r="C291" s="138"/>
-      <c r="D291" s="138"/>
-      <c r="E291" s="138"/>
-      <c r="F291" s="138"/>
-      <c r="G291" s="138"/>
-      <c r="H291" s="138"/>
-      <c r="I291" s="138"/>
-      <c r="J291" s="138"/>
+      <c r="B291" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C291" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D291" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E291" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F291" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G291" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I291" s="138">
+        <v>873</v>
+      </c>
+      <c r="J291" s="144">
+        <v>636000000</v>
+      </c>
       <c r="K291" s="138"/>
-      <c r="L291" s="138"/>
+      <c r="L291" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M291" s="138"/>
-      <c r="N291" s="138"/>
+      <c r="N291" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O291" s="138"/>
       <c r="P291" s="138"/>
       <c r="Q291" s="138"/>
@@ -16132,19 +16339,38 @@
     </row>
     <row r="292" spans="1:20" ht="18" customHeight="1">
       <c r="A292" s="138"/>
-      <c r="B292" s="138"/>
-      <c r="C292" s="138"/>
-      <c r="D292" s="138"/>
-      <c r="E292" s="138"/>
-      <c r="F292" s="138"/>
-      <c r="G292" s="138"/>
-      <c r="H292" s="138"/>
-      <c r="I292" s="138"/>
-      <c r="J292" s="138"/>
+      <c r="B292" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C292" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D292" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E292" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F292" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G292" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I292" s="138">
+        <v>873</v>
+      </c>
+      <c r="J292" s="138">
+        <v>7.5</v>
+      </c>
       <c r="K292" s="138"/>
-      <c r="L292" s="138"/>
+      <c r="L292" s="142" t="s">
+        <v>71</v>
+      </c>
       <c r="M292" s="138"/>
-      <c r="N292" s="138"/>
+      <c r="N292" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O292" s="138"/>
       <c r="P292" s="138"/>
       <c r="Q292" s="138"/>
@@ -16154,19 +16380,38 @@
     </row>
     <row r="293" spans="1:20" ht="18" customHeight="1">
       <c r="A293" s="138"/>
-      <c r="B293" s="138"/>
-      <c r="C293" s="138"/>
-      <c r="D293" s="138"/>
-      <c r="E293" s="138"/>
-      <c r="F293" s="138"/>
-      <c r="G293" s="138"/>
-      <c r="H293" s="138"/>
-      <c r="I293" s="138"/>
-      <c r="J293" s="138"/>
+      <c r="B293" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C293" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D293" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E293" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F293" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G293" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="I293" s="138">
+        <v>873</v>
+      </c>
+      <c r="J293" s="144">
+        <v>679000000</v>
+      </c>
       <c r="K293" s="138"/>
-      <c r="L293" s="138"/>
+      <c r="L293" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M293" s="138"/>
-      <c r="N293" s="138"/>
+      <c r="N293" s="142" t="s">
+        <v>202</v>
+      </c>
       <c r="O293" s="138"/>
       <c r="P293" s="138"/>
       <c r="Q293" s="138"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s12598-024-03153-2`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6678C2C-8414-5848-90E9-E1E71880E7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163485D4-8E60-C141-B47D-2375F4C8F245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="7960" windowWidth="43540" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="10620" windowWidth="43540" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="204">
   <si>
     <r>
       <rPr>
@@ -740,6 +740,9 @@
   <si>
     <t>10.1016/j.msea.2024.147225</t>
   </si>
+  <si>
+    <t>10.1007/s12598-024-03153-2</t>
+  </si>
 </sst>
 </file>
 
@@ -911,7 +914,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1599,11 +1602,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1913,6 +1927,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3075,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A270" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G299" sqref="G299"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A279" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H298" sqref="H298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -15947,6 +15962,9 @@
       <c r="G282" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H282" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I282" s="138">
         <v>298</v>
       </c>
@@ -15988,6 +16006,9 @@
       <c r="G283" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H283" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I283" s="138">
         <v>298</v>
       </c>
@@ -16029,6 +16050,9 @@
       <c r="G284" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H284" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I284" s="138">
         <v>298</v>
       </c>
@@ -16070,6 +16094,9 @@
       <c r="G285" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H285" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I285" s="138">
         <v>673</v>
       </c>
@@ -16111,6 +16138,9 @@
       <c r="G286" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H286" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I286" s="138">
         <v>673</v>
       </c>
@@ -16152,6 +16182,9 @@
       <c r="G287" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H287" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I287" s="138">
         <v>673</v>
       </c>
@@ -16193,6 +16226,9 @@
       <c r="G288" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H288" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I288" s="138">
         <v>773</v>
       </c>
@@ -16234,6 +16270,9 @@
       <c r="G289" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H289" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I289" s="138">
         <v>773</v>
       </c>
@@ -16275,6 +16314,9 @@
       <c r="G290" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H290" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I290" s="138">
         <v>773</v>
       </c>
@@ -16316,6 +16358,9 @@
       <c r="G291" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H291" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I291" s="138">
         <v>873</v>
       </c>
@@ -16357,6 +16402,9 @@
       <c r="G292" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H292" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I292" s="138">
         <v>873</v>
       </c>
@@ -16398,6 +16446,9 @@
       <c r="G293" s="142" t="s">
         <v>29</v>
       </c>
+      <c r="H293" s="145" t="s">
+        <v>173</v>
+      </c>
       <c r="I293" s="138">
         <v>873</v>
       </c>
@@ -16421,41 +16472,91 @@
     </row>
     <row r="294" spans="1:20" ht="18" customHeight="1">
       <c r="A294" s="138"/>
-      <c r="B294" s="138"/>
-      <c r="C294" s="138"/>
-      <c r="D294" s="138"/>
-      <c r="E294" s="138"/>
-      <c r="F294" s="138"/>
-      <c r="G294" s="138"/>
+      <c r="B294" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C294" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D294" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E294" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F294" s="142" t="s">
+        <v>63</v>
+      </c>
+      <c r="G294" s="142" t="s">
+        <v>29</v>
+      </c>
       <c r="H294" s="138"/>
-      <c r="I294" s="138"/>
-      <c r="J294" s="138"/>
-      <c r="K294" s="138"/>
-      <c r="L294" s="138"/>
+      <c r="I294" s="138">
+        <v>298</v>
+      </c>
+      <c r="J294" s="64">
+        <f t="shared" ref="J294:K294" si="21">P294*9807000</f>
+        <v>3599169000</v>
+      </c>
+      <c r="K294" s="64">
+        <f t="shared" si="21"/>
+        <v>33343800</v>
+      </c>
+      <c r="L294" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M294" s="138"/>
-      <c r="N294" s="138"/>
+      <c r="N294" s="142" t="s">
+        <v>203</v>
+      </c>
       <c r="O294" s="138"/>
-      <c r="P294" s="138"/>
-      <c r="Q294" s="138"/>
+      <c r="P294" s="138">
+        <v>367</v>
+      </c>
+      <c r="Q294" s="138">
+        <v>3.4</v>
+      </c>
       <c r="R294" s="138"/>
       <c r="S294" s="139"/>
       <c r="T294" s="139"/>
     </row>
     <row r="295" spans="1:20" ht="18" customHeight="1">
       <c r="A295" s="138"/>
-      <c r="B295" s="138"/>
-      <c r="C295" s="138"/>
-      <c r="D295" s="138"/>
-      <c r="E295" s="138"/>
-      <c r="F295" s="138"/>
-      <c r="G295" s="138"/>
+      <c r="B295" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C295" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D295" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E295" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F295" s="142" t="s">
+        <v>64</v>
+      </c>
+      <c r="G295" s="142" t="s">
+        <v>29</v>
+      </c>
       <c r="H295" s="138"/>
-      <c r="I295" s="138"/>
-      <c r="J295" s="138"/>
-      <c r="K295" s="138"/>
-      <c r="L295" s="138"/>
+      <c r="I295" s="138">
+        <v>298</v>
+      </c>
+      <c r="J295" s="144">
+        <v>4400000000</v>
+      </c>
+      <c r="K295" s="144">
+        <v>60000000</v>
+      </c>
+      <c r="L295" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M295" s="138"/>
-      <c r="N295" s="138"/>
+      <c r="N295" s="142" t="s">
+        <v>203</v>
+      </c>
       <c r="O295" s="138"/>
       <c r="P295" s="138"/>
       <c r="Q295" s="138"/>
@@ -16465,19 +16566,41 @@
     </row>
     <row r="296" spans="1:20" ht="18" customHeight="1">
       <c r="A296" s="138"/>
-      <c r="B296" s="138"/>
-      <c r="C296" s="138"/>
-      <c r="D296" s="138"/>
-      <c r="E296" s="138"/>
-      <c r="F296" s="138"/>
-      <c r="G296" s="138"/>
+      <c r="B296" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="C296" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D296" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="E296" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="F296" s="142" t="s">
+        <v>192</v>
+      </c>
+      <c r="G296" s="142" t="s">
+        <v>29</v>
+      </c>
       <c r="H296" s="138"/>
-      <c r="I296" s="138"/>
-      <c r="J296" s="138"/>
-      <c r="K296" s="138"/>
-      <c r="L296" s="138"/>
+      <c r="I296" s="138">
+        <v>298</v>
+      </c>
+      <c r="J296" s="144">
+        <v>107000000000</v>
+      </c>
+      <c r="K296" s="144">
+        <v>870000000</v>
+      </c>
+      <c r="L296" s="142" t="s">
+        <v>33</v>
+      </c>
       <c r="M296" s="138"/>
-      <c r="N296" s="138"/>
+      <c r="N296" s="142" t="s">
+        <v>203</v>
+      </c>
       <c r="O296" s="138"/>
       <c r="P296" s="138"/>
       <c r="Q296" s="138"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.actamat.2022.118449`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163485D4-8E60-C141-B47D-2375F4C8F245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B655E0-B354-C149-A9AD-0489F14121D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="10620" windowWidth="43540" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="6920" windowWidth="43540" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="210">
   <si>
     <r>
       <rPr>
@@ -742,6 +742,24 @@
   </si>
   <si>
     <t>10.1007/s12598-024-03153-2</t>
+  </si>
+  <si>
+    <t>Fe41.26 Ni28.2 Co17 Al11 Ta2.5 B0.04</t>
+  </si>
+  <si>
+    <t>FCC+B2</t>
+  </si>
+  <si>
+    <t>AAM+H+HR+A+AT</t>
+  </si>
+  <si>
+    <t>homogenized at 1573K for 1h twice then hot rolled at 1573K with around 25% reduction then cold rolled with 90% reduction then annealed at 1473K for 10min and aged at 873K for 2h</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2022.118449</t>
+  </si>
+  <si>
+    <t>F3a</t>
   </si>
 </sst>
 </file>
@@ -3090,8 +3108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A279" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H298" sqref="H298"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A290" zoomScale="75" workbookViewId="0">
+      <selection activeCell="L314" sqref="L314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -16610,21 +16628,48 @@
     </row>
     <row r="297" spans="1:20" ht="18" customHeight="1">
       <c r="A297" s="138"/>
-      <c r="B297" s="138"/>
-      <c r="C297" s="138"/>
-      <c r="D297" s="138"/>
-      <c r="E297" s="138"/>
-      <c r="F297" s="138"/>
-      <c r="G297" s="138"/>
-      <c r="H297" s="138"/>
-      <c r="I297" s="138"/>
-      <c r="J297" s="138"/>
+      <c r="B297" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C297" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D297" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E297" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F297" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G297" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H297" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I297" s="138">
+        <v>77</v>
+      </c>
+      <c r="J297" s="138">
+        <f>P297*1000000</f>
+        <v>1141618497.1098201</v>
+      </c>
       <c r="K297" s="138"/>
-      <c r="L297" s="138"/>
-      <c r="M297" s="138"/>
-      <c r="N297" s="138"/>
+      <c r="L297" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M297" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N297" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O297" s="138"/>
-      <c r="P297" s="138"/>
+      <c r="P297" s="138">
+        <v>1141.6184971098201</v>
+      </c>
       <c r="Q297" s="138"/>
       <c r="R297" s="138"/>
       <c r="S297" s="139"/>
@@ -16632,21 +16677,48 @@
     </row>
     <row r="298" spans="1:20" ht="18" customHeight="1">
       <c r="A298" s="138"/>
-      <c r="B298" s="138"/>
-      <c r="C298" s="138"/>
-      <c r="D298" s="138"/>
-      <c r="E298" s="138"/>
-      <c r="F298" s="138"/>
-      <c r="G298" s="138"/>
-      <c r="H298" s="138"/>
-      <c r="I298" s="138"/>
-      <c r="J298" s="138"/>
+      <c r="B298" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C298" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D298" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E298" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F298" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G298" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H298" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I298" s="138">
+        <v>298</v>
+      </c>
+      <c r="J298" s="138">
+        <f t="shared" ref="J298:J304" si="22">P298*1000000</f>
+        <v>1005780346.8207999</v>
+      </c>
       <c r="K298" s="138"/>
-      <c r="L298" s="138"/>
-      <c r="M298" s="138"/>
-      <c r="N298" s="138"/>
+      <c r="L298" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M298" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N298" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O298" s="138"/>
-      <c r="P298" s="138"/>
+      <c r="P298" s="138">
+        <v>1005.7803468208</v>
+      </c>
       <c r="Q298" s="138"/>
       <c r="R298" s="138"/>
       <c r="S298" s="139"/>
@@ -16654,21 +16726,48 @@
     </row>
     <row r="299" spans="1:20" ht="18" customHeight="1">
       <c r="A299" s="138"/>
-      <c r="B299" s="138"/>
-      <c r="C299" s="138"/>
-      <c r="D299" s="138"/>
-      <c r="E299" s="138"/>
-      <c r="F299" s="138"/>
-      <c r="G299" s="138"/>
-      <c r="H299" s="138"/>
-      <c r="I299" s="138"/>
-      <c r="J299" s="138"/>
+      <c r="B299" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C299" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D299" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E299" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F299" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G299" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H299" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I299" s="138">
+        <v>873</v>
+      </c>
+      <c r="J299" s="138">
+        <f t="shared" si="22"/>
+        <v>598265895.95375693</v>
+      </c>
       <c r="K299" s="138"/>
-      <c r="L299" s="138"/>
-      <c r="M299" s="138"/>
-      <c r="N299" s="138"/>
+      <c r="L299" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M299" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N299" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O299" s="138"/>
-      <c r="P299" s="138"/>
+      <c r="P299" s="138">
+        <v>598.26589595375697</v>
+      </c>
       <c r="Q299" s="138"/>
       <c r="R299" s="138"/>
       <c r="S299" s="139"/>
@@ -16676,21 +16775,48 @@
     </row>
     <row r="300" spans="1:20" ht="18" customHeight="1">
       <c r="A300" s="138"/>
-      <c r="B300" s="138"/>
-      <c r="C300" s="138"/>
-      <c r="D300" s="138"/>
-      <c r="E300" s="138"/>
-      <c r="F300" s="138"/>
-      <c r="G300" s="138"/>
-      <c r="H300" s="138"/>
-      <c r="I300" s="138"/>
-      <c r="J300" s="138"/>
+      <c r="B300" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C300" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D300" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E300" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F300" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G300" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H300" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I300" s="138">
+        <v>1073</v>
+      </c>
+      <c r="J300" s="138">
+        <f t="shared" si="22"/>
+        <v>485549132.94797701</v>
+      </c>
       <c r="K300" s="138"/>
-      <c r="L300" s="138"/>
-      <c r="M300" s="138"/>
-      <c r="N300" s="138"/>
+      <c r="L300" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M300" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N300" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O300" s="138"/>
-      <c r="P300" s="138"/>
+      <c r="P300" s="138">
+        <v>485.549132947977</v>
+      </c>
       <c r="Q300" s="138"/>
       <c r="R300" s="138"/>
       <c r="S300" s="139"/>
@@ -16698,21 +16824,48 @@
     </row>
     <row r="301" spans="1:20" ht="18" customHeight="1">
       <c r="A301" s="138"/>
-      <c r="B301" s="138"/>
-      <c r="C301" s="138"/>
-      <c r="D301" s="138"/>
-      <c r="E301" s="138"/>
-      <c r="F301" s="138"/>
-      <c r="G301" s="138"/>
-      <c r="H301" s="138"/>
-      <c r="I301" s="138"/>
-      <c r="J301" s="138"/>
+      <c r="B301" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C301" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D301" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E301" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F301" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G301" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H301" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I301" s="138">
+        <v>77</v>
+      </c>
+      <c r="J301" s="138">
+        <f t="shared" si="22"/>
+        <v>2187861271.6763</v>
+      </c>
       <c r="K301" s="138"/>
-      <c r="L301" s="138"/>
-      <c r="M301" s="138"/>
-      <c r="N301" s="138"/>
+      <c r="L301" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M301" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N301" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O301" s="138"/>
-      <c r="P301" s="138"/>
+      <c r="P301" s="138">
+        <v>2187.8612716763</v>
+      </c>
       <c r="Q301" s="138"/>
       <c r="R301" s="138"/>
       <c r="S301" s="139"/>
@@ -16720,21 +16873,48 @@
     </row>
     <row r="302" spans="1:20" ht="18" customHeight="1">
       <c r="A302" s="138"/>
-      <c r="B302" s="138"/>
-      <c r="C302" s="138"/>
-      <c r="D302" s="138"/>
-      <c r="E302" s="138"/>
-      <c r="F302" s="138"/>
-      <c r="G302" s="138"/>
-      <c r="H302" s="138"/>
-      <c r="I302" s="138"/>
-      <c r="J302" s="138"/>
+      <c r="B302" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C302" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D302" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E302" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F302" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G302" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H302" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I302" s="138">
+        <v>298</v>
+      </c>
+      <c r="J302" s="138">
+        <f t="shared" si="22"/>
+        <v>1447976878.61271</v>
+      </c>
       <c r="K302" s="138"/>
-      <c r="L302" s="138"/>
-      <c r="M302" s="138"/>
-      <c r="N302" s="138"/>
+      <c r="L302" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M302" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N302" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O302" s="138"/>
-      <c r="P302" s="138"/>
+      <c r="P302" s="138">
+        <v>1447.9768786127099</v>
+      </c>
       <c r="Q302" s="138"/>
       <c r="R302" s="138"/>
       <c r="S302" s="139"/>
@@ -16742,21 +16922,48 @@
     </row>
     <row r="303" spans="1:20" ht="18" customHeight="1">
       <c r="A303" s="138"/>
-      <c r="B303" s="138"/>
-      <c r="C303" s="138"/>
-      <c r="D303" s="138"/>
-      <c r="E303" s="138"/>
-      <c r="F303" s="138"/>
-      <c r="G303" s="138"/>
-      <c r="H303" s="138"/>
-      <c r="I303" s="138"/>
-      <c r="J303" s="138"/>
+      <c r="B303" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C303" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D303" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E303" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F303" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G303" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H303" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I303" s="138">
+        <v>873</v>
+      </c>
+      <c r="J303" s="138">
+        <f t="shared" si="22"/>
+        <v>823699421.96531701</v>
+      </c>
       <c r="K303" s="138"/>
-      <c r="L303" s="138"/>
-      <c r="M303" s="138"/>
-      <c r="N303" s="138"/>
+      <c r="L303" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M303" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N303" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O303" s="138"/>
-      <c r="P303" s="138"/>
+      <c r="P303" s="138">
+        <v>823.69942196531701</v>
+      </c>
       <c r="Q303" s="138"/>
       <c r="R303" s="138"/>
       <c r="S303" s="139"/>
@@ -16764,21 +16971,48 @@
     </row>
     <row r="304" spans="1:20" ht="18" customHeight="1">
       <c r="A304" s="138"/>
-      <c r="B304" s="138"/>
-      <c r="C304" s="138"/>
-      <c r="D304" s="138"/>
-      <c r="E304" s="138"/>
-      <c r="F304" s="138"/>
-      <c r="G304" s="138"/>
-      <c r="H304" s="138"/>
-      <c r="I304" s="138"/>
-      <c r="J304" s="138"/>
+      <c r="B304" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C304" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D304" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E304" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F304" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G304" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H304" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I304" s="138">
+        <v>1073</v>
+      </c>
+      <c r="J304" s="138">
+        <f t="shared" si="22"/>
+        <v>523121387.28323704</v>
+      </c>
       <c r="K304" s="138"/>
-      <c r="L304" s="138"/>
-      <c r="M304" s="138"/>
-      <c r="N304" s="138"/>
+      <c r="L304" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M304" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N304" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O304" s="138"/>
-      <c r="P304" s="138"/>
+      <c r="P304" s="138">
+        <v>523.12138728323703</v>
+      </c>
       <c r="Q304" s="138"/>
       <c r="R304" s="138"/>
       <c r="S304" s="139"/>
@@ -16786,19 +17020,43 @@
     </row>
     <row r="305" spans="1:20" ht="18" customHeight="1">
       <c r="A305" s="138"/>
-      <c r="B305" s="138"/>
-      <c r="C305" s="138"/>
-      <c r="D305" s="138"/>
-      <c r="E305" s="138"/>
-      <c r="F305" s="138"/>
-      <c r="G305" s="138"/>
-      <c r="H305" s="138"/>
-      <c r="I305" s="138"/>
-      <c r="J305" s="138"/>
+      <c r="B305" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C305" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D305" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E305" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F305" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G305" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H305" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I305" s="138">
+        <v>77</v>
+      </c>
+      <c r="J305" s="138">
+        <v>12.4774774774774</v>
+      </c>
       <c r="K305" s="138"/>
-      <c r="L305" s="138"/>
-      <c r="M305" s="138"/>
-      <c r="N305" s="138"/>
+      <c r="L305" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M305" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N305" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O305" s="138"/>
       <c r="P305" s="138"/>
       <c r="Q305" s="138"/>
@@ -16808,19 +17066,43 @@
     </row>
     <row r="306" spans="1:20" ht="18" customHeight="1">
       <c r="A306" s="138"/>
-      <c r="B306" s="138"/>
-      <c r="C306" s="138"/>
-      <c r="D306" s="138"/>
-      <c r="E306" s="138"/>
-      <c r="F306" s="138"/>
-      <c r="G306" s="138"/>
-      <c r="H306" s="138"/>
-      <c r="I306" s="138"/>
-      <c r="J306" s="138"/>
+      <c r="B306" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C306" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D306" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E306" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F306" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G306" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H306" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I306" s="138">
+        <v>298</v>
+      </c>
+      <c r="J306" s="138">
+        <v>21.2612612612612</v>
+      </c>
       <c r="K306" s="138"/>
-      <c r="L306" s="138"/>
-      <c r="M306" s="138"/>
-      <c r="N306" s="138"/>
+      <c r="L306" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M306" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N306" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O306" s="138"/>
       <c r="P306" s="138"/>
       <c r="Q306" s="138"/>
@@ -16830,19 +17112,43 @@
     </row>
     <row r="307" spans="1:20" ht="18" customHeight="1">
       <c r="A307" s="138"/>
-      <c r="B307" s="138"/>
-      <c r="C307" s="138"/>
-      <c r="D307" s="138"/>
-      <c r="E307" s="138"/>
-      <c r="F307" s="138"/>
-      <c r="G307" s="138"/>
-      <c r="H307" s="138"/>
-      <c r="I307" s="138"/>
-      <c r="J307" s="138"/>
+      <c r="B307" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C307" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D307" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E307" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F307" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G307" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H307" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I307" s="138">
+        <v>873</v>
+      </c>
+      <c r="J307" s="138">
+        <v>24.234234234234201</v>
+      </c>
       <c r="K307" s="138"/>
-      <c r="L307" s="138"/>
-      <c r="M307" s="138"/>
-      <c r="N307" s="138"/>
+      <c r="L307" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M307" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N307" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O307" s="138"/>
       <c r="P307" s="138"/>
       <c r="Q307" s="138"/>
@@ -16852,19 +17158,43 @@
     </row>
     <row r="308" spans="1:20" ht="18" customHeight="1">
       <c r="A308" s="138"/>
-      <c r="B308" s="138"/>
-      <c r="C308" s="138"/>
-      <c r="D308" s="138"/>
-      <c r="E308" s="138"/>
-      <c r="F308" s="138"/>
-      <c r="G308" s="138"/>
-      <c r="H308" s="138"/>
-      <c r="I308" s="138"/>
-      <c r="J308" s="138"/>
+      <c r="B308" s="142" t="s">
+        <v>204</v>
+      </c>
+      <c r="C308" s="142" t="s">
+        <v>205</v>
+      </c>
+      <c r="D308" s="142" t="s">
+        <v>206</v>
+      </c>
+      <c r="E308" s="142" t="s">
+        <v>207</v>
+      </c>
+      <c r="F308" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G308" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H308" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I308" s="138">
+        <v>1073</v>
+      </c>
+      <c r="J308" s="138">
+        <v>22.387387387387299</v>
+      </c>
       <c r="K308" s="138"/>
-      <c r="L308" s="138"/>
-      <c r="M308" s="138"/>
-      <c r="N308" s="138"/>
+      <c r="L308" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M308" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="N308" s="142" t="s">
+        <v>208</v>
+      </c>
       <c r="O308" s="138"/>
       <c r="P308" s="138"/>
       <c r="Q308" s="138"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.actamat.2022.118602`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B655E0-B354-C149-A9AD-0489F14121D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BEA1E5-958B-284E-AA5B-9103067CC6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="6920" windowWidth="43540" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="5680" windowWidth="43540" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2914" uniqueCount="222">
   <si>
     <r>
       <rPr>
@@ -760,6 +760,42 @@
   </si>
   <si>
     <t>F3a</t>
+  </si>
+  <si>
+    <t>Hf15 Nb40 Ta25 Ti15 Zr5</t>
+  </si>
+  <si>
+    <t>NTTHZ</t>
+  </si>
+  <si>
+    <t>cold rolled with 90% reduction and annealed at 900*C for 60min forming heterogeneous lamella (HL) structure</t>
+  </si>
+  <si>
+    <t>cold rolled with 90% reduction and annealed at 1150*C for 60min forming fine grain (FG) structure</t>
+  </si>
+  <si>
+    <t>cold rolled with 90% reduction and annealed at 1300*C for 30min forming coarse grain (CG) structure</t>
+  </si>
+  <si>
+    <t>minimum tensile ductility</t>
+  </si>
+  <si>
+    <t>AAM+CR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cold rolled with 90% reduction </t>
+  </si>
+  <si>
+    <t>S7a</t>
+  </si>
+  <si>
+    <t>F6a</t>
+  </si>
+  <si>
+    <t>S11a</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2022.118602</t>
   </si>
 </sst>
 </file>
@@ -3108,8 +3144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A290" zoomScale="75" workbookViewId="0">
-      <selection activeCell="L314" sqref="L314"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A302" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N337" sqref="N337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -17203,20 +17239,46 @@
       <c r="T308" s="139"/>
     </row>
     <row r="309" spans="1:20" ht="18" customHeight="1">
-      <c r="A309" s="138"/>
-      <c r="B309" s="138"/>
-      <c r="C309" s="138"/>
-      <c r="D309" s="138"/>
-      <c r="E309" s="138"/>
-      <c r="F309" s="138"/>
-      <c r="G309" s="138"/>
-      <c r="H309" s="138"/>
-      <c r="I309" s="138"/>
-      <c r="J309" s="138"/>
+      <c r="A309" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B309" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C309" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D309" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E309" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F309" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G309" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H309" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I309" s="138">
+        <v>298</v>
+      </c>
+      <c r="J309" s="138">
+        <v>944444444.44444394</v>
+      </c>
       <c r="K309" s="138"/>
-      <c r="L309" s="138"/>
-      <c r="M309" s="138"/>
-      <c r="N309" s="138"/>
+      <c r="L309" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M309" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N309" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O309" s="138"/>
       <c r="P309" s="138"/>
       <c r="Q309" s="138"/>
@@ -17225,20 +17287,46 @@
       <c r="T309" s="139"/>
     </row>
     <row r="310" spans="1:20" ht="18" customHeight="1">
-      <c r="A310" s="138"/>
-      <c r="B310" s="138"/>
-      <c r="C310" s="138"/>
-      <c r="D310" s="138"/>
-      <c r="E310" s="138"/>
-      <c r="F310" s="138"/>
-      <c r="G310" s="138"/>
-      <c r="H310" s="138"/>
-      <c r="I310" s="138"/>
-      <c r="J310" s="138"/>
+      <c r="A310" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B310" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C310" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D310" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E310" s="142" t="s">
+        <v>213</v>
+      </c>
+      <c r="F310" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G310" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H310" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I310" s="138">
+        <v>298</v>
+      </c>
+      <c r="J310" s="138">
+        <v>776353276.35327601</v>
+      </c>
       <c r="K310" s="138"/>
-      <c r="L310" s="138"/>
-      <c r="M310" s="138"/>
-      <c r="N310" s="138"/>
+      <c r="L310" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M310" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N310" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O310" s="138"/>
       <c r="P310" s="138"/>
       <c r="Q310" s="138"/>
@@ -17247,20 +17335,46 @@
       <c r="T310" s="139"/>
     </row>
     <row r="311" spans="1:20" ht="18" customHeight="1">
-      <c r="A311" s="138"/>
-      <c r="B311" s="138"/>
-      <c r="C311" s="138"/>
-      <c r="D311" s="138"/>
-      <c r="E311" s="138"/>
-      <c r="F311" s="138"/>
-      <c r="G311" s="138"/>
-      <c r="H311" s="138"/>
-      <c r="I311" s="138"/>
-      <c r="J311" s="138"/>
+      <c r="A311" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B311" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C311" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D311" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E311" s="142" t="s">
+        <v>214</v>
+      </c>
+      <c r="F311" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G311" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H311" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I311" s="138">
+        <v>298</v>
+      </c>
+      <c r="J311" s="138">
+        <v>732193732.19373202</v>
+      </c>
       <c r="K311" s="138"/>
-      <c r="L311" s="138"/>
-      <c r="M311" s="138"/>
-      <c r="N311" s="138"/>
+      <c r="L311" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M311" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N311" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O311" s="138"/>
       <c r="P311" s="138"/>
       <c r="Q311" s="138"/>
@@ -17269,20 +17383,46 @@
       <c r="T311" s="139"/>
     </row>
     <row r="312" spans="1:20" ht="18" customHeight="1">
-      <c r="A312" s="138"/>
-      <c r="B312" s="138"/>
-      <c r="C312" s="138"/>
-      <c r="D312" s="138"/>
-      <c r="E312" s="138"/>
-      <c r="F312" s="138"/>
-      <c r="G312" s="138"/>
-      <c r="H312" s="138"/>
-      <c r="I312" s="138"/>
-      <c r="J312" s="138"/>
+      <c r="A312" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B312" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C312" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D312" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E312" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F312" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G312" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H312" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I312" s="138">
+        <v>1073</v>
+      </c>
+      <c r="J312" s="138">
+        <v>414529914.52991402</v>
+      </c>
       <c r="K312" s="138"/>
-      <c r="L312" s="138"/>
-      <c r="M312" s="138"/>
-      <c r="N312" s="138"/>
+      <c r="L312" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M312" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N312" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O312" s="138"/>
       <c r="P312" s="138"/>
       <c r="Q312" s="138"/>
@@ -17291,20 +17431,46 @@
       <c r="T312" s="139"/>
     </row>
     <row r="313" spans="1:20" ht="18" customHeight="1">
-      <c r="A313" s="138"/>
-      <c r="B313" s="138"/>
-      <c r="C313" s="138"/>
-      <c r="D313" s="138"/>
-      <c r="E313" s="138"/>
-      <c r="F313" s="138"/>
-      <c r="G313" s="138"/>
-      <c r="H313" s="138"/>
-      <c r="I313" s="138"/>
-      <c r="J313" s="138"/>
+      <c r="A313" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B313" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C313" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D313" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E313" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F313" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G313" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H313" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I313" s="138">
+        <v>1173</v>
+      </c>
+      <c r="J313" s="138">
+        <v>351851851.851852</v>
+      </c>
       <c r="K313" s="138"/>
-      <c r="L313" s="138"/>
-      <c r="M313" s="138"/>
-      <c r="N313" s="138"/>
+      <c r="L313" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M313" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N313" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O313" s="138"/>
       <c r="P313" s="138"/>
       <c r="Q313" s="138"/>
@@ -17313,20 +17479,46 @@
       <c r="T313" s="139"/>
     </row>
     <row r="314" spans="1:20" ht="18" customHeight="1">
-      <c r="A314" s="138"/>
-      <c r="B314" s="138"/>
-      <c r="C314" s="138"/>
-      <c r="D314" s="138"/>
-      <c r="E314" s="138"/>
-      <c r="F314" s="138"/>
-      <c r="G314" s="138"/>
-      <c r="H314" s="138"/>
-      <c r="I314" s="138"/>
-      <c r="J314" s="138"/>
+      <c r="A314" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B314" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C314" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D314" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E314" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F314" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G314" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H314" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I314" s="138">
+        <v>1273</v>
+      </c>
+      <c r="J314" s="138">
+        <v>243589743.58974299</v>
+      </c>
       <c r="K314" s="138"/>
-      <c r="L314" s="138"/>
-      <c r="M314" s="138"/>
-      <c r="N314" s="138"/>
+      <c r="L314" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M314" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N314" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O314" s="138"/>
       <c r="P314" s="138"/>
       <c r="Q314" s="138"/>
@@ -17335,20 +17527,46 @@
       <c r="T314" s="139"/>
     </row>
     <row r="315" spans="1:20" ht="18" customHeight="1">
-      <c r="A315" s="138"/>
-      <c r="B315" s="138"/>
-      <c r="C315" s="138"/>
-      <c r="D315" s="138"/>
-      <c r="E315" s="138"/>
-      <c r="F315" s="138"/>
-      <c r="G315" s="138"/>
-      <c r="H315" s="138"/>
-      <c r="I315" s="138"/>
-      <c r="J315" s="138"/>
+      <c r="A315" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B315" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C315" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D315" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E315" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F315" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G315" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H315" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I315" s="138">
+        <v>1373</v>
+      </c>
+      <c r="J315" s="138">
+        <v>142450142.450142</v>
+      </c>
       <c r="K315" s="138"/>
-      <c r="L315" s="138"/>
-      <c r="M315" s="138"/>
-      <c r="N315" s="138"/>
+      <c r="L315" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M315" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N315" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O315" s="138"/>
       <c r="P315" s="138"/>
       <c r="Q315" s="138"/>
@@ -17357,20 +17575,46 @@
       <c r="T315" s="139"/>
     </row>
     <row r="316" spans="1:20" ht="18" customHeight="1">
-      <c r="A316" s="138"/>
-      <c r="B316" s="138"/>
-      <c r="C316" s="138"/>
-      <c r="D316" s="138"/>
-      <c r="E316" s="138"/>
-      <c r="F316" s="138"/>
-      <c r="G316" s="138"/>
-      <c r="H316" s="138"/>
-      <c r="I316" s="138"/>
-      <c r="J316" s="138"/>
+      <c r="A316" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B316" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C316" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D316" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E316" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F316" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G316" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H316" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I316" s="138">
+        <v>298</v>
+      </c>
+      <c r="J316" s="138">
+        <v>1059829059.8290499</v>
+      </c>
       <c r="K316" s="138"/>
-      <c r="L316" s="138"/>
-      <c r="M316" s="138"/>
-      <c r="N316" s="138"/>
+      <c r="L316" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M316" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N316" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O316" s="138"/>
       <c r="P316" s="138"/>
       <c r="Q316" s="138"/>
@@ -17379,20 +17623,46 @@
       <c r="T316" s="139"/>
     </row>
     <row r="317" spans="1:20" ht="18" customHeight="1">
-      <c r="A317" s="138"/>
-      <c r="B317" s="138"/>
-      <c r="C317" s="138"/>
-      <c r="D317" s="138"/>
-      <c r="E317" s="138"/>
-      <c r="F317" s="138"/>
-      <c r="G317" s="138"/>
-      <c r="H317" s="138"/>
-      <c r="I317" s="138"/>
-      <c r="J317" s="138"/>
+      <c r="A317" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B317" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C317" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D317" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E317" s="142" t="s">
+        <v>213</v>
+      </c>
+      <c r="F317" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G317" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H317" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I317" s="138">
+        <v>298</v>
+      </c>
+      <c r="J317" s="138">
+        <v>913105413.10541296</v>
+      </c>
       <c r="K317" s="138"/>
-      <c r="L317" s="138"/>
-      <c r="M317" s="138"/>
-      <c r="N317" s="138"/>
+      <c r="L317" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M317" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N317" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O317" s="138"/>
       <c r="P317" s="138"/>
       <c r="Q317" s="138"/>
@@ -17401,20 +17671,46 @@
       <c r="T317" s="139"/>
     </row>
     <row r="318" spans="1:20" ht="18" customHeight="1">
-      <c r="A318" s="138"/>
-      <c r="B318" s="138"/>
-      <c r="C318" s="138"/>
-      <c r="D318" s="138"/>
-      <c r="E318" s="138"/>
-      <c r="F318" s="138"/>
-      <c r="G318" s="138"/>
-      <c r="H318" s="138"/>
-      <c r="I318" s="138"/>
-      <c r="J318" s="138"/>
+      <c r="A318" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B318" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C318" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D318" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E318" s="142" t="s">
+        <v>214</v>
+      </c>
+      <c r="F318" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G318" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H318" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I318" s="138">
+        <v>298</v>
+      </c>
+      <c r="J318" s="138">
+        <v>867521367.52136695</v>
+      </c>
       <c r="K318" s="138"/>
-      <c r="L318" s="138"/>
-      <c r="M318" s="138"/>
-      <c r="N318" s="138"/>
+      <c r="L318" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M318" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N318" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O318" s="138"/>
       <c r="P318" s="138"/>
       <c r="Q318" s="138"/>
@@ -17423,20 +17719,46 @@
       <c r="T318" s="139"/>
     </row>
     <row r="319" spans="1:20" ht="18" customHeight="1">
-      <c r="A319" s="138"/>
-      <c r="B319" s="138"/>
-      <c r="C319" s="138"/>
-      <c r="D319" s="138"/>
-      <c r="E319" s="138"/>
-      <c r="F319" s="138"/>
-      <c r="G319" s="138"/>
-      <c r="H319" s="138"/>
-      <c r="I319" s="138"/>
-      <c r="J319" s="138"/>
+      <c r="A319" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B319" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C319" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D319" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E319" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F319" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G319" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H319" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I319" s="138">
+        <v>1073</v>
+      </c>
+      <c r="J319" s="138">
+        <v>538461538.46153796</v>
+      </c>
       <c r="K319" s="138"/>
-      <c r="L319" s="138"/>
-      <c r="M319" s="138"/>
-      <c r="N319" s="138"/>
+      <c r="L319" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M319" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N319" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O319" s="138"/>
       <c r="P319" s="138"/>
       <c r="Q319" s="138"/>
@@ -17445,20 +17767,46 @@
       <c r="T319" s="139"/>
     </row>
     <row r="320" spans="1:20" ht="18" customHeight="1">
-      <c r="A320" s="138"/>
-      <c r="B320" s="138"/>
-      <c r="C320" s="138"/>
-      <c r="D320" s="138"/>
-      <c r="E320" s="138"/>
-      <c r="F320" s="138"/>
-      <c r="G320" s="138"/>
-      <c r="H320" s="138"/>
-      <c r="I320" s="138"/>
-      <c r="J320" s="138"/>
+      <c r="A320" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B320" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C320" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D320" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E320" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F320" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G320" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H320" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I320" s="138">
+        <v>1173</v>
+      </c>
+      <c r="J320" s="138">
+        <v>450142450.14244998</v>
+      </c>
       <c r="K320" s="138"/>
-      <c r="L320" s="138"/>
-      <c r="M320" s="138"/>
-      <c r="N320" s="138"/>
+      <c r="L320" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M320" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N320" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O320" s="138"/>
       <c r="P320" s="138"/>
       <c r="Q320" s="138"/>
@@ -17467,20 +17815,46 @@
       <c r="T320" s="139"/>
     </row>
     <row r="321" spans="1:20" ht="18" customHeight="1">
-      <c r="A321" s="138"/>
-      <c r="B321" s="138"/>
-      <c r="C321" s="138"/>
-      <c r="D321" s="138"/>
-      <c r="E321" s="138"/>
-      <c r="F321" s="138"/>
-      <c r="G321" s="138"/>
-      <c r="H321" s="138"/>
-      <c r="I321" s="138"/>
-      <c r="J321" s="138"/>
+      <c r="A321" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B321" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C321" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D321" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E321" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F321" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G321" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H321" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I321" s="138">
+        <v>1273</v>
+      </c>
+      <c r="J321" s="138">
+        <v>313390313.39031303</v>
+      </c>
       <c r="K321" s="138"/>
-      <c r="L321" s="138"/>
-      <c r="M321" s="138"/>
-      <c r="N321" s="138"/>
+      <c r="L321" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M321" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N321" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O321" s="138"/>
       <c r="P321" s="138"/>
       <c r="Q321" s="138"/>
@@ -17489,20 +17863,46 @@
       <c r="T321" s="139"/>
     </row>
     <row r="322" spans="1:20" ht="18" customHeight="1">
-      <c r="A322" s="138"/>
-      <c r="B322" s="138"/>
-      <c r="C322" s="138"/>
-      <c r="D322" s="138"/>
-      <c r="E322" s="138"/>
-      <c r="F322" s="138"/>
-      <c r="G322" s="138"/>
-      <c r="H322" s="138"/>
-      <c r="I322" s="138"/>
-      <c r="J322" s="138"/>
+      <c r="A322" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B322" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C322" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D322" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E322" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F322" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G322" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H322" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I322" s="138">
+        <v>1373</v>
+      </c>
+      <c r="J322" s="138">
+        <v>249287749.28774899</v>
+      </c>
       <c r="K322" s="138"/>
-      <c r="L322" s="138"/>
-      <c r="M322" s="138"/>
-      <c r="N322" s="138"/>
+      <c r="L322" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M322" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N322" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O322" s="138"/>
       <c r="P322" s="138"/>
       <c r="Q322" s="138"/>
@@ -17511,20 +17911,46 @@
       <c r="T322" s="139"/>
     </row>
     <row r="323" spans="1:20" ht="18" customHeight="1">
-      <c r="A323" s="138"/>
-      <c r="B323" s="138"/>
-      <c r="C323" s="138"/>
-      <c r="D323" s="138"/>
-      <c r="E323" s="138"/>
-      <c r="F323" s="138"/>
-      <c r="G323" s="138"/>
-      <c r="H323" s="138"/>
-      <c r="I323" s="138"/>
-      <c r="J323" s="138"/>
+      <c r="A323" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B323" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C323" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D323" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E323" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F323" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G323" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H323" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I323" s="138">
+        <v>298</v>
+      </c>
+      <c r="J323" s="138">
+        <v>13.988549618320601</v>
+      </c>
       <c r="K323" s="138"/>
-      <c r="L323" s="138"/>
-      <c r="M323" s="138"/>
-      <c r="N323" s="138"/>
+      <c r="L323" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M323" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N323" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O323" s="138"/>
       <c r="P323" s="138"/>
       <c r="Q323" s="138"/>
@@ -17533,20 +17959,46 @@
       <c r="T323" s="139"/>
     </row>
     <row r="324" spans="1:20" ht="18" customHeight="1">
-      <c r="A324" s="138"/>
-      <c r="B324" s="138"/>
-      <c r="C324" s="138"/>
-      <c r="D324" s="138"/>
-      <c r="E324" s="138"/>
-      <c r="F324" s="138"/>
-      <c r="G324" s="138"/>
-      <c r="H324" s="138"/>
-      <c r="I324" s="138"/>
-      <c r="J324" s="138"/>
+      <c r="A324" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B324" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C324" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D324" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E324" s="142" t="s">
+        <v>213</v>
+      </c>
+      <c r="F324" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G324" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H324" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I324" s="138">
+        <v>298</v>
+      </c>
+      <c r="J324" s="138">
+        <v>13.568702290076301</v>
+      </c>
       <c r="K324" s="138"/>
-      <c r="L324" s="138"/>
-      <c r="M324" s="138"/>
-      <c r="N324" s="138"/>
+      <c r="L324" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M324" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N324" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O324" s="138"/>
       <c r="P324" s="138"/>
       <c r="Q324" s="138"/>
@@ -17555,20 +18007,46 @@
       <c r="T324" s="139"/>
     </row>
     <row r="325" spans="1:20" ht="18" customHeight="1">
-      <c r="A325" s="138"/>
-      <c r="B325" s="138"/>
-      <c r="C325" s="138"/>
-      <c r="D325" s="138"/>
-      <c r="E325" s="138"/>
-      <c r="F325" s="138"/>
-      <c r="G325" s="138"/>
-      <c r="H325" s="138"/>
-      <c r="I325" s="138"/>
-      <c r="J325" s="138"/>
+      <c r="A325" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B325" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C325" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D325" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E325" s="142" t="s">
+        <v>214</v>
+      </c>
+      <c r="F325" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G325" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H325" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I325" s="138">
+        <v>298</v>
+      </c>
+      <c r="J325" s="138">
+        <v>15.706106870229</v>
+      </c>
       <c r="K325" s="138"/>
-      <c r="L325" s="138"/>
-      <c r="M325" s="138"/>
-      <c r="N325" s="138"/>
+      <c r="L325" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M325" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N325" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O325" s="138"/>
       <c r="P325" s="138"/>
       <c r="Q325" s="138"/>
@@ -17577,20 +18055,46 @@
       <c r="T325" s="139"/>
     </row>
     <row r="326" spans="1:20" ht="18" customHeight="1">
-      <c r="A326" s="138"/>
-      <c r="B326" s="138"/>
-      <c r="C326" s="138"/>
-      <c r="D326" s="138"/>
-      <c r="E326" s="138"/>
-      <c r="F326" s="138"/>
-      <c r="G326" s="138"/>
-      <c r="H326" s="138"/>
-      <c r="I326" s="138"/>
-      <c r="J326" s="138"/>
+      <c r="A326" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B326" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C326" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D326" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E326" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F326" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G326" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H326" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I326" s="138">
+        <v>1073</v>
+      </c>
+      <c r="J326" s="138">
+        <v>9.2366412213740396</v>
+      </c>
       <c r="K326" s="138"/>
-      <c r="L326" s="138"/>
-      <c r="M326" s="138"/>
-      <c r="N326" s="138"/>
+      <c r="L326" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M326" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N326" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O326" s="138"/>
       <c r="P326" s="138"/>
       <c r="Q326" s="138"/>
@@ -17599,20 +18103,46 @@
       <c r="T326" s="139"/>
     </row>
     <row r="327" spans="1:20" ht="18" customHeight="1">
-      <c r="A327" s="138"/>
-      <c r="B327" s="138"/>
-      <c r="C327" s="138"/>
-      <c r="D327" s="138"/>
-      <c r="E327" s="138"/>
-      <c r="F327" s="138"/>
-      <c r="G327" s="138"/>
-      <c r="H327" s="138"/>
-      <c r="I327" s="138"/>
-      <c r="J327" s="138"/>
+      <c r="A327" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B327" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C327" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D327" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E327" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F327" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G327" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H327" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I327" s="138">
+        <v>1173</v>
+      </c>
+      <c r="J327" s="138">
+        <v>10.7251908396946</v>
+      </c>
       <c r="K327" s="138"/>
-      <c r="L327" s="138"/>
-      <c r="M327" s="138"/>
-      <c r="N327" s="138"/>
+      <c r="L327" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M327" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N327" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O327" s="138"/>
       <c r="P327" s="138"/>
       <c r="Q327" s="138"/>
@@ -17621,20 +18151,46 @@
       <c r="T327" s="139"/>
     </row>
     <row r="328" spans="1:20" ht="18" customHeight="1">
-      <c r="A328" s="138"/>
-      <c r="B328" s="138"/>
-      <c r="C328" s="138"/>
-      <c r="D328" s="138"/>
-      <c r="E328" s="138"/>
-      <c r="F328" s="138"/>
-      <c r="G328" s="138"/>
-      <c r="H328" s="138"/>
-      <c r="I328" s="138"/>
-      <c r="J328" s="138"/>
+      <c r="A328" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B328" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C328" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D328" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E328" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F328" s="142" t="s">
+        <v>215</v>
+      </c>
+      <c r="G328" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H328" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I328" s="138">
+        <v>1273</v>
+      </c>
+      <c r="J328" s="138">
+        <v>20</v>
+      </c>
       <c r="K328" s="138"/>
-      <c r="L328" s="138"/>
-      <c r="M328" s="138"/>
-      <c r="N328" s="138"/>
+      <c r="L328" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M328" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N328" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O328" s="138"/>
       <c r="P328" s="138"/>
       <c r="Q328" s="138"/>
@@ -17643,20 +18199,46 @@
       <c r="T328" s="139"/>
     </row>
     <row r="329" spans="1:20" ht="18" customHeight="1">
-      <c r="A329" s="138"/>
-      <c r="B329" s="138"/>
-      <c r="C329" s="138"/>
-      <c r="D329" s="138"/>
-      <c r="E329" s="138"/>
-      <c r="F329" s="138"/>
-      <c r="G329" s="138"/>
-      <c r="H329" s="138"/>
-      <c r="I329" s="138"/>
-      <c r="J329" s="138"/>
+      <c r="A329" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B329" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C329" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D329" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E329" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F329" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G329" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H329" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I329" s="138">
+        <v>1373</v>
+      </c>
+      <c r="J329" s="138">
+        <v>9.1603053435114408</v>
+      </c>
       <c r="K329" s="138"/>
-      <c r="L329" s="138"/>
-      <c r="M329" s="138"/>
-      <c r="N329" s="138"/>
+      <c r="L329" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M329" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="N329" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O329" s="138"/>
       <c r="P329" s="138"/>
       <c r="Q329" s="138"/>
@@ -17665,64 +18247,140 @@
       <c r="T329" s="139"/>
     </row>
     <row r="330" spans="1:20" ht="18" customHeight="1">
-      <c r="A330" s="138"/>
-      <c r="B330" s="138"/>
-      <c r="C330" s="138"/>
-      <c r="D330" s="138"/>
+      <c r="A330" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B330" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C330" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D330" s="142" t="s">
+        <v>66</v>
+      </c>
       <c r="E330" s="138"/>
-      <c r="F330" s="138"/>
-      <c r="G330" s="138"/>
+      <c r="F330" s="142" t="s">
+        <v>63</v>
+      </c>
+      <c r="G330" s="142" t="s">
+        <v>29</v>
+      </c>
       <c r="H330" s="138"/>
-      <c r="I330" s="138"/>
-      <c r="J330" s="138"/>
-      <c r="K330" s="138"/>
-      <c r="L330" s="138"/>
-      <c r="M330" s="138"/>
-      <c r="N330" s="138"/>
+      <c r="I330" s="138">
+        <v>298</v>
+      </c>
+      <c r="J330" s="64">
+        <f t="shared" ref="J330:J331" si="23">P330*9807000</f>
+        <v>2932293000</v>
+      </c>
+      <c r="L330" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M330" s="142" t="s">
+        <v>218</v>
+      </c>
+      <c r="N330" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O330" s="138"/>
-      <c r="P330" s="138"/>
+      <c r="P330" s="138">
+        <v>299</v>
+      </c>
       <c r="Q330" s="138"/>
       <c r="R330" s="138"/>
       <c r="S330" s="139"/>
       <c r="T330" s="139"/>
     </row>
     <row r="331" spans="1:20" ht="18" customHeight="1">
-      <c r="A331" s="138"/>
-      <c r="B331" s="138"/>
-      <c r="C331" s="138"/>
-      <c r="D331" s="138"/>
-      <c r="E331" s="138"/>
-      <c r="F331" s="138"/>
-      <c r="G331" s="138"/>
+      <c r="A331" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B331" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C331" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D331" s="142" t="s">
+        <v>216</v>
+      </c>
+      <c r="E331" s="142" t="s">
+        <v>217</v>
+      </c>
+      <c r="F331" s="142" t="s">
+        <v>63</v>
+      </c>
+      <c r="G331" s="142" t="s">
+        <v>29</v>
+      </c>
       <c r="H331" s="138"/>
-      <c r="I331" s="138"/>
-      <c r="J331" s="138"/>
-      <c r="K331" s="138"/>
-      <c r="L331" s="138"/>
-      <c r="M331" s="138"/>
-      <c r="N331" s="138"/>
+      <c r="I331" s="138">
+        <v>298</v>
+      </c>
+      <c r="J331" s="64">
+        <f t="shared" si="23"/>
+        <v>3461871000</v>
+      </c>
+      <c r="L331" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M331" s="142" t="s">
+        <v>218</v>
+      </c>
+      <c r="N331" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O331" s="138"/>
-      <c r="P331" s="138"/>
+      <c r="P331" s="138">
+        <v>353</v>
+      </c>
       <c r="Q331" s="138"/>
       <c r="R331" s="138"/>
       <c r="S331" s="139"/>
       <c r="T331" s="139"/>
     </row>
     <row r="332" spans="1:20" ht="18" customHeight="1">
-      <c r="A332" s="138"/>
-      <c r="B332" s="138"/>
-      <c r="C332" s="138"/>
-      <c r="D332" s="138"/>
-      <c r="E332" s="138"/>
-      <c r="F332" s="138"/>
-      <c r="G332" s="138"/>
-      <c r="H332" s="138"/>
-      <c r="I332" s="138"/>
-      <c r="J332" s="138"/>
+      <c r="A332" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B332" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C332" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D332" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E332" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F332" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G332" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H332" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I332" s="138">
+        <v>77</v>
+      </c>
+      <c r="J332" s="144">
+        <v>1407000000</v>
+      </c>
       <c r="K332" s="138"/>
-      <c r="L332" s="138"/>
-      <c r="M332" s="138"/>
-      <c r="N332" s="138"/>
+      <c r="L332" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M332" s="142" t="s">
+        <v>220</v>
+      </c>
+      <c r="N332" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O332" s="138"/>
       <c r="P332" s="138"/>
       <c r="Q332" s="138"/>
@@ -17731,20 +18389,46 @@
       <c r="T332" s="139"/>
     </row>
     <row r="333" spans="1:20" ht="18" customHeight="1">
-      <c r="A333" s="138"/>
-      <c r="B333" s="138"/>
-      <c r="C333" s="138"/>
-      <c r="D333" s="138"/>
-      <c r="E333" s="138"/>
-      <c r="F333" s="138"/>
-      <c r="G333" s="138"/>
-      <c r="H333" s="138"/>
-      <c r="I333" s="138"/>
-      <c r="J333" s="138"/>
+      <c r="A333" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B333" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C333" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D333" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E333" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F333" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G333" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H333" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I333" s="138">
+        <v>77</v>
+      </c>
+      <c r="J333" s="144">
+        <v>1493000000</v>
+      </c>
       <c r="K333" s="138"/>
-      <c r="L333" s="138"/>
-      <c r="M333" s="138"/>
-      <c r="N333" s="138"/>
+      <c r="L333" s="142" t="s">
+        <v>33</v>
+      </c>
+      <c r="M333" s="142" t="s">
+        <v>220</v>
+      </c>
+      <c r="N333" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O333" s="138"/>
       <c r="P333" s="138"/>
       <c r="Q333" s="138"/>
@@ -17753,20 +18437,46 @@
       <c r="T333" s="139"/>
     </row>
     <row r="334" spans="1:20" ht="18" customHeight="1">
-      <c r="A334" s="138"/>
-      <c r="B334" s="138"/>
-      <c r="C334" s="138"/>
-      <c r="D334" s="138"/>
-      <c r="E334" s="138"/>
-      <c r="F334" s="138"/>
-      <c r="G334" s="138"/>
-      <c r="H334" s="138"/>
-      <c r="I334" s="138"/>
-      <c r="J334" s="138"/>
+      <c r="A334" s="142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B334" s="142" t="s">
+        <v>210</v>
+      </c>
+      <c r="C334" s="142" t="s">
+        <v>68</v>
+      </c>
+      <c r="D334" s="142" t="s">
+        <v>88</v>
+      </c>
+      <c r="E334" s="142" t="s">
+        <v>212</v>
+      </c>
+      <c r="F334" s="142" t="s">
+        <v>79</v>
+      </c>
+      <c r="G334" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H334" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="I334" s="138">
+        <v>77</v>
+      </c>
+      <c r="J334" s="138">
+        <v>12.4</v>
+      </c>
       <c r="K334" s="138"/>
-      <c r="L334" s="138"/>
-      <c r="M334" s="138"/>
-      <c r="N334" s="138"/>
+      <c r="L334" s="142" t="s">
+        <v>71</v>
+      </c>
+      <c r="M334" s="142" t="s">
+        <v>220</v>
+      </c>
+      <c r="N334" s="142" t="s">
+        <v>221</v>
+      </c>
       <c r="O334" s="138"/>
       <c r="P334" s="138"/>
       <c r="Q334" s="138"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.intermet.2021.107397`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883D8A11-4528-8C41-B405-9DD8A06F847D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E756088-C5E0-7042-83A1-FA701CBA6E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="5800" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="7300" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3148" uniqueCount="249">
   <si>
     <r>
       <rPr>
@@ -859,6 +859,24 @@
   </si>
   <si>
     <t>Al0.8CrCuFeMn1.5Ni</t>
+  </si>
+  <si>
+    <t>AlCrFeNiTi</t>
+  </si>
+  <si>
+    <t>AlCrFeNiTiCu0.5</t>
+  </si>
+  <si>
+    <t>AlCrFeNiTiCu1</t>
+  </si>
+  <si>
+    <t>AlCrFeNiTiCu1.5</t>
+  </si>
+  <si>
+    <t>AlCrFeNiTiCu2</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2021.107397</t>
   </si>
 </sst>
 </file>
@@ -3207,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A331" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J360" sqref="J360"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A346" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G372" sqref="G372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -19642,7 +19660,7 @@
         <v>5300852586.206893</v>
       </c>
       <c r="K356" s="64">
-        <f t="shared" ref="K356:K357" si="28">(Q356-P356)*9807000</f>
+        <f t="shared" ref="K356:K362" si="28">(Q356-P356)*9807000</f>
         <v>54953017.241378427</v>
       </c>
       <c r="L356" s="105" t="s">
@@ -19690,7 +19708,7 @@
         <v>298</v>
       </c>
       <c r="J357" s="64">
-        <f t="shared" ref="J357" si="29">P357*9807000</f>
+        <f t="shared" ref="J357:J362" si="29">P357*9807000</f>
         <v>4865455603.4482718</v>
       </c>
       <c r="K357" s="64">
@@ -19719,110 +19737,250 @@
     </row>
     <row r="358" spans="1:20" ht="18" customHeight="1">
       <c r="A358" s="101"/>
-      <c r="B358" s="101"/>
-      <c r="C358" s="101"/>
-      <c r="D358" s="101"/>
+      <c r="B358" s="105" t="s">
+        <v>243</v>
+      </c>
+      <c r="C358" s="105" t="s">
+        <v>235</v>
+      </c>
+      <c r="D358" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E358" s="101"/>
-      <c r="F358" s="101"/>
-      <c r="G358" s="101"/>
+      <c r="F358" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G358" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H358" s="101"/>
-      <c r="I358" s="101"/>
-      <c r="J358" s="101"/>
-      <c r="K358" s="101"/>
-      <c r="L358" s="101"/>
-      <c r="M358" s="101"/>
-      <c r="N358" s="101"/>
+      <c r="I358" s="101">
+        <v>298</v>
+      </c>
+      <c r="J358" s="64">
+        <f t="shared" si="29"/>
+        <v>4257718301.8867884</v>
+      </c>
+      <c r="K358" s="64">
+        <f t="shared" si="28"/>
+        <v>130451603.77358647</v>
+      </c>
+      <c r="L358" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M358" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="N358" s="105" t="s">
+        <v>248</v>
+      </c>
       <c r="O358" s="101"/>
-      <c r="P358" s="101"/>
-      <c r="Q358" s="101"/>
+      <c r="P358" s="101">
+        <v>434.15094339622601</v>
+      </c>
+      <c r="Q358" s="101">
+        <v>447.452830188679</v>
+      </c>
       <c r="R358" s="101"/>
       <c r="S358" s="102"/>
       <c r="T358" s="102"/>
     </row>
     <row r="359" spans="1:20" ht="18" customHeight="1">
       <c r="A359" s="101"/>
-      <c r="B359" s="101"/>
-      <c r="C359" s="101"/>
-      <c r="D359" s="101"/>
+      <c r="B359" s="105" t="s">
+        <v>244</v>
+      </c>
+      <c r="C359" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="D359" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E359" s="101"/>
-      <c r="F359" s="101"/>
-      <c r="G359" s="101"/>
+      <c r="F359" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G359" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H359" s="101"/>
-      <c r="I359" s="101"/>
-      <c r="J359" s="101"/>
-      <c r="K359" s="101"/>
-      <c r="L359" s="101"/>
-      <c r="M359" s="101"/>
-      <c r="N359" s="101"/>
+      <c r="I359" s="101">
+        <v>298</v>
+      </c>
+      <c r="J359" s="64">
+        <f t="shared" si="29"/>
+        <v>3755340849.0565963</v>
+      </c>
+      <c r="K359" s="64">
+        <f t="shared" si="28"/>
+        <v>105471509.43396145</v>
+      </c>
+      <c r="L359" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M359" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="N359" s="105" t="s">
+        <v>248</v>
+      </c>
       <c r="O359" s="101"/>
-      <c r="P359" s="101"/>
-      <c r="Q359" s="101"/>
+      <c r="P359" s="101">
+        <v>382.92452830188603</v>
+      </c>
+      <c r="Q359" s="101">
+        <v>393.67924528301802</v>
+      </c>
       <c r="R359" s="101"/>
       <c r="S359" s="102"/>
       <c r="T359" s="102"/>
     </row>
     <row r="360" spans="1:20" ht="18" customHeight="1">
       <c r="A360" s="101"/>
-      <c r="B360" s="101"/>
-      <c r="C360" s="101"/>
-      <c r="D360" s="101"/>
+      <c r="B360" s="105" t="s">
+        <v>245</v>
+      </c>
+      <c r="C360" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="D360" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E360" s="101"/>
-      <c r="F360" s="101"/>
-      <c r="G360" s="101"/>
+      <c r="F360" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G360" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H360" s="101"/>
-      <c r="I360" s="101"/>
-      <c r="J360" s="101"/>
-      <c r="K360" s="101"/>
-      <c r="L360" s="101"/>
-      <c r="M360" s="101"/>
-      <c r="N360" s="101"/>
+      <c r="I360" s="101">
+        <v>298</v>
+      </c>
+      <c r="J360" s="64">
+        <f t="shared" si="29"/>
+        <v>3469457547.1698079</v>
+      </c>
+      <c r="K360" s="64">
+        <f t="shared" si="28"/>
+        <v>113798207.54717295</v>
+      </c>
+      <c r="L360" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M360" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="N360" s="105" t="s">
+        <v>248</v>
+      </c>
       <c r="O360" s="101"/>
-      <c r="P360" s="101"/>
-      <c r="Q360" s="101"/>
+      <c r="P360" s="101">
+        <v>353.77358490566002</v>
+      </c>
+      <c r="Q360" s="101">
+        <v>365.377358490566</v>
+      </c>
       <c r="R360" s="101"/>
       <c r="S360" s="102"/>
       <c r="T360" s="102"/>
     </row>
     <row r="361" spans="1:20" ht="18" customHeight="1">
       <c r="A361" s="101"/>
-      <c r="B361" s="101"/>
-      <c r="C361" s="101"/>
-      <c r="D361" s="101"/>
+      <c r="B361" s="105" t="s">
+        <v>246</v>
+      </c>
+      <c r="C361" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="D361" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E361" s="101"/>
-      <c r="F361" s="101"/>
-      <c r="G361" s="101"/>
+      <c r="F361" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G361" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H361" s="101"/>
-      <c r="I361" s="101"/>
-      <c r="J361" s="101"/>
-      <c r="K361" s="101"/>
-      <c r="L361" s="101"/>
-      <c r="M361" s="101"/>
-      <c r="N361" s="101"/>
+      <c r="I361" s="101">
+        <v>298</v>
+      </c>
+      <c r="J361" s="64">
+        <f t="shared" si="29"/>
+        <v>3069776037.7358465</v>
+      </c>
+      <c r="K361" s="64">
+        <f t="shared" si="28"/>
+        <v>86042547.169807225</v>
+      </c>
+      <c r="L361" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M361" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="N361" s="105" t="s">
+        <v>248</v>
+      </c>
       <c r="O361" s="101"/>
-      <c r="P361" s="101"/>
-      <c r="Q361" s="101"/>
+      <c r="P361" s="101">
+        <v>313.01886792452802</v>
+      </c>
+      <c r="Q361" s="101">
+        <v>321.79245283018798</v>
+      </c>
       <c r="R361" s="101"/>
       <c r="S361" s="102"/>
       <c r="T361" s="102"/>
     </row>
     <row r="362" spans="1:20" ht="18" customHeight="1">
       <c r="A362" s="101"/>
-      <c r="B362" s="101"/>
-      <c r="C362" s="101"/>
-      <c r="D362" s="101"/>
+      <c r="B362" s="105" t="s">
+        <v>247</v>
+      </c>
+      <c r="C362" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="D362" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E362" s="101"/>
-      <c r="F362" s="101"/>
-      <c r="G362" s="101"/>
+      <c r="F362" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G362" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H362" s="101"/>
-      <c r="I362" s="101"/>
-      <c r="J362" s="101"/>
-      <c r="K362" s="101"/>
-      <c r="L362" s="101"/>
-      <c r="M362" s="101"/>
-      <c r="N362" s="101"/>
+      <c r="I362" s="101">
+        <v>298</v>
+      </c>
+      <c r="J362" s="64">
+        <f t="shared" si="29"/>
+        <v>2747810377.3584905</v>
+      </c>
+      <c r="K362" s="64">
+        <f t="shared" si="28"/>
+        <v>108247075.4716921</v>
+      </c>
+      <c r="L362" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M362" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="N362" s="105" t="s">
+        <v>248</v>
+      </c>
       <c r="O362" s="101"/>
-      <c r="P362" s="101"/>
-      <c r="Q362" s="101"/>
+      <c r="P362" s="101">
+        <v>280.18867924528303</v>
+      </c>
+      <c r="Q362" s="101">
+        <v>291.22641509433902</v>
+      </c>
       <c r="R362" s="101"/>
       <c r="S362" s="102"/>
       <c r="T362" s="102"/>
@@ -19904,7 +20062,7 @@
       <c r="H366" s="101"/>
       <c r="I366" s="101"/>
       <c r="J366" s="101"/>
-      <c r="K366" s="101"/>
+      <c r="K366" s="105"/>
       <c r="L366" s="101"/>
       <c r="M366" s="101"/>
       <c r="N366" s="101"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1016/j.intermet.2016.12.015`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E756088-C5E0-7042-83A1-FA701CBA6E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A75E514-6A9A-174A-B1BB-97328C4D0D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="7300" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3148" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3160" uniqueCount="253">
   <si>
     <r>
       <rPr>
@@ -877,6 +877,18 @@
   </si>
   <si>
     <t>10.1016/j.intermet.2021.107397</t>
+  </si>
+  <si>
+    <t>AlCoCrFeNi</t>
+  </si>
+  <si>
+    <t>AlCoCrCu0.5FeNi</t>
+  </si>
+  <si>
+    <t>BCC+FCC</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2016.12.015</t>
   </si>
 </sst>
 </file>
@@ -3225,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A346" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G372" sqref="G372"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A349" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N369" sqref="N369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -19987,9 +19999,15 @@
     </row>
     <row r="363" spans="1:20" ht="18" customHeight="1">
       <c r="A363" s="101"/>
-      <c r="B363" s="101"/>
-      <c r="C363" s="101"/>
-      <c r="D363" s="101"/>
+      <c r="B363" s="105" t="s">
+        <v>249</v>
+      </c>
+      <c r="C363" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="D363" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E363" s="101"/>
       <c r="F363" s="101"/>
       <c r="G363" s="101"/>
@@ -19999,7 +20017,9 @@
       <c r="K363" s="101"/>
       <c r="L363" s="101"/>
       <c r="M363" s="101"/>
-      <c r="N363" s="101"/>
+      <c r="N363" s="105" t="s">
+        <v>252</v>
+      </c>
       <c r="O363" s="101"/>
       <c r="P363" s="101"/>
       <c r="Q363" s="101"/>
@@ -20009,9 +20029,15 @@
     </row>
     <row r="364" spans="1:20" ht="18" customHeight="1">
       <c r="A364" s="101"/>
-      <c r="B364" s="101"/>
-      <c r="C364" s="101"/>
-      <c r="D364" s="101"/>
+      <c r="B364" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="C364" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="D364" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E364" s="101"/>
       <c r="F364" s="101"/>
       <c r="G364" s="101"/>
@@ -20021,7 +20047,9 @@
       <c r="K364" s="101"/>
       <c r="L364" s="101"/>
       <c r="M364" s="101"/>
-      <c r="N364" s="101"/>
+      <c r="N364" s="105" t="s">
+        <v>252</v>
+      </c>
       <c r="O364" s="101"/>
       <c r="P364" s="101"/>
       <c r="Q364" s="101"/>
@@ -20031,9 +20059,15 @@
     </row>
     <row r="365" spans="1:20" ht="18" customHeight="1">
       <c r="A365" s="101"/>
-      <c r="B365" s="101"/>
-      <c r="C365" s="101"/>
-      <c r="D365" s="101"/>
+      <c r="B365" s="105" t="s">
+        <v>232</v>
+      </c>
+      <c r="C365" s="105" t="s">
+        <v>251</v>
+      </c>
+      <c r="D365" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E365" s="101"/>
       <c r="F365" s="101"/>
       <c r="G365" s="101"/>
@@ -20043,7 +20077,9 @@
       <c r="K365" s="101"/>
       <c r="L365" s="101"/>
       <c r="M365" s="101"/>
-      <c r="N365" s="101"/>
+      <c r="N365" s="105" t="s">
+        <v>252</v>
+      </c>
       <c r="O365" s="101"/>
       <c r="P365" s="101"/>
       <c r="Q365" s="101"/>

</xml_diff>

<commit_message>
- extracted structural data from `10.1134/S1029959921060035`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A75E514-6A9A-174A-B1BB-97328C4D0D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3A4E39-12AE-4548-9BB1-9AE788D87F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="7300" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3160" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3175" uniqueCount="260">
   <si>
     <r>
       <rPr>
@@ -889,6 +889,27 @@
   </si>
   <si>
     <t>10.1016/j.intermet.2016.12.015</t>
+  </si>
+  <si>
+    <t>Al0.25CoCrFeNiCu</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNi1.6Ti0.7</t>
+  </si>
+  <si>
+    <t>Al0.25CoCrFeNiV</t>
+  </si>
+  <si>
+    <t>metal granules and powders by molten in alumina crucibles with graphite lids in induction furnace in a reducing atmosphere at up to 1873K</t>
+  </si>
+  <si>
+    <t>BCC is mostly V; metal granules and powders by molten in alumina crucibles with graphite lids in induction furnace in a reducing atmosphere at up to 1873K</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>10.1134/S1029959921060035</t>
   </si>
 </sst>
 </file>
@@ -3238,7 +3259,7 @@
   <dimension ref="A1:T926"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A349" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N369" sqref="N369"/>
+      <selection activeCell="H372" sqref="H372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -19414,7 +19435,7 @@
         <v>298</v>
       </c>
       <c r="J351" s="64">
-        <f t="shared" ref="J351:J354" si="26">P351*9807000</f>
+        <f t="shared" ref="J351" si="26">P351*9807000</f>
         <v>1409161165.0485384</v>
       </c>
       <c r="K351" s="64">
@@ -20089,10 +20110,18 @@
     </row>
     <row r="366" spans="1:20" ht="18" customHeight="1">
       <c r="A366" s="101"/>
-      <c r="B366" s="101"/>
-      <c r="C366" s="101"/>
-      <c r="D366" s="101"/>
-      <c r="E366" s="101"/>
+      <c r="B366" s="105" t="s">
+        <v>253</v>
+      </c>
+      <c r="C366" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D366" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E366" s="105" t="s">
+        <v>256</v>
+      </c>
       <c r="F366" s="101"/>
       <c r="G366" s="101"/>
       <c r="H366" s="101"/>
@@ -20101,7 +20130,9 @@
       <c r="K366" s="105"/>
       <c r="L366" s="101"/>
       <c r="M366" s="101"/>
-      <c r="N366" s="101"/>
+      <c r="N366" s="105" t="s">
+        <v>259</v>
+      </c>
       <c r="O366" s="101"/>
       <c r="P366" s="101"/>
       <c r="Q366" s="101"/>
@@ -20111,10 +20142,18 @@
     </row>
     <row r="367" spans="1:20" ht="18" customHeight="1">
       <c r="A367" s="101"/>
-      <c r="B367" s="101"/>
-      <c r="C367" s="101"/>
-      <c r="D367" s="101"/>
-      <c r="E367" s="101"/>
+      <c r="B367" s="105" t="s">
+        <v>254</v>
+      </c>
+      <c r="C367" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D367" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E367" s="105" t="s">
+        <v>256</v>
+      </c>
       <c r="F367" s="101"/>
       <c r="G367" s="101"/>
       <c r="H367" s="101"/>
@@ -20123,7 +20162,9 @@
       <c r="K367" s="101"/>
       <c r="L367" s="101"/>
       <c r="M367" s="101"/>
-      <c r="N367" s="101"/>
+      <c r="N367" s="105" t="s">
+        <v>259</v>
+      </c>
       <c r="O367" s="101"/>
       <c r="P367" s="101"/>
       <c r="Q367" s="101"/>
@@ -20133,10 +20174,18 @@
     </row>
     <row r="368" spans="1:20" ht="18" customHeight="1">
       <c r="A368" s="101"/>
-      <c r="B368" s="101"/>
-      <c r="C368" s="101"/>
-      <c r="D368" s="101"/>
-      <c r="E368" s="101"/>
+      <c r="B368" s="105" t="s">
+        <v>255</v>
+      </c>
+      <c r="C368" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D368" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E368" s="105" t="s">
+        <v>257</v>
+      </c>
       <c r="F368" s="101"/>
       <c r="G368" s="101"/>
       <c r="H368" s="101"/>
@@ -20145,7 +20194,9 @@
       <c r="K368" s="101"/>
       <c r="L368" s="101"/>
       <c r="M368" s="101"/>
-      <c r="N368" s="101"/>
+      <c r="N368" s="105" t="s">
+        <v>259</v>
+      </c>
       <c r="O368" s="101"/>
       <c r="P368" s="101"/>
       <c r="Q368" s="101"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s43452-024-01102-5`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3A4E39-12AE-4548-9BB1-9AE788D87F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB76766-1151-AA44-87E1-B110EE127E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="7300" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="8500" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3175" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3256" uniqueCount="271">
   <si>
     <r>
       <rPr>
@@ -910,6 +910,39 @@
   </si>
   <si>
     <t>10.1134/S1029959921060035</t>
+  </si>
+  <si>
+    <t>AlCoCrFeNiSi0.5Cu0.01</t>
+  </si>
+  <si>
+    <t>AlCoCrFeNiSi0.5Cu0.05</t>
+  </si>
+  <si>
+    <t>AlCoCrFeNiSi0.5Cu0.1</t>
+  </si>
+  <si>
+    <t>IM in Ar</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>saturation magnetization</t>
+  </si>
+  <si>
+    <t>Am^2/kg</t>
+  </si>
+  <si>
+    <t>coercivity</t>
+  </si>
+  <si>
+    <t>A/m</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>10.1007/s43452-024-01102-5</t>
   </si>
 </sst>
 </file>
@@ -3258,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A349" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H372" sqref="H372"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B360" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N380" sqref="N380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -20206,19 +20239,41 @@
     </row>
     <row r="369" spans="1:20" ht="18" customHeight="1">
       <c r="A369" s="101"/>
-      <c r="B369" s="101"/>
-      <c r="C369" s="101"/>
-      <c r="D369" s="101"/>
-      <c r="E369" s="101"/>
-      <c r="F369" s="101"/>
-      <c r="G369" s="101"/>
+      <c r="B369" s="105" t="s">
+        <v>260</v>
+      </c>
+      <c r="C369" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D369" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E369" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F369" s="105" t="s">
+        <v>265</v>
+      </c>
+      <c r="G369" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H369" s="101"/>
-      <c r="I369" s="101"/>
-      <c r="J369" s="101"/>
+      <c r="I369" s="101">
+        <v>298</v>
+      </c>
+      <c r="J369" s="101">
+        <v>39.299999999999997</v>
+      </c>
       <c r="K369" s="101"/>
-      <c r="L369" s="101"/>
-      <c r="M369" s="101"/>
-      <c r="N369" s="101"/>
+      <c r="L369" s="105" t="s">
+        <v>266</v>
+      </c>
+      <c r="M369" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="N369" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O369" s="101"/>
       <c r="P369" s="101"/>
       <c r="Q369" s="101"/>
@@ -20228,19 +20283,41 @@
     </row>
     <row r="370" spans="1:20" ht="18" customHeight="1">
       <c r="A370" s="101"/>
-      <c r="B370" s="101"/>
-      <c r="C370" s="101"/>
-      <c r="D370" s="101"/>
-      <c r="E370" s="101"/>
-      <c r="F370" s="101"/>
-      <c r="G370" s="101"/>
+      <c r="B370" s="105" t="s">
+        <v>261</v>
+      </c>
+      <c r="C370" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D370" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E370" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F370" s="105" t="s">
+        <v>265</v>
+      </c>
+      <c r="G370" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H370" s="101"/>
-      <c r="I370" s="101"/>
-      <c r="J370" s="101"/>
+      <c r="I370" s="101">
+        <v>298</v>
+      </c>
+      <c r="J370" s="101">
+        <v>38.9</v>
+      </c>
       <c r="K370" s="101"/>
-      <c r="L370" s="101"/>
-      <c r="M370" s="101"/>
-      <c r="N370" s="101"/>
+      <c r="L370" s="105" t="s">
+        <v>266</v>
+      </c>
+      <c r="M370" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="N370" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O370" s="101"/>
       <c r="P370" s="101"/>
       <c r="Q370" s="101"/>
@@ -20250,19 +20327,41 @@
     </row>
     <row r="371" spans="1:20" ht="18" customHeight="1">
       <c r="A371" s="101"/>
-      <c r="B371" s="101"/>
-      <c r="C371" s="101"/>
-      <c r="D371" s="101"/>
-      <c r="E371" s="101"/>
-      <c r="F371" s="101"/>
-      <c r="G371" s="101"/>
+      <c r="B371" s="105" t="s">
+        <v>262</v>
+      </c>
+      <c r="C371" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D371" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E371" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F371" s="105" t="s">
+        <v>265</v>
+      </c>
+      <c r="G371" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H371" s="101"/>
-      <c r="I371" s="101"/>
-      <c r="J371" s="101"/>
+      <c r="I371" s="101">
+        <v>298</v>
+      </c>
+      <c r="J371" s="101">
+        <v>35.299999999999997</v>
+      </c>
       <c r="K371" s="101"/>
-      <c r="L371" s="101"/>
-      <c r="M371" s="101"/>
-      <c r="N371" s="101"/>
+      <c r="L371" s="105" t="s">
+        <v>266</v>
+      </c>
+      <c r="M371" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="N371" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O371" s="101"/>
       <c r="P371" s="101"/>
       <c r="Q371" s="101"/>
@@ -20272,21 +20371,46 @@
     </row>
     <row r="372" spans="1:20" ht="18" customHeight="1">
       <c r="A372" s="101"/>
-      <c r="B372" s="101"/>
-      <c r="C372" s="101"/>
-      <c r="D372" s="101"/>
-      <c r="E372" s="101"/>
-      <c r="F372" s="101"/>
-      <c r="G372" s="101"/>
+      <c r="B372" s="105" t="s">
+        <v>260</v>
+      </c>
+      <c r="C372" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D372" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E372" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F372" s="105" t="s">
+        <v>267</v>
+      </c>
+      <c r="G372" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H372" s="101"/>
-      <c r="I372" s="101"/>
-      <c r="J372" s="101"/>
+      <c r="I372" s="101">
+        <v>298</v>
+      </c>
+      <c r="J372" s="101">
+        <f>P372*79.57747</f>
+        <v>6238.8736480000007</v>
+      </c>
       <c r="K372" s="101"/>
-      <c r="L372" s="101"/>
-      <c r="M372" s="101"/>
-      <c r="N372" s="101"/>
+      <c r="L372" s="105" t="s">
+        <v>268</v>
+      </c>
+      <c r="M372" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="N372" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O372" s="101"/>
-      <c r="P372" s="101"/>
+      <c r="P372" s="101">
+        <v>78.400000000000006</v>
+      </c>
       <c r="Q372" s="101"/>
       <c r="R372" s="101"/>
       <c r="S372" s="102"/>
@@ -20294,21 +20418,46 @@
     </row>
     <row r="373" spans="1:20" ht="18" customHeight="1">
       <c r="A373" s="101"/>
-      <c r="B373" s="101"/>
-      <c r="C373" s="101"/>
-      <c r="D373" s="101"/>
-      <c r="E373" s="101"/>
-      <c r="F373" s="101"/>
-      <c r="G373" s="101"/>
+      <c r="B373" s="105" t="s">
+        <v>261</v>
+      </c>
+      <c r="C373" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D373" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E373" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F373" s="105" t="s">
+        <v>267</v>
+      </c>
+      <c r="G373" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H373" s="101"/>
-      <c r="I373" s="101"/>
-      <c r="J373" s="101"/>
+      <c r="I373" s="101">
+        <v>298</v>
+      </c>
+      <c r="J373" s="101">
+        <f t="shared" ref="J373:J374" si="30">P373*79.57747</f>
+        <v>5944.4370090000002</v>
+      </c>
       <c r="K373" s="101"/>
-      <c r="L373" s="101"/>
-      <c r="M373" s="101"/>
-      <c r="N373" s="101"/>
+      <c r="L373" s="105" t="s">
+        <v>268</v>
+      </c>
+      <c r="M373" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="N373" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O373" s="101"/>
-      <c r="P373" s="101"/>
+      <c r="P373" s="101">
+        <v>74.7</v>
+      </c>
       <c r="Q373" s="101"/>
       <c r="R373" s="101"/>
       <c r="S373" s="102"/>
@@ -20316,21 +20465,46 @@
     </row>
     <row r="374" spans="1:20" ht="18" customHeight="1">
       <c r="A374" s="101"/>
-      <c r="B374" s="101"/>
-      <c r="C374" s="101"/>
-      <c r="D374" s="101"/>
-      <c r="E374" s="101"/>
-      <c r="F374" s="101"/>
-      <c r="G374" s="101"/>
+      <c r="B374" s="105" t="s">
+        <v>262</v>
+      </c>
+      <c r="C374" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D374" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E374" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F374" s="105" t="s">
+        <v>267</v>
+      </c>
+      <c r="G374" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H374" s="101"/>
-      <c r="I374" s="101"/>
-      <c r="J374" s="101"/>
+      <c r="I374" s="101">
+        <v>298</v>
+      </c>
+      <c r="J374" s="101">
+        <f t="shared" si="30"/>
+        <v>5172.5355500000005</v>
+      </c>
       <c r="K374" s="101"/>
-      <c r="L374" s="101"/>
-      <c r="M374" s="101"/>
-      <c r="N374" s="101"/>
+      <c r="L374" s="105" t="s">
+        <v>268</v>
+      </c>
+      <c r="M374" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="N374" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O374" s="101"/>
-      <c r="P374" s="101"/>
+      <c r="P374" s="101">
+        <v>65</v>
+      </c>
       <c r="Q374" s="101"/>
       <c r="R374" s="101"/>
       <c r="S374" s="102"/>
@@ -20338,66 +20512,156 @@
     </row>
     <row r="375" spans="1:20" ht="18" customHeight="1">
       <c r="A375" s="101"/>
-      <c r="B375" s="101"/>
-      <c r="C375" s="101"/>
-      <c r="D375" s="101"/>
-      <c r="E375" s="101"/>
-      <c r="F375" s="101"/>
-      <c r="G375" s="101"/>
+      <c r="B375" s="105" t="s">
+        <v>260</v>
+      </c>
+      <c r="C375" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D375" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E375" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F375" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G375" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H375" s="101"/>
-      <c r="I375" s="101"/>
-      <c r="J375" s="101"/>
-      <c r="K375" s="101"/>
-      <c r="L375" s="101"/>
-      <c r="M375" s="101"/>
-      <c r="N375" s="101"/>
+      <c r="I375" s="101">
+        <v>298</v>
+      </c>
+      <c r="J375" s="64">
+        <f t="shared" ref="J375:J377" si="31">P375*9807000</f>
+        <v>6961921122.9946499</v>
+      </c>
+      <c r="K375" s="64">
+        <f t="shared" ref="K375:K377" si="32">(Q375-P375)*9807000</f>
+        <v>432661764.70587683</v>
+      </c>
+      <c r="L375" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M375" s="105" t="s">
+        <v>269</v>
+      </c>
+      <c r="N375" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O375" s="101"/>
-      <c r="P375" s="101"/>
-      <c r="Q375" s="101"/>
+      <c r="P375" s="101">
+        <v>709.893048128342</v>
+      </c>
+      <c r="Q375" s="101">
+        <v>754.01069518716497</v>
+      </c>
       <c r="R375" s="101"/>
       <c r="S375" s="102"/>
       <c r="T375" s="102"/>
     </row>
     <row r="376" spans="1:20" ht="18" customHeight="1">
       <c r="A376" s="101"/>
-      <c r="B376" s="101"/>
-      <c r="C376" s="101"/>
-      <c r="D376" s="101"/>
-      <c r="E376" s="101"/>
-      <c r="F376" s="101"/>
-      <c r="G376" s="101"/>
+      <c r="B376" s="105" t="s">
+        <v>261</v>
+      </c>
+      <c r="C376" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D376" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E376" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F376" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G376" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H376" s="101"/>
-      <c r="I376" s="101"/>
-      <c r="J376" s="101"/>
-      <c r="K376" s="101"/>
-      <c r="L376" s="101"/>
-      <c r="M376" s="101"/>
-      <c r="N376" s="101"/>
+      <c r="I376" s="101">
+        <v>298</v>
+      </c>
+      <c r="J376" s="64">
+        <f t="shared" si="31"/>
+        <v>6975032085.5614948</v>
+      </c>
+      <c r="K376" s="64">
+        <f t="shared" si="32"/>
+        <v>471994652.40641487</v>
+      </c>
+      <c r="L376" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M376" s="105" t="s">
+        <v>269</v>
+      </c>
+      <c r="N376" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O376" s="101"/>
-      <c r="P376" s="101"/>
-      <c r="Q376" s="101"/>
+      <c r="P376" s="101">
+        <v>711.22994652406396</v>
+      </c>
+      <c r="Q376" s="101">
+        <v>759.35828877005304</v>
+      </c>
       <c r="R376" s="101"/>
       <c r="S376" s="102"/>
       <c r="T376" s="102"/>
     </row>
     <row r="377" spans="1:20" ht="18" customHeight="1">
       <c r="A377" s="101"/>
-      <c r="B377" s="101"/>
-      <c r="C377" s="101"/>
-      <c r="D377" s="101"/>
-      <c r="E377" s="101"/>
-      <c r="F377" s="101"/>
-      <c r="G377" s="101"/>
+      <c r="B377" s="105" t="s">
+        <v>262</v>
+      </c>
+      <c r="C377" s="105" t="s">
+        <v>264</v>
+      </c>
+      <c r="D377" s="105" t="s">
+        <v>258</v>
+      </c>
+      <c r="E377" s="105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F377" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G377" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H377" s="101"/>
-      <c r="I377" s="101"/>
-      <c r="J377" s="101"/>
-      <c r="K377" s="101"/>
-      <c r="L377" s="101"/>
-      <c r="M377" s="101"/>
-      <c r="N377" s="101"/>
+      <c r="I377" s="101">
+        <v>298</v>
+      </c>
+      <c r="J377" s="64">
+        <f t="shared" si="31"/>
+        <v>7053697860.9625597</v>
+      </c>
+      <c r="K377" s="64">
+        <f t="shared" si="32"/>
+        <v>747324866.31016302</v>
+      </c>
+      <c r="L377" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M377" s="105" t="s">
+        <v>269</v>
+      </c>
+      <c r="N377" s="105" t="s">
+        <v>270</v>
+      </c>
       <c r="O377" s="101"/>
-      <c r="P377" s="101"/>
-      <c r="Q377" s="101"/>
+      <c r="P377" s="101">
+        <v>719.25133689839504</v>
+      </c>
+      <c r="Q377" s="101">
+        <v>795.45454545454504</v>
+      </c>
       <c r="R377" s="101"/>
       <c r="S377" s="102"/>
       <c r="T377" s="102"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.matchemphys.2017.08.011`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB76766-1151-AA44-87E1-B110EE127E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348B9FF2-05B4-5548-B15B-48DB23951436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="8500" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3256" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="279">
   <si>
     <r>
       <rPr>
@@ -943,6 +943,30 @@
   </si>
   <si>
     <t>10.1007/s43452-024-01102-5</t>
+  </si>
+  <si>
+    <t>CoCrFeNiMn</t>
+  </si>
+  <si>
+    <t>CoCrFeNiMnC0.05</t>
+  </si>
+  <si>
+    <t>CoCrFeNiMnC0.1</t>
+  </si>
+  <si>
+    <t>CoCrFeNiMnC0.15</t>
+  </si>
+  <si>
+    <t>CoCrFeNiMnC0.2</t>
+  </si>
+  <si>
+    <t>FCC+carbide</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchemphys.2017.08.011</t>
   </si>
 </sst>
 </file>
@@ -3291,8 +3315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B360" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N380" sqref="N380"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A370" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N398" sqref="N398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -20668,19 +20692,39 @@
     </row>
     <row r="378" spans="1:20" ht="18" customHeight="1">
       <c r="A378" s="101"/>
-      <c r="B378" s="101"/>
-      <c r="C378" s="101"/>
-      <c r="D378" s="101"/>
+      <c r="B378" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="C378" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D378" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E378" s="101"/>
-      <c r="F378" s="101"/>
-      <c r="G378" s="101"/>
+      <c r="F378" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G378" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H378" s="101"/>
-      <c r="I378" s="101"/>
-      <c r="J378" s="101"/>
+      <c r="I378" s="101">
+        <v>298</v>
+      </c>
+      <c r="J378" s="101">
+        <v>487261146.49681503</v>
+      </c>
       <c r="K378" s="101"/>
-      <c r="L378" s="101"/>
-      <c r="M378" s="101"/>
-      <c r="N378" s="101"/>
+      <c r="L378" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M378" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N378" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O378" s="101"/>
       <c r="P378" s="101"/>
       <c r="Q378" s="101"/>
@@ -20690,19 +20734,39 @@
     </row>
     <row r="379" spans="1:20" ht="18" customHeight="1">
       <c r="A379" s="101"/>
-      <c r="B379" s="101"/>
-      <c r="C379" s="101"/>
-      <c r="D379" s="101"/>
+      <c r="B379" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="C379" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D379" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E379" s="101"/>
-      <c r="F379" s="101"/>
-      <c r="G379" s="101"/>
+      <c r="F379" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G379" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H379" s="101"/>
-      <c r="I379" s="101"/>
-      <c r="J379" s="101"/>
+      <c r="I379" s="101">
+        <v>298</v>
+      </c>
+      <c r="J379" s="101">
+        <v>573885350.31847095</v>
+      </c>
       <c r="K379" s="101"/>
-      <c r="L379" s="101"/>
-      <c r="M379" s="101"/>
-      <c r="N379" s="101"/>
+      <c r="L379" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M379" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N379" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O379" s="101"/>
       <c r="P379" s="101"/>
       <c r="Q379" s="101"/>
@@ -20712,19 +20776,39 @@
     </row>
     <row r="380" spans="1:20" ht="18" customHeight="1">
       <c r="A380" s="101"/>
-      <c r="B380" s="101"/>
-      <c r="C380" s="101"/>
-      <c r="D380" s="101"/>
+      <c r="B380" s="105" t="s">
+        <v>273</v>
+      </c>
+      <c r="C380" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D380" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E380" s="101"/>
-      <c r="F380" s="101"/>
-      <c r="G380" s="101"/>
+      <c r="F380" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G380" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H380" s="101"/>
-      <c r="I380" s="101"/>
-      <c r="J380" s="101"/>
+      <c r="I380" s="101">
+        <v>298</v>
+      </c>
+      <c r="J380" s="101">
+        <v>664331210.191082</v>
+      </c>
       <c r="K380" s="101"/>
-      <c r="L380" s="101"/>
-      <c r="M380" s="101"/>
-      <c r="N380" s="101"/>
+      <c r="L380" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M380" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N380" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O380" s="101"/>
       <c r="P380" s="101"/>
       <c r="Q380" s="101"/>
@@ -20734,19 +20818,39 @@
     </row>
     <row r="381" spans="1:20" ht="18" customHeight="1">
       <c r="A381" s="101"/>
-      <c r="B381" s="101"/>
-      <c r="C381" s="101"/>
-      <c r="D381" s="101"/>
+      <c r="B381" s="105" t="s">
+        <v>274</v>
+      </c>
+      <c r="C381" s="105" t="s">
+        <v>276</v>
+      </c>
+      <c r="D381" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E381" s="101"/>
-      <c r="F381" s="101"/>
-      <c r="G381" s="101"/>
+      <c r="F381" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G381" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H381" s="101"/>
-      <c r="I381" s="101"/>
-      <c r="J381" s="101"/>
+      <c r="I381" s="101">
+        <v>298</v>
+      </c>
+      <c r="J381" s="101">
+        <v>621019108.28025401</v>
+      </c>
       <c r="K381" s="101"/>
-      <c r="L381" s="101"/>
-      <c r="M381" s="101"/>
-      <c r="N381" s="101"/>
+      <c r="L381" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M381" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N381" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O381" s="101"/>
       <c r="P381" s="101"/>
       <c r="Q381" s="101"/>
@@ -20756,19 +20860,39 @@
     </row>
     <row r="382" spans="1:20" ht="18" customHeight="1">
       <c r="A382" s="101"/>
-      <c r="B382" s="101"/>
-      <c r="C382" s="101"/>
-      <c r="D382" s="101"/>
+      <c r="B382" s="105" t="s">
+        <v>275</v>
+      </c>
+      <c r="C382" s="105" t="s">
+        <v>276</v>
+      </c>
+      <c r="D382" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E382" s="101"/>
-      <c r="F382" s="101"/>
-      <c r="G382" s="101"/>
+      <c r="F382" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G382" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H382" s="101"/>
-      <c r="I382" s="101"/>
-      <c r="J382" s="101"/>
+      <c r="I382" s="101">
+        <v>298</v>
+      </c>
+      <c r="J382" s="101">
+        <v>733121019.10827994</v>
+      </c>
       <c r="K382" s="101"/>
-      <c r="L382" s="101"/>
-      <c r="M382" s="101"/>
-      <c r="N382" s="101"/>
+      <c r="L382" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M382" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N382" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O382" s="101"/>
       <c r="P382" s="101"/>
       <c r="Q382" s="101"/>
@@ -20778,19 +20902,39 @@
     </row>
     <row r="383" spans="1:20" ht="18" customHeight="1">
       <c r="A383" s="101"/>
-      <c r="B383" s="101"/>
-      <c r="C383" s="101"/>
-      <c r="D383" s="101"/>
+      <c r="B383" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="C383" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D383" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E383" s="101"/>
-      <c r="F383" s="101"/>
-      <c r="G383" s="101"/>
+      <c r="F383" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="G383" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H383" s="101"/>
-      <c r="I383" s="101"/>
-      <c r="J383" s="101"/>
+      <c r="I383" s="101">
+        <v>298</v>
+      </c>
+      <c r="J383" s="101">
+        <v>277500000</v>
+      </c>
       <c r="K383" s="101"/>
-      <c r="L383" s="101"/>
-      <c r="M383" s="101"/>
-      <c r="N383" s="101"/>
+      <c r="L383" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M383" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N383" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O383" s="101"/>
       <c r="P383" s="101"/>
       <c r="Q383" s="101"/>
@@ -20800,19 +20944,39 @@
     </row>
     <row r="384" spans="1:20" ht="18" customHeight="1">
       <c r="A384" s="101"/>
-      <c r="B384" s="101"/>
-      <c r="C384" s="101"/>
-      <c r="D384" s="101"/>
+      <c r="B384" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="C384" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D384" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E384" s="101"/>
-      <c r="F384" s="101"/>
-      <c r="G384" s="101"/>
+      <c r="F384" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="G384" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H384" s="101"/>
-      <c r="I384" s="101"/>
-      <c r="J384" s="101"/>
+      <c r="I384" s="101">
+        <v>298</v>
+      </c>
+      <c r="J384" s="101">
+        <v>311249999.99999899</v>
+      </c>
       <c r="K384" s="101"/>
-      <c r="L384" s="101"/>
-      <c r="M384" s="101"/>
-      <c r="N384" s="101"/>
+      <c r="L384" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M384" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N384" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O384" s="101"/>
       <c r="P384" s="101"/>
       <c r="Q384" s="101"/>
@@ -20822,19 +20986,39 @@
     </row>
     <row r="385" spans="1:20" ht="18" customHeight="1">
       <c r="A385" s="101"/>
-      <c r="B385" s="101"/>
-      <c r="C385" s="101"/>
-      <c r="D385" s="101"/>
+      <c r="B385" s="105" t="s">
+        <v>273</v>
+      </c>
+      <c r="C385" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D385" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E385" s="101"/>
-      <c r="F385" s="101"/>
-      <c r="G385" s="101"/>
+      <c r="F385" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="G385" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H385" s="101"/>
-      <c r="I385" s="101"/>
-      <c r="J385" s="101"/>
+      <c r="I385" s="101">
+        <v>298</v>
+      </c>
+      <c r="J385" s="101">
+        <v>391874999.99999899</v>
+      </c>
       <c r="K385" s="101"/>
-      <c r="L385" s="101"/>
-      <c r="M385" s="101"/>
-      <c r="N385" s="101"/>
+      <c r="L385" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M385" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N385" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O385" s="101"/>
       <c r="P385" s="101"/>
       <c r="Q385" s="101"/>
@@ -20844,19 +21028,39 @@
     </row>
     <row r="386" spans="1:20" ht="18" customHeight="1">
       <c r="A386" s="101"/>
-      <c r="B386" s="101"/>
-      <c r="C386" s="101"/>
-      <c r="D386" s="101"/>
+      <c r="B386" s="105" t="s">
+        <v>274</v>
+      </c>
+      <c r="C386" s="105" t="s">
+        <v>276</v>
+      </c>
+      <c r="D386" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E386" s="101"/>
-      <c r="F386" s="101"/>
-      <c r="G386" s="101"/>
+      <c r="F386" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="G386" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H386" s="101"/>
-      <c r="I386" s="101"/>
-      <c r="J386" s="101"/>
+      <c r="I386" s="101">
+        <v>298</v>
+      </c>
+      <c r="J386" s="101">
+        <v>470625000</v>
+      </c>
       <c r="K386" s="101"/>
-      <c r="L386" s="101"/>
-      <c r="M386" s="101"/>
-      <c r="N386" s="101"/>
+      <c r="L386" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M386" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N386" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O386" s="101"/>
       <c r="P386" s="101"/>
       <c r="Q386" s="101"/>
@@ -20866,19 +21070,39 @@
     </row>
     <row r="387" spans="1:20" ht="18" customHeight="1">
       <c r="A387" s="101"/>
-      <c r="B387" s="101"/>
-      <c r="C387" s="101"/>
-      <c r="D387" s="101"/>
+      <c r="B387" s="105" t="s">
+        <v>275</v>
+      </c>
+      <c r="C387" s="105" t="s">
+        <v>276</v>
+      </c>
+      <c r="D387" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E387" s="101"/>
-      <c r="F387" s="101"/>
-      <c r="G387" s="101"/>
+      <c r="F387" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="G387" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H387" s="101"/>
-      <c r="I387" s="101"/>
-      <c r="J387" s="101"/>
+      <c r="I387" s="101">
+        <v>298</v>
+      </c>
+      <c r="J387" s="101">
+        <v>650625000</v>
+      </c>
       <c r="K387" s="101"/>
-      <c r="L387" s="101"/>
-      <c r="M387" s="101"/>
-      <c r="N387" s="101"/>
+      <c r="L387" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M387" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N387" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O387" s="101"/>
       <c r="P387" s="101"/>
       <c r="Q387" s="101"/>
@@ -20888,19 +21112,39 @@
     </row>
     <row r="388" spans="1:20" ht="18" customHeight="1">
       <c r="A388" s="101"/>
-      <c r="B388" s="101"/>
-      <c r="C388" s="101"/>
-      <c r="D388" s="101"/>
+      <c r="B388" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="C388" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D388" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E388" s="101"/>
-      <c r="F388" s="101"/>
-      <c r="G388" s="101"/>
+      <c r="F388" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="G388" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H388" s="101"/>
-      <c r="I388" s="101"/>
-      <c r="J388" s="101"/>
+      <c r="I388" s="101">
+        <v>298</v>
+      </c>
+      <c r="J388" s="101">
+        <v>52.676767676767597</v>
+      </c>
       <c r="K388" s="101"/>
-      <c r="L388" s="101"/>
-      <c r="M388" s="101"/>
-      <c r="N388" s="101"/>
+      <c r="L388" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M388" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N388" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O388" s="101"/>
       <c r="P388" s="101"/>
       <c r="Q388" s="101"/>
@@ -20910,19 +21154,39 @@
     </row>
     <row r="389" spans="1:20" ht="18" customHeight="1">
       <c r="A389" s="101"/>
-      <c r="B389" s="101"/>
-      <c r="C389" s="101"/>
-      <c r="D389" s="101"/>
+      <c r="B389" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="C389" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D389" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E389" s="101"/>
-      <c r="F389" s="101"/>
-      <c r="G389" s="101"/>
+      <c r="F389" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="G389" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H389" s="101"/>
-      <c r="I389" s="101"/>
-      <c r="J389" s="101"/>
+      <c r="I389" s="101">
+        <v>298</v>
+      </c>
+      <c r="J389" s="101">
+        <v>60.505050505050498</v>
+      </c>
       <c r="K389" s="101"/>
-      <c r="L389" s="101"/>
-      <c r="M389" s="101"/>
-      <c r="N389" s="101"/>
+      <c r="L389" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M389" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N389" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O389" s="101"/>
       <c r="P389" s="101"/>
       <c r="Q389" s="101"/>
@@ -20932,19 +21196,39 @@
     </row>
     <row r="390" spans="1:20" ht="18" customHeight="1">
       <c r="A390" s="101"/>
-      <c r="B390" s="101"/>
-      <c r="C390" s="101"/>
-      <c r="D390" s="101"/>
+      <c r="B390" s="105" t="s">
+        <v>273</v>
+      </c>
+      <c r="C390" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D390" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E390" s="101"/>
-      <c r="F390" s="101"/>
-      <c r="G390" s="101"/>
+      <c r="F390" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="G390" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H390" s="101"/>
-      <c r="I390" s="101"/>
-      <c r="J390" s="101"/>
+      <c r="I390" s="101">
+        <v>298</v>
+      </c>
+      <c r="J390" s="101">
+        <v>47.121212121212103</v>
+      </c>
       <c r="K390" s="101"/>
-      <c r="L390" s="101"/>
-      <c r="M390" s="101"/>
-      <c r="N390" s="101"/>
+      <c r="L390" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M390" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N390" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O390" s="101"/>
       <c r="P390" s="101"/>
       <c r="Q390" s="101"/>
@@ -20954,19 +21238,39 @@
     </row>
     <row r="391" spans="1:20" ht="18" customHeight="1">
       <c r="A391" s="101"/>
-      <c r="B391" s="101"/>
-      <c r="C391" s="101"/>
-      <c r="D391" s="101"/>
+      <c r="B391" s="105" t="s">
+        <v>274</v>
+      </c>
+      <c r="C391" s="105" t="s">
+        <v>276</v>
+      </c>
+      <c r="D391" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E391" s="101"/>
-      <c r="F391" s="101"/>
-      <c r="G391" s="101"/>
+      <c r="F391" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="G391" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H391" s="101"/>
-      <c r="I391" s="101"/>
-      <c r="J391" s="101"/>
+      <c r="I391" s="101">
+        <v>298</v>
+      </c>
+      <c r="J391" s="101">
+        <v>20.101010101010001</v>
+      </c>
       <c r="K391" s="101"/>
-      <c r="L391" s="101"/>
-      <c r="M391" s="101"/>
-      <c r="N391" s="101"/>
+      <c r="L391" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M391" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N391" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O391" s="101"/>
       <c r="P391" s="101"/>
       <c r="Q391" s="101"/>
@@ -20976,19 +21280,39 @@
     </row>
     <row r="392" spans="1:20" ht="18" customHeight="1">
       <c r="A392" s="101"/>
-      <c r="B392" s="101"/>
-      <c r="C392" s="101"/>
-      <c r="D392" s="101"/>
+      <c r="B392" s="105" t="s">
+        <v>275</v>
+      </c>
+      <c r="C392" s="105" t="s">
+        <v>276</v>
+      </c>
+      <c r="D392" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E392" s="101"/>
-      <c r="F392" s="101"/>
-      <c r="G392" s="101"/>
+      <c r="F392" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="G392" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H392" s="101"/>
-      <c r="I392" s="101"/>
-      <c r="J392" s="101"/>
+      <c r="I392" s="101">
+        <v>298</v>
+      </c>
+      <c r="J392" s="101">
+        <v>12.525252525252499</v>
+      </c>
       <c r="K392" s="101"/>
-      <c r="L392" s="101"/>
-      <c r="M392" s="101"/>
-      <c r="N392" s="101"/>
+      <c r="L392" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M392" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="N392" s="105" t="s">
+        <v>278</v>
+      </c>
       <c r="O392" s="101"/>
       <c r="P392" s="101"/>
       <c r="Q392" s="101"/>

</xml_diff>

<commit_message>
- extracted data from `10.1007/s11665-023-08899-x`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348B9FF2-05B4-5548-B15B-48DB23951436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AE79FA-BF36-4C40-A57B-3776DC3376F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="8500" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3552" uniqueCount="288">
   <si>
     <r>
       <rPr>
@@ -967,6 +967,33 @@
   </si>
   <si>
     <t>10.1016/j.matchemphys.2017.08.011</t>
+  </si>
+  <si>
+    <t>Al15Cr15Fe50Ni20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al15Cr15Fe50Ni18B2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al15Cr15Fe50Ni16B4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al15Cr15Fe50Ni15B5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al15Cr15Fe50Ni14B6 </t>
+  </si>
+  <si>
+    <t>Al15Cr15Fe50Ni12B8</t>
+  </si>
+  <si>
+    <t>FCC+BCC+Cr2B</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>10.1007/s11665-023-08899-x</t>
   </si>
 </sst>
 </file>
@@ -3315,8 +3342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A370" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N398" sqref="N398"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A393" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N418" sqref="N418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -21322,21 +21349,44 @@
     </row>
     <row r="393" spans="1:20" ht="18" customHeight="1">
       <c r="A393" s="101"/>
-      <c r="B393" s="101"/>
-      <c r="C393" s="101"/>
-      <c r="D393" s="101"/>
+      <c r="B393" s="105" t="s">
+        <v>279</v>
+      </c>
+      <c r="C393" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D393" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E393" s="101"/>
-      <c r="F393" s="101"/>
-      <c r="G393" s="101"/>
+      <c r="F393" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G393" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H393" s="101"/>
-      <c r="I393" s="101"/>
-      <c r="J393" s="101"/>
+      <c r="I393" s="101">
+        <v>298</v>
+      </c>
+      <c r="J393" s="64">
+        <f t="shared" ref="J393:J398" si="33">P393*9807000</f>
+        <v>4246431000</v>
+      </c>
       <c r="K393" s="101"/>
-      <c r="L393" s="101"/>
-      <c r="M393" s="101"/>
-      <c r="N393" s="101"/>
+      <c r="L393" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M393" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N393" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O393" s="101"/>
-      <c r="P393" s="101"/>
+      <c r="P393" s="101">
+        <v>433</v>
+      </c>
       <c r="Q393" s="101"/>
       <c r="R393" s="101"/>
       <c r="S393" s="102"/>
@@ -21344,21 +21394,44 @@
     </row>
     <row r="394" spans="1:20" ht="18" customHeight="1">
       <c r="A394" s="101"/>
-      <c r="B394" s="101"/>
-      <c r="C394" s="101"/>
-      <c r="D394" s="101"/>
+      <c r="B394" s="105" t="s">
+        <v>280</v>
+      </c>
+      <c r="C394" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D394" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E394" s="101"/>
-      <c r="F394" s="101"/>
-      <c r="G394" s="101"/>
+      <c r="F394" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G394" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H394" s="101"/>
-      <c r="I394" s="101"/>
-      <c r="J394" s="101"/>
+      <c r="I394" s="101">
+        <v>298</v>
+      </c>
+      <c r="J394" s="64">
+        <f t="shared" si="33"/>
+        <v>4756395000</v>
+      </c>
       <c r="K394" s="101"/>
-      <c r="L394" s="101"/>
-      <c r="M394" s="101"/>
-      <c r="N394" s="101"/>
+      <c r="L394" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M394" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N394" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O394" s="101"/>
-      <c r="P394" s="101"/>
+      <c r="P394" s="101">
+        <v>485</v>
+      </c>
       <c r="Q394" s="101"/>
       <c r="R394" s="101"/>
       <c r="S394" s="102"/>
@@ -21366,21 +21439,44 @@
     </row>
     <row r="395" spans="1:20" ht="18" customHeight="1">
       <c r="A395" s="101"/>
-      <c r="B395" s="101"/>
-      <c r="C395" s="101"/>
-      <c r="D395" s="101"/>
+      <c r="B395" s="105" t="s">
+        <v>281</v>
+      </c>
+      <c r="C395" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D395" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E395" s="101"/>
-      <c r="F395" s="101"/>
-      <c r="G395" s="101"/>
+      <c r="F395" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G395" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H395" s="101"/>
-      <c r="I395" s="101"/>
-      <c r="J395" s="101"/>
+      <c r="I395" s="101">
+        <v>298</v>
+      </c>
+      <c r="J395" s="64">
+        <f t="shared" si="33"/>
+        <v>4825044000</v>
+      </c>
       <c r="K395" s="101"/>
-      <c r="L395" s="101"/>
-      <c r="M395" s="101"/>
-      <c r="N395" s="101"/>
+      <c r="L395" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M395" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N395" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O395" s="101"/>
-      <c r="P395" s="101"/>
+      <c r="P395" s="101">
+        <v>492</v>
+      </c>
       <c r="Q395" s="101"/>
       <c r="R395" s="101"/>
       <c r="S395" s="102"/>
@@ -21388,21 +21484,44 @@
     </row>
     <row r="396" spans="1:20" ht="18" customHeight="1">
       <c r="A396" s="101"/>
-      <c r="B396" s="101"/>
-      <c r="C396" s="101"/>
-      <c r="D396" s="101"/>
+      <c r="B396" s="105" t="s">
+        <v>282</v>
+      </c>
+      <c r="C396" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D396" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E396" s="101"/>
-      <c r="F396" s="101"/>
-      <c r="G396" s="101"/>
+      <c r="F396" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G396" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H396" s="101"/>
-      <c r="I396" s="101"/>
-      <c r="J396" s="101"/>
+      <c r="I396" s="101">
+        <v>298</v>
+      </c>
+      <c r="J396" s="64">
+        <f t="shared" si="33"/>
+        <v>5639025000</v>
+      </c>
       <c r="K396" s="101"/>
-      <c r="L396" s="101"/>
-      <c r="M396" s="101"/>
-      <c r="N396" s="101"/>
+      <c r="L396" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M396" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N396" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O396" s="101"/>
-      <c r="P396" s="101"/>
+      <c r="P396" s="101">
+        <v>575</v>
+      </c>
       <c r="Q396" s="101"/>
       <c r="R396" s="101"/>
       <c r="S396" s="102"/>
@@ -21410,21 +21529,44 @@
     </row>
     <row r="397" spans="1:20" ht="18" customHeight="1">
       <c r="A397" s="101"/>
-      <c r="B397" s="101"/>
-      <c r="C397" s="101"/>
-      <c r="D397" s="101"/>
+      <c r="B397" s="105" t="s">
+        <v>283</v>
+      </c>
+      <c r="C397" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D397" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E397" s="101"/>
-      <c r="F397" s="101"/>
-      <c r="G397" s="101"/>
+      <c r="F397" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G397" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H397" s="101"/>
-      <c r="I397" s="101"/>
-      <c r="J397" s="101"/>
+      <c r="I397" s="101">
+        <v>298</v>
+      </c>
+      <c r="J397" s="64">
+        <f t="shared" si="33"/>
+        <v>5266359000</v>
+      </c>
       <c r="K397" s="101"/>
-      <c r="L397" s="101"/>
-      <c r="M397" s="101"/>
-      <c r="N397" s="101"/>
+      <c r="L397" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M397" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N397" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O397" s="101"/>
-      <c r="P397" s="101"/>
+      <c r="P397" s="101">
+        <v>537</v>
+      </c>
       <c r="Q397" s="101"/>
       <c r="R397" s="101"/>
       <c r="S397" s="102"/>
@@ -21432,21 +21574,44 @@
     </row>
     <row r="398" spans="1:20" ht="18" customHeight="1">
       <c r="A398" s="101"/>
-      <c r="B398" s="101"/>
-      <c r="C398" s="101"/>
-      <c r="D398" s="101"/>
+      <c r="B398" s="105" t="s">
+        <v>284</v>
+      </c>
+      <c r="C398" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D398" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E398" s="101"/>
-      <c r="F398" s="101"/>
-      <c r="G398" s="101"/>
+      <c r="F398" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G398" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H398" s="101"/>
-      <c r="I398" s="101"/>
-      <c r="J398" s="101"/>
+      <c r="I398" s="101">
+        <v>298</v>
+      </c>
+      <c r="J398" s="64">
+        <f t="shared" si="33"/>
+        <v>4883886000</v>
+      </c>
       <c r="K398" s="101"/>
-      <c r="L398" s="101"/>
-      <c r="M398" s="101"/>
-      <c r="N398" s="101"/>
+      <c r="L398" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M398" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N398" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O398" s="101"/>
-      <c r="P398" s="101"/>
+      <c r="P398" s="101">
+        <v>498</v>
+      </c>
       <c r="Q398" s="101"/>
       <c r="R398" s="101"/>
       <c r="S398" s="102"/>
@@ -21454,21 +21619,44 @@
     </row>
     <row r="399" spans="1:20" ht="18" customHeight="1">
       <c r="A399" s="101"/>
-      <c r="B399" s="101"/>
-      <c r="C399" s="101"/>
-      <c r="D399" s="101"/>
+      <c r="B399" s="105" t="s">
+        <v>279</v>
+      </c>
+      <c r="C399" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D399" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E399" s="101"/>
-      <c r="F399" s="101"/>
-      <c r="G399" s="101"/>
+      <c r="F399" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G399" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H399" s="101"/>
-      <c r="I399" s="101"/>
-      <c r="J399" s="101"/>
+      <c r="I399" s="101">
+        <v>298</v>
+      </c>
+      <c r="J399" s="101">
+        <f>P399*1000000</f>
+        <v>1096000000</v>
+      </c>
       <c r="K399" s="101"/>
-      <c r="L399" s="101"/>
-      <c r="M399" s="101"/>
-      <c r="N399" s="101"/>
+      <c r="L399" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M399" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N399" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O399" s="101"/>
-      <c r="P399" s="101"/>
+      <c r="P399" s="101">
+        <v>1096</v>
+      </c>
       <c r="Q399" s="101"/>
       <c r="R399" s="101"/>
       <c r="S399" s="102"/>
@@ -21476,21 +21664,44 @@
     </row>
     <row r="400" spans="1:20" ht="18" customHeight="1">
       <c r="A400" s="101"/>
-      <c r="B400" s="101"/>
-      <c r="C400" s="101"/>
-      <c r="D400" s="101"/>
+      <c r="B400" s="105" t="s">
+        <v>280</v>
+      </c>
+      <c r="C400" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D400" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E400" s="101"/>
-      <c r="F400" s="101"/>
-      <c r="G400" s="101"/>
+      <c r="F400" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G400" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H400" s="101"/>
-      <c r="I400" s="101"/>
-      <c r="J400" s="101"/>
+      <c r="I400" s="101">
+        <v>298</v>
+      </c>
+      <c r="J400" s="101">
+        <f t="shared" ref="J400:J408" si="34">P400*1000000</f>
+        <v>1243000000</v>
+      </c>
       <c r="K400" s="101"/>
-      <c r="L400" s="101"/>
-      <c r="M400" s="101"/>
-      <c r="N400" s="101"/>
+      <c r="L400" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M400" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N400" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O400" s="101"/>
-      <c r="P400" s="101"/>
+      <c r="P400" s="101">
+        <v>1243</v>
+      </c>
       <c r="Q400" s="101"/>
       <c r="R400" s="101"/>
       <c r="S400" s="102"/>
@@ -21498,21 +21709,44 @@
     </row>
     <row r="401" spans="1:20" ht="18" customHeight="1">
       <c r="A401" s="101"/>
-      <c r="B401" s="101"/>
-      <c r="C401" s="101"/>
-      <c r="D401" s="101"/>
+      <c r="B401" s="105" t="s">
+        <v>281</v>
+      </c>
+      <c r="C401" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D401" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E401" s="101"/>
-      <c r="F401" s="101"/>
-      <c r="G401" s="101"/>
+      <c r="F401" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G401" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H401" s="101"/>
-      <c r="I401" s="101"/>
-      <c r="J401" s="101"/>
+      <c r="I401" s="101">
+        <v>298</v>
+      </c>
+      <c r="J401" s="101">
+        <f t="shared" si="34"/>
+        <v>1258000000</v>
+      </c>
       <c r="K401" s="101"/>
-      <c r="L401" s="101"/>
-      <c r="M401" s="101"/>
-      <c r="N401" s="101"/>
+      <c r="L401" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M401" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N401" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O401" s="101"/>
-      <c r="P401" s="101"/>
+      <c r="P401" s="101">
+        <v>1258</v>
+      </c>
       <c r="Q401" s="101"/>
       <c r="R401" s="101"/>
       <c r="S401" s="102"/>
@@ -21520,21 +21754,44 @@
     </row>
     <row r="402" spans="1:20" ht="18" customHeight="1">
       <c r="A402" s="101"/>
-      <c r="B402" s="101"/>
-      <c r="C402" s="101"/>
-      <c r="D402" s="101"/>
+      <c r="B402" s="105" t="s">
+        <v>282</v>
+      </c>
+      <c r="C402" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D402" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E402" s="101"/>
-      <c r="F402" s="101"/>
-      <c r="G402" s="101"/>
+      <c r="F402" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G402" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H402" s="101"/>
-      <c r="I402" s="101"/>
-      <c r="J402" s="101"/>
+      <c r="I402" s="101">
+        <v>298</v>
+      </c>
+      <c r="J402" s="101">
+        <f t="shared" si="34"/>
+        <v>1330000000</v>
+      </c>
       <c r="K402" s="101"/>
-      <c r="L402" s="101"/>
-      <c r="M402" s="101"/>
-      <c r="N402" s="101"/>
+      <c r="L402" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M402" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N402" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O402" s="101"/>
-      <c r="P402" s="101"/>
+      <c r="P402" s="101">
+        <v>1330</v>
+      </c>
       <c r="Q402" s="101"/>
       <c r="R402" s="101"/>
       <c r="S402" s="102"/>
@@ -21542,21 +21799,44 @@
     </row>
     <row r="403" spans="1:20" ht="18" customHeight="1">
       <c r="A403" s="101"/>
-      <c r="B403" s="101"/>
-      <c r="C403" s="101"/>
-      <c r="D403" s="101"/>
+      <c r="B403" s="105" t="s">
+        <v>283</v>
+      </c>
+      <c r="C403" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D403" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E403" s="101"/>
-      <c r="F403" s="101"/>
-      <c r="G403" s="101"/>
+      <c r="F403" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G403" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H403" s="101"/>
-      <c r="I403" s="101"/>
-      <c r="J403" s="101"/>
+      <c r="I403" s="101">
+        <v>298</v>
+      </c>
+      <c r="J403" s="101">
+        <f t="shared" si="34"/>
+        <v>1778000000</v>
+      </c>
       <c r="K403" s="101"/>
-      <c r="L403" s="101"/>
-      <c r="M403" s="101"/>
-      <c r="N403" s="101"/>
+      <c r="L403" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M403" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N403" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O403" s="101"/>
-      <c r="P403" s="101"/>
+      <c r="P403" s="101">
+        <v>1778</v>
+      </c>
       <c r="Q403" s="101"/>
       <c r="R403" s="101"/>
       <c r="S403" s="102"/>
@@ -21564,21 +21844,44 @@
     </row>
     <row r="404" spans="1:20" ht="18" customHeight="1">
       <c r="A404" s="101"/>
-      <c r="B404" s="101"/>
-      <c r="C404" s="101"/>
-      <c r="D404" s="101"/>
+      <c r="B404" s="105" t="s">
+        <v>284</v>
+      </c>
+      <c r="C404" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D404" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E404" s="101"/>
-      <c r="F404" s="101"/>
-      <c r="G404" s="101"/>
+      <c r="F404" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G404" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H404" s="101"/>
-      <c r="I404" s="101"/>
-      <c r="J404" s="101"/>
+      <c r="I404" s="101">
+        <v>298</v>
+      </c>
+      <c r="J404" s="101">
+        <f t="shared" si="34"/>
+        <v>1912000000</v>
+      </c>
       <c r="K404" s="101"/>
-      <c r="L404" s="101"/>
-      <c r="M404" s="101"/>
-      <c r="N404" s="101"/>
+      <c r="L404" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M404" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N404" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O404" s="101"/>
-      <c r="P404" s="101"/>
+      <c r="P404" s="101">
+        <v>1912</v>
+      </c>
       <c r="Q404" s="101"/>
       <c r="R404" s="101"/>
       <c r="S404" s="102"/>
@@ -21586,21 +21889,44 @@
     </row>
     <row r="405" spans="1:20" ht="18" customHeight="1">
       <c r="A405" s="101"/>
-      <c r="B405" s="101"/>
-      <c r="C405" s="101"/>
-      <c r="D405" s="101"/>
+      <c r="B405" s="105" t="s">
+        <v>281</v>
+      </c>
+      <c r="C405" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D405" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E405" s="101"/>
-      <c r="F405" s="101"/>
-      <c r="G405" s="101"/>
+      <c r="F405" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="G405" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H405" s="101"/>
-      <c r="I405" s="101"/>
-      <c r="J405" s="101"/>
+      <c r="I405" s="101">
+        <v>298</v>
+      </c>
+      <c r="J405" s="101">
+        <f t="shared" si="34"/>
+        <v>2564000000</v>
+      </c>
       <c r="K405" s="101"/>
-      <c r="L405" s="101"/>
-      <c r="M405" s="101"/>
-      <c r="N405" s="101"/>
+      <c r="L405" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M405" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N405" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O405" s="101"/>
-      <c r="P405" s="101"/>
+      <c r="P405" s="101">
+        <v>2564</v>
+      </c>
       <c r="Q405" s="101"/>
       <c r="R405" s="101"/>
       <c r="S405" s="102"/>
@@ -21608,21 +21934,44 @@
     </row>
     <row r="406" spans="1:20" ht="18" customHeight="1">
       <c r="A406" s="101"/>
-      <c r="B406" s="101"/>
-      <c r="C406" s="101"/>
-      <c r="D406" s="101"/>
+      <c r="B406" s="105" t="s">
+        <v>282</v>
+      </c>
+      <c r="C406" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D406" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E406" s="101"/>
-      <c r="F406" s="101"/>
-      <c r="G406" s="101"/>
+      <c r="F406" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="G406" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H406" s="101"/>
-      <c r="I406" s="101"/>
-      <c r="J406" s="101"/>
+      <c r="I406" s="101">
+        <v>298</v>
+      </c>
+      <c r="J406" s="101">
+        <f t="shared" si="34"/>
+        <v>2595000000</v>
+      </c>
       <c r="K406" s="101"/>
-      <c r="L406" s="101"/>
-      <c r="M406" s="101"/>
-      <c r="N406" s="101"/>
+      <c r="L406" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M406" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N406" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O406" s="101"/>
-      <c r="P406" s="101"/>
+      <c r="P406" s="101">
+        <v>2595</v>
+      </c>
       <c r="Q406" s="101"/>
       <c r="R406" s="101"/>
       <c r="S406" s="102"/>
@@ -21630,21 +21979,44 @@
     </row>
     <row r="407" spans="1:20" ht="18" customHeight="1">
       <c r="A407" s="101"/>
-      <c r="B407" s="101"/>
-      <c r="C407" s="101"/>
-      <c r="D407" s="101"/>
+      <c r="B407" s="105" t="s">
+        <v>283</v>
+      </c>
+      <c r="C407" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D407" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E407" s="101"/>
-      <c r="F407" s="101"/>
-      <c r="G407" s="101"/>
+      <c r="F407" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="G407" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H407" s="101"/>
-      <c r="I407" s="101"/>
-      <c r="J407" s="101"/>
+      <c r="I407" s="101">
+        <v>298</v>
+      </c>
+      <c r="J407" s="101">
+        <f t="shared" si="34"/>
+        <v>2414000000</v>
+      </c>
       <c r="K407" s="101"/>
-      <c r="L407" s="101"/>
-      <c r="M407" s="101"/>
-      <c r="N407" s="101"/>
+      <c r="L407" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M407" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N407" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O407" s="101"/>
-      <c r="P407" s="101"/>
+      <c r="P407" s="101">
+        <v>2414</v>
+      </c>
       <c r="Q407" s="101"/>
       <c r="R407" s="101"/>
       <c r="S407" s="102"/>
@@ -21652,21 +22024,44 @@
     </row>
     <row r="408" spans="1:20" ht="18" customHeight="1">
       <c r="A408" s="101"/>
-      <c r="B408" s="101"/>
-      <c r="C408" s="101"/>
-      <c r="D408" s="101"/>
+      <c r="B408" s="105" t="s">
+        <v>284</v>
+      </c>
+      <c r="C408" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D408" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E408" s="101"/>
-      <c r="F408" s="101"/>
-      <c r="G408" s="101"/>
+      <c r="F408" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="G408" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H408" s="101"/>
-      <c r="I408" s="101"/>
-      <c r="J408" s="101"/>
+      <c r="I408" s="101">
+        <v>298</v>
+      </c>
+      <c r="J408" s="101">
+        <f t="shared" si="34"/>
+        <v>2070000000</v>
+      </c>
       <c r="K408" s="101"/>
-      <c r="L408" s="101"/>
-      <c r="M408" s="101"/>
-      <c r="N408" s="101"/>
+      <c r="L408" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M408" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N408" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O408" s="101"/>
-      <c r="P408" s="101"/>
+      <c r="P408" s="101">
+        <v>2070</v>
+      </c>
       <c r="Q408" s="101"/>
       <c r="R408" s="101"/>
       <c r="S408" s="102"/>
@@ -21674,19 +22069,39 @@
     </row>
     <row r="409" spans="1:20" ht="18" customHeight="1">
       <c r="A409" s="101"/>
-      <c r="B409" s="101"/>
-      <c r="C409" s="101"/>
-      <c r="D409" s="101"/>
+      <c r="B409" s="105" t="s">
+        <v>281</v>
+      </c>
+      <c r="C409" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D409" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E409" s="101"/>
-      <c r="F409" s="101"/>
-      <c r="G409" s="101"/>
+      <c r="F409" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G409" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H409" s="101"/>
-      <c r="I409" s="101"/>
-      <c r="J409" s="101"/>
+      <c r="I409" s="101">
+        <v>298</v>
+      </c>
+      <c r="J409" s="101">
+        <v>42</v>
+      </c>
       <c r="K409" s="101"/>
-      <c r="L409" s="101"/>
-      <c r="M409" s="101"/>
-      <c r="N409" s="101"/>
+      <c r="L409" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M409" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N409" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O409" s="101"/>
       <c r="P409" s="101"/>
       <c r="Q409" s="101"/>
@@ -21696,19 +22111,39 @@
     </row>
     <row r="410" spans="1:20" ht="18" customHeight="1">
       <c r="A410" s="101"/>
-      <c r="B410" s="101"/>
-      <c r="C410" s="101"/>
-      <c r="D410" s="101"/>
+      <c r="B410" s="105" t="s">
+        <v>282</v>
+      </c>
+      <c r="C410" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D410" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E410" s="101"/>
-      <c r="F410" s="101"/>
-      <c r="G410" s="101"/>
+      <c r="F410" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G410" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H410" s="101"/>
-      <c r="I410" s="101"/>
-      <c r="J410" s="101"/>
+      <c r="I410" s="101">
+        <v>298</v>
+      </c>
+      <c r="J410" s="101">
+        <v>31</v>
+      </c>
       <c r="K410" s="101"/>
-      <c r="L410" s="101"/>
-      <c r="M410" s="101"/>
-      <c r="N410" s="101"/>
+      <c r="L410" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M410" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N410" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O410" s="101"/>
       <c r="P410" s="101"/>
       <c r="Q410" s="101"/>
@@ -21718,19 +22153,39 @@
     </row>
     <row r="411" spans="1:20" ht="18" customHeight="1">
       <c r="A411" s="101"/>
-      <c r="B411" s="101"/>
-      <c r="C411" s="101"/>
-      <c r="D411" s="101"/>
+      <c r="B411" s="105" t="s">
+        <v>283</v>
+      </c>
+      <c r="C411" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D411" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E411" s="101"/>
-      <c r="F411" s="101"/>
-      <c r="G411" s="101"/>
+      <c r="F411" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G411" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H411" s="101"/>
-      <c r="I411" s="101"/>
-      <c r="J411" s="101"/>
+      <c r="I411" s="101">
+        <v>298</v>
+      </c>
+      <c r="J411" s="101">
+        <v>23</v>
+      </c>
       <c r="K411" s="101"/>
-      <c r="L411" s="101"/>
-      <c r="M411" s="101"/>
-      <c r="N411" s="101"/>
+      <c r="L411" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M411" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N411" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O411" s="101"/>
       <c r="P411" s="101"/>
       <c r="Q411" s="101"/>
@@ -21740,19 +22195,39 @@
     </row>
     <row r="412" spans="1:20" ht="18" customHeight="1">
       <c r="A412" s="101"/>
-      <c r="B412" s="101"/>
-      <c r="C412" s="101"/>
-      <c r="D412" s="101"/>
+      <c r="B412" s="105" t="s">
+        <v>284</v>
+      </c>
+      <c r="C412" s="105" t="s">
+        <v>285</v>
+      </c>
+      <c r="D412" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E412" s="101"/>
-      <c r="F412" s="101"/>
-      <c r="G412" s="101"/>
+      <c r="F412" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G412" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H412" s="101"/>
-      <c r="I412" s="101"/>
-      <c r="J412" s="101"/>
+      <c r="I412" s="101">
+        <v>298</v>
+      </c>
+      <c r="J412" s="101">
+        <v>16</v>
+      </c>
       <c r="K412" s="101"/>
-      <c r="L412" s="101"/>
-      <c r="M412" s="101"/>
-      <c r="N412" s="101"/>
+      <c r="L412" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M412" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N412" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O412" s="101"/>
       <c r="P412" s="101"/>
       <c r="Q412" s="101"/>
@@ -21762,19 +22237,39 @@
     </row>
     <row r="413" spans="1:20" ht="18" customHeight="1">
       <c r="A413" s="101"/>
-      <c r="B413" s="101"/>
-      <c r="C413" s="101"/>
-      <c r="D413" s="101"/>
+      <c r="B413" s="105" t="s">
+        <v>279</v>
+      </c>
+      <c r="C413" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D413" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E413" s="101"/>
-      <c r="F413" s="101"/>
-      <c r="G413" s="101"/>
+      <c r="F413" s="105" t="s">
+        <v>76</v>
+      </c>
+      <c r="G413" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H413" s="101"/>
-      <c r="I413" s="101"/>
-      <c r="J413" s="101"/>
+      <c r="I413" s="101">
+        <v>298</v>
+      </c>
+      <c r="J413" s="101">
+        <v>80</v>
+      </c>
       <c r="K413" s="101"/>
-      <c r="L413" s="101"/>
-      <c r="M413" s="101"/>
-      <c r="N413" s="101"/>
+      <c r="L413" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M413" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N413" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O413" s="101"/>
       <c r="P413" s="101"/>
       <c r="Q413" s="101"/>
@@ -21784,19 +22279,39 @@
     </row>
     <row r="414" spans="1:20" ht="18" customHeight="1">
       <c r="A414" s="101"/>
-      <c r="B414" s="101"/>
-      <c r="C414" s="101"/>
-      <c r="D414" s="101"/>
+      <c r="B414" s="105" t="s">
+        <v>280</v>
+      </c>
+      <c r="C414" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D414" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="E414" s="101"/>
-      <c r="F414" s="101"/>
-      <c r="G414" s="101"/>
+      <c r="F414" s="105" t="s">
+        <v>76</v>
+      </c>
+      <c r="G414" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H414" s="101"/>
-      <c r="I414" s="101"/>
-      <c r="J414" s="101"/>
+      <c r="I414" s="101">
+        <v>298</v>
+      </c>
+      <c r="J414" s="101">
+        <v>80</v>
+      </c>
       <c r="K414" s="101"/>
-      <c r="L414" s="101"/>
-      <c r="M414" s="101"/>
-      <c r="N414" s="101"/>
+      <c r="L414" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M414" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N414" s="105" t="s">
+        <v>287</v>
+      </c>
       <c r="O414" s="101"/>
       <c r="P414" s="101"/>
       <c r="Q414" s="101"/>
@@ -33026,9 +33541,6 @@
     </row>
     <row r="925" spans="1:20" ht="15" customHeight="1">
       <c r="A925" s="101"/>
-      <c r="B925" s="101"/>
-      <c r="C925" s="101"/>
-      <c r="D925" s="101"/>
       <c r="E925" s="101"/>
       <c r="F925" s="101"/>
       <c r="G925" s="101"/>
@@ -33048,9 +33560,6 @@
     </row>
     <row r="926" spans="1:20" ht="15" customHeight="1">
       <c r="A926" s="101"/>
-      <c r="B926" s="101"/>
-      <c r="C926" s="101"/>
-      <c r="D926" s="101"/>
       <c r="E926" s="101"/>
       <c r="F926" s="101"/>
       <c r="G926" s="101"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.jmst.2020.10.038`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AE79FA-BF36-4C40-A57B-3776DC3376F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A384942-58D3-8C4F-A4A8-EDE30538A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="8500" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3552" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3633" uniqueCount="296">
   <si>
     <r>
       <rPr>
@@ -994,6 +994,30 @@
   </si>
   <si>
     <t>10.1007/s11665-023-08899-x</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmst.2020.10.038</t>
+  </si>
+  <si>
+    <t>Si2 V7 Cr10Mn5Fe46Co30</t>
+  </si>
+  <si>
+    <t>Si4 V5 Cr10Mn5Fe46Co30</t>
+  </si>
+  <si>
+    <t>Si7 V2 Cr10Mn5Fe46Co30</t>
+  </si>
+  <si>
+    <t>VIM+HR+H+CR+A+WQ</t>
+  </si>
+  <si>
+    <t>IM in VIM under Ar and hot rolled at around 1000*C with around 90% reduction then homogenized at 1473K for 2h and cold rolled with over 50% reduction and annealed at 1173K for 15min and water quenched</t>
+  </si>
+  <si>
+    <t>FCC+HCP</t>
+  </si>
+  <si>
+    <t>F5</t>
   </si>
 </sst>
 </file>
@@ -3342,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A393" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N418" sqref="N418"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A399" zoomScale="60" workbookViewId="0">
+      <selection activeCell="J438" sqref="J438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -22321,19 +22345,43 @@
     </row>
     <row r="415" spans="1:20" ht="18" customHeight="1">
       <c r="A415" s="101"/>
-      <c r="B415" s="101"/>
-      <c r="C415" s="101"/>
-      <c r="D415" s="101"/>
-      <c r="E415" s="101"/>
-      <c r="F415" s="101"/>
-      <c r="G415" s="101"/>
+      <c r="B415" s="105" t="s">
+        <v>289</v>
+      </c>
+      <c r="C415" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D415" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E415" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F415" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="G415" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H415" s="101"/>
-      <c r="I415" s="101"/>
-      <c r="J415" s="101"/>
-      <c r="K415" s="101"/>
-      <c r="L415" s="101"/>
-      <c r="M415" s="101"/>
-      <c r="N415" s="101"/>
+      <c r="I415" s="101">
+        <v>298</v>
+      </c>
+      <c r="J415" s="107">
+        <v>435000000</v>
+      </c>
+      <c r="K415" s="107">
+        <v>7000000</v>
+      </c>
+      <c r="L415" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M415" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N415" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O415" s="101"/>
       <c r="P415" s="101"/>
       <c r="Q415" s="101"/>
@@ -22343,19 +22391,43 @@
     </row>
     <row r="416" spans="1:20" ht="18" customHeight="1">
       <c r="A416" s="101"/>
-      <c r="B416" s="101"/>
-      <c r="C416" s="101"/>
-      <c r="D416" s="101"/>
-      <c r="E416" s="101"/>
-      <c r="F416" s="101"/>
-      <c r="G416" s="101"/>
+      <c r="B416" s="105" t="s">
+        <v>290</v>
+      </c>
+      <c r="C416" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D416" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E416" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F416" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="G416" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H416" s="101"/>
-      <c r="I416" s="101"/>
-      <c r="J416" s="101"/>
-      <c r="K416" s="101"/>
-      <c r="L416" s="101"/>
-      <c r="M416" s="101"/>
-      <c r="N416" s="101"/>
+      <c r="I416" s="101">
+        <v>298</v>
+      </c>
+      <c r="J416" s="107">
+        <v>392000000</v>
+      </c>
+      <c r="K416" s="107">
+        <v>4000000</v>
+      </c>
+      <c r="L416" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M416" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N416" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O416" s="101"/>
       <c r="P416" s="101"/>
       <c r="Q416" s="101"/>
@@ -22365,19 +22437,43 @@
     </row>
     <row r="417" spans="1:20" ht="18" customHeight="1">
       <c r="A417" s="101"/>
-      <c r="B417" s="101"/>
-      <c r="C417" s="101"/>
-      <c r="D417" s="101"/>
-      <c r="E417" s="101"/>
-      <c r="F417" s="101"/>
-      <c r="G417" s="101"/>
+      <c r="B417" s="105" t="s">
+        <v>291</v>
+      </c>
+      <c r="C417" s="105" t="s">
+        <v>294</v>
+      </c>
+      <c r="D417" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E417" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F417" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="G417" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H417" s="101"/>
-      <c r="I417" s="101"/>
-      <c r="J417" s="101"/>
-      <c r="K417" s="101"/>
-      <c r="L417" s="101"/>
-      <c r="M417" s="101"/>
-      <c r="N417" s="101"/>
+      <c r="I417" s="101">
+        <v>298</v>
+      </c>
+      <c r="J417" s="107">
+        <v>403000000</v>
+      </c>
+      <c r="K417" s="107">
+        <v>9000000</v>
+      </c>
+      <c r="L417" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M417" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N417" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O417" s="101"/>
       <c r="P417" s="101"/>
       <c r="Q417" s="101"/>
@@ -22387,19 +22483,43 @@
     </row>
     <row r="418" spans="1:20" ht="18" customHeight="1">
       <c r="A418" s="101"/>
-      <c r="B418" s="101"/>
-      <c r="C418" s="101"/>
-      <c r="D418" s="101"/>
-      <c r="E418" s="101"/>
-      <c r="F418" s="101"/>
-      <c r="G418" s="101"/>
+      <c r="B418" s="105" t="s">
+        <v>289</v>
+      </c>
+      <c r="C418" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D418" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E418" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F418" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G418" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H418" s="101"/>
-      <c r="I418" s="101"/>
-      <c r="J418" s="101"/>
-      <c r="K418" s="101"/>
-      <c r="L418" s="101"/>
-      <c r="M418" s="101"/>
-      <c r="N418" s="101"/>
+      <c r="I418" s="101">
+        <v>298</v>
+      </c>
+      <c r="J418" s="107">
+        <v>1085000000</v>
+      </c>
+      <c r="K418" s="107">
+        <v>6000000</v>
+      </c>
+      <c r="L418" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M418" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N418" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O418" s="101"/>
       <c r="P418" s="101"/>
       <c r="Q418" s="101"/>
@@ -22409,19 +22529,43 @@
     </row>
     <row r="419" spans="1:20" ht="18" customHeight="1">
       <c r="A419" s="101"/>
-      <c r="B419" s="101"/>
-      <c r="C419" s="101"/>
-      <c r="D419" s="101"/>
-      <c r="E419" s="101"/>
-      <c r="F419" s="101"/>
-      <c r="G419" s="101"/>
+      <c r="B419" s="105" t="s">
+        <v>290</v>
+      </c>
+      <c r="C419" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D419" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E419" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F419" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G419" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H419" s="101"/>
-      <c r="I419" s="101"/>
-      <c r="J419" s="101"/>
-      <c r="K419" s="101"/>
-      <c r="L419" s="101"/>
-      <c r="M419" s="101"/>
-      <c r="N419" s="101"/>
+      <c r="I419" s="101">
+        <v>298</v>
+      </c>
+      <c r="J419" s="107">
+        <v>962000000</v>
+      </c>
+      <c r="K419" s="107">
+        <v>8000000</v>
+      </c>
+      <c r="L419" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M419" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N419" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O419" s="101"/>
       <c r="P419" s="101"/>
       <c r="Q419" s="101"/>
@@ -22431,19 +22575,43 @@
     </row>
     <row r="420" spans="1:20" ht="18" customHeight="1">
       <c r="A420" s="101"/>
-      <c r="B420" s="101"/>
-      <c r="C420" s="101"/>
-      <c r="D420" s="101"/>
-      <c r="E420" s="101"/>
-      <c r="F420" s="101"/>
-      <c r="G420" s="101"/>
+      <c r="B420" s="105" t="s">
+        <v>291</v>
+      </c>
+      <c r="C420" s="105" t="s">
+        <v>294</v>
+      </c>
+      <c r="D420" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E420" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F420" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="G420" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H420" s="101"/>
-      <c r="I420" s="101"/>
-      <c r="J420" s="101"/>
-      <c r="K420" s="101"/>
-      <c r="L420" s="101"/>
-      <c r="M420" s="101"/>
-      <c r="N420" s="101"/>
+      <c r="I420" s="101">
+        <v>298</v>
+      </c>
+      <c r="J420" s="107">
+        <v>860000000</v>
+      </c>
+      <c r="K420" s="107">
+        <v>2000000</v>
+      </c>
+      <c r="L420" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M420" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N420" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O420" s="101"/>
       <c r="P420" s="101"/>
       <c r="Q420" s="101"/>
@@ -22453,19 +22621,43 @@
     </row>
     <row r="421" spans="1:20" ht="18" customHeight="1">
       <c r="A421" s="101"/>
-      <c r="B421" s="101"/>
-      <c r="C421" s="101"/>
-      <c r="D421" s="101"/>
-      <c r="E421" s="101"/>
-      <c r="F421" s="101"/>
-      <c r="G421" s="101"/>
+      <c r="B421" s="105" t="s">
+        <v>289</v>
+      </c>
+      <c r="C421" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D421" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E421" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F421" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="G421" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H421" s="101"/>
-      <c r="I421" s="101"/>
-      <c r="J421" s="101"/>
-      <c r="K421" s="101"/>
-      <c r="L421" s="101"/>
-      <c r="M421" s="101"/>
-      <c r="N421" s="101"/>
+      <c r="I421" s="101">
+        <v>298</v>
+      </c>
+      <c r="J421" s="101">
+        <v>57.3</v>
+      </c>
+      <c r="K421" s="101">
+        <v>1.6</v>
+      </c>
+      <c r="L421" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M421" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N421" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O421" s="101"/>
       <c r="P421" s="101"/>
       <c r="Q421" s="101"/>
@@ -22475,19 +22667,43 @@
     </row>
     <row r="422" spans="1:20" ht="18" customHeight="1">
       <c r="A422" s="101"/>
-      <c r="B422" s="101"/>
-      <c r="C422" s="101"/>
-      <c r="D422" s="101"/>
-      <c r="E422" s="101"/>
-      <c r="F422" s="101"/>
-      <c r="G422" s="101"/>
+      <c r="B422" s="105" t="s">
+        <v>290</v>
+      </c>
+      <c r="C422" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D422" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E422" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F422" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="G422" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H422" s="101"/>
-      <c r="I422" s="101"/>
-      <c r="J422" s="101"/>
-      <c r="K422" s="101"/>
-      <c r="L422" s="101"/>
-      <c r="M422" s="101"/>
-      <c r="N422" s="101"/>
+      <c r="I422" s="101">
+        <v>298</v>
+      </c>
+      <c r="J422" s="101">
+        <v>54.8</v>
+      </c>
+      <c r="K422" s="101">
+        <v>0.9</v>
+      </c>
+      <c r="L422" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M422" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N422" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O422" s="101"/>
       <c r="P422" s="101"/>
       <c r="Q422" s="101"/>
@@ -22497,19 +22713,43 @@
     </row>
     <row r="423" spans="1:20" ht="15" customHeight="1">
       <c r="A423" s="101"/>
-      <c r="B423" s="101"/>
-      <c r="C423" s="101"/>
-      <c r="D423" s="101"/>
-      <c r="E423" s="101"/>
-      <c r="F423" s="101"/>
-      <c r="G423" s="101"/>
+      <c r="B423" s="105" t="s">
+        <v>291</v>
+      </c>
+      <c r="C423" s="105" t="s">
+        <v>294</v>
+      </c>
+      <c r="D423" s="105" t="s">
+        <v>292</v>
+      </c>
+      <c r="E423" s="105" t="s">
+        <v>293</v>
+      </c>
+      <c r="F423" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="G423" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H423" s="101"/>
-      <c r="I423" s="101"/>
-      <c r="J423" s="101"/>
-      <c r="K423" s="101"/>
-      <c r="L423" s="101"/>
-      <c r="M423" s="101"/>
-      <c r="N423" s="101"/>
+      <c r="I423" s="101">
+        <v>298</v>
+      </c>
+      <c r="J423" s="101">
+        <v>61.8</v>
+      </c>
+      <c r="K423" s="101">
+        <v>0.2</v>
+      </c>
+      <c r="L423" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M423" s="105" t="s">
+        <v>295</v>
+      </c>
+      <c r="N423" s="105" t="s">
+        <v>288</v>
+      </c>
       <c r="O423" s="101"/>
       <c r="P423" s="101"/>
       <c r="Q423" s="101"/>

</xml_diff>

<commit_message>
- extracted data from `10.1016/j.msea.2019.138566`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jan2025.xlsx
+++ b/MiscSmallUploads_Jan2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A384942-58D3-8C4F-A4A8-EDE30538A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE53C19-1531-0647-BB7D-A8C63B5AD1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="8500" windowWidth="34560" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3633" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="311">
   <si>
     <r>
       <rPr>
@@ -1019,6 +1019,51 @@
   <si>
     <t>F5</t>
   </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>CrFeNi</t>
+  </si>
+  <si>
+    <t>CrFeNiAl0.2</t>
+  </si>
+  <si>
+    <t>CrFeNiAl0.4</t>
+  </si>
+  <si>
+    <t>CrFeNiAl0.3Ti0.3</t>
+  </si>
+  <si>
+    <t>CrFeNiAl0.4Ti0.2</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Mal2</t>
+  </si>
+  <si>
+    <t>MAl4</t>
+  </si>
+  <si>
+    <t>Mal3Ti3</t>
+  </si>
+  <si>
+    <t>MAl4Ti2</t>
+  </si>
+  <si>
+    <t>AAM in liqid state for over 1h</t>
+  </si>
+  <si>
+    <t>BCC+B2</t>
+  </si>
+  <si>
+    <t>FCC+BCC+B2</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2019.138566</t>
+  </si>
 </sst>
 </file>
 
@@ -1893,7 +1938,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2204,6 +2249,7 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3366,8 +3412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T926"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A399" zoomScale="60" workbookViewId="0">
-      <selection activeCell="J438" sqref="J438"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A413" zoomScale="60" workbookViewId="0">
+      <selection activeCell="O447" sqref="O447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -22758,130 +22804,314 @@
       <c r="T423" s="102"/>
     </row>
     <row r="424" spans="1:20" ht="15" customHeight="1">
-      <c r="A424" s="101"/>
-      <c r="B424" s="101"/>
-      <c r="C424" s="101"/>
-      <c r="D424" s="101"/>
-      <c r="E424" s="101"/>
-      <c r="F424" s="101"/>
-      <c r="G424" s="101"/>
+      <c r="A424" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="B424" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C424" s="108" t="s">
+        <v>236</v>
+      </c>
+      <c r="D424" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E424" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F424" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G424" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H424" s="101"/>
-      <c r="I424" s="101"/>
-      <c r="J424" s="101"/>
-      <c r="K424" s="101"/>
-      <c r="L424" s="101"/>
-      <c r="M424" s="101"/>
-      <c r="N424" s="101"/>
+      <c r="I424" s="101">
+        <v>298</v>
+      </c>
+      <c r="J424" s="64">
+        <f t="shared" ref="J424:K428" si="35">P424*9807000</f>
+        <v>1833909000</v>
+      </c>
+      <c r="K424" s="64">
+        <f t="shared" si="35"/>
+        <v>39228000</v>
+      </c>
+      <c r="L424" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M424" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N424" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O424" s="101"/>
-      <c r="P424" s="101"/>
-      <c r="Q424" s="101"/>
+      <c r="P424" s="101">
+        <v>187</v>
+      </c>
+      <c r="Q424" s="101">
+        <v>4</v>
+      </c>
       <c r="R424" s="101"/>
       <c r="S424" s="102"/>
       <c r="T424" s="102"/>
     </row>
     <row r="425" spans="1:20" ht="15" customHeight="1">
-      <c r="A425" s="101"/>
-      <c r="B425" s="101"/>
-      <c r="C425" s="101"/>
-      <c r="D425" s="101"/>
-      <c r="E425" s="101"/>
-      <c r="F425" s="101"/>
-      <c r="G425" s="101"/>
+      <c r="A425" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="B425" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C425" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D425" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E425" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F425" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G425" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H425" s="101"/>
-      <c r="I425" s="101"/>
-      <c r="J425" s="101"/>
-      <c r="K425" s="101"/>
-      <c r="L425" s="101"/>
-      <c r="M425" s="101"/>
-      <c r="N425" s="101"/>
+      <c r="I425" s="101">
+        <v>298</v>
+      </c>
+      <c r="J425" s="64">
+        <f t="shared" si="35"/>
+        <v>2118312000</v>
+      </c>
+      <c r="K425" s="64">
+        <f t="shared" si="35"/>
+        <v>88263000</v>
+      </c>
+      <c r="L425" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M425" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N425" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O425" s="101"/>
-      <c r="P425" s="101"/>
-      <c r="Q425" s="101"/>
+      <c r="P425" s="101">
+        <v>216</v>
+      </c>
+      <c r="Q425" s="101">
+        <v>9</v>
+      </c>
       <c r="R425" s="101"/>
       <c r="S425" s="102"/>
       <c r="T425" s="102"/>
     </row>
     <row r="426" spans="1:20" ht="15" customHeight="1">
-      <c r="A426" s="101"/>
-      <c r="B426" s="101"/>
-      <c r="C426" s="101"/>
-      <c r="D426" s="101"/>
-      <c r="E426" s="101"/>
-      <c r="F426" s="101"/>
-      <c r="G426" s="101"/>
+      <c r="A426" s="105" t="s">
+        <v>304</v>
+      </c>
+      <c r="B426" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C426" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D426" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E426" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F426" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G426" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H426" s="101"/>
-      <c r="I426" s="101"/>
-      <c r="J426" s="101"/>
-      <c r="K426" s="101"/>
-      <c r="L426" s="101"/>
-      <c r="M426" s="101"/>
-      <c r="N426" s="101"/>
+      <c r="I426" s="101">
+        <v>298</v>
+      </c>
+      <c r="J426" s="64">
+        <f t="shared" si="35"/>
+        <v>5315394000</v>
+      </c>
+      <c r="K426" s="64">
+        <f t="shared" si="35"/>
+        <v>98070000</v>
+      </c>
+      <c r="L426" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M426" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N426" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O426" s="101"/>
-      <c r="P426" s="101"/>
-      <c r="Q426" s="101"/>
+      <c r="P426" s="101">
+        <v>542</v>
+      </c>
+      <c r="Q426" s="101">
+        <v>10</v>
+      </c>
       <c r="R426" s="101"/>
       <c r="S426" s="102"/>
       <c r="T426" s="102"/>
     </row>
     <row r="427" spans="1:20" ht="15" customHeight="1">
-      <c r="A427" s="101"/>
-      <c r="B427" s="101"/>
-      <c r="C427" s="101"/>
-      <c r="D427" s="101"/>
-      <c r="E427" s="101"/>
-      <c r="F427" s="101"/>
-      <c r="G427" s="101"/>
+      <c r="A427" s="105" t="s">
+        <v>305</v>
+      </c>
+      <c r="B427" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C427" s="105" t="s">
+        <v>309</v>
+      </c>
+      <c r="D427" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E427" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F427" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G427" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H427" s="101"/>
-      <c r="I427" s="101"/>
-      <c r="J427" s="101"/>
-      <c r="K427" s="101"/>
-      <c r="L427" s="101"/>
-      <c r="M427" s="101"/>
-      <c r="N427" s="101"/>
+      <c r="I427" s="101">
+        <v>298</v>
+      </c>
+      <c r="J427" s="64">
+        <f t="shared" si="35"/>
+        <v>5403657000</v>
+      </c>
+      <c r="K427" s="64">
+        <f t="shared" si="35"/>
+        <v>68649000</v>
+      </c>
+      <c r="L427" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M427" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N427" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O427" s="101"/>
-      <c r="P427" s="101"/>
-      <c r="Q427" s="101"/>
+      <c r="P427" s="101">
+        <v>551</v>
+      </c>
+      <c r="Q427" s="101">
+        <v>7</v>
+      </c>
       <c r="R427" s="101"/>
       <c r="S427" s="102"/>
       <c r="T427" s="102"/>
     </row>
     <row r="428" spans="1:20" ht="15" customHeight="1">
-      <c r="A428" s="101"/>
-      <c r="B428" s="101"/>
-      <c r="C428" s="101"/>
-      <c r="D428" s="101"/>
-      <c r="E428" s="101"/>
-      <c r="F428" s="101"/>
-      <c r="G428" s="101"/>
+      <c r="A428" s="105" t="s">
+        <v>306</v>
+      </c>
+      <c r="B428" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C428" s="105" t="s">
+        <v>308</v>
+      </c>
+      <c r="D428" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E428" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F428" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="G428" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H428" s="101"/>
-      <c r="I428" s="101"/>
-      <c r="J428" s="101"/>
-      <c r="K428" s="101"/>
-      <c r="L428" s="101"/>
-      <c r="M428" s="101"/>
-      <c r="N428" s="101"/>
+      <c r="I428" s="101">
+        <v>298</v>
+      </c>
+      <c r="J428" s="64">
+        <f t="shared" si="35"/>
+        <v>5688060000</v>
+      </c>
+      <c r="K428" s="64">
+        <f t="shared" si="35"/>
+        <v>78456000</v>
+      </c>
+      <c r="L428" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M428" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N428" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O428" s="101"/>
-      <c r="P428" s="101"/>
-      <c r="Q428" s="101"/>
+      <c r="P428" s="101">
+        <v>580</v>
+      </c>
+      <c r="Q428" s="101">
+        <v>8</v>
+      </c>
       <c r="R428" s="101"/>
       <c r="S428" s="102"/>
       <c r="T428" s="102"/>
     </row>
     <row r="429" spans="1:20" ht="15" customHeight="1">
-      <c r="A429" s="101"/>
-      <c r="B429" s="101"/>
-      <c r="C429" s="101"/>
-      <c r="D429" s="101"/>
-      <c r="E429" s="101"/>
-      <c r="F429" s="101"/>
-      <c r="G429" s="101"/>
+      <c r="A429" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="B429" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C429" s="108" t="s">
+        <v>236</v>
+      </c>
+      <c r="D429" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E429" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F429" s="105" t="s">
+        <v>64</v>
+      </c>
+      <c r="G429" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H429" s="101"/>
-      <c r="I429" s="101"/>
-      <c r="J429" s="101"/>
+      <c r="I429" s="101">
+        <v>298</v>
+      </c>
+      <c r="J429" s="101">
+        <v>3108614232.2097301</v>
+      </c>
       <c r="K429" s="101"/>
-      <c r="L429" s="101"/>
-      <c r="M429" s="101"/>
-      <c r="N429" s="101"/>
+      <c r="L429" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M429" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="N429" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O429" s="101"/>
       <c r="P429" s="101"/>
       <c r="Q429" s="101"/>
@@ -22890,20 +23120,44 @@
       <c r="T429" s="102"/>
     </row>
     <row r="430" spans="1:20" ht="15" customHeight="1">
-      <c r="A430" s="101"/>
-      <c r="B430" s="101"/>
-      <c r="C430" s="101"/>
-      <c r="D430" s="101"/>
-      <c r="E430" s="101"/>
-      <c r="F430" s="101"/>
-      <c r="G430" s="101"/>
+      <c r="A430" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="B430" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C430" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D430" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E430" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F430" s="105" t="s">
+        <v>64</v>
+      </c>
+      <c r="G430" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H430" s="101"/>
-      <c r="I430" s="101"/>
-      <c r="J430" s="101"/>
+      <c r="I430" s="101">
+        <v>298</v>
+      </c>
+      <c r="J430" s="101">
+        <v>4456928838.9513102</v>
+      </c>
       <c r="K430" s="101"/>
-      <c r="L430" s="101"/>
-      <c r="M430" s="101"/>
-      <c r="N430" s="101"/>
+      <c r="L430" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M430" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="N430" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O430" s="101"/>
       <c r="P430" s="101"/>
       <c r="Q430" s="101"/>
@@ -22912,20 +23166,44 @@
       <c r="T430" s="102"/>
     </row>
     <row r="431" spans="1:20" ht="15" customHeight="1">
-      <c r="A431" s="101"/>
-      <c r="B431" s="101"/>
-      <c r="C431" s="101"/>
-      <c r="D431" s="101"/>
-      <c r="E431" s="101"/>
-      <c r="F431" s="101"/>
-      <c r="G431" s="101"/>
+      <c r="A431" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="B431" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C431" s="108" t="s">
+        <v>236</v>
+      </c>
+      <c r="D431" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E431" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F431" s="105" t="s">
+        <v>192</v>
+      </c>
+      <c r="G431" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H431" s="101"/>
-      <c r="I431" s="101"/>
-      <c r="J431" s="101"/>
+      <c r="I431" s="101">
+        <v>298</v>
+      </c>
+      <c r="J431" s="101">
+        <v>105614973262.032</v>
+      </c>
       <c r="K431" s="101"/>
-      <c r="L431" s="101"/>
-      <c r="M431" s="101"/>
-      <c r="N431" s="101"/>
+      <c r="L431" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M431" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="N431" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O431" s="101"/>
       <c r="P431" s="101"/>
       <c r="Q431" s="101"/>
@@ -22934,20 +23212,44 @@
       <c r="T431" s="102"/>
     </row>
     <row r="432" spans="1:20" ht="15" customHeight="1">
-      <c r="A432" s="101"/>
-      <c r="B432" s="101"/>
-      <c r="C432" s="101"/>
-      <c r="D432" s="101"/>
-      <c r="E432" s="101"/>
-      <c r="F432" s="101"/>
-      <c r="G432" s="101"/>
+      <c r="A432" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="B432" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C432" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D432" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E432" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F432" s="105" t="s">
+        <v>192</v>
+      </c>
+      <c r="G432" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H432" s="101"/>
-      <c r="I432" s="101"/>
-      <c r="J432" s="101"/>
+      <c r="I432" s="101">
+        <v>298</v>
+      </c>
+      <c r="J432" s="101">
+        <v>175133689839.57199</v>
+      </c>
       <c r="K432" s="101"/>
-      <c r="L432" s="101"/>
-      <c r="M432" s="101"/>
-      <c r="N432" s="101"/>
+      <c r="L432" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M432" s="105" t="s">
+        <v>296</v>
+      </c>
+      <c r="N432" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O432" s="101"/>
       <c r="P432" s="101"/>
       <c r="Q432" s="101"/>
@@ -22956,20 +23258,46 @@
       <c r="T432" s="102"/>
     </row>
     <row r="433" spans="1:20" ht="15" customHeight="1">
-      <c r="A433" s="101"/>
-      <c r="B433" s="101"/>
-      <c r="C433" s="101"/>
-      <c r="D433" s="101"/>
-      <c r="E433" s="101"/>
-      <c r="F433" s="101"/>
-      <c r="G433" s="101"/>
+      <c r="A433" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="B433" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C433" s="108" t="s">
+        <v>236</v>
+      </c>
+      <c r="D433" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E433" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F433" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G433" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H433" s="101"/>
-      <c r="I433" s="101"/>
-      <c r="J433" s="101"/>
-      <c r="K433" s="101"/>
-      <c r="L433" s="101"/>
-      <c r="M433" s="101"/>
-      <c r="N433" s="101"/>
+      <c r="I433" s="101">
+        <v>298</v>
+      </c>
+      <c r="J433" s="107">
+        <v>160000000</v>
+      </c>
+      <c r="K433" s="107">
+        <v>5000000</v>
+      </c>
+      <c r="L433" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M433" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N433" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O433" s="101"/>
       <c r="P433" s="101"/>
       <c r="Q433" s="101"/>
@@ -22978,20 +23306,46 @@
       <c r="T433" s="102"/>
     </row>
     <row r="434" spans="1:20" ht="15" customHeight="1">
-      <c r="A434" s="101"/>
-      <c r="B434" s="101"/>
-      <c r="C434" s="101"/>
-      <c r="D434" s="101"/>
-      <c r="E434" s="101"/>
-      <c r="F434" s="101"/>
-      <c r="G434" s="101"/>
+      <c r="A434" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="B434" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C434" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D434" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E434" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F434" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G434" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H434" s="101"/>
-      <c r="I434" s="101"/>
-      <c r="J434" s="101"/>
-      <c r="K434" s="101"/>
-      <c r="L434" s="101"/>
-      <c r="M434" s="101"/>
-      <c r="N434" s="101"/>
+      <c r="I434" s="101">
+        <v>298</v>
+      </c>
+      <c r="J434" s="107">
+        <v>280000000</v>
+      </c>
+      <c r="K434" s="146">
+        <v>7000000</v>
+      </c>
+      <c r="L434" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M434" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N434" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O434" s="101"/>
       <c r="P434" s="101"/>
       <c r="Q434" s="101"/>
@@ -23000,20 +23354,46 @@
       <c r="T434" s="102"/>
     </row>
     <row r="435" spans="1:20" ht="15" customHeight="1">
-      <c r="A435" s="101"/>
-      <c r="B435" s="101"/>
-      <c r="C435" s="101"/>
-      <c r="D435" s="101"/>
-      <c r="E435" s="101"/>
-      <c r="F435" s="101"/>
-      <c r="G435" s="101"/>
+      <c r="A435" s="105" t="s">
+        <v>304</v>
+      </c>
+      <c r="B435" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C435" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D435" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E435" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F435" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G435" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H435" s="101"/>
-      <c r="I435" s="101"/>
-      <c r="J435" s="101"/>
-      <c r="K435" s="101"/>
-      <c r="L435" s="101"/>
-      <c r="M435" s="101"/>
-      <c r="N435" s="101"/>
+      <c r="I435" s="101">
+        <v>298</v>
+      </c>
+      <c r="J435" s="107">
+        <v>1350000000</v>
+      </c>
+      <c r="K435" s="107">
+        <v>9000000</v>
+      </c>
+      <c r="L435" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M435" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N435" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O435" s="101"/>
       <c r="P435" s="101"/>
       <c r="Q435" s="101"/>
@@ -23022,20 +23402,46 @@
       <c r="T435" s="102"/>
     </row>
     <row r="436" spans="1:20" ht="15" customHeight="1">
-      <c r="A436" s="101"/>
-      <c r="B436" s="101"/>
-      <c r="C436" s="101"/>
-      <c r="D436" s="101"/>
-      <c r="E436" s="101"/>
-      <c r="F436" s="101"/>
-      <c r="G436" s="101"/>
+      <c r="A436" s="105" t="s">
+        <v>305</v>
+      </c>
+      <c r="B436" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C436" s="105" t="s">
+        <v>309</v>
+      </c>
+      <c r="D436" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E436" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F436" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G436" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H436" s="101"/>
-      <c r="I436" s="101"/>
-      <c r="J436" s="101"/>
-      <c r="K436" s="101"/>
-      <c r="L436" s="101"/>
-      <c r="M436" s="101"/>
-      <c r="N436" s="101"/>
+      <c r="I436" s="101">
+        <v>298</v>
+      </c>
+      <c r="J436" s="107">
+        <v>1712000000</v>
+      </c>
+      <c r="K436" s="107">
+        <v>8000000</v>
+      </c>
+      <c r="L436" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M436" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N436" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O436" s="101"/>
       <c r="P436" s="101"/>
       <c r="Q436" s="101"/>
@@ -23044,20 +23450,46 @@
       <c r="T436" s="102"/>
     </row>
     <row r="437" spans="1:20" ht="15" customHeight="1">
-      <c r="A437" s="101"/>
-      <c r="B437" s="101"/>
-      <c r="C437" s="101"/>
-      <c r="D437" s="101"/>
-      <c r="E437" s="101"/>
-      <c r="F437" s="101"/>
-      <c r="G437" s="101"/>
+      <c r="A437" s="105" t="s">
+        <v>306</v>
+      </c>
+      <c r="B437" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C437" s="105" t="s">
+        <v>308</v>
+      </c>
+      <c r="D437" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E437" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F437" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G437" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H437" s="101"/>
-      <c r="I437" s="101"/>
-      <c r="J437" s="101"/>
-      <c r="K437" s="101"/>
-      <c r="L437" s="101"/>
-      <c r="M437" s="101"/>
-      <c r="N437" s="101"/>
+      <c r="I437" s="101">
+        <v>298</v>
+      </c>
+      <c r="J437" s="107">
+        <v>1600000000</v>
+      </c>
+      <c r="K437" s="107">
+        <v>6000000</v>
+      </c>
+      <c r="L437" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M437" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N437" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O437" s="101"/>
       <c r="P437" s="101"/>
       <c r="Q437" s="101"/>
@@ -23066,20 +23498,46 @@
       <c r="T437" s="102"/>
     </row>
     <row r="438" spans="1:20" ht="15" customHeight="1">
-      <c r="A438" s="101"/>
-      <c r="B438" s="101"/>
-      <c r="C438" s="101"/>
-      <c r="D438" s="101"/>
-      <c r="E438" s="101"/>
-      <c r="F438" s="101"/>
-      <c r="G438" s="101"/>
+      <c r="A438" s="105" t="s">
+        <v>304</v>
+      </c>
+      <c r="B438" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C438" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D438" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E438" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F438" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="G438" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H438" s="101"/>
-      <c r="I438" s="101"/>
-      <c r="J438" s="101"/>
-      <c r="K438" s="101"/>
-      <c r="L438" s="101"/>
-      <c r="M438" s="101"/>
-      <c r="N438" s="101"/>
+      <c r="I438" s="101">
+        <v>298</v>
+      </c>
+      <c r="J438" s="107">
+        <v>3219000000</v>
+      </c>
+      <c r="K438" s="107">
+        <v>7000000</v>
+      </c>
+      <c r="L438" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M438" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N438" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O438" s="101"/>
       <c r="P438" s="101"/>
       <c r="Q438" s="101"/>
@@ -23088,20 +23546,46 @@
       <c r="T438" s="102"/>
     </row>
     <row r="439" spans="1:20" ht="15" customHeight="1">
-      <c r="A439" s="101"/>
-      <c r="B439" s="101"/>
-      <c r="C439" s="101"/>
-      <c r="D439" s="101"/>
-      <c r="E439" s="101"/>
-      <c r="F439" s="101"/>
-      <c r="G439" s="101"/>
+      <c r="A439" s="105" t="s">
+        <v>305</v>
+      </c>
+      <c r="B439" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C439" s="105" t="s">
+        <v>309</v>
+      </c>
+      <c r="D439" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E439" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F439" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="G439" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H439" s="101"/>
-      <c r="I439" s="101"/>
-      <c r="J439" s="101"/>
-      <c r="K439" s="101"/>
-      <c r="L439" s="101"/>
-      <c r="M439" s="101"/>
-      <c r="N439" s="101"/>
+      <c r="I439" s="101">
+        <v>298</v>
+      </c>
+      <c r="J439" s="107">
+        <v>3700000000</v>
+      </c>
+      <c r="K439" s="107">
+        <v>9000000</v>
+      </c>
+      <c r="L439" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M439" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N439" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O439" s="101"/>
       <c r="P439" s="101"/>
       <c r="Q439" s="101"/>
@@ -23110,20 +23594,46 @@
       <c r="T439" s="102"/>
     </row>
     <row r="440" spans="1:20" ht="15" customHeight="1">
-      <c r="A440" s="101"/>
-      <c r="B440" s="101"/>
-      <c r="C440" s="101"/>
-      <c r="D440" s="101"/>
-      <c r="E440" s="101"/>
-      <c r="F440" s="101"/>
-      <c r="G440" s="101"/>
+      <c r="A440" s="105" t="s">
+        <v>306</v>
+      </c>
+      <c r="B440" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C440" s="105" t="s">
+        <v>308</v>
+      </c>
+      <c r="D440" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E440" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F440" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="G440" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H440" s="101"/>
-      <c r="I440" s="101"/>
-      <c r="J440" s="101"/>
-      <c r="K440" s="101"/>
-      <c r="L440" s="101"/>
-      <c r="M440" s="101"/>
-      <c r="N440" s="101"/>
+      <c r="I440" s="101">
+        <v>298</v>
+      </c>
+      <c r="J440" s="107">
+        <v>3819000000</v>
+      </c>
+      <c r="K440" s="107">
+        <v>6000000</v>
+      </c>
+      <c r="L440" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M440" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N440" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O440" s="101"/>
       <c r="P440" s="101"/>
       <c r="Q440" s="101"/>
@@ -23132,20 +23642,44 @@
       <c r="T440" s="102"/>
     </row>
     <row r="441" spans="1:20" ht="15" customHeight="1">
-      <c r="A441" s="101"/>
-      <c r="B441" s="101"/>
-      <c r="C441" s="101"/>
-      <c r="D441" s="101"/>
-      <c r="E441" s="101"/>
-      <c r="F441" s="101"/>
-      <c r="G441" s="101"/>
+      <c r="A441" s="105" t="s">
+        <v>302</v>
+      </c>
+      <c r="B441" s="105" t="s">
+        <v>297</v>
+      </c>
+      <c r="C441" s="108" t="s">
+        <v>236</v>
+      </c>
+      <c r="D441" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E441" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F441" s="105" t="s">
+        <v>76</v>
+      </c>
+      <c r="G441" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H441" s="101"/>
-      <c r="I441" s="101"/>
-      <c r="J441" s="101"/>
+      <c r="I441" s="101">
+        <v>298</v>
+      </c>
+      <c r="J441" s="101">
+        <v>50</v>
+      </c>
       <c r="K441" s="101"/>
-      <c r="L441" s="101"/>
-      <c r="M441" s="101"/>
-      <c r="N441" s="101"/>
+      <c r="L441" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M441" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N441" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O441" s="101"/>
       <c r="P441" s="101"/>
       <c r="Q441" s="101"/>
@@ -23154,20 +23688,44 @@
       <c r="T441" s="102"/>
     </row>
     <row r="442" spans="1:20" ht="15" customHeight="1">
-      <c r="A442" s="101"/>
-      <c r="B442" s="101"/>
-      <c r="C442" s="101"/>
-      <c r="D442" s="101"/>
-      <c r="E442" s="101"/>
-      <c r="F442" s="101"/>
-      <c r="G442" s="101"/>
+      <c r="A442" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="B442" s="105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C442" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="D442" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E442" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F442" s="105" t="s">
+        <v>76</v>
+      </c>
+      <c r="G442" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H442" s="101"/>
-      <c r="I442" s="101"/>
-      <c r="J442" s="101"/>
+      <c r="I442" s="101">
+        <v>298</v>
+      </c>
+      <c r="J442" s="101">
+        <v>50</v>
+      </c>
       <c r="K442" s="101"/>
-      <c r="L442" s="101"/>
-      <c r="M442" s="101"/>
-      <c r="N442" s="101"/>
+      <c r="L442" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M442" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N442" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O442" s="101"/>
       <c r="P442" s="101"/>
       <c r="Q442" s="101"/>
@@ -23176,20 +23734,46 @@
       <c r="T442" s="102"/>
     </row>
     <row r="443" spans="1:20" ht="15" customHeight="1">
-      <c r="A443" s="101"/>
-      <c r="B443" s="101"/>
-      <c r="C443" s="101"/>
-      <c r="D443" s="101"/>
-      <c r="E443" s="101"/>
-      <c r="F443" s="101"/>
-      <c r="G443" s="101"/>
+      <c r="A443" s="105" t="s">
+        <v>304</v>
+      </c>
+      <c r="B443" s="105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C443" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="D443" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E443" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F443" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G443" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H443" s="101"/>
-      <c r="I443" s="101"/>
-      <c r="J443" s="101"/>
-      <c r="K443" s="101"/>
-      <c r="L443" s="101"/>
-      <c r="M443" s="101"/>
-      <c r="N443" s="101"/>
+      <c r="I443" s="101">
+        <v>298</v>
+      </c>
+      <c r="J443" s="101">
+        <v>37</v>
+      </c>
+      <c r="K443" s="101">
+        <v>0.5</v>
+      </c>
+      <c r="L443" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M443" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N443" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O443" s="101"/>
       <c r="P443" s="101"/>
       <c r="Q443" s="101"/>
@@ -23198,20 +23782,46 @@
       <c r="T443" s="102"/>
     </row>
     <row r="444" spans="1:20" ht="15" customHeight="1">
-      <c r="A444" s="101"/>
-      <c r="B444" s="101"/>
-      <c r="C444" s="101"/>
-      <c r="D444" s="101"/>
-      <c r="E444" s="101"/>
-      <c r="F444" s="101"/>
-      <c r="G444" s="101"/>
+      <c r="A444" s="105" t="s">
+        <v>305</v>
+      </c>
+      <c r="B444" s="105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C444" s="105" t="s">
+        <v>309</v>
+      </c>
+      <c r="D444" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E444" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F444" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G444" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H444" s="101"/>
-      <c r="I444" s="101"/>
-      <c r="J444" s="101"/>
-      <c r="K444" s="101"/>
-      <c r="L444" s="101"/>
-      <c r="M444" s="101"/>
-      <c r="N444" s="101"/>
+      <c r="I444" s="101">
+        <v>298</v>
+      </c>
+      <c r="J444" s="101">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="K444" s="101">
+        <v>0.6</v>
+      </c>
+      <c r="L444" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M444" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N444" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O444" s="101"/>
       <c r="P444" s="101"/>
       <c r="Q444" s="101"/>
@@ -23220,20 +23830,46 @@
       <c r="T444" s="102"/>
     </row>
     <row r="445" spans="1:20" ht="15" customHeight="1">
-      <c r="A445" s="101"/>
-      <c r="B445" s="101"/>
-      <c r="C445" s="101"/>
-      <c r="D445" s="101"/>
-      <c r="E445" s="101"/>
-      <c r="F445" s="101"/>
-      <c r="G445" s="101"/>
+      <c r="A445" s="105" t="s">
+        <v>306</v>
+      </c>
+      <c r="B445" s="105" t="s">
+        <v>301</v>
+      </c>
+      <c r="C445" s="105" t="s">
+        <v>308</v>
+      </c>
+      <c r="D445" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E445" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="F445" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G445" s="105" t="s">
+        <v>29</v>
+      </c>
       <c r="H445" s="101"/>
-      <c r="I445" s="101"/>
-      <c r="J445" s="101"/>
-      <c r="K445" s="101"/>
-      <c r="L445" s="101"/>
-      <c r="M445" s="101"/>
-      <c r="N445" s="101"/>
+      <c r="I445" s="101">
+        <v>298</v>
+      </c>
+      <c r="J445" s="101">
+        <v>45</v>
+      </c>
+      <c r="K445" s="101">
+        <v>0.9</v>
+      </c>
+      <c r="L445" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="M445" s="105" t="s">
+        <v>286</v>
+      </c>
+      <c r="N445" s="105" t="s">
+        <v>310</v>
+      </c>
       <c r="O445" s="101"/>
       <c r="P445" s="101"/>
       <c r="Q445" s="101"/>

</xml_diff>